<commit_message>
Added input/output requirements for Budgeting and Target Settings.
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="577">
   <si>
     <t>Term</t>
   </si>
@@ -1553,15 +1553,24 @@
     <t>System will calculate provision for total purcahse cost for specific period (default is 12 months). Merchant can override it for value (i.e. total provision – e.g. 5 lakh instead of 3 lakhs recommended by system), or period (e.g. 6 montsh instead of 12 months recommended by system).</t>
   </si>
   <si>
+    <t>To be done (new batch will be written)</t>
+  </si>
+  <si>
     <t>System will calculate provision for fixed operating expenses (i.e. common operarting expenses) for specific period (default is 12 months). Merchant can override it for value (i.e. total provision – e.g. 5 lakh instead of 3 lakhs recommended by system), or period (e.g. 6 montsh instead of 12 months recommended by system).</t>
   </si>
   <si>
     <t>System will calculate provision for variable operating expenses (i.e. subscription specific operarting expenses) for specific period (default is 12 months). Merchant can override it for value (i.e. total provision – e.g. 5 lakh instead of 3 lakhs recommended by system), or period (e.g. 6 montsh instead of 12 months recommended by system).</t>
   </si>
   <si>
+    <t>Will be provided by integration domain (OperatingExpenseReceivedEvent)</t>
+  </si>
+  <si>
     <t>Merchant will make provision for losses.</t>
   </si>
   <si>
+    <t>To be done (from admin console – will come via REST controller)</t>
+  </si>
+  <si>
     <t>Merchant will make provision for benefits.</t>
   </si>
   <si>
@@ -1574,19 +1583,31 @@
     <t>When system receives incoming inventory details from main application, their total purchase cost is debited under 'purchase cost' and respective provision account.</t>
   </si>
   <si>
+    <t>ProductStatusReceivedEvent from integration domain (to be revisit)</t>
+  </si>
+  <si>
     <t>When system receives incoming operating expenses details from main application, they are debited under respective expense categories and respective provision account.</t>
   </si>
   <si>
     <t>When system receives common taxes paid from main application, their total taxes paid is debited under 'taxes cost' and respective provision account.</t>
   </si>
   <si>
+    <t>Will be provided by integration domain (to be done)</t>
+  </si>
+  <si>
     <t>When a product exceeds its revenue beyond its forecast by x% then additional amount will be credited to nodal account.</t>
   </si>
   <si>
+    <t>Will be calculated in business account domain for each event</t>
+  </si>
+  <si>
     <t>When a product's revenue falls behind its forecast by x% then difference  amount will be debited from nodal account and respective provision account.</t>
   </si>
   <si>
-    <t>When a subscriber does subscription, but has not yet made payment yet, his total subscription value is credited to provisional revenue.</t>
+    <t>When a subscriber does subscription, but has not yet made payment, his total subscription value is credited to provisional revenue.</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedEvent from subscriber domain</t>
   </si>
   <si>
     <t>When a subscriber does subscription and has made partial/full advanced payment, then the payment amount is credited to booking amount.</t>
@@ -1595,25 +1616,67 @@
     <t>When a delivery is made to subscriber(s),  the delivery amount should be debited from provisional revenue and respective provision account.</t>
   </si>
   <si>
+    <t>BasketDeliveryStatusEvent from subscriber domain</t>
+  </si>
+  <si>
     <t>When a delivery is made to subscriber(s), its revenue is credited under “revenue” subject to receipt of payment. In case some of advanced payment made by subscriber still exists under booking amount, the delivery amount should be debited from booking amount and respective provision account.</t>
   </si>
   <si>
     <t>When interest is gained on booking amount, it will be credited to “interests”.</t>
   </si>
   <si>
+    <t>To be done (via integration domain)</t>
+  </si>
+  <si>
     <t>Debit delivery expense from subscription specific expenses upon successful delivery. Also debit from respective provision account.</t>
   </si>
   <si>
-    <t>Debit fixed operating expense when the same are received from main application. Also debit from respective provision account.</t>
-  </si>
-  <si>
     <t>Debit benefits when subscriber(s) get specific benefit. Also debit from respective provision account.</t>
   </si>
   <si>
     <t>Upon every debit, if balance in respective provision account is approaching to zero, then notification should be sent to merchant to make additional provisions.</t>
   </si>
   <si>
+    <t>Output will be ProvisionNotSufficientNotificationEvent (to be done)</t>
+  </si>
+  <si>
     <t>When the subscription forecast as well as expense forecast is adjusted by the forecast correction job, it should also correct the provisions required under each category and send it to merchant for approval. Once it is approved by merchant, the provisions elements will be credited under respective provisions.</t>
+  </si>
+  <si>
+    <t>When an item is cancelled or replaced from subscription, appropriate item cancellation event should be fired from subscriber domain and they should debit provisional revenue.</t>
+  </si>
+  <si>
+    <t>BasketDeletedEvent and DeliveryCreatedEvent in subscriber domain</t>
+  </si>
+  <si>
+    <t>When an item is replaced or added to current subscription, appropriate item addition event should be fired from subscriber domain and they should credit provisional revenue.</t>
+  </si>
+  <si>
+    <t>When subscriber cancells subscription, appropriate subscription cancelled event should be fired from subscriber domain and they should debit the total sum amount of remaining subscription amount from provisional revenue.</t>
+  </si>
+  <si>
+    <t>Multiple instances of BasketDeletedEvent from subscriber domain</t>
+  </si>
+  <si>
+    <t>When a refund is made to a subscriber subject to cancellation of subscription, appropriate amount is debited from booking amount.</t>
+  </si>
+  <si>
+    <t>To be done (from subscriber domain)</t>
+  </si>
+  <si>
+    <t>When an new subscription is made, any benefits other than product level discount made to the customer are debited from provision for benefits.</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedEvent from subscriber domain (to be done)</t>
+  </si>
+  <si>
+    <t>When an item is cancelled from subscription, the difference of previous benefit offered and newly calculated benefit will be credited to provision for benefits.</t>
+  </si>
+  <si>
+    <t>When a subscription is cancelled from subscription, the difference of previous benefit offered and newly calculated benefit will be credited to provision for benefits.</t>
+  </si>
+  <si>
+    <t>BasketDeletedEvent in subscriber domain</t>
   </si>
   <si>
     <t>Subscriber fills registration form to register on subscription website.</t>
@@ -1870,16 +1933,16 @@
     <t>Debit from revenue account in case of cancelation of Subscription</t>
   </si>
   <si>
-    <t>Credit delivery expense to subscription specific operating expense on successful delivery. </t>
-  </si>
-  <si>
-    <t>Debit delivery expense from provisional subscription specific operating expense on successful delivery. </t>
-  </si>
-  <si>
-    <t>Credit Fixed expenses to Fixed operating expense when received from site. </t>
-  </si>
-  <si>
-    <t>Debit Fixed expenses from Fixed operating expense when received from site. </t>
+    <t>Credit delivery expense to subscription specific operating expense on successful delivery.</t>
+  </si>
+  <si>
+    <t>Debit delivery expense from provisional subscription specific operating expense on successful delivery.</t>
+  </si>
+  <si>
+    <t>Credit Fixed expenses to Fixed operating expense when received from site.</t>
+  </si>
+  <si>
+    <t>Debit Fixed expenses from Fixed operating expense when received from site.</t>
   </si>
   <si>
     <t>Debit from provision of basket level benefit when subscriber get basket level benefits.</t>
@@ -1889,6 +1952,9 @@
   </si>
   <si>
     <t>Credit to benefit's provisions when subscriber cancels the subscription.</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t>Provision for losses would be used as a last resort (i.e. losses occurred and no money for provision)</t>
@@ -1901,7 +1967,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1973,6 +2039,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1996,7 +2069,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -2054,7 +2127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2235,6 +2308,18 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2266,7 +2351,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -2438,61 +2523,61 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
-        <v>524</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>525</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>526</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>527</v>
+      <c r="A1" s="48" t="s">
+        <v>545</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>547</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>528</v>
+        <v>549</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>222</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>529</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>530</v>
+        <v>551</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>222</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>531</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>532</v>
+        <v>553</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>222</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>533</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>534</v>
+        <v>555</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>222</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>535</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -2547,7 +2632,7 @@
       <c r="E2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="46"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="28" t="s">
         <v>20</v>
       </c>
@@ -2574,664 +2659,666 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="s">
-        <v>536</v>
-      </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
-        <v>537</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
+      <c r="A3" s="49" t="s">
+        <v>557</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49" t="s">
+        <v>558</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46" t="s">
-        <v>538</v>
-      </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49" t="s">
+        <v>559</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46" t="s">
-        <v>539</v>
-      </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49" t="s">
+        <v>560</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46" t="s">
-        <v>540</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49" t="s">
+        <v>561</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46" t="s">
-        <v>541</v>
-      </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49" t="s">
+        <v>562</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46" t="s">
-        <v>542</v>
-      </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49" t="s">
+        <v>563</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46" t="s">
-        <v>543</v>
-      </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49" t="s">
+        <v>564</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46" t="s">
-        <v>544</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49" t="s">
+        <v>565</v>
+      </c>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
     </row>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46" t="s">
-        <v>545</v>
-      </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49" t="s">
+        <v>566</v>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46" t="s">
-        <v>546</v>
-      </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49" t="s">
+        <v>567</v>
+      </c>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46" t="s">
-        <v>547</v>
-      </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49" t="s">
+        <v>568</v>
+      </c>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
     </row>
     <row r="19" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46" t="s">
-        <v>548</v>
-      </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49" t="s">
+        <v>569</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
     </row>
     <row r="21" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46" t="s">
-        <v>549</v>
-      </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49" t="s">
+        <v>570</v>
+      </c>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46" t="s">
-        <v>550</v>
-      </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49" t="s">
+        <v>571</v>
+      </c>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
     </row>
     <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46" t="s">
-        <v>551</v>
-      </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49" t="s">
+        <v>572</v>
+      </c>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
     </row>
     <row r="25" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46" t="s">
-        <v>552</v>
-      </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49" t="s">
+        <v>573</v>
+      </c>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46" t="s">
-        <v>553</v>
-      </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
+    <row r="26" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49" t="s">
+        <v>574</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>575</v>
+      </c>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="46"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="46"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="46"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="46"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="46"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="50"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="46"/>
-      <c r="B36" s="46"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="46"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="47"/>
-      <c r="N37" s="47"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="46"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
-      <c r="N38" s="47"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="46"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="47"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="46"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="47"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="50"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3264,7 +3351,7 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="28.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="26" t="s">
-        <v>554</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -33273,10 +33360,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33473,502 +33560,643 @@
         <v>444</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="55.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="55.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="40"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>445</v>
       </c>
       <c r="C11" s="40" t="s">
         <v>446</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="40" t="s">
+        <v>447</v>
+      </c>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
       <c r="G11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="40"/>
-      <c r="B12" s="44"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="40" t="s">
+        <v>448</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>447</v>
       </c>
-      <c r="D12" s="40"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="40"/>
-      <c r="B13" s="44"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="40" t="s">
-        <v>448</v>
-      </c>
-      <c r="D13" s="40"/>
+        <v>449</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>450</v>
+      </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="40"/>
-      <c r="B14" s="44"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="40" t="s">
-        <v>449</v>
-      </c>
-      <c r="D14" s="40"/>
+        <v>451</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>452</v>
+      </c>
       <c r="E14" s="40"/>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
     </row>
-    <row r="15" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="40"/>
-      <c r="B15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="40" t="s">
-        <v>450</v>
-      </c>
-      <c r="D15" s="40"/>
+        <v>453</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>452</v>
+      </c>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
       <c r="G15" s="40"/>
     </row>
-    <row r="16" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40"/>
-      <c r="B16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="40" t="s">
-        <v>451</v>
-      </c>
-      <c r="D16" s="40"/>
+        <v>454</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>452</v>
+      </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
       <c r="G16" s="40"/>
     </row>
-    <row r="17" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40"/>
-      <c r="B17" s="44"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="40" t="s">
+        <v>455</v>
+      </c>
+      <c r="D17" s="40" t="s">
         <v>452</v>
       </c>
-      <c r="D17" s="40"/>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
       <c r="G17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40"/>
-      <c r="B18" s="44"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="40" t="s">
-        <v>453</v>
-      </c>
-      <c r="D18" s="40"/>
+        <v>456</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>457</v>
+      </c>
       <c r="E18" s="40"/>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40"/>
-      <c r="B19" s="44"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="40" t="s">
-        <v>454</v>
-      </c>
-      <c r="D19" s="40"/>
+        <v>458</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>450</v>
+      </c>
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40"/>
-      <c r="B20" s="44"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="40" t="s">
-        <v>455</v>
-      </c>
-      <c r="D20" s="40"/>
+        <v>459</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>460</v>
+      </c>
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
       <c r="G20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40"/>
-      <c r="B21" s="44"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="40" t="s">
-        <v>456</v>
-      </c>
-      <c r="D21" s="40"/>
+        <v>461</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>462</v>
+      </c>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="40"/>
-      <c r="B22" s="44"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="40" t="s">
-        <v>457</v>
-      </c>
-      <c r="D22" s="40"/>
+        <v>463</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>462</v>
+      </c>
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
       <c r="G22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40"/>
-      <c r="B23" s="44"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="40" t="s">
-        <v>458</v>
-      </c>
-      <c r="D23" s="40"/>
+        <v>464</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>465</v>
+      </c>
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
       <c r="G23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40"/>
-      <c r="B24" s="44"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="40" t="s">
-        <v>459</v>
-      </c>
-      <c r="D24" s="40"/>
+        <v>466</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>465</v>
+      </c>
       <c r="E24" s="40"/>
       <c r="F24" s="40"/>
       <c r="G24" s="40"/>
     </row>
     <row r="25" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40"/>
-      <c r="B25" s="44"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="40" t="s">
-        <v>460</v>
-      </c>
-      <c r="D25" s="40"/>
+        <v>467</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>468</v>
+      </c>
       <c r="E25" s="40"/>
       <c r="F25" s="40"/>
       <c r="G25" s="40"/>
     </row>
     <row r="26" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40"/>
-      <c r="B26" s="44"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="40" t="s">
-        <v>461</v>
-      </c>
-      <c r="D26" s="40"/>
+        <v>469</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>468</v>
+      </c>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
       <c r="G26" s="40"/>
     </row>
     <row r="27" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40"/>
-      <c r="B27" s="44"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="40" t="s">
-        <v>462</v>
-      </c>
-      <c r="D27" s="40"/>
+        <v>470</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>471</v>
+      </c>
       <c r="E27" s="40"/>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
     </row>
     <row r="28" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40"/>
-      <c r="B28" s="44"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="40" t="s">
-        <v>463</v>
-      </c>
-      <c r="D28" s="40"/>
+        <v>472</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>468</v>
+      </c>
       <c r="E28" s="40"/>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
     </row>
     <row r="29" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40"/>
-      <c r="B29" s="44"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="40" t="s">
-        <v>464</v>
-      </c>
-      <c r="D29" s="40"/>
+        <v>473</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>465</v>
+      </c>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
     </row>
-    <row r="30" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40"/>
-      <c r="B30" s="44"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="40" t="s">
-        <v>465</v>
-      </c>
-      <c r="D30" s="40"/>
+        <v>474</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>475</v>
+      </c>
       <c r="E30" s="40"/>
       <c r="F30" s="40"/>
       <c r="G30" s="40"/>
     </row>
-    <row r="31" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40"/>
-      <c r="B31" s="44"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="40" t="s">
-        <v>466</v>
-      </c>
-      <c r="D31" s="40"/>
+        <v>476</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>447</v>
+      </c>
       <c r="E31" s="40"/>
       <c r="F31" s="40"/>
       <c r="G31" s="40"/>
     </row>
-    <row r="32" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="40"/>
-      <c r="B32" s="44"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="40" t="s">
-        <v>467</v>
-      </c>
-      <c r="D32" s="40"/>
+        <v>477</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>478</v>
+      </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
       <c r="G32" s="40"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="40"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="40" t="s">
+        <v>479</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>478</v>
+      </c>
       <c r="E33" s="40"/>
       <c r="F33" s="40"/>
       <c r="G33" s="40"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="55.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="40" t="s">
+        <v>480</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>481</v>
+      </c>
       <c r="E34" s="40"/>
       <c r="F34" s="40"/>
       <c r="G34" s="40"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="40"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="40" t="s">
+        <v>482</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>483</v>
+      </c>
       <c r="E35" s="40"/>
       <c r="F35" s="40"/>
       <c r="G35" s="40"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="28.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="40"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="40" t="s">
+        <v>484</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>485</v>
+      </c>
       <c r="E36" s="40"/>
       <c r="F36" s="40"/>
       <c r="G36" s="40"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="40"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="40" t="s">
+        <v>486</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>478</v>
+      </c>
       <c r="E37" s="40"/>
       <c r="F37" s="40"/>
       <c r="G37" s="40"/>
     </row>
     <row r="38" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="40" t="n">
-        <v>2</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>44</v>
-      </c>
+      <c r="A38" s="40"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="40" t="s">
-        <v>468</v>
+        <v>487</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>469</v>
-      </c>
-      <c r="E38" s="40" t="s">
-        <v>470</v>
-      </c>
-      <c r="F38" s="40" t="s">
-        <v>471</v>
-      </c>
+        <v>488</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
       <c r="G38" s="40"/>
     </row>
-    <row r="39" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="40"/>
-      <c r="B39" s="40" t="s">
-        <v>472</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>473</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>474</v>
-      </c>
-      <c r="E39" s="40" t="s">
-        <v>475</v>
-      </c>
+      <c r="B39" s="44"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
       <c r="F39" s="40"/>
       <c r="G39" s="40"/>
     </row>
-    <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="40"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40" t="s">
-        <v>476</v>
-      </c>
-      <c r="D40" s="40" t="s">
-        <v>477</v>
-      </c>
-      <c r="E40" s="40" t="s">
-        <v>478</v>
-      </c>
+      <c r="B40" s="44"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
       <c r="F40" s="40"/>
       <c r="G40" s="40"/>
     </row>
-    <row r="41" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="40"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40" t="s">
-        <v>479</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>480</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>481</v>
-      </c>
+      <c r="B41" s="44"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
       <c r="F41" s="40"/>
       <c r="G41" s="40"/>
     </row>
-    <row r="42" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40" t="s">
-        <v>482</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>483</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>484</v>
-      </c>
+      <c r="B42" s="44"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
       <c r="F42" s="40"/>
       <c r="G42" s="40"/>
     </row>
-    <row r="43" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>486</v>
-      </c>
-      <c r="E43" s="40" t="s">
-        <v>487</v>
-      </c>
+      <c r="B43" s="44"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="40"/>
       <c r="G43" s="40"/>
     </row>
-    <row r="44" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40" t="s">
-        <v>488</v>
-      </c>
-      <c r="D44" s="40" t="s">
-        <v>489</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>490</v>
-      </c>
+      <c r="B44" s="44"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
       <c r="F44" s="40"/>
       <c r="G44" s="40"/>
     </row>
-    <row r="45" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>491</v>
-      </c>
-      <c r="E45" s="40" t="s">
-        <v>492</v>
-      </c>
+      <c r="B45" s="44"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
       <c r="F45" s="40"/>
       <c r="G45" s="40"/>
     </row>
-    <row r="46" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="40"/>
+    <row r="46" customFormat="false" ht="42.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="40" t="n">
+        <v>2</v>
+      </c>
       <c r="B46" s="40" t="s">
-        <v>493</v>
+        <v>44</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E46" s="40" t="s">
-        <v>496</v>
-      </c>
-      <c r="F46" s="40"/>
+        <v>491</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>492</v>
+      </c>
       <c r="G46" s="40"/>
     </row>
-    <row r="47" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="40"/>
       <c r="B47" s="40" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="E47" s="40" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F47" s="40"/>
       <c r="G47" s="40"/>
     </row>
-    <row r="48" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="40"/>
-      <c r="B48" s="40" t="s">
-        <v>501</v>
-      </c>
+      <c r="B48" s="40"/>
       <c r="C48" s="40" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F48" s="40"/>
       <c r="G48" s="40"/>
     </row>
-    <row r="49" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="40"/>
       <c r="B49" s="40"/>
       <c r="C49" s="40" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E49" s="40" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F49" s="40"/>
       <c r="G49" s="40"/>
     </row>
-    <row r="50" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="40"/>
-      <c r="B50" s="40" t="s">
-        <v>508</v>
-      </c>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40" t="s">
+        <v>503</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>504</v>
+      </c>
+      <c r="E50" s="40" t="s">
+        <v>505</v>
+      </c>
       <c r="F50" s="40"/>
       <c r="G50" s="40"/>
     </row>
+    <row r="51" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40" t="s">
+        <v>506</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>507</v>
+      </c>
+      <c r="E51" s="40" t="s">
+        <v>508</v>
+      </c>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+    </row>
+    <row r="52" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40" t="s">
+        <v>509</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>510</v>
+      </c>
+      <c r="E52" s="40" t="s">
+        <v>511</v>
+      </c>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+    </row>
+    <row r="53" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>512</v>
+      </c>
+      <c r="E53" s="40" t="s">
+        <v>513</v>
+      </c>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+    </row>
+    <row r="54" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="40"/>
+      <c r="B54" s="40" t="s">
+        <v>514</v>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>515</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>516</v>
+      </c>
+      <c r="E54" s="40" t="s">
+        <v>517</v>
+      </c>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+    </row>
+    <row r="55" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="40"/>
+      <c r="B55" s="40" t="s">
+        <v>518</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>519</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>520</v>
+      </c>
+      <c r="E55" s="40" t="s">
+        <v>521</v>
+      </c>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+    </row>
+    <row r="56" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="40"/>
+      <c r="B56" s="40" t="s">
+        <v>522</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>523</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>524</v>
+      </c>
+      <c r="E56" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+    </row>
+    <row r="57" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40" t="s">
+        <v>526</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>527</v>
+      </c>
+      <c r="E57" s="40" t="s">
+        <v>528</v>
+      </c>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+    </row>
+    <row r="58" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="40"/>
+      <c r="B58" s="40" t="s">
+        <v>529</v>
+      </c>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
@@ -33976,8 +34204,9 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="F4:F8"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B11:B38"/>
+    <mergeCell ref="B47:B53"/>
+    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -34017,7 +34246,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>509</v>
+        <v>530</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34025,7 +34254,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>510</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34033,7 +34262,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>511</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34041,7 +34270,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>512</v>
+        <v>533</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34049,7 +34278,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>513</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34057,7 +34286,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>514</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34065,7 +34294,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>515</v>
+        <v>536</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34073,7 +34302,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>516</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34081,7 +34310,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>517</v>
+        <v>538</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34089,7 +34318,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>518</v>
+        <v>539</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34097,7 +34326,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>519</v>
+        <v>540</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34105,7 +34334,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>520</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34113,7 +34342,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>521</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34121,7 +34350,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>522</v>
+        <v>543</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34129,7 +34358,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>523</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on user stories for business accounting
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="584">
   <si>
     <t xml:space="preserve">Term</t>
   </si>
@@ -1916,7 +1916,28 @@
     <t xml:space="preserve">Admin is able to see specific product(s) which are pending to complete the reconfiguration (e.g. forecast and expense distribution needs to be changed/reconfigured etc.)</t>
   </si>
   <si>
+    <t xml:space="preserve">Domain</t>
+  </si>
+  <si>
     <t xml:space="preserve">BDGT_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receiving inventory details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProductStatusReceivedEvent is received at business domain (from integration domain). The event contains inventory details (total purchase cost).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total purchase cost is debited under ‘purchase cost’ and provision account for the same (i.e. purchase cost).</t>
   </si>
   <si>
     <t xml:space="preserve">Merchant make provision for initial investment</t>
@@ -2092,7 +2113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2111,6 +2132,13 @@
       <left style="thin"/>
       <right style="thin"/>
       <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -2140,7 +2168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2337,12 +2365,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2431,8 +2471,8 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="103.368421052632"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="105.19028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -2528,10 +2568,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -2609,19 +2649,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N41"/>
+  <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
@@ -2629,7 +2671,7 @@
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2687,9 @@
       <c r="E2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="49"/>
+      <c r="F2" s="49" t="s">
+        <v>558</v>
+      </c>
       <c r="G2" s="28" t="s">
         <v>20</v>
       </c>
@@ -2671,16 +2715,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="95.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="49" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="28" t="s">
         <v>446</v>
       </c>
-      <c r="E3" s="49"/>
+      <c r="E3" s="28" t="s">
+        <v>447</v>
+      </c>
       <c r="F3" s="49"/>
       <c r="G3" s="49"/>
       <c r="H3" s="49"/>
@@ -2691,14 +2737,16 @@
       <c r="M3" s="50"/>
       <c r="N3" s="50"/>
     </row>
-    <row r="4" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="49"/>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="28" t="s">
         <v>448</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="28" t="s">
+        <v>447</v>
+      </c>
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
@@ -2709,14 +2757,16 @@
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
     </row>
-    <row r="5" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="49"/>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="28" t="s">
         <v>449</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="28" t="s">
+        <v>450</v>
+      </c>
       <c r="F5" s="49"/>
       <c r="G5" s="49"/>
       <c r="H5" s="49"/>
@@ -2727,14 +2777,16 @@
       <c r="M5" s="50"/>
       <c r="N5" s="50"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="49"/>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="28" t="s">
         <v>451</v>
       </c>
-      <c r="E6" s="49"/>
+      <c r="E6" s="28" t="s">
+        <v>452</v>
+      </c>
       <c r="F6" s="49"/>
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
@@ -2745,14 +2797,16 @@
       <c r="M6" s="50"/>
       <c r="N6" s="50"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="49"/>
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="28" t="s">
         <v>453</v>
       </c>
-      <c r="E7" s="49"/>
+      <c r="E7" s="28" t="s">
+        <v>452</v>
+      </c>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
       <c r="H7" s="49"/>
@@ -2763,14 +2817,16 @@
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
     </row>
-    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="49"/>
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="28" t="s">
+        <v>452</v>
+      </c>
       <c r="F8" s="49"/>
       <c r="G8" s="49"/>
       <c r="H8" s="49"/>
@@ -2781,14 +2837,16 @@
       <c r="M8" s="50"/>
       <c r="N8" s="50"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="49"/>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="E9" s="49"/>
+      <c r="E9" s="28" t="s">
+        <v>452</v>
+      </c>
       <c r="F9" s="49"/>
       <c r="G9" s="49"/>
       <c r="H9" s="49"/>
@@ -2799,14 +2857,16 @@
       <c r="M9" s="50"/>
       <c r="N9" s="50"/>
     </row>
-    <row r="10" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49"/>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="28" t="s">
+        <v>560</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="E10" s="49"/>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
       <c r="H10" s="49"/>
@@ -2817,14 +2877,14 @@
       <c r="M10" s="50"/>
       <c r="N10" s="50"/>
     </row>
-    <row r="11" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="49"/>
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
-      <c r="D11" s="40" t="s">
-        <v>458</v>
-      </c>
-      <c r="E11" s="49"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="51" t="s">
+        <v>457</v>
+      </c>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
       <c r="H11" s="49"/>
@@ -2835,50 +2895,62 @@
       <c r="M11" s="50"/>
       <c r="N11" s="50"/>
     </row>
-    <row r="12" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="49"/>
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
-      <c r="D12" s="40" t="s">
-        <v>459</v>
-      </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="52" t="s">
+        <v>561</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>562</v>
+      </c>
+      <c r="G12" s="49" t="s">
+        <v>563</v>
+      </c>
       <c r="H12" s="49"/>
-      <c r="I12" s="50"/>
+      <c r="I12" s="50" t="s">
+        <v>564</v>
+      </c>
       <c r="J12" s="50"/>
       <c r="K12" s="50"/>
       <c r="L12" s="50"/>
       <c r="M12" s="50"/>
       <c r="N12" s="50"/>
     </row>
-    <row r="13" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="49"/>
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
-      <c r="D13" s="40" t="s">
-        <v>461</v>
-      </c>
-      <c r="E13" s="49"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="52" t="s">
+        <v>565</v>
+      </c>
       <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="G13" s="49" t="s">
+        <v>563</v>
+      </c>
       <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
+      <c r="I13" s="50" t="s">
+        <v>564</v>
+      </c>
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
       <c r="L13" s="50"/>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
     </row>
-    <row r="14" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="49"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
-      <c r="D14" s="40" t="s">
-        <v>463</v>
-      </c>
-      <c r="E14" s="49"/>
+      <c r="D14" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>450</v>
+      </c>
       <c r="F14" s="49"/>
       <c r="G14" s="49"/>
       <c r="H14" s="49"/>
@@ -2889,14 +2961,16 @@
       <c r="M14" s="50"/>
       <c r="N14" s="50"/>
     </row>
-    <row r="15" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="49"/>
       <c r="B15" s="49"/>
       <c r="C15" s="49"/>
-      <c r="D15" s="40" t="s">
-        <v>464</v>
-      </c>
-      <c r="E15" s="49"/>
+      <c r="D15" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>460</v>
+      </c>
       <c r="F15" s="49"/>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
@@ -2907,14 +2981,16 @@
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
     </row>
-    <row r="16" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="49"/>
       <c r="B16" s="49"/>
       <c r="C16" s="49"/>
-      <c r="D16" s="40" t="s">
-        <v>466</v>
-      </c>
-      <c r="E16" s="49"/>
+      <c r="D16" s="28" t="s">
+        <v>461</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>462</v>
+      </c>
       <c r="F16" s="49"/>
       <c r="G16" s="49"/>
       <c r="H16" s="49"/>
@@ -2925,14 +3001,16 @@
       <c r="M16" s="50"/>
       <c r="N16" s="50"/>
     </row>
-    <row r="17" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="49"/>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
-      <c r="D17" s="40" t="s">
-        <v>468</v>
-      </c>
-      <c r="E17" s="49"/>
+      <c r="D17" s="28" t="s">
+        <v>463</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>462</v>
+      </c>
       <c r="F17" s="49"/>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -2943,14 +3021,16 @@
       <c r="M17" s="50"/>
       <c r="N17" s="50"/>
     </row>
-    <row r="18" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="49"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
-      <c r="D18" s="40" t="s">
-        <v>470</v>
-      </c>
-      <c r="E18" s="49"/>
+      <c r="D18" s="28" t="s">
+        <v>464</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>465</v>
+      </c>
       <c r="F18" s="49"/>
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
@@ -2961,14 +3041,16 @@
       <c r="M18" s="50"/>
       <c r="N18" s="50"/>
     </row>
-    <row r="19" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="49"/>
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
-      <c r="D19" s="40" t="s">
-        <v>471</v>
-      </c>
-      <c r="E19" s="49"/>
+      <c r="D19" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>467</v>
+      </c>
       <c r="F19" s="49"/>
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
@@ -2979,14 +3061,16 @@
       <c r="M19" s="50"/>
       <c r="N19" s="50"/>
     </row>
-    <row r="20" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="49"/>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
-      <c r="D20" s="40" t="s">
-        <v>473</v>
-      </c>
-      <c r="E20" s="49"/>
+      <c r="D20" s="28" t="s">
+        <v>468</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>469</v>
+      </c>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
@@ -2997,14 +3081,16 @@
       <c r="M20" s="50"/>
       <c r="N20" s="50"/>
     </row>
-    <row r="21" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="49"/>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
-      <c r="D21" s="40" t="s">
-        <v>474</v>
-      </c>
-      <c r="E21" s="49"/>
+      <c r="D21" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>469</v>
+      </c>
       <c r="F21" s="49"/>
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
@@ -3015,14 +3101,16 @@
       <c r="M21" s="50"/>
       <c r="N21" s="50"/>
     </row>
-    <row r="22" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="49"/>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
-      <c r="D22" s="40" t="s">
-        <v>475</v>
-      </c>
-      <c r="E22" s="49"/>
+      <c r="D22" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>472</v>
+      </c>
       <c r="F22" s="49"/>
       <c r="G22" s="49"/>
       <c r="H22" s="49"/>
@@ -3033,14 +3121,16 @@
       <c r="M22" s="50"/>
       <c r="N22" s="50"/>
     </row>
-    <row r="23" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="49"/>
       <c r="B23" s="49"/>
       <c r="C23" s="49"/>
-      <c r="D23" s="40" t="s">
-        <v>477</v>
-      </c>
-      <c r="E23" s="49"/>
+      <c r="D23" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>469</v>
+      </c>
       <c r="F23" s="49"/>
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
@@ -3051,14 +3141,16 @@
       <c r="M23" s="50"/>
       <c r="N23" s="50"/>
     </row>
-    <row r="24" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="49"/>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
-      <c r="D24" s="40" t="s">
-        <v>478</v>
-      </c>
-      <c r="E24" s="49"/>
+      <c r="D24" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>465</v>
+      </c>
       <c r="F24" s="49"/>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
@@ -3069,14 +3161,16 @@
       <c r="M24" s="50"/>
       <c r="N24" s="50"/>
     </row>
-    <row r="25" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="49"/>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
-      <c r="D25" s="40" t="s">
-        <v>480</v>
-      </c>
-      <c r="E25" s="49"/>
+      <c r="D25" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>476</v>
+      </c>
       <c r="F25" s="49"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
@@ -3087,14 +3181,16 @@
       <c r="M25" s="50"/>
       <c r="N25" s="50"/>
     </row>
-    <row r="26" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="49"/>
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
-      <c r="D26" s="40" t="s">
-        <v>481</v>
-      </c>
-      <c r="E26" s="49"/>
+      <c r="D26" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>447</v>
+      </c>
       <c r="F26" s="49"/>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -3105,14 +3201,16 @@
       <c r="M26" s="50"/>
       <c r="N26" s="50"/>
     </row>
-    <row r="27" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="49"/>
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
-      <c r="D27" s="40" t="s">
-        <v>483</v>
-      </c>
-      <c r="E27" s="49"/>
+      <c r="D27" s="28" t="s">
+        <v>478</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>479</v>
+      </c>
       <c r="F27" s="49"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
@@ -3123,14 +3221,16 @@
       <c r="M27" s="50"/>
       <c r="N27" s="50"/>
     </row>
-    <row r="28" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="49"/>
       <c r="B28" s="49"/>
       <c r="C28" s="49"/>
-      <c r="D28" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="E28" s="49"/>
+      <c r="D28" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>479</v>
+      </c>
       <c r="F28" s="49"/>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
@@ -3141,14 +3241,16 @@
       <c r="M28" s="50"/>
       <c r="N28" s="50"/>
     </row>
-    <row r="29" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="82.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="49"/>
       <c r="B29" s="49"/>
       <c r="C29" s="49"/>
-      <c r="D29" s="40" t="s">
-        <v>487</v>
-      </c>
-      <c r="E29" s="49"/>
+      <c r="D29" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>482</v>
+      </c>
       <c r="F29" s="49"/>
       <c r="G29" s="49"/>
       <c r="H29" s="49"/>
@@ -3159,14 +3261,16 @@
       <c r="M29" s="50"/>
       <c r="N29" s="50"/>
     </row>
-    <row r="30" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="49"/>
       <c r="B30" s="49"/>
       <c r="C30" s="49"/>
-      <c r="D30" s="40" t="s">
-        <v>488</v>
-      </c>
-      <c r="E30" s="49"/>
+      <c r="D30" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>484</v>
+      </c>
       <c r="F30" s="49"/>
       <c r="G30" s="49"/>
       <c r="H30" s="49"/>
@@ -3177,12 +3281,16 @@
       <c r="M30" s="50"/>
       <c r="N30" s="50"/>
     </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="49"/>
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
+      <c r="D31" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>486</v>
+      </c>
       <c r="F31" s="49"/>
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
@@ -3193,12 +3301,16 @@
       <c r="M31" s="50"/>
       <c r="N31" s="50"/>
     </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="49"/>
       <c r="B32" s="49"/>
       <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
+      <c r="D32" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>479</v>
+      </c>
       <c r="F32" s="49"/>
       <c r="G32" s="49"/>
       <c r="H32" s="49"/>
@@ -3209,12 +3321,16 @@
       <c r="M32" s="50"/>
       <c r="N32" s="50"/>
     </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="49"/>
       <c r="B33" s="49"/>
       <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
+      <c r="D33" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>489</v>
+      </c>
       <c r="F33" s="49"/>
       <c r="G33" s="49"/>
       <c r="H33" s="49"/>
@@ -3338,14 +3454,14 @@
       <c r="N40" s="50"/>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="50"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
       <c r="I41" s="50"/>
       <c r="J41" s="50"/>
       <c r="K41" s="50"/>
@@ -3353,7 +3469,58 @@
       <c r="M41" s="50"/>
       <c r="N41" s="50"/>
     </row>
+    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="50"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="49"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="50"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="50"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D10:D13"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3378,10 +3545,10 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.7368421052632"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
@@ -3433,12 +3600,12 @@
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="49" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="E3" s="49"/>
       <c r="F3" s="49"/>
@@ -3472,7 +3639,7 @@
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
       <c r="D5" s="49" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="E5" s="49"/>
       <c r="F5" s="49"/>
@@ -3522,7 +3689,7 @@
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
       <c r="D8" s="49" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="E8" s="49"/>
       <c r="F8" s="49"/>
@@ -3540,7 +3707,7 @@
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
       <c r="D9" s="49" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="49"/>
@@ -3558,7 +3725,7 @@
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
       <c r="D10" s="49" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
@@ -3576,7 +3743,7 @@
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
       <c r="D11" s="49" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="E11" s="49"/>
       <c r="F11" s="49"/>
@@ -3610,7 +3777,7 @@
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="E13" s="49"/>
       <c r="F13" s="49"/>
@@ -3628,7 +3795,7 @@
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="E14" s="49"/>
       <c r="F14" s="49"/>
@@ -3646,7 +3813,7 @@
       <c r="B15" s="49"/>
       <c r="C15" s="49"/>
       <c r="D15" s="49" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="49"/>
@@ -3664,7 +3831,7 @@
       <c r="B16" s="49"/>
       <c r="C16" s="49"/>
       <c r="D16" s="49" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="E16" s="49"/>
       <c r="F16" s="49"/>
@@ -3698,7 +3865,7 @@
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="49" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="E18" s="49"/>
       <c r="F18" s="49"/>
@@ -3716,7 +3883,7 @@
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
       <c r="D19" s="49" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
@@ -3750,7 +3917,7 @@
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
       <c r="D21" s="49" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -3768,7 +3935,7 @@
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
       <c r="D22" s="49" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="E22" s="49"/>
       <c r="F22" s="49"/>
@@ -3802,7 +3969,7 @@
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
       <c r="D24" s="49" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="E24" s="49"/>
       <c r="F24" s="49"/>
@@ -3820,7 +3987,7 @@
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="49"/>
@@ -3838,7 +4005,7 @@
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
       <c r="D26" s="49" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="E26" s="49"/>
       <c r="F26" s="49"/>
@@ -4115,13 +4282,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -4150,15 +4317,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="75.8421052631579"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="4" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="4" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="4" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="77.2307692307692"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="4" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="4" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="4" width="16.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32735,17 +32902,17 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.2388663967611"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -32801,7 +32968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="26" t="s">
         <v>192</v>
       </c>
@@ -32810,29 +32977,29 @@
       </c>
       <c r="E3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="26"/>
       <c r="D4" s="26" t="s">
         <v>194</v>
       </c>
       <c r="E4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="26"/>
       <c r="D5" s="26" t="s">
         <v>195</v>
       </c>
       <c r="E5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0"/>
+    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="26"/>
       <c r="D6" s="4" t="s">
         <v>196</v>
       </c>
       <c r="E6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0"/>
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="26"/>
       <c r="D7" s="4" t="s">
         <v>197</v>
       </c>
@@ -32885,8 +33052,8 @@
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4" t="s">
+    <row r="15" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C15" s="25" t="s">
         <v>204</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -32896,37 +33063,47 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="25"/>
       <c r="D16" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="25"/>
       <c r="D17" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="25"/>
       <c r="D18" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="25"/>
       <c r="D19" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="25"/>
       <c r="D20" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="25"/>
       <c r="D21" s="1" t="s">
         <v>212</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C15:C21"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -32954,18 +33131,18 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="27" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="27" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="73.8056680161943"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="45.2024291497976"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="75.0890688259109"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="27" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="27" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="27" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="27" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="27" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="27" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="27" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="27" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="27" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="26.6720647773279"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="27.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="27" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -33707,9 +33884,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="98.6558704453441"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="100.477732793522"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -33854,10 +34031,10 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.2024291497976"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="81.1943319838057"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -34021,10 +34198,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.4858299595142"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -34132,20 +34309,20 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.8825910931174"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="87.9433198380567"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="89.4453441295547"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -35001,7 +35178,7 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.1943319838057"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added 'provision for losses' flow in business domain
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="596">
   <si>
     <t>Term</t>
   </si>
@@ -1909,52 +1909,55 @@
     <t>BDGT_01</t>
   </si>
   <si>
+    <t>Value of provision for purchase cost and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>BusinessAccountProvisionController</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommand</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler</t>
+  </si>
+  <si>
+    <t>BusinessAccount</t>
+  </si>
+  <si>
+    <t>CreateProvisionEvent</t>
+  </si>
+  <si>
+    <t>CreateProvisionEventListener</t>
+  </si>
+  <si>
+    <t>REST controller fires command CreateProvisionCommand</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for purchase cost and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
     <t>Merchant will make provision for purchase cost.</t>
   </si>
   <si>
-    <t>Value of provision for purchase cost and provision date are received via REST controller</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>BusinessAccountProvisionController</t>
-  </si>
-  <si>
-    <t>CreateProvisionCommand</t>
-  </si>
-  <si>
-    <t>CreateProvisionCommandHandler</t>
-  </si>
-  <si>
-    <t>BusinessAccount</t>
-  </si>
-  <si>
-    <t>CreateProvisionEvent</t>
-  </si>
-  <si>
-    <t>CreateProvisionEventListener</t>
-  </si>
-  <si>
-    <t>REST controller fires command CreateProvisionForPurchaseCostCommand</t>
-  </si>
-  <si>
-    <t>CreateProvisionForPurchaseCostCommandHandler fires CreateProvisionForPurchaseCostEvent which will update provision for purchase cost and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
-  </si>
-  <si>
     <t>Receiving inventory details</t>
   </si>
   <si>
     <t>ProductStatusReceivedEvent is received at business domain (from integration domain). The event contains inventory details (total purchase cost).</t>
   </si>
   <si>
-    <t>Not started</t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>ProductStatusReceivedEvent</t>
+  </si>
+  <si>
+    <t>ProductStatusReceivedEventListener</t>
   </si>
   <si>
     <t>Total purchase cost is debited under ‘purchase cost’ and provision account for the same (i.e. purchase cost).</t>
@@ -2690,10 +2693,10 @@
   </sheetPr>
   <dimension ref="A2:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2820,7 +2823,7 @@
       <c r="M5" s="52"/>
       <c r="N5" s="52"/>
     </row>
-    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="51"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -2828,27 +2831,41 @@
         <v>451</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>452</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
+        <v>560</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H6" s="51"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
+      <c r="I6" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K6" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L6" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M6" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N6" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
-      <c r="D7" s="30" t="s">
-        <v>453</v>
-      </c>
+      <c r="D7" s="30"/>
       <c r="E7" s="30" t="s">
-        <v>452</v>
+        <v>569</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -2860,15 +2877,13 @@
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
     </row>
-    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
-      <c r="D8" s="30" t="s">
-        <v>454</v>
-      </c>
+      <c r="D8" s="30"/>
       <c r="E8" s="30" t="s">
-        <v>452</v>
+        <v>570</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -2880,12 +2895,12 @@
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
     </row>
-    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="30" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>452</v>
@@ -2900,49 +2915,35 @@
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="30" t="s">
-        <v>560</v>
+        <v>454</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>561</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>562</v>
-      </c>
-      <c r="G10" s="51" t="s">
-        <v>563</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
       <c r="H10" s="51"/>
-      <c r="I10" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="J10" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="K10" s="53" t="s">
-        <v>566</v>
-      </c>
-      <c r="L10" s="53" t="s">
-        <v>567</v>
-      </c>
-      <c r="M10" s="53" t="s">
-        <v>568</v>
-      </c>
-      <c r="N10" s="53" t="s">
-        <v>569</v>
-      </c>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>455</v>
+      </c>
       <c r="E11" s="30" t="s">
-        <v>570</v>
+        <v>452</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -2954,33 +2955,49 @@
       <c r="M11" s="52"/>
       <c r="N11" s="52"/>
     </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="30" t="s">
+        <v>571</v>
+      </c>
       <c r="E12" s="30" t="s">
-        <v>571</v>
-      </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
+        <v>560</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H12" s="51"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
+      <c r="I12" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K12" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L12" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M12" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N12" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="30" t="s">
-        <v>572</v>
-      </c>
+      <c r="D13" s="30"/>
       <c r="E13" s="30" t="s">
-        <v>456</v>
+        <v>569</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -2992,13 +3009,13 @@
       <c r="M13" s="52"/>
       <c r="N13" s="52"/>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="30"/>
-      <c r="E14" s="54" t="s">
-        <v>457</v>
+      <c r="E14" s="30" t="s">
+        <v>570</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -3010,24 +3027,20 @@
       <c r="M14" s="52"/>
       <c r="N14" s="52"/>
     </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="55" t="s">
-        <v>573</v>
-      </c>
-      <c r="F15" s="51" t="s">
-        <v>562</v>
-      </c>
-      <c r="G15" s="51" t="s">
-        <v>574</v>
-      </c>
+      <c r="D15" s="30" t="s">
+        <v>572</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
       <c r="H15" s="51"/>
-      <c r="I15" s="52" t="s">
-        <v>575</v>
-      </c>
+      <c r="I15" s="52"/>
       <c r="J15" s="52"/>
       <c r="K15" s="52"/>
       <c r="L15" s="52"/>
@@ -3039,72 +3052,96 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="55" t="s">
-        <v>576</v>
+      <c r="E16" s="54" t="s">
+        <v>457</v>
       </c>
       <c r="F16" s="51"/>
-      <c r="G16" s="51" t="s">
-        <v>574</v>
-      </c>
+      <c r="G16" s="51"/>
       <c r="H16" s="51"/>
-      <c r="I16" s="52" t="s">
-        <v>575</v>
-      </c>
+      <c r="I16" s="52"/>
       <c r="J16" s="52"/>
       <c r="K16" s="52"/>
       <c r="L16" s="52"/>
       <c r="M16" s="52"/>
       <c r="N16" s="52"/>
     </row>
-    <row r="17" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
-      <c r="D17" s="30" t="s">
-        <v>458</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>450</v>
-      </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="55" t="s">
+        <v>573</v>
+      </c>
+      <c r="F17" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
+      <c r="I17" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="J17" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="L17" s="52" t="s">
+        <v>566</v>
+      </c>
+      <c r="M17" s="53" t="s">
+        <v>575</v>
+      </c>
+      <c r="N17" s="53" t="s">
+        <v>576</v>
+      </c>
     </row>
-    <row r="18" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
-      <c r="D18" s="30" t="s">
-        <v>459</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>460</v>
-      </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="55" t="s">
+        <v>577</v>
+      </c>
+      <c r="F18" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
+      <c r="I18" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="J18" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="K18" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="L18" s="52" t="s">
+        <v>566</v>
+      </c>
+      <c r="M18" s="53" t="s">
+        <v>575</v>
+      </c>
+      <c r="N18" s="53" t="s">
+        <v>576</v>
+      </c>
     </row>
-    <row r="19" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>462</v>
+        <v>458</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>450</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -3116,15 +3153,15 @@
       <c r="M19" s="52"/>
       <c r="N19" s="52"/>
     </row>
-    <row r="20" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
       <c r="D20" s="30" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -3136,15 +3173,15 @@
       <c r="M20" s="52"/>
       <c r="N20" s="52"/>
     </row>
-    <row r="21" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="30" t="s">
-        <v>464</v>
-      </c>
-      <c r="E21" s="49" t="s">
-        <v>465</v>
+        <v>461</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>462</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -3156,15 +3193,15 @@
       <c r="M21" s="52"/>
       <c r="N21" s="52"/>
     </row>
-    <row r="22" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="30" t="s">
-        <v>466</v>
-      </c>
-      <c r="E22" s="49" t="s">
-        <v>467</v>
+        <v>463</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>462</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -3176,15 +3213,15 @@
       <c r="M22" s="52"/>
       <c r="N22" s="52"/>
     </row>
-    <row r="23" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
       <c r="D23" s="30" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -3196,15 +3233,15 @@
       <c r="M23" s="52"/>
       <c r="N23" s="52"/>
     </row>
-    <row r="24" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="51"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="30" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -3216,15 +3253,15 @@
       <c r="M24" s="52"/>
       <c r="N24" s="52"/>
     </row>
-    <row r="25" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="51"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>472</v>
+        <v>468</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>469</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -3236,12 +3273,12 @@
       <c r="M25" s="52"/>
       <c r="N25" s="52"/>
     </row>
-    <row r="26" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="30" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E26" s="49" t="s">
         <v>469</v>
@@ -3256,15 +3293,15 @@
       <c r="M26" s="52"/>
       <c r="N26" s="52"/>
     </row>
-    <row r="27" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="51"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
       <c r="D27" s="30" t="s">
-        <v>474</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>465</v>
+        <v>471</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>472</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -3276,15 +3313,15 @@
       <c r="M27" s="52"/>
       <c r="N27" s="52"/>
     </row>
-    <row r="28" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
       <c r="D28" s="30" t="s">
-        <v>475</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>476</v>
+        <v>473</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>469</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -3296,15 +3333,15 @@
       <c r="M28" s="52"/>
       <c r="N28" s="52"/>
     </row>
-    <row r="29" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
       <c r="D29" s="30" t="s">
-        <v>477</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>447</v>
+        <v>474</v>
+      </c>
+      <c r="E29" s="49" t="s">
+        <v>465</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -3316,15 +3353,15 @@
       <c r="M29" s="52"/>
       <c r="N29" s="52"/>
     </row>
-    <row r="30" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="51"/>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="30" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -3336,15 +3373,15 @@
       <c r="M30" s="52"/>
       <c r="N30" s="52"/>
     </row>
-    <row r="31" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
       <c r="D31" s="30" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>479</v>
+        <v>447</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -3356,15 +3393,15 @@
       <c r="M31" s="52"/>
       <c r="N31" s="52"/>
     </row>
-    <row r="32" customFormat="false" ht="82.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="51"/>
       <c r="B32" s="51"/>
       <c r="C32" s="51"/>
       <c r="D32" s="30" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -3376,15 +3413,15 @@
       <c r="M32" s="52"/>
       <c r="N32" s="52"/>
     </row>
-    <row r="33" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="51"/>
       <c r="B33" s="51"/>
       <c r="C33" s="51"/>
       <c r="D33" s="30" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -3396,15 +3433,15 @@
       <c r="M33" s="52"/>
       <c r="N33" s="52"/>
     </row>
-    <row r="34" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="51"/>
       <c r="B34" s="51"/>
       <c r="C34" s="51"/>
       <c r="D34" s="30" t="s">
-        <v>485</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>486</v>
+        <v>481</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>482</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -3416,15 +3453,15 @@
       <c r="M34" s="52"/>
       <c r="N34" s="52"/>
     </row>
-    <row r="35" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="51"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
       <c r="D35" s="30" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -3436,15 +3473,15 @@
       <c r="M35" s="52"/>
       <c r="N35" s="52"/>
     </row>
-    <row r="36" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51"/>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
       <c r="D36" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>489</v>
+        <v>485</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>486</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -3456,12 +3493,16 @@
       <c r="M36" s="52"/>
       <c r="N36" s="52"/>
     </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="51"/>
       <c r="B37" s="51"/>
       <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
+      <c r="D37" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>479</v>
+      </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
       <c r="H37" s="51"/>
@@ -3472,12 +3513,16 @@
       <c r="M37" s="52"/>
       <c r="N37" s="52"/>
     </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="51"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
+      <c r="D38" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>489</v>
+      </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
       <c r="H38" s="51"/>
@@ -3488,7 +3533,7 @@
       <c r="M38" s="52"/>
       <c r="N38" s="52"/>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="51"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
@@ -3504,7 +3549,7 @@
       <c r="M39" s="52"/>
       <c r="N39" s="52"/>
     </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="51"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
@@ -3520,7 +3565,7 @@
       <c r="M40" s="52"/>
       <c r="N40" s="52"/>
     </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="51"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -3536,7 +3581,7 @@
       <c r="M41" s="52"/>
       <c r="N41" s="52"/>
     </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="51"/>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -3552,7 +3597,7 @@
       <c r="M42" s="52"/>
       <c r="N42" s="52"/>
     </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="51"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
@@ -3568,7 +3613,7 @@
       <c r="M43" s="52"/>
       <c r="N43" s="52"/>
     </row>
-    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="51"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -3584,7 +3629,7 @@
       <c r="M44" s="52"/>
       <c r="N44" s="52"/>
     </row>
-    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="51"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
@@ -3600,7 +3645,7 @@
       <c r="M45" s="52"/>
       <c r="N45" s="52"/>
     </row>
-    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -3616,15 +3661,15 @@
       <c r="M46" s="52"/>
       <c r="N46" s="52"/>
     </row>
-    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="52"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="51"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
       <c r="I47" s="52"/>
       <c r="J47" s="52"/>
       <c r="K47" s="52"/>
@@ -3632,11 +3677,44 @@
       <c r="M47" s="52"/>
       <c r="N47" s="52"/>
     </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="51"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="52"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D16"/>
+  <mergeCells count="3">
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3722,7 +3800,7 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -3756,7 +3834,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -3806,7 +3884,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -3824,7 +3902,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -3842,7 +3920,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -3860,7 +3938,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -3894,7 +3972,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -3912,7 +3990,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -3930,7 +4008,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -3948,7 +4026,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -3982,7 +4060,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -4000,7 +4078,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -4034,7 +4112,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -4052,7 +4130,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -4086,7 +4164,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -4104,7 +4182,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -4122,7 +4200,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -4405,7 +4483,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'provision for benefits' flow in business domain
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="596">
   <si>
     <t>Term</t>
   </si>
@@ -2691,12 +2691,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N65536"/>
+  <dimension ref="A2:N51"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2895,7 +2895,7 @@
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
@@ -2903,27 +2903,41 @@
         <v>453</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>452</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+        <v>560</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H9" s="51"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
+      <c r="I9" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J9" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K9" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L9" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M9" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N9" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
-      <c r="D10" s="30" t="s">
-        <v>454</v>
-      </c>
+      <c r="D10" s="30"/>
       <c r="E10" s="30" t="s">
-        <v>452</v>
+        <v>569</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -2935,15 +2949,13 @@
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="30" t="s">
-        <v>455</v>
-      </c>
+      <c r="D11" s="30"/>
       <c r="E11" s="30" t="s">
-        <v>452</v>
+        <v>570</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -2955,49 +2967,35 @@
       <c r="M11" s="52"/>
       <c r="N11" s="52"/>
     </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
       <c r="D12" s="30" t="s">
-        <v>571</v>
+        <v>454</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>560</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G12" s="51" t="s">
-        <v>562</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="51"/>
-      <c r="I12" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K12" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L12" s="53" t="s">
-        <v>566</v>
-      </c>
-      <c r="M12" s="53" t="s">
-        <v>567</v>
-      </c>
-      <c r="N12" s="53" t="s">
-        <v>568</v>
-      </c>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="30" t="s">
+        <v>455</v>
+      </c>
       <c r="E13" s="30" t="s">
-        <v>569</v>
+        <v>452</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -3009,33 +3007,49 @@
       <c r="M13" s="52"/>
       <c r="N13" s="52"/>
     </row>
-    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30" t="s">
+        <v>571</v>
+      </c>
       <c r="E14" s="30" t="s">
-        <v>570</v>
-      </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
+        <v>560</v>
+      </c>
+      <c r="F14" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
+      <c r="I14" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K14" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L14" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M14" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N14" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="15" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="30" t="s">
-        <v>572</v>
-      </c>
+      <c r="D15" s="30"/>
       <c r="E15" s="30" t="s">
-        <v>456</v>
+        <v>569</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -3047,13 +3061,13 @@
       <c r="M15" s="52"/>
       <c r="N15" s="52"/>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="54" t="s">
-        <v>457</v>
+      <c r="E16" s="30" t="s">
+        <v>570</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -3065,123 +3079,121 @@
       <c r="M16" s="52"/>
       <c r="N16" s="52"/>
     </row>
-    <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="55" t="s">
-        <v>573</v>
-      </c>
-      <c r="F17" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G17" s="51" t="s">
-        <v>562</v>
-      </c>
+      <c r="D17" s="30" t="s">
+        <v>572</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="51"/>
-      <c r="I17" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="J17" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="K17" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="L17" s="52" t="s">
-        <v>566</v>
-      </c>
-      <c r="M17" s="53" t="s">
-        <v>575</v>
-      </c>
-      <c r="N17" s="53" t="s">
-        <v>576</v>
-      </c>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="30"/>
-      <c r="E18" s="55" t="s">
-        <v>577</v>
-      </c>
-      <c r="F18" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G18" s="51" t="s">
-        <v>562</v>
-      </c>
+      <c r="E18" s="54" t="s">
+        <v>457</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="51"/>
-      <c r="I18" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="J18" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="K18" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="L18" s="52" t="s">
-        <v>566</v>
-      </c>
-      <c r="M18" s="53" t="s">
-        <v>575</v>
-      </c>
-      <c r="N18" s="53" t="s">
-        <v>576</v>
-      </c>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
     </row>
-    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
-      <c r="D19" s="30" t="s">
-        <v>458</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>450</v>
-      </c>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="55" t="s">
+        <v>573</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
+      <c r="I19" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="J19" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="K19" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="L19" s="52" t="s">
+        <v>566</v>
+      </c>
+      <c r="M19" s="53" t="s">
+        <v>575</v>
+      </c>
+      <c r="N19" s="53" t="s">
+        <v>576</v>
+      </c>
     </row>
-    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
-      <c r="D20" s="30" t="s">
-        <v>459</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>460</v>
-      </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="55" t="s">
+        <v>577</v>
+      </c>
+      <c r="F20" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G20" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H20" s="51"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
+      <c r="I20" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="J20" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="K20" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="L20" s="52" t="s">
+        <v>566</v>
+      </c>
+      <c r="M20" s="53" t="s">
+        <v>575</v>
+      </c>
+      <c r="N20" s="53" t="s">
+        <v>576</v>
+      </c>
     </row>
-    <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>462</v>
+        <v>458</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>450</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -3198,10 +3210,10 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="30" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -3213,15 +3225,15 @@
       <c r="M22" s="52"/>
       <c r="N22" s="52"/>
     </row>
-    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
       <c r="D23" s="30" t="s">
-        <v>464</v>
-      </c>
-      <c r="E23" s="49" t="s">
-        <v>465</v>
+        <v>461</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>462</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -3238,10 +3250,10 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="30" t="s">
-        <v>466</v>
-      </c>
-      <c r="E24" s="49" t="s">
-        <v>467</v>
+        <v>463</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>462</v>
       </c>
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
@@ -3258,10 +3270,10 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="30" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -3273,15 +3285,15 @@
       <c r="M25" s="52"/>
       <c r="N25" s="52"/>
     </row>
-    <row r="26" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="30" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -3293,15 +3305,15 @@
       <c r="M26" s="52"/>
       <c r="N26" s="52"/>
     </row>
-    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="51"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
       <c r="D27" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>472</v>
+        <v>468</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>469</v>
       </c>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
@@ -3313,12 +3325,12 @@
       <c r="M27" s="52"/>
       <c r="N27" s="52"/>
     </row>
-    <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
       <c r="D28" s="30" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E28" s="49" t="s">
         <v>469</v>
@@ -3333,15 +3345,15 @@
       <c r="M28" s="52"/>
       <c r="N28" s="52"/>
     </row>
-    <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
       <c r="D29" s="30" t="s">
-        <v>474</v>
-      </c>
-      <c r="E29" s="49" t="s">
-        <v>465</v>
+        <v>471</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>472</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -3358,10 +3370,10 @@
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="30" t="s">
-        <v>475</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>476</v>
+        <v>473</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>469</v>
       </c>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
@@ -3373,15 +3385,15 @@
       <c r="M30" s="52"/>
       <c r="N30" s="52"/>
     </row>
-    <row r="31" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
       <c r="D31" s="30" t="s">
-        <v>477</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>447</v>
+        <v>474</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>465</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -3393,15 +3405,15 @@
       <c r="M31" s="52"/>
       <c r="N31" s="52"/>
     </row>
-    <row r="32" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="51"/>
       <c r="B32" s="51"/>
       <c r="C32" s="51"/>
       <c r="D32" s="30" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -3413,15 +3425,15 @@
       <c r="M32" s="52"/>
       <c r="N32" s="52"/>
     </row>
-    <row r="33" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="51"/>
       <c r="B33" s="51"/>
       <c r="C33" s="51"/>
       <c r="D33" s="30" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>479</v>
+        <v>447</v>
       </c>
       <c r="F33" s="51"/>
       <c r="G33" s="51"/>
@@ -3433,15 +3445,15 @@
       <c r="M33" s="52"/>
       <c r="N33" s="52"/>
     </row>
-    <row r="34" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="51"/>
       <c r="B34" s="51"/>
       <c r="C34" s="51"/>
       <c r="D34" s="30" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -3453,15 +3465,15 @@
       <c r="M34" s="52"/>
       <c r="N34" s="52"/>
     </row>
-    <row r="35" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="51"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
       <c r="D35" s="30" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -3473,15 +3485,15 @@
       <c r="M35" s="52"/>
       <c r="N35" s="52"/>
     </row>
-    <row r="36" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="51"/>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
       <c r="D36" s="30" t="s">
-        <v>485</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>486</v>
+        <v>481</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>482</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -3498,10 +3510,10 @@
       <c r="B37" s="51"/>
       <c r="C37" s="51"/>
       <c r="D37" s="30" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -3518,10 +3530,10 @@
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
       <c r="D38" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>489</v>
+        <v>485</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>486</v>
       </c>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
@@ -3533,12 +3545,16 @@
       <c r="M38" s="52"/>
       <c r="N38" s="52"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="51"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
+      <c r="D39" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>479</v>
+      </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
       <c r="H39" s="51"/>
@@ -3549,12 +3565,16 @@
       <c r="M39" s="52"/>
       <c r="N39" s="52"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="51"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
+      <c r="D40" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>489</v>
+      </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
       <c r="H40" s="51"/>
@@ -3694,14 +3714,14 @@
       <c r="N48" s="52"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="52"/>
-      <c r="B49" s="52"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
+      <c r="A49" s="51"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
       <c r="I49" s="52"/>
       <c r="J49" s="52"/>
       <c r="K49" s="52"/>
@@ -3709,12 +3729,44 @@
       <c r="M49" s="52"/>
       <c r="N49" s="52"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="51"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="52"/>
+      <c r="L50" s="52"/>
+      <c r="M50" s="52"/>
+      <c r="N50" s="52"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="52"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Completed user stories for provisions (to be set by merchant)
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="620">
   <si>
     <t>Term</t>
   </si>
@@ -1909,42 +1909,111 @@
     <t>BDGT_01</t>
   </si>
   <si>
+    <t>Value of provision for losses and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>BusinessAccountProvisionController</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommand</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler</t>
+  </si>
+  <si>
+    <t>BusinessAccount</t>
+  </si>
+  <si>
+    <t>CreateProvisionEvent</t>
+  </si>
+  <si>
+    <t>CreateProvisionEventListener</t>
+  </si>
+  <si>
+    <t>REST controller fires command CreateProvisionCommand</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for losses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Value of provision for benefits and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for benefits and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Value of provision for taxes and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for taxes and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Value of provision for others and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for others and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Merchant will make provision for common expenses.</t>
+  </si>
+  <si>
+    <t>Value of provision for common expenses and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for common expenses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Merchant will make provision for nodal account.</t>
+  </si>
+  <si>
+    <t>Value of provision for nodal account and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for nodal account and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Merchant will make provision for revenue.</t>
+  </si>
+  <si>
+    <t>Value of provision for revenue and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for revenue and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Merchant will make provision for booking amount.</t>
+  </si>
+  <si>
+    <t>Value of provision for booking amount and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for booking amount and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Merchant will make provision for subscription specific expenses.</t>
+  </si>
+  <si>
+    <t>Value of provision for subscription specific expenses and provision date are received via REST controller</t>
+  </si>
+  <si>
+    <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for subscription specific expenses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
+  </si>
+  <si>
+    <t>Merchant will make provision for purchase cost.</t>
+  </si>
+  <si>
     <t>Value of provision for purchase cost and provision date are received via REST controller</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>BusinessAccountProvisionController</t>
-  </si>
-  <si>
-    <t>CreateProvisionCommand</t>
-  </si>
-  <si>
-    <t>CreateProvisionCommandHandler</t>
-  </si>
-  <si>
-    <t>BusinessAccount</t>
-  </si>
-  <si>
-    <t>CreateProvisionEvent</t>
-  </si>
-  <si>
-    <t>CreateProvisionEventListener</t>
-  </si>
-  <si>
-    <t>REST controller fires command CreateProvisionCommand</t>
-  </si>
-  <si>
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for purchase cost and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
-    <t>Merchant will make provision for purchase cost.</t>
-  </si>
-  <si>
     <t>Receiving inventory details</t>
   </si>
   <si>
@@ -1961,6 +2030,9 @@
   </si>
   <si>
     <t>Total purchase cost is debited under ‘purchase cost’ and provision account for the same (i.e. purchase cost).</t>
+  </si>
+  <si>
+    <t>When system receives incoming operating expenses details from main application, they are debited under respective operating expense categories and respective provision account.</t>
   </si>
   <si>
     <t>Merchant make provision for initial investment</t>
@@ -2691,12 +2763,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N51"/>
+  <dimension ref="A2:N70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2877,7 +2949,7 @@
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
     </row>
-    <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -2903,7 +2975,7 @@
         <v>453</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="F9" s="51" t="s">
         <v>561</v>
@@ -2955,7 +3027,7 @@
       <c r="C11" s="51"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -2967,7 +3039,7 @@
       <c r="M11" s="52"/>
       <c r="N11" s="52"/>
     </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
@@ -2975,27 +3047,41 @@
         <v>454</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>452</v>
-      </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
+        <v>573</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H12" s="51"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
+      <c r="I12" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K12" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L12" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M12" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N12" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="30" t="s">
-        <v>455</v>
-      </c>
+      <c r="D13" s="30"/>
       <c r="E13" s="30" t="s">
-        <v>452</v>
+        <v>569</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -3007,67 +3093,67 @@
       <c r="M13" s="52"/>
       <c r="N13" s="52"/>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
-      <c r="D14" s="30" t="s">
-        <v>571</v>
-      </c>
+      <c r="D14" s="30"/>
       <c r="E14" s="30" t="s">
-        <v>560</v>
-      </c>
-      <c r="F14" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G14" s="51" t="s">
-        <v>562</v>
-      </c>
+        <v>574</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="51"/>
-      <c r="I14" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J14" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K14" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L14" s="53" t="s">
-        <v>566</v>
-      </c>
-      <c r="M14" s="53" t="s">
-        <v>567</v>
-      </c>
-      <c r="N14" s="53" t="s">
-        <v>568</v>
-      </c>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="30"/>
+      <c r="D15" s="30" t="s">
+        <v>455</v>
+      </c>
       <c r="E15" s="30" t="s">
-        <v>569</v>
-      </c>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
+        <v>575</v>
+      </c>
+      <c r="F15" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
+      <c r="I15" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J15" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K15" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L15" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M15" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N15" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -3079,15 +3165,13 @@
       <c r="M16" s="52"/>
       <c r="N16" s="52"/>
     </row>
-    <row r="17" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
-      <c r="D17" s="30" t="s">
-        <v>572</v>
-      </c>
+      <c r="D17" s="30"/>
       <c r="E17" s="30" t="s">
-        <v>456</v>
+        <v>576</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -3099,121 +3183,121 @@
       <c r="M17" s="52"/>
       <c r="N17" s="52"/>
     </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="54" t="s">
-        <v>457</v>
-      </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
+      <c r="D18" s="30" t="s">
+        <v>577</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>578</v>
+      </c>
+      <c r="F18" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
+      <c r="I18" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K18" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L18" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M18" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N18" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="30"/>
-      <c r="E19" s="55" t="s">
-        <v>573</v>
-      </c>
-      <c r="F19" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G19" s="51" t="s">
-        <v>562</v>
-      </c>
+      <c r="E19" s="30" t="s">
+        <v>569</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="51"/>
-      <c r="I19" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="J19" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="K19" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="L19" s="52" t="s">
-        <v>566</v>
-      </c>
-      <c r="M19" s="53" t="s">
-        <v>575</v>
-      </c>
-      <c r="N19" s="53" t="s">
-        <v>576</v>
-      </c>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
       <c r="D20" s="30"/>
-      <c r="E20" s="55" t="s">
-        <v>577</v>
-      </c>
-      <c r="F20" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G20" s="51" t="s">
-        <v>562</v>
-      </c>
+      <c r="E20" s="30" t="s">
+        <v>579</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="51"/>
-      <c r="I20" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="J20" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="K20" s="52" t="s">
-        <v>574</v>
-      </c>
-      <c r="L20" s="52" t="s">
-        <v>566</v>
-      </c>
-      <c r="M20" s="53" t="s">
-        <v>575</v>
-      </c>
-      <c r="N20" s="53" t="s">
-        <v>576</v>
-      </c>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
     </row>
-    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="30" t="s">
-        <v>458</v>
-      </c>
-      <c r="E21" s="56" t="s">
-        <v>450</v>
-      </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
+        <v>580</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>581</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H21" s="51"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
+      <c r="I21" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J21" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K21" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L21" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M21" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N21" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="22" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
-      <c r="D22" s="30" t="s">
-        <v>459</v>
-      </c>
+      <c r="D22" s="30"/>
       <c r="E22" s="30" t="s">
-        <v>460</v>
+        <v>569</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -3225,15 +3309,13 @@
       <c r="M22" s="52"/>
       <c r="N22" s="52"/>
     </row>
-    <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
-      <c r="D23" s="30" t="s">
-        <v>461</v>
-      </c>
+      <c r="D23" s="30"/>
       <c r="E23" s="30" t="s">
-        <v>462</v>
+        <v>582</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -3245,35 +3327,49 @@
       <c r="M23" s="52"/>
       <c r="N23" s="52"/>
     </row>
-    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="51"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="30" t="s">
-        <v>463</v>
+        <v>583</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>462</v>
-      </c>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
+        <v>584</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G24" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H24" s="51"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
+      <c r="I24" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J24" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K24" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L24" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M24" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N24" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="51"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
-      <c r="D25" s="30" t="s">
-        <v>464</v>
-      </c>
-      <c r="E25" s="49" t="s">
-        <v>465</v>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30" t="s">
+        <v>569</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -3289,11 +3385,9 @@
       <c r="A26" s="51"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
-      <c r="D26" s="30" t="s">
-        <v>466</v>
-      </c>
-      <c r="E26" s="49" t="s">
-        <v>467</v>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30" t="s">
+        <v>585</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -3305,35 +3399,49 @@
       <c r="M26" s="52"/>
       <c r="N26" s="52"/>
     </row>
-    <row r="27" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="51"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
       <c r="D27" s="30" t="s">
-        <v>468</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>469</v>
-      </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
+        <v>586</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="F27" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G27" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H27" s="51"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
+      <c r="I27" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J27" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K27" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L27" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M27" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N27" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="28" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
-      <c r="D28" s="30" t="s">
-        <v>470</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>469</v>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30" t="s">
+        <v>569</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -3345,15 +3453,13 @@
       <c r="M28" s="52"/>
       <c r="N28" s="52"/>
     </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
-      <c r="D29" s="30" t="s">
-        <v>471</v>
-      </c>
+      <c r="D29" s="30"/>
       <c r="E29" s="30" t="s">
-        <v>472</v>
+        <v>588</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -3365,35 +3471,49 @@
       <c r="M29" s="52"/>
       <c r="N29" s="52"/>
     </row>
-    <row r="30" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="51"/>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="30" t="s">
-        <v>473</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>469</v>
-      </c>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
+        <v>589</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>590</v>
+      </c>
+      <c r="F30" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G30" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H30" s="51"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
+      <c r="I30" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J30" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K30" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L30" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M30" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N30" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
-      <c r="D31" s="30" t="s">
-        <v>474</v>
-      </c>
-      <c r="E31" s="49" t="s">
-        <v>465</v>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30" t="s">
+        <v>569</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -3409,11 +3529,9 @@
       <c r="A32" s="51"/>
       <c r="B32" s="51"/>
       <c r="C32" s="51"/>
-      <c r="D32" s="30" t="s">
-        <v>475</v>
-      </c>
+      <c r="D32" s="30"/>
       <c r="E32" s="30" t="s">
-        <v>476</v>
+        <v>591</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -3425,35 +3543,49 @@
       <c r="M32" s="52"/>
       <c r="N32" s="52"/>
     </row>
-    <row r="33" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="51"/>
       <c r="B33" s="51"/>
       <c r="C33" s="51"/>
       <c r="D33" s="30" t="s">
-        <v>477</v>
+        <v>592</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
+        <v>593</v>
+      </c>
+      <c r="F33" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H33" s="51"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
+      <c r="I33" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="J33" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="K33" s="53" t="s">
+        <v>565</v>
+      </c>
+      <c r="L33" s="53" t="s">
+        <v>566</v>
+      </c>
+      <c r="M33" s="53" t="s">
+        <v>567</v>
+      </c>
+      <c r="N33" s="53" t="s">
+        <v>568</v>
+      </c>
     </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="51"/>
       <c r="B34" s="51"/>
       <c r="C34" s="51"/>
-      <c r="D34" s="30" t="s">
-        <v>478</v>
-      </c>
+      <c r="D34" s="30"/>
       <c r="E34" s="30" t="s">
-        <v>479</v>
+        <v>569</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -3465,15 +3597,13 @@
       <c r="M34" s="52"/>
       <c r="N34" s="52"/>
     </row>
-    <row r="35" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="51"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
-      <c r="D35" s="30" t="s">
-        <v>480</v>
-      </c>
+      <c r="D35" s="30"/>
       <c r="E35" s="30" t="s">
-        <v>479</v>
+        <v>594</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -3485,15 +3615,15 @@
       <c r="M35" s="52"/>
       <c r="N35" s="52"/>
     </row>
-    <row r="36" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="51"/>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
       <c r="D36" s="30" t="s">
-        <v>481</v>
+        <v>595</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="51"/>
@@ -3505,15 +3635,13 @@
       <c r="M36" s="52"/>
       <c r="N36" s="52"/>
     </row>
-    <row r="37" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="51"/>
       <c r="B37" s="51"/>
       <c r="C37" s="51"/>
-      <c r="D37" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>484</v>
+      <c r="D37" s="30"/>
+      <c r="E37" s="54" t="s">
+        <v>457</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
@@ -3525,55 +3653,83 @@
       <c r="M37" s="52"/>
       <c r="N37" s="52"/>
     </row>
-    <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="51"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
-      <c r="D38" s="30" t="s">
-        <v>485</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="55" t="s">
+        <v>596</v>
+      </c>
+      <c r="F38" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G38" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H38" s="51"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="52"/>
-      <c r="N38" s="52"/>
+      <c r="I38" s="52" t="s">
+        <v>597</v>
+      </c>
+      <c r="J38" s="52" t="s">
+        <v>597</v>
+      </c>
+      <c r="K38" s="52" t="s">
+        <v>597</v>
+      </c>
+      <c r="L38" s="52" t="s">
+        <v>566</v>
+      </c>
+      <c r="M38" s="53" t="s">
+        <v>598</v>
+      </c>
+      <c r="N38" s="53" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="39" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="51"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
-      <c r="D39" s="30" t="s">
-        <v>487</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>479</v>
-      </c>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="55" t="s">
+        <v>600</v>
+      </c>
+      <c r="F39" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="G39" s="51" t="s">
+        <v>562</v>
+      </c>
       <c r="H39" s="51"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
+      <c r="I39" s="52" t="s">
+        <v>597</v>
+      </c>
+      <c r="J39" s="52" t="s">
+        <v>597</v>
+      </c>
+      <c r="K39" s="52" t="s">
+        <v>597</v>
+      </c>
+      <c r="L39" s="52" t="s">
+        <v>566</v>
+      </c>
+      <c r="M39" s="53" t="s">
+        <v>598</v>
+      </c>
+      <c r="N39" s="53" t="s">
+        <v>599</v>
+      </c>
     </row>
-    <row r="40" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="51"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
       <c r="D40" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>489</v>
+        <v>601</v>
+      </c>
+      <c r="E40" s="56" t="s">
+        <v>450</v>
       </c>
       <c r="F40" s="51"/>
       <c r="G40" s="51"/>
@@ -3585,12 +3741,16 @@
       <c r="M40" s="52"/>
       <c r="N40" s="52"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="51"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
+      <c r="D41" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>460</v>
+      </c>
       <c r="F41" s="51"/>
       <c r="G41" s="51"/>
       <c r="H41" s="51"/>
@@ -3601,12 +3761,16 @@
       <c r="M41" s="52"/>
       <c r="N41" s="52"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="51"/>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
+      <c r="D42" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>462</v>
+      </c>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
       <c r="H42" s="51"/>
@@ -3617,12 +3781,16 @@
       <c r="M42" s="52"/>
       <c r="N42" s="52"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="51"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
+      <c r="D43" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>462</v>
+      </c>
       <c r="F43" s="51"/>
       <c r="G43" s="51"/>
       <c r="H43" s="51"/>
@@ -3633,12 +3801,16 @@
       <c r="M43" s="52"/>
       <c r="N43" s="52"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="51"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
+      <c r="D44" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="E44" s="49" t="s">
+        <v>465</v>
+      </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
       <c r="H44" s="51"/>
@@ -3649,12 +3821,16 @@
       <c r="M44" s="52"/>
       <c r="N44" s="52"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="51"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
+      <c r="D45" s="30" t="s">
+        <v>466</v>
+      </c>
+      <c r="E45" s="49" t="s">
+        <v>467</v>
+      </c>
       <c r="F45" s="51"/>
       <c r="G45" s="51"/>
       <c r="H45" s="51"/>
@@ -3665,12 +3841,16 @@
       <c r="M45" s="52"/>
       <c r="N45" s="52"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
+      <c r="D46" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E46" s="49" t="s">
+        <v>469</v>
+      </c>
       <c r="F46" s="51"/>
       <c r="G46" s="51"/>
       <c r="H46" s="51"/>
@@ -3681,12 +3861,16 @@
       <c r="M46" s="52"/>
       <c r="N46" s="52"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="51"/>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
+      <c r="D47" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="E47" s="49" t="s">
+        <v>469</v>
+      </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
       <c r="H47" s="51"/>
@@ -3697,12 +3881,16 @@
       <c r="M47" s="52"/>
       <c r="N47" s="52"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="51"/>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
+      <c r="D48" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>472</v>
+      </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
       <c r="H48" s="51"/>
@@ -3713,12 +3901,16 @@
       <c r="M48" s="52"/>
       <c r="N48" s="52"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="51"/>
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
+      <c r="D49" s="30" t="s">
+        <v>473</v>
+      </c>
+      <c r="E49" s="49" t="s">
+        <v>469</v>
+      </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
       <c r="H49" s="51"/>
@@ -3729,12 +3921,16 @@
       <c r="M49" s="52"/>
       <c r="N49" s="52"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="51"/>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
+      <c r="D50" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="E50" s="49" t="s">
+        <v>465</v>
+      </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
       <c r="H50" s="51"/>
@@ -3745,15 +3941,19 @@
       <c r="M50" s="52"/>
       <c r="N50" s="52"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="52"/>
+    <row r="51" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="30" t="s">
+        <v>475</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
       <c r="I51" s="52"/>
       <c r="J51" s="52"/>
       <c r="K51" s="52"/>
@@ -3761,12 +3961,355 @@
       <c r="M51" s="52"/>
       <c r="N51" s="52"/>
     </row>
+    <row r="52" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="51"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="52"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+    </row>
+    <row r="53" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="51"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="51"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
+    </row>
+    <row r="54" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="51"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="30" t="s">
+        <v>480</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="52"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="52"/>
+      <c r="L54" s="52"/>
+      <c r="M54" s="52"/>
+      <c r="N54" s="52"/>
+    </row>
+    <row r="55" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="51"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="30" t="s">
+        <v>481</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>482</v>
+      </c>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="52"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="52"/>
+      <c r="M55" s="52"/>
+      <c r="N55" s="52"/>
+    </row>
+    <row r="56" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="51"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>484</v>
+      </c>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
+      <c r="M56" s="52"/>
+      <c r="N56" s="52"/>
+    </row>
+    <row r="57" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="51"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="30" t="s">
+        <v>485</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="51"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="52"/>
+    </row>
+    <row r="58" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="51"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="52"/>
+      <c r="L58" s="52"/>
+      <c r="M58" s="52"/>
+      <c r="N58" s="52"/>
+    </row>
+    <row r="59" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="51"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>489</v>
+      </c>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="52"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="51"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="52"/>
+      <c r="N60" s="52"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="51"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="52"/>
+      <c r="M61" s="52"/>
+      <c r="N61" s="52"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="51"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="52"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="51"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="51"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="52"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="51"/>
+      <c r="B64" s="51"/>
+      <c r="C64" s="51"/>
+      <c r="D64" s="51"/>
+      <c r="E64" s="51"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="51"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="52"/>
+      <c r="N64" s="52"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="51"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="52"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="51"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="52"/>
+      <c r="N66" s="52"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="51"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
+      <c r="K67" s="52"/>
+      <c r="L67" s="52"/>
+      <c r="M67" s="52"/>
+      <c r="N67" s="52"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="51"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="52"/>
+      <c r="J68" s="52"/>
+      <c r="K68" s="52"/>
+      <c r="L68" s="52"/>
+      <c r="M68" s="52"/>
+      <c r="N68" s="52"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="51"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="52"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="52"/>
+      <c r="L69" s="52"/>
+      <c r="M69" s="52"/>
+      <c r="N69" s="52"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="52"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
+      <c r="I70" s="52"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="52"/>
+      <c r="L70" s="52"/>
+      <c r="M70" s="52"/>
+      <c r="N70" s="52"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="11">
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D36:D39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3852,7 +4395,7 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>578</v>
+        <v>602</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -3886,7 +4429,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>579</v>
+        <v>603</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -3936,7 +4479,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>580</v>
+        <v>604</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -3954,7 +4497,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>581</v>
+        <v>605</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -3972,7 +4515,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>582</v>
+        <v>606</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -3990,7 +4533,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>583</v>
+        <v>607</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -4024,7 +4567,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>584</v>
+        <v>608</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -4042,7 +4585,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -4060,7 +4603,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>586</v>
+        <v>610</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -4078,7 +4621,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -4112,7 +4655,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -4130,7 +4673,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -4164,7 +4707,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>590</v>
+        <v>614</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -4182,7 +4725,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>591</v>
+        <v>615</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -4216,7 +4759,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -4234,7 +4777,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>593</v>
+        <v>617</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -4252,7 +4795,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -4535,7 +5078,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>595</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Business domain - Completed flow for recieving inventory details, operating expenses and partial/full advanced payment
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="637">
   <si>
     <t>Term</t>
   </si>
@@ -1619,12 +1619,15 @@
     <t>When a delivery is made to subscriber(s),  the delivery amount should be debited from provisional revenue and respective provision account.</t>
   </si>
   <si>
+    <t>BasketDispatchStatusUpdatedEvent from subscriber domain (to revisit for adding basket cost – which will be credited to revenue and debited from booking amount – by business domain)</t>
+  </si>
+  <si>
+    <t>When a delivery is made to subscriber(s), its revenue is credited under “revenue” subject to receipt of payment. In case some of advanced payment made by subscriber still exists under booking amount, the delivery amount should be debited from booking amount and respective provision account.</t>
+  </si>
+  <si>
     <t>BasketDeliveryStatusEvent from subscriber domain</t>
   </si>
   <si>
-    <t>When a delivery is made to subscriber(s), its revenue is credited under “revenue” subject to receipt of payment. In case some of advanced payment made by subscriber still exists under booking amount, the delivery amount should be debited from booking amount and respective provision account.</t>
-  </si>
-  <si>
     <t>When interest is gained on booking amount, it will be credited to “interests”.</t>
   </si>
   <si>
@@ -1680,6 +1683,12 @@
   </si>
   <si>
     <t>BasketDeletedEvent in subscriber domain</t>
+  </si>
+  <si>
+    <t>External replenishment for account (via REST/UI etc.) - i.e. merchant will be able to either define provisions etc. Externally, or flow would handle it internally (i.e. carry forward after year end)</t>
+  </si>
+  <si>
+    <t>To be done</t>
   </si>
   <si>
     <t>Subscriber fills registration form to register on subscription website.</t>
@@ -1969,7 +1978,7 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for common expenses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
-    <t>Merchant will make provision for nodal account.</t>
+    <t>REMOVE : Merchant will make provision for nodal account.</t>
   </si>
   <si>
     <t>Value of provision for nodal account and provision date are received via REST controller</t>
@@ -1978,7 +1987,7 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for nodal account and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
-    <t>Merchant will make provision for revenue.</t>
+    <t>REMOVE : Merchant will make provision for revenue.</t>
   </si>
   <si>
     <t>Value of provision for revenue and provision date are received via REST controller</t>
@@ -1987,7 +1996,7 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for revenue and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
-    <t>Merchant will make provision for booking amount.</t>
+    <t>REMOVE : Merchant will make provision for booking amount.</t>
   </si>
   <si>
     <t>Value of provision for booking amount and provision date are received via REST controller</t>
@@ -2020,19 +2029,61 @@
     <t>ProductStatusReceivedEvent is received at business domain (from integration domain). The event contains inventory details (total purchase cost).</t>
   </si>
   <si>
+    <t>Total purchase cost is debited under ‘purchase cost’ and provision account for the same (i.e. purchase cost).</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>ProductStatusReceivedEvent</t>
-  </si>
-  <si>
-    <t>ProductStatusReceivedEventListener</t>
-  </si>
-  <si>
-    <t>Total purchase cost is debited under ‘purchase cost’ and provision account for the same (i.e. purchase cost).</t>
+    <t>ProductStatusReceivedCommand</t>
+  </si>
+  <si>
+    <t>ProductStatusReceivedCommandHandler</t>
+  </si>
+  <si>
+    <t>ProductStatusReceivedEvent, PurchaseCostCreditedEvent, PurchaseCostDebitedEvent</t>
+  </si>
+  <si>
+    <t>ProductStatusReceivedEventListener, PurchaseCostCreditedEventListener, PurchaseCostDebitedEventListener</t>
   </si>
   <si>
     <t>When system receives incoming operating expenses details from main application, they are debited under respective operating expense categories and respective provision account.</t>
+  </si>
+  <si>
+    <t>OperatingExpenseReceivedCommand</t>
+  </si>
+  <si>
+    <t>OperatingExpenseReceivedCommandHandler</t>
+  </si>
+  <si>
+    <t>OperatingExpenseReceivedEvent, OperatingExpenseCreditedEvent, OperatingExpenseDebitedEvent</t>
+  </si>
+  <si>
+    <t>OperatingExpenseReceivedEventListener, OperatingExpenseCreditedEventListener, OperatingExpenseDebitedEventListener</t>
+  </si>
+  <si>
+    <t>REMOVE : When a subscriber does subscription, but has not yet made payment, his total subscription value is credited to provisional revenue.</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedEvent from subscriber domain (to revisit)</t>
+  </si>
+  <si>
+    <t>PaymentProcessedCommand</t>
+  </si>
+  <si>
+    <t>PaymentProcessedCommandHandler</t>
+  </si>
+  <si>
+    <t>PaymentProcessedEvent, BookingAmountCreditedEvent</t>
+  </si>
+  <si>
+    <t>PaymentProcessedEventListener, BookingAmountCreditedEventListener</t>
+  </si>
+  <si>
+    <t>When a delivery is made to subscriber(s),  the delivery amount should be debited from booking amount and credited to revenue.</t>
+  </si>
+  <si>
+    <t>BasketDispatchStatusUpdatedEvent from subscriber domain</t>
   </si>
   <si>
     <t>Merchant make provision for initial investment</t>
@@ -2096,7 +2147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2175,8 +2226,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2204,6 +2261,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -2270,7 +2333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2483,6 +2546,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2495,8 +2562,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2691,60 +2766,60 @@
   <sheetData>
     <row r="1" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -2765,10 +2840,10 @@
   </sheetPr>
   <dimension ref="A2:N70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2806,7 +2881,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>20</v>
@@ -2835,7 +2910,7 @@
     </row>
     <row r="3" customFormat="false" ht="95.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="51" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
@@ -2899,45 +2974,45 @@
       <c r="A6" s="51"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="53" t="s">
         <v>451</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H6" s="51"/>
-      <c r="I6" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J6" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K6" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L6" s="53" t="s">
+      <c r="I6" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M6" s="53" t="s">
+      <c r="J6" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N6" s="53" t="s">
+      <c r="K6" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L6" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M6" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N6" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
-      <c r="D7" s="30"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -2953,9 +3028,9 @@
       <c r="A8" s="51"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="30" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -2971,45 +3046,45 @@
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="53" t="s">
         <v>453</v>
       </c>
       <c r="E9" s="30" t="s">
+        <v>574</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>565</v>
+      </c>
+      <c r="H9" s="51"/>
+      <c r="I9" s="54" t="s">
+        <v>566</v>
+      </c>
+      <c r="J9" s="54" t="s">
+        <v>567</v>
+      </c>
+      <c r="K9" s="54" t="s">
+        <v>568</v>
+      </c>
+      <c r="L9" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M9" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N9" s="54" t="s">
         <v>571</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G9" s="51" t="s">
-        <v>562</v>
-      </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J9" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K9" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L9" s="53" t="s">
-        <v>566</v>
-      </c>
-      <c r="M9" s="53" t="s">
-        <v>567</v>
-      </c>
-      <c r="N9" s="53" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -3025,9 +3100,9 @@
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -3043,45 +3118,45 @@
       <c r="A12" s="51"/>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="53" t="s">
         <v>454</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G12" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H12" s="51"/>
-      <c r="I12" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K12" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L12" s="53" t="s">
+      <c r="I12" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M12" s="53" t="s">
+      <c r="J12" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N12" s="53" t="s">
+      <c r="K12" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L12" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M12" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N12" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="51"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -3097,9 +3172,9 @@
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="30" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -3115,45 +3190,45 @@
       <c r="A15" s="51"/>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="53" t="s">
         <v>455</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H15" s="51"/>
-      <c r="I15" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J15" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K15" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L15" s="53" t="s">
+      <c r="I15" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M15" s="53" t="s">
+      <c r="J15" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N15" s="53" t="s">
+      <c r="K15" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L15" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M15" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N15" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51"/>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -3169,9 +3244,9 @@
       <c r="A17" s="51"/>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="53"/>
       <c r="E17" s="30" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -3187,45 +3262,45 @@
       <c r="A18" s="51"/>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
-      <c r="D18" s="30" t="s">
-        <v>577</v>
+      <c r="D18" s="53" t="s">
+        <v>580</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H18" s="51"/>
-      <c r="I18" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J18" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K18" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L18" s="53" t="s">
+      <c r="I18" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M18" s="53" t="s">
+      <c r="J18" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N18" s="53" t="s">
+      <c r="K18" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L18" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M18" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N18" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51"/>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
-      <c r="D19" s="30"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -3241,9 +3316,9 @@
       <c r="A20" s="51"/>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
-      <c r="D20" s="30"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="30" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -3259,45 +3334,45 @@
       <c r="A21" s="51"/>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
-      <c r="D21" s="30" t="s">
-        <v>580</v>
+      <c r="D21" s="53" t="s">
+        <v>583</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G21" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H21" s="51"/>
-      <c r="I21" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J21" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K21" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L21" s="53" t="s">
+      <c r="I21" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M21" s="53" t="s">
+      <c r="J21" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N21" s="53" t="s">
+      <c r="K21" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L21" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M21" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N21" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51"/>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
-      <c r="D22" s="30"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -3313,9 +3388,9 @@
       <c r="A23" s="51"/>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
-      <c r="D23" s="30"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="30" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -3331,45 +3406,45 @@
       <c r="A24" s="51"/>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
-      <c r="D24" s="30" t="s">
-        <v>583</v>
+      <c r="D24" s="53" t="s">
+        <v>586</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H24" s="51"/>
-      <c r="I24" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J24" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K24" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L24" s="53" t="s">
+      <c r="I24" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M24" s="53" t="s">
+      <c r="J24" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N24" s="53" t="s">
+      <c r="K24" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L24" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M24" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N24" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="51"/>
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
-      <c r="D25" s="30"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -3385,9 +3460,9 @@
       <c r="A26" s="51"/>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
-      <c r="D26" s="30"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="30" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -3403,45 +3478,45 @@
       <c r="A27" s="51"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
-      <c r="D27" s="30" t="s">
-        <v>586</v>
+      <c r="D27" s="53" t="s">
+        <v>589</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G27" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H27" s="51"/>
-      <c r="I27" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J27" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K27" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L27" s="53" t="s">
+      <c r="I27" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M27" s="53" t="s">
+      <c r="J27" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N27" s="53" t="s">
+      <c r="K27" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L27" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M27" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N27" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
-      <c r="D28" s="30"/>
+      <c r="D28" s="53"/>
       <c r="E28" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -3457,9 +3532,9 @@
       <c r="A29" s="51"/>
       <c r="B29" s="51"/>
       <c r="C29" s="51"/>
-      <c r="D29" s="30"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="30" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -3475,45 +3550,45 @@
       <c r="A30" s="51"/>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
-      <c r="D30" s="30" t="s">
-        <v>589</v>
+      <c r="D30" s="53" t="s">
+        <v>592</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="F30" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G30" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H30" s="51"/>
-      <c r="I30" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J30" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K30" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L30" s="53" t="s">
+      <c r="I30" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M30" s="53" t="s">
+      <c r="J30" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N30" s="53" t="s">
+      <c r="K30" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L30" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M30" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N30" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="51"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
-      <c r="D31" s="30"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -3529,9 +3604,9 @@
       <c r="A32" s="51"/>
       <c r="B32" s="51"/>
       <c r="C32" s="51"/>
-      <c r="D32" s="30"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="30" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -3547,45 +3622,45 @@
       <c r="A33" s="51"/>
       <c r="B33" s="51"/>
       <c r="C33" s="51"/>
-      <c r="D33" s="30" t="s">
-        <v>592</v>
+      <c r="D33" s="53" t="s">
+        <v>595</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="F33" s="51" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="G33" s="51" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="H33" s="51"/>
-      <c r="I33" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="J33" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="K33" s="53" t="s">
-        <v>565</v>
-      </c>
-      <c r="L33" s="53" t="s">
+      <c r="I33" s="54" t="s">
         <v>566</v>
       </c>
-      <c r="M33" s="53" t="s">
+      <c r="J33" s="54" t="s">
         <v>567</v>
       </c>
-      <c r="N33" s="53" t="s">
+      <c r="K33" s="54" t="s">
         <v>568</v>
+      </c>
+      <c r="L33" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M33" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="N33" s="54" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="51"/>
       <c r="B34" s="51"/>
       <c r="C34" s="51"/>
-      <c r="D34" s="30"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="30" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -3601,9 +3676,9 @@
       <c r="A35" s="51"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
-      <c r="D35" s="30"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="30" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -3619,8 +3694,8 @@
       <c r="A36" s="51"/>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
-      <c r="D36" s="30" t="s">
-        <v>595</v>
+      <c r="D36" s="53" t="s">
+        <v>598</v>
       </c>
       <c r="E36" s="30" t="s">
         <v>456</v>
@@ -3639,8 +3714,8 @@
       <c r="A37" s="51"/>
       <c r="B37" s="51"/>
       <c r="C37" s="51"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="54" t="s">
+      <c r="D37" s="53"/>
+      <c r="E37" s="55" t="s">
         <v>457</v>
       </c>
       <c r="F37" s="51"/>
@@ -3657,89 +3732,89 @@
       <c r="A38" s="51"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="55" t="s">
-        <v>596</v>
-      </c>
-      <c r="F38" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G38" s="51" t="s">
-        <v>562</v>
-      </c>
-      <c r="H38" s="51"/>
-      <c r="I38" s="52" t="s">
-        <v>597</v>
-      </c>
-      <c r="J38" s="52" t="s">
-        <v>597</v>
-      </c>
-      <c r="K38" s="52" t="s">
-        <v>597</v>
-      </c>
-      <c r="L38" s="52" t="s">
-        <v>566</v>
-      </c>
-      <c r="M38" s="53" t="s">
-        <v>598</v>
-      </c>
-      <c r="N38" s="53" t="s">
+      <c r="D38" s="53"/>
+      <c r="E38" s="56" t="s">
         <v>599</v>
       </c>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
     </row>
-    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="51"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="55" t="s">
+      <c r="D39" s="53"/>
+      <c r="E39" s="56" t="s">
         <v>600</v>
       </c>
-      <c r="F39" s="51" t="s">
-        <v>561</v>
-      </c>
-      <c r="G39" s="51" t="s">
-        <v>562</v>
-      </c>
-      <c r="H39" s="51"/>
-      <c r="I39" s="52" t="s">
-        <v>597</v>
-      </c>
-      <c r="J39" s="52" t="s">
-        <v>597</v>
-      </c>
-      <c r="K39" s="52" t="s">
-        <v>597</v>
-      </c>
-      <c r="L39" s="52" t="s">
-        <v>566</v>
-      </c>
-      <c r="M39" s="53" t="s">
-        <v>598</v>
-      </c>
-      <c r="N39" s="53" t="s">
-        <v>599</v>
+      <c r="F39" s="54" t="s">
+        <v>564</v>
+      </c>
+      <c r="G39" s="54" t="s">
+        <v>565</v>
+      </c>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54" t="s">
+        <v>601</v>
+      </c>
+      <c r="J39" s="54" t="s">
+        <v>602</v>
+      </c>
+      <c r="K39" s="54" t="s">
+        <v>603</v>
+      </c>
+      <c r="L39" s="54" t="s">
+        <v>569</v>
+      </c>
+      <c r="M39" s="54" t="s">
+        <v>604</v>
+      </c>
+      <c r="N39" s="54" t="s">
+        <v>605</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="51"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="53" t="s">
+        <v>606</v>
+      </c>
+      <c r="E40" s="58" t="s">
+        <v>450</v>
+      </c>
+      <c r="F40" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="G40" s="51" t="s">
+        <v>565</v>
+      </c>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51" t="s">
         <v>601</v>
       </c>
-      <c r="E40" s="56" t="s">
-        <v>450</v>
-      </c>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
+      <c r="J40" s="54" t="s">
+        <v>607</v>
+      </c>
+      <c r="K40" s="54" t="s">
+        <v>608</v>
+      </c>
+      <c r="L40" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="M40" s="51" t="s">
+        <v>609</v>
+      </c>
+      <c r="N40" s="51" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="51"/>
@@ -3805,11 +3880,11 @@
       <c r="A44" s="51"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
-      <c r="D44" s="30" t="s">
-        <v>464</v>
+      <c r="D44" s="53" t="s">
+        <v>611</v>
       </c>
       <c r="E44" s="49" t="s">
-        <v>465</v>
+        <v>612</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -3825,30 +3900,46 @@
       <c r="A45" s="51"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="53" t="s">
         <v>466</v>
       </c>
       <c r="E45" s="49" t="s">
         <v>467</v>
       </c>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
+      <c r="F45" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="G45" s="51" t="s">
+        <v>565</v>
+      </c>
       <c r="H45" s="51"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
+      <c r="I45" s="51" t="s">
+        <v>601</v>
+      </c>
+      <c r="J45" s="51" t="s">
+        <v>613</v>
+      </c>
+      <c r="K45" s="51" t="s">
+        <v>614</v>
+      </c>
+      <c r="L45" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="M45" s="51" t="s">
+        <v>615</v>
+      </c>
+      <c r="N45" s="59" t="s">
+        <v>616</v>
+      </c>
     </row>
-    <row r="46" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
       <c r="D46" s="30" t="s">
-        <v>468</v>
-      </c>
-      <c r="E46" s="49" t="s">
+        <v>617</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>469</v>
       </c>
       <c r="F46" s="51"/>
@@ -3869,7 +3960,7 @@
         <v>470</v>
       </c>
       <c r="E47" s="49" t="s">
-        <v>469</v>
+        <v>618</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -3886,10 +3977,10 @@
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
       <c r="D48" s="30" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F48" s="51"/>
       <c r="G48" s="51"/>
@@ -3906,10 +3997,10 @@
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
       <c r="D49" s="30" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>469</v>
+        <v>618</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -3926,7 +4017,7 @@
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
       <c r="D50" s="30" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E50" s="49" t="s">
         <v>465</v>
@@ -3946,10 +4037,10 @@
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
       <c r="D51" s="30" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -3966,7 +4057,7 @@
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
       <c r="D52" s="30" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E52" s="30" t="s">
         <v>447</v>
@@ -3986,10 +4077,10 @@
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
       <c r="D53" s="30" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -4006,10 +4097,10 @@
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
       <c r="D54" s="30" t="s">
+        <v>481</v>
+      </c>
+      <c r="E54" s="30" t="s">
         <v>480</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>479</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -4026,10 +4117,10 @@
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
       <c r="D55" s="30" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -4046,10 +4137,10 @@
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
       <c r="D56" s="30" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E56" s="30" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -4066,10 +4157,10 @@
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
       <c r="D57" s="30" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -4086,10 +4177,10 @@
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
       <c r="D58" s="30" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -4106,10 +4197,10 @@
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
       <c r="D59" s="30" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -4390,12 +4481,12 @@
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="51" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>602</v>
+        <v>619</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -4429,7 +4520,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>603</v>
+        <v>620</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -4479,7 +4570,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>604</v>
+        <v>621</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -4497,7 +4588,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>605</v>
+        <v>622</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -4515,7 +4606,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>606</v>
+        <v>623</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -4533,7 +4624,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>607</v>
+        <v>624</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -4567,7 +4658,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>608</v>
+        <v>625</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -4585,7 +4676,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>609</v>
+        <v>626</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -4603,7 +4694,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>610</v>
+        <v>627</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -4621,7 +4712,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>611</v>
+        <v>628</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -4655,7 +4746,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -4673,7 +4764,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -4707,7 +4798,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>614</v>
+        <v>631</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -4725,7 +4816,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>615</v>
+        <v>632</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -4759,7 +4850,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>616</v>
+        <v>633</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -4777,7 +4868,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>617</v>
+        <v>634</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -4795,7 +4886,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>618</v>
+        <v>635</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -5078,7 +5169,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>619</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -35099,8 +35190,8 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35312,7 +35403,7 @@
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
     </row>
-    <row r="12" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="42"/>
       <c r="B12" s="47"/>
       <c r="C12" s="42" t="s">
@@ -35325,7 +35416,7 @@
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
     </row>
-    <row r="13" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="42"/>
       <c r="B13" s="47"/>
       <c r="C13" s="42" t="s">
@@ -35338,7 +35429,7 @@
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
     </row>
-    <row r="14" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
       <c r="B14" s="47"/>
       <c r="C14" s="42" t="s">
@@ -35351,7 +35442,7 @@
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
     </row>
-    <row r="15" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="42"/>
       <c r="B15" s="47"/>
       <c r="C15" s="42" t="s">
@@ -35364,7 +35455,7 @@
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
     </row>
-    <row r="16" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
       <c r="B16" s="47"/>
       <c r="C16" s="42" t="s">
@@ -35377,7 +35468,7 @@
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
     </row>
-    <row r="17" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
       <c r="B17" s="47"/>
       <c r="C17" s="42" t="s">
@@ -35390,7 +35481,7 @@
       <c r="F17" s="42"/>
       <c r="G17" s="42"/>
     </row>
-    <row r="18" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="47"/>
       <c r="C18" s="42" t="s">
@@ -35403,7 +35494,7 @@
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
     </row>
-    <row r="19" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="47"/>
       <c r="C19" s="42" t="s">
@@ -35416,7 +35507,7 @@
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
     </row>
-    <row r="20" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
       <c r="B20" s="47"/>
       <c r="C20" s="42" t="s">
@@ -35429,7 +35520,7 @@
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
     </row>
-    <row r="21" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
       <c r="B21" s="47"/>
       <c r="C21" s="42" t="s">
@@ -35442,7 +35533,7 @@
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
     </row>
-    <row r="22" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
       <c r="B22" s="47"/>
       <c r="C22" s="42" t="s">
@@ -35455,7 +35546,7 @@
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
     </row>
-    <row r="23" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="42"/>
       <c r="B23" s="47"/>
       <c r="C23" s="42" t="s">
@@ -35468,7 +35559,7 @@
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
     </row>
-    <row r="24" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="42"/>
       <c r="B24" s="47"/>
       <c r="C24" s="42" t="s">
@@ -35481,63 +35572,63 @@
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
     </row>
-    <row r="25" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="42"/>
       <c r="B25" s="47"/>
       <c r="C25" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="4" t="s">
         <v>469</v>
       </c>
       <c r="E25" s="42"/>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
     </row>
-    <row r="26" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="42"/>
       <c r="B26" s="47"/>
       <c r="C26" s="42" t="s">
         <v>470</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E26" s="42"/>
       <c r="F26" s="42"/>
       <c r="G26" s="42"/>
     </row>
-    <row r="27" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="42"/>
       <c r="B27" s="47"/>
       <c r="C27" s="42" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E27" s="42"/>
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
     </row>
-    <row r="28" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="42"/>
       <c r="B28" s="47"/>
       <c r="C28" s="42" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E28" s="42"/>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
     </row>
-    <row r="29" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="42"/>
       <c r="B29" s="47"/>
       <c r="C29" s="42" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D29" s="49" t="s">
         <v>465</v>
@@ -35546,24 +35637,24 @@
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
     </row>
-    <row r="30" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="42"/>
       <c r="B30" s="47"/>
       <c r="C30" s="42" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
     </row>
-    <row r="31" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="42"/>
       <c r="B31" s="47"/>
       <c r="C31" s="42" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D31" s="42" t="s">
         <v>447</v>
@@ -35572,102 +35663,106 @@
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
     </row>
-    <row r="32" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="42"/>
       <c r="B32" s="47"/>
       <c r="C32" s="42" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E32" s="42"/>
       <c r="F32" s="42"/>
       <c r="G32" s="42"/>
     </row>
-    <row r="33" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="42"/>
       <c r="B33" s="47"/>
       <c r="C33" s="42" t="s">
+        <v>481</v>
+      </c>
+      <c r="D33" s="42" t="s">
         <v>480</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>479</v>
       </c>
       <c r="E33" s="42"/>
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
     </row>
-    <row r="34" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="42"/>
       <c r="B34" s="47"/>
       <c r="C34" s="42" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E34" s="42"/>
       <c r="F34" s="42"/>
       <c r="G34" s="42"/>
     </row>
-    <row r="35" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="42"/>
       <c r="B35" s="47"/>
       <c r="C35" s="42" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E35" s="42"/>
       <c r="F35" s="42"/>
       <c r="G35" s="42"/>
     </row>
-    <row r="36" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="42"/>
       <c r="B36" s="47"/>
       <c r="C36" s="42" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
     </row>
-    <row r="37" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="42"/>
       <c r="B37" s="47"/>
       <c r="C37" s="42" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
     </row>
-    <row r="38" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="42"/>
       <c r="B38" s="47"/>
       <c r="C38" s="42" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D38" s="42" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E38" s="42"/>
       <c r="F38" s="42"/>
       <c r="G38" s="42"/>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="42"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="42" t="s">
+        <v>491</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>492</v>
+      </c>
       <c r="E39" s="42"/>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
@@ -35734,32 +35829,32 @@
         <v>44</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="G46" s="42"/>
     </row>
     <row r="47" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="42"/>
       <c r="B47" s="42" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="E47" s="42" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
@@ -35768,13 +35863,13 @@
       <c r="A48" s="42"/>
       <c r="B48" s="42"/>
       <c r="C48" s="42" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="F48" s="42"/>
       <c r="G48" s="42"/>
@@ -35783,13 +35878,13 @@
       <c r="A49" s="42"/>
       <c r="B49" s="42"/>
       <c r="C49" s="42" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="F49" s="42"/>
       <c r="G49" s="42"/>
@@ -35798,13 +35893,13 @@
       <c r="A50" s="42"/>
       <c r="B50" s="42"/>
       <c r="C50" s="42" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="F50" s="42"/>
       <c r="G50" s="42"/>
@@ -35813,13 +35908,13 @@
       <c r="A51" s="42"/>
       <c r="B51" s="42"/>
       <c r="C51" s="42" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="E51" s="42" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
@@ -35828,13 +35923,13 @@
       <c r="A52" s="42"/>
       <c r="B52" s="42"/>
       <c r="C52" s="42" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
@@ -35846,10 +35941,10 @@
         <v>132</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
@@ -35857,16 +35952,16 @@
     <row r="54" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="42"/>
       <c r="B54" s="42" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
@@ -35874,16 +35969,16 @@
     <row r="55" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="42"/>
       <c r="B55" s="42" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E55" s="42" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="F55" s="42"/>
       <c r="G55" s="42"/>
@@ -35891,16 +35986,16 @@
     <row r="56" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="42"/>
       <c r="B56" s="42" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C56" s="42" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E56" s="42" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="F56" s="42"/>
       <c r="G56" s="42"/>
@@ -35909,13 +36004,13 @@
       <c r="A57" s="42"/>
       <c r="B57" s="42"/>
       <c r="C57" s="42" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="E57" s="42" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="F57" s="42"/>
       <c r="G57" s="42"/>
@@ -35923,7 +36018,7 @@
     <row r="58" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="42"/>
       <c r="B58" s="42" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
@@ -35940,7 +36035,7 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="F4:F8"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B11:B38"/>
+    <mergeCell ref="B11:B39"/>
     <mergeCell ref="B47:B53"/>
     <mergeCell ref="B56:B57"/>
   </mergeCells>
@@ -35982,7 +36077,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35990,7 +36085,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35998,7 +36093,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36006,7 +36101,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36014,7 +36109,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36022,7 +36117,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36030,7 +36125,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36038,7 +36133,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36046,7 +36141,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36054,7 +36149,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36062,7 +36157,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36070,7 +36165,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36078,7 +36173,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36086,7 +36181,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36094,7 +36189,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Business domain - Completed flow for recieving delivery details
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="641">
   <si>
     <t>Term</t>
   </si>
@@ -2081,6 +2081,18 @@
   </si>
   <si>
     <t>When a delivery is made to subscriber(s),  the delivery amount should be debited from booking amount and credited to revenue.</t>
+  </si>
+  <si>
+    <t>BasketDispatchStatusUpdatedCommand</t>
+  </si>
+  <si>
+    <t>BasketDispatchStatusUpdatedCommandHandler</t>
+  </si>
+  <si>
+    <t>BasketDispatchStatusUpdatedEvent, BookingAmountDebitedEvent, RevenueCreditEvent</t>
+  </si>
+  <si>
+    <t>BasketDispatchStatusUpdatedEventListener, BookingAmountDebitedEventListener, RevenueCreditEventListener</t>
   </si>
   <si>
     <t>BasketDispatchStatusUpdatedEvent from subscriber domain</t>
@@ -3928,29 +3940,45 @@
       <c r="M45" s="51" t="s">
         <v>615</v>
       </c>
-      <c r="N45" s="59" t="s">
+      <c r="N45" s="51" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="53" t="s">
         <v>617</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
+      <c r="F46" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="G46" s="51" t="s">
+        <v>565</v>
+      </c>
       <c r="H46" s="51"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
+      <c r="I46" s="51" t="s">
+        <v>601</v>
+      </c>
+      <c r="J46" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="K46" s="51" t="s">
+        <v>619</v>
+      </c>
+      <c r="L46" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="M46" s="51" t="s">
+        <v>620</v>
+      </c>
+      <c r="N46" s="59" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="51"/>
@@ -3960,7 +3988,7 @@
         <v>470</v>
       </c>
       <c r="E47" s="49" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="F47" s="51"/>
       <c r="G47" s="51"/>
@@ -4000,7 +4028,7 @@
         <v>474</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -4486,7 +4514,7 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -4520,7 +4548,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -4570,7 +4598,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -4588,7 +4616,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -4606,7 +4634,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -4624,7 +4652,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -4658,7 +4686,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -4676,7 +4704,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -4694,7 +4722,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -4712,7 +4740,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -4746,7 +4774,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -4764,7 +4792,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -4798,7 +4826,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -4816,7 +4844,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -4850,7 +4878,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -4868,7 +4896,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -4886,7 +4914,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -5169,7 +5197,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Business domain - Completed flow for recieving benefits
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="647">
   <si>
     <t>Term</t>
   </si>
@@ -2096,6 +2096,24 @@
   </si>
   <si>
     <t>BasketDispatchStatusUpdatedEvent from subscriber domain</t>
+  </si>
+  <si>
+    <t>BasketDispatchStatusUpdatedEvent from subscriber domain (to revisit – whether expense should be part of BasketDispachStatusUpdatedEvent – or should subscriber domain fire another OperatingExpenseReceivedEvent?)</t>
+  </si>
+  <si>
+    <t>NA/</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedCommand</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedCommandHandler</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedEvent, BenefitDebitedEvent, BenefitCreditedEvent</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedEventListener, BenefitDebitedEventListener, BenefitCreditedEventListener</t>
   </si>
   <si>
     <t>Merchant make provision for initial investment</t>
@@ -2852,10 +2870,10 @@
   </sheetPr>
   <dimension ref="A2:N70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D46" activeCellId="0" sqref="D46"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3976,7 +3994,7 @@
       <c r="M46" s="51" t="s">
         <v>620</v>
       </c>
-      <c r="N46" s="59" t="s">
+      <c r="N46" s="51" t="s">
         <v>621</v>
       </c>
     </row>
@@ -3984,21 +4002,37 @@
       <c r="A47" s="51"/>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="53" t="s">
         <v>470</v>
       </c>
       <c r="E47" s="49" t="s">
         <v>622</v>
       </c>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
+      <c r="F47" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="G47" s="51" t="s">
+        <v>565</v>
+      </c>
       <c r="H47" s="51"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
-      <c r="K47" s="52"/>
-      <c r="L47" s="52"/>
-      <c r="M47" s="52"/>
-      <c r="N47" s="52"/>
+      <c r="I47" s="51" t="s">
+        <v>601</v>
+      </c>
+      <c r="J47" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="K47" s="51" t="s">
+        <v>619</v>
+      </c>
+      <c r="L47" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="M47" s="51" t="s">
+        <v>620</v>
+      </c>
+      <c r="N47" s="51" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="51"/>
@@ -4027,8 +4061,8 @@
       <c r="D49" s="30" t="s">
         <v>474</v>
       </c>
-      <c r="E49" s="49" t="s">
-        <v>622</v>
+      <c r="E49" s="4" t="s">
+        <v>623</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -4040,25 +4074,41 @@
       <c r="M49" s="52"/>
       <c r="N49" s="52"/>
     </row>
-    <row r="50" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="51"/>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="53" t="s">
         <v>475</v>
       </c>
       <c r="E50" s="49" t="s">
         <v>465</v>
       </c>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
+      <c r="F50" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="G50" s="51" t="s">
+        <v>565</v>
+      </c>
       <c r="H50" s="51"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="52"/>
-      <c r="L50" s="52"/>
-      <c r="M50" s="52"/>
-      <c r="N50" s="52"/>
+      <c r="I50" s="51" t="s">
+        <v>624</v>
+      </c>
+      <c r="J50" s="51" t="s">
+        <v>625</v>
+      </c>
+      <c r="K50" s="51" t="s">
+        <v>626</v>
+      </c>
+      <c r="L50" s="51" t="s">
+        <v>569</v>
+      </c>
+      <c r="M50" s="51" t="s">
+        <v>627</v>
+      </c>
+      <c r="N50" s="59" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="51"/>
@@ -4514,7 +4564,7 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -4548,7 +4598,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -4598,7 +4648,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -4616,7 +4666,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -4634,7 +4684,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -4652,7 +4702,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>628</v>
+        <v>634</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -4686,7 +4736,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -4704,7 +4754,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>630</v>
+        <v>636</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -4722,7 +4772,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -4740,7 +4790,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -4774,7 +4824,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -4792,7 +4842,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -4826,7 +4876,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -4844,7 +4894,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -4878,7 +4928,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -4896,7 +4946,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -4914,7 +4964,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -5197,7 +5247,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Business domain - Refactored accounts and events. Also made relevant changes in user stories.
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="681">
   <si>
     <t>Term</t>
   </si>
@@ -1918,6 +1918,15 @@
     <t>BDGT_01</t>
   </si>
   <si>
+    <t>BDGT_02</t>
+  </si>
+  <si>
+    <t>BDGT_03</t>
+  </si>
+  <si>
+    <t>BDGT_04</t>
+  </si>
+  <si>
     <t>Value of provision for losses and provision date are received via REST controller</t>
   </si>
   <si>
@@ -1951,24 +1960,36 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for losses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_05</t>
+  </si>
+  <si>
     <t>Value of provision for benefits and provision date are received via REST controller</t>
   </si>
   <si>
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for benefits and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_06</t>
+  </si>
+  <si>
     <t>Value of provision for taxes and provision date are received via REST controller</t>
   </si>
   <si>
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for taxes and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_07</t>
+  </si>
+  <si>
     <t>Value of provision for others and provision date are received via REST controller</t>
   </si>
   <si>
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for others and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_08</t>
+  </si>
+  <si>
     <t>Merchant will make provision for common expenses.</t>
   </si>
   <si>
@@ -1978,6 +1999,9 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for common expenses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_09</t>
+  </si>
+  <si>
     <t>REMOVE : Merchant will make provision for nodal account.</t>
   </si>
   <si>
@@ -1987,6 +2011,9 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for nodal account and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_10</t>
+  </si>
+  <si>
     <t>REMOVE : Merchant will make provision for revenue.</t>
   </si>
   <si>
@@ -1996,6 +2023,9 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for revenue and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_11</t>
+  </si>
+  <si>
     <t>REMOVE : Merchant will make provision for booking amount.</t>
   </si>
   <si>
@@ -2005,6 +2035,9 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for booking amount and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_12</t>
+  </si>
+  <si>
     <t>Merchant will make provision for subscription specific expenses.</t>
   </si>
   <si>
@@ -2014,6 +2047,9 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for subscription specific expenses and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_13</t>
+  </si>
+  <si>
     <t>Merchant will make provision for purchase cost.</t>
   </si>
   <si>
@@ -2023,6 +2059,9 @@
     <t>CreateProvisionCommandHandler fires CreateProvisionEvent which will update provision for purchase cost and provision date to both – aggregate (BusinessAccount) and view (BusinessAccountView)</t>
   </si>
   <si>
+    <t>BDGT_14</t>
+  </si>
+  <si>
     <t>Receiving inventory details</t>
   </si>
   <si>
@@ -2047,6 +2086,9 @@
     <t>ProductStatusReceivedEventListener, PurchaseCostCreditedEventListener, PurchaseCostDebitedEventListener</t>
   </si>
   <si>
+    <t>BDGT_15</t>
+  </si>
+  <si>
     <t>When system receives incoming operating expenses details from main application, they are debited under respective operating expense categories and respective provision account.</t>
   </si>
   <si>
@@ -2062,12 +2104,27 @@
     <t>OperatingExpenseReceivedEventListener, OperatingExpenseCreditedEventListener, OperatingExpenseDebitedEventListener</t>
   </si>
   <si>
+    <t>BDGT_16</t>
+  </si>
+  <si>
+    <t>BDGT_17</t>
+  </si>
+  <si>
+    <t>BDGT_18</t>
+  </si>
+  <si>
+    <t>BDGT_19</t>
+  </si>
+  <si>
     <t>REMOVE : When a subscriber does subscription, but has not yet made payment, his total subscription value is credited to provisional revenue.</t>
   </si>
   <si>
     <t>SubscriptionActivatedEvent from subscriber domain (to revisit)</t>
   </si>
   <si>
+    <t>BDGT_20</t>
+  </si>
+  <si>
     <t>PaymentProcessedCommand</t>
   </si>
   <si>
@@ -2080,6 +2137,9 @@
     <t>PaymentProcessedEventListener, BookingAmountCreditedEventListener</t>
   </si>
   <si>
+    <t>BDGT_21</t>
+  </si>
+  <si>
     <t>When a delivery is made to subscriber(s),  the delivery amount should be debited from booking amount and credited to revenue.</t>
   </si>
   <si>
@@ -2095,12 +2155,24 @@
     <t>BasketDispatchStatusUpdatedEventListener, BookingAmountDebitedEventListener, RevenueCreditEventListener</t>
   </si>
   <si>
+    <t>BDGT_22</t>
+  </si>
+  <si>
     <t>BasketDispatchStatusUpdatedEvent from subscriber domain</t>
   </si>
   <si>
+    <t>BDGT_23</t>
+  </si>
+  <si>
+    <t>BDGT_24</t>
+  </si>
+  <si>
     <t>BasketDispatchStatusUpdatedEvent from subscriber domain (to revisit – whether expense should be part of BasketDispachStatusUpdatedEvent – or should subscriber domain fire another OperatingExpenseReceivedEvent?)</t>
   </si>
   <si>
+    <t>BDGT_25</t>
+  </si>
+  <si>
     <t>NA/</t>
   </si>
   <si>
@@ -2114,6 +2186,36 @@
   </si>
   <si>
     <t>SubscriptionActivatedEventListener, BenefitDebitedEventListener, BenefitCreditedEventListener</t>
+  </si>
+  <si>
+    <t>BDGT_26</t>
+  </si>
+  <si>
+    <t>BDGT_27</t>
+  </si>
+  <si>
+    <t>BDGT_28</t>
+  </si>
+  <si>
+    <t>BDGT_29</t>
+  </si>
+  <si>
+    <t>BDGT_30</t>
+  </si>
+  <si>
+    <t>BDGT_31</t>
+  </si>
+  <si>
+    <t>BDGT_32</t>
+  </si>
+  <si>
+    <t>SubscriptionActivatedEvent from subscriber domain (to be done) – check if duplicate of BDGT_25</t>
+  </si>
+  <si>
+    <t>BDGT_33</t>
+  </si>
+  <si>
+    <t>BDGT_34</t>
   </si>
   <si>
     <t>Merchant make provision for initial investment</t>
@@ -2177,7 +2279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2255,12 +2357,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2363,7 +2459,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2600,10 +2696,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2684,7 +2776,7 @@
   <dimension ref="C1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+      <selection pane="topLeft" activeCell="D47" activeCellId="1" sqref="F57:N57 D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2782,7 +2874,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F57:N57 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2870,10 +2962,10 @@
   </sheetPr>
   <dimension ref="A2:N70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F57" activeCellId="0" sqref="F57:N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2960,8 +3052,10 @@
       <c r="M3" s="52"/>
       <c r="N3" s="52"/>
     </row>
-    <row r="4" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51"/>
+    <row r="4" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="51" t="s">
+        <v>563</v>
+      </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
       <c r="D4" s="30" t="s">
@@ -2980,8 +3074,10 @@
       <c r="M4" s="52"/>
       <c r="N4" s="52"/>
     </row>
-    <row r="5" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51"/>
+    <row r="5" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="51" t="s">
+        <v>564</v>
+      </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="30" t="s">
@@ -3001,39 +3097,41 @@
       <c r="N5" s="52"/>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51"/>
+      <c r="A6" s="51" t="s">
+        <v>565</v>
+      </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="53" t="s">
         <v>451</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H6" s="51"/>
       <c r="I6" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J6" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K6" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L6" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N6" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3042,7 +3140,7 @@
       <c r="C7" s="51"/>
       <c r="D7" s="53"/>
       <c r="E7" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -3060,7 +3158,7 @@
       <c r="C8" s="51"/>
       <c r="D8" s="53"/>
       <c r="E8" s="30" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -3073,39 +3171,41 @@
       <c r="N8" s="52"/>
     </row>
     <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51"/>
+      <c r="A9" s="51" t="s">
+        <v>577</v>
+      </c>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="53" t="s">
         <v>453</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G9" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H9" s="51"/>
       <c r="I9" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J9" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K9" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L9" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M9" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N9" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,7 +3214,7 @@
       <c r="C10" s="51"/>
       <c r="D10" s="53"/>
       <c r="E10" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -3132,7 +3232,7 @@
       <c r="C11" s="51"/>
       <c r="D11" s="53"/>
       <c r="E11" s="30" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -3145,39 +3245,41 @@
       <c r="N11" s="52"/>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51"/>
+      <c r="A12" s="51" t="s">
+        <v>580</v>
+      </c>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
       <c r="D12" s="53" t="s">
         <v>454</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G12" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H12" s="51"/>
       <c r="I12" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J12" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K12" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L12" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M12" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N12" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3288,7 @@
       <c r="C13" s="51"/>
       <c r="D13" s="53"/>
       <c r="E13" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
@@ -3204,7 +3306,7 @@
       <c r="C14" s="51"/>
       <c r="D14" s="53"/>
       <c r="E14" s="30" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -3217,39 +3319,41 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="51"/>
+      <c r="A15" s="51" t="s">
+        <v>583</v>
+      </c>
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="53" t="s">
         <v>455</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H15" s="51"/>
       <c r="I15" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J15" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K15" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L15" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N15" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,7 +3362,7 @@
       <c r="C16" s="51"/>
       <c r="D16" s="53"/>
       <c r="E16" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -3276,7 +3380,7 @@
       <c r="C17" s="51"/>
       <c r="D17" s="53"/>
       <c r="E17" s="30" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -3289,39 +3393,41 @@
       <c r="N17" s="52"/>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="51"/>
+      <c r="A18" s="51" t="s">
+        <v>586</v>
+      </c>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="53" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H18" s="51"/>
       <c r="I18" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J18" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K18" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M18" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N18" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,7 +3436,7 @@
       <c r="C19" s="51"/>
       <c r="D19" s="53"/>
       <c r="E19" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -3348,7 +3454,7 @@
       <c r="C20" s="51"/>
       <c r="D20" s="53"/>
       <c r="E20" s="30" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -3361,39 +3467,41 @@
       <c r="N20" s="52"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="51"/>
+      <c r="A21" s="51" t="s">
+        <v>590</v>
+      </c>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="53" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G21" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H21" s="51"/>
       <c r="I21" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J21" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K21" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L21" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M21" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N21" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,7 +3510,7 @@
       <c r="C22" s="51"/>
       <c r="D22" s="53"/>
       <c r="E22" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -3420,7 +3528,7 @@
       <c r="C23" s="51"/>
       <c r="D23" s="53"/>
       <c r="E23" s="30" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -3433,39 +3541,41 @@
       <c r="N23" s="52"/>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="51"/>
+      <c r="A24" s="51" t="s">
+        <v>594</v>
+      </c>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="53" t="s">
-        <v>586</v>
+        <v>595</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>587</v>
+        <v>596</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H24" s="51"/>
       <c r="I24" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J24" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K24" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L24" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M24" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N24" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3474,7 +3584,7 @@
       <c r="C25" s="51"/>
       <c r="D25" s="53"/>
       <c r="E25" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
@@ -3492,7 +3602,7 @@
       <c r="C26" s="51"/>
       <c r="D26" s="53"/>
       <c r="E26" s="30" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
@@ -3505,39 +3615,41 @@
       <c r="N26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="51"/>
+      <c r="A27" s="51" t="s">
+        <v>598</v>
+      </c>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
       <c r="D27" s="53" t="s">
-        <v>589</v>
+        <v>599</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G27" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H27" s="51"/>
       <c r="I27" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J27" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K27" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L27" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M27" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N27" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,7 +3658,7 @@
       <c r="C28" s="51"/>
       <c r="D28" s="53"/>
       <c r="E28" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
@@ -3564,7 +3676,7 @@
       <c r="C29" s="51"/>
       <c r="D29" s="53"/>
       <c r="E29" s="30" t="s">
-        <v>591</v>
+        <v>601</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
@@ -3577,39 +3689,41 @@
       <c r="N29" s="52"/>
     </row>
     <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="51"/>
+      <c r="A30" s="51" t="s">
+        <v>602</v>
+      </c>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
       <c r="D30" s="53" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="F30" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G30" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H30" s="51"/>
       <c r="I30" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J30" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K30" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L30" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M30" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N30" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3732,7 @@
       <c r="C31" s="51"/>
       <c r="D31" s="53"/>
       <c r="E31" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F31" s="51"/>
       <c r="G31" s="51"/>
@@ -3636,7 +3750,7 @@
       <c r="C32" s="51"/>
       <c r="D32" s="53"/>
       <c r="E32" s="30" t="s">
-        <v>594</v>
+        <v>605</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="51"/>
@@ -3649,39 +3763,41 @@
       <c r="N32" s="52"/>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="51"/>
+      <c r="A33" s="51" t="s">
+        <v>606</v>
+      </c>
       <c r="B33" s="51"/>
       <c r="C33" s="51"/>
       <c r="D33" s="53" t="s">
-        <v>595</v>
+        <v>607</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>596</v>
+        <v>608</v>
       </c>
       <c r="F33" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G33" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H33" s="51"/>
       <c r="I33" s="54" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="J33" s="54" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K33" s="54" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="L33" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M33" s="54" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="N33" s="54" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3690,7 +3806,7 @@
       <c r="C34" s="51"/>
       <c r="D34" s="53"/>
       <c r="E34" s="30" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
@@ -3708,7 +3824,7 @@
       <c r="C35" s="51"/>
       <c r="D35" s="53"/>
       <c r="E35" s="30" t="s">
-        <v>597</v>
+        <v>609</v>
       </c>
       <c r="F35" s="51"/>
       <c r="G35" s="51"/>
@@ -3721,11 +3837,13 @@
       <c r="N35" s="52"/>
     </row>
     <row r="36" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="51"/>
+      <c r="A36" s="51" t="s">
+        <v>610</v>
+      </c>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
       <c r="D36" s="53" t="s">
-        <v>598</v>
+        <v>611</v>
       </c>
       <c r="E36" s="30" t="s">
         <v>456</v>
@@ -3764,7 +3882,7 @@
       <c r="C38" s="51"/>
       <c r="D38" s="53"/>
       <c r="E38" s="56" t="s">
-        <v>599</v>
+        <v>612</v>
       </c>
       <c r="F38" s="57"/>
       <c r="G38" s="57"/>
@@ -3782,72 +3900,76 @@
       <c r="C39" s="51"/>
       <c r="D39" s="53"/>
       <c r="E39" s="56" t="s">
-        <v>600</v>
+        <v>613</v>
       </c>
       <c r="F39" s="54" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G39" s="54" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H39" s="54"/>
       <c r="I39" s="54" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
       <c r="J39" s="54" t="s">
-        <v>602</v>
+        <v>615</v>
       </c>
       <c r="K39" s="54" t="s">
-        <v>603</v>
+        <v>616</v>
       </c>
       <c r="L39" s="54" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M39" s="54" t="s">
-        <v>604</v>
+        <v>617</v>
       </c>
       <c r="N39" s="54" t="s">
-        <v>605</v>
+        <v>618</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="51"/>
+      <c r="A40" s="51" t="s">
+        <v>619</v>
+      </c>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
       <c r="D40" s="53" t="s">
-        <v>606</v>
+        <v>620</v>
       </c>
       <c r="E40" s="58" t="s">
         <v>450</v>
       </c>
       <c r="F40" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G40" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H40" s="51"/>
       <c r="I40" s="51" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
       <c r="J40" s="54" t="s">
-        <v>607</v>
+        <v>621</v>
       </c>
       <c r="K40" s="54" t="s">
-        <v>608</v>
+        <v>622</v>
       </c>
       <c r="L40" s="51" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M40" s="51" t="s">
-        <v>609</v>
+        <v>623</v>
       </c>
       <c r="N40" s="51" t="s">
-        <v>610</v>
+        <v>624</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="51"/>
+      <c r="A41" s="51" t="s">
+        <v>625</v>
+      </c>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
       <c r="D41" s="30" t="s">
@@ -3867,7 +3989,9 @@
       <c r="N41" s="52"/>
     </row>
     <row r="42" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="51"/>
+      <c r="A42" s="51" t="s">
+        <v>626</v>
+      </c>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
       <c r="D42" s="30" t="s">
@@ -3887,7 +4011,9 @@
       <c r="N42" s="52"/>
     </row>
     <row r="43" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="51"/>
+      <c r="A43" s="51" t="s">
+        <v>627</v>
+      </c>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
       <c r="D43" s="30" t="s">
@@ -3907,14 +4033,16 @@
       <c r="N43" s="52"/>
     </row>
     <row r="44" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="51"/>
+      <c r="A44" s="51" t="s">
+        <v>628</v>
+      </c>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
       <c r="D44" s="53" t="s">
-        <v>611</v>
+        <v>629</v>
       </c>
       <c r="E44" s="49" t="s">
-        <v>612</v>
+        <v>630</v>
       </c>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
@@ -3927,7 +4055,9 @@
       <c r="N44" s="52"/>
     </row>
     <row r="45" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="51"/>
+      <c r="A45" s="51" t="s">
+        <v>631</v>
+      </c>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
       <c r="D45" s="53" t="s">
@@ -3937,105 +4067,111 @@
         <v>467</v>
       </c>
       <c r="F45" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G45" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H45" s="51"/>
       <c r="I45" s="51" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
       <c r="J45" s="51" t="s">
-        <v>613</v>
+        <v>632</v>
       </c>
       <c r="K45" s="51" t="s">
-        <v>614</v>
+        <v>633</v>
       </c>
       <c r="L45" s="51" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M45" s="51" t="s">
-        <v>615</v>
+        <v>634</v>
       </c>
       <c r="N45" s="51" t="s">
-        <v>616</v>
+        <v>635</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="51"/>
+      <c r="A46" s="51" t="s">
+        <v>636</v>
+      </c>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
       <c r="D46" s="53" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>469</v>
       </c>
       <c r="F46" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G46" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H46" s="51"/>
       <c r="I46" s="51" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
       <c r="J46" s="51" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
       <c r="K46" s="51" t="s">
-        <v>619</v>
+        <v>639</v>
       </c>
       <c r="L46" s="51" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M46" s="51" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="N46" s="51" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="51"/>
+      <c r="A47" s="51" t="s">
+        <v>642</v>
+      </c>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
       <c r="D47" s="53" t="s">
         <v>470</v>
       </c>
       <c r="E47" s="49" t="s">
-        <v>622</v>
+        <v>643</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G47" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H47" s="51"/>
       <c r="I47" s="51" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
       <c r="J47" s="51" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
       <c r="K47" s="51" t="s">
-        <v>619</v>
+        <v>639</v>
       </c>
       <c r="L47" s="51" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M47" s="51" t="s">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="N47" s="51" t="s">
-        <v>621</v>
+        <v>641</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="51"/>
+      <c r="A48" s="51" t="s">
+        <v>644</v>
+      </c>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
       <c r="D48" s="30" t="s">
@@ -4055,14 +4191,16 @@
       <c r="N48" s="52"/>
     </row>
     <row r="49" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="51"/>
+      <c r="A49" s="51" t="s">
+        <v>645</v>
+      </c>
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
       <c r="D49" s="30" t="s">
         <v>474</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>623</v>
+        <v>646</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -4075,7 +4213,9 @@
       <c r="N49" s="52"/>
     </row>
     <row r="50" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="51"/>
+      <c r="A50" s="51" t="s">
+        <v>647</v>
+      </c>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
       <c r="D50" s="53" t="s">
@@ -4085,33 +4225,35 @@
         <v>465</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G50" s="51" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="H50" s="51"/>
       <c r="I50" s="51" t="s">
-        <v>624</v>
+        <v>648</v>
       </c>
       <c r="J50" s="51" t="s">
-        <v>625</v>
+        <v>649</v>
       </c>
       <c r="K50" s="51" t="s">
-        <v>626</v>
+        <v>650</v>
       </c>
       <c r="L50" s="51" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="M50" s="51" t="s">
-        <v>627</v>
-      </c>
-      <c r="N50" s="59" t="s">
-        <v>628</v>
+        <v>651</v>
+      </c>
+      <c r="N50" s="51" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="51"/>
+      <c r="A51" s="51" t="s">
+        <v>653</v>
+      </c>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
       <c r="D51" s="30" t="s">
@@ -4131,7 +4273,9 @@
       <c r="N51" s="52"/>
     </row>
     <row r="52" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="51"/>
+      <c r="A52" s="51" t="s">
+        <v>654</v>
+      </c>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
       <c r="D52" s="30" t="s">
@@ -4151,7 +4295,9 @@
       <c r="N52" s="52"/>
     </row>
     <row r="53" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="51"/>
+      <c r="A53" s="51" t="s">
+        <v>655</v>
+      </c>
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
       <c r="D53" s="30" t="s">
@@ -4171,7 +4317,9 @@
       <c r="N53" s="52"/>
     </row>
     <row r="54" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="51"/>
+      <c r="A54" s="51" t="s">
+        <v>656</v>
+      </c>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
       <c r="D54" s="30" t="s">
@@ -4191,7 +4339,9 @@
       <c r="N54" s="52"/>
     </row>
     <row r="55" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="51"/>
+      <c r="A55" s="51" t="s">
+        <v>657</v>
+      </c>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
       <c r="D55" s="30" t="s">
@@ -4211,7 +4361,9 @@
       <c r="N55" s="52"/>
     </row>
     <row r="56" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="51"/>
+      <c r="A56" s="51" t="s">
+        <v>658</v>
+      </c>
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
       <c r="D56" s="30" t="s">
@@ -4230,28 +4382,48 @@
       <c r="M56" s="52"/>
       <c r="N56" s="52"/>
     </row>
-    <row r="57" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="51"/>
+    <row r="57" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="51" t="s">
+        <v>659</v>
+      </c>
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="53" t="s">
         <v>486</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="F57" s="51"/>
-      <c r="G57" s="51"/>
+        <v>660</v>
+      </c>
+      <c r="F57" s="51" t="s">
+        <v>567</v>
+      </c>
+      <c r="G57" s="51" t="s">
+        <v>568</v>
+      </c>
       <c r="H57" s="51"/>
-      <c r="I57" s="52"/>
-      <c r="J57" s="52"/>
-      <c r="K57" s="52"/>
-      <c r="L57" s="52"/>
-      <c r="M57" s="52"/>
-      <c r="N57" s="52"/>
+      <c r="I57" s="51" t="s">
+        <v>648</v>
+      </c>
+      <c r="J57" s="51" t="s">
+        <v>649</v>
+      </c>
+      <c r="K57" s="51" t="s">
+        <v>650</v>
+      </c>
+      <c r="L57" s="51" t="s">
+        <v>572</v>
+      </c>
+      <c r="M57" s="51" t="s">
+        <v>651</v>
+      </c>
+      <c r="N57" s="51" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="51"/>
+      <c r="A58" s="51" t="s">
+        <v>661</v>
+      </c>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
       <c r="D58" s="30" t="s">
@@ -4271,7 +4443,9 @@
       <c r="N58" s="52"/>
     </row>
     <row r="59" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="51"/>
+      <c r="A59" s="51" t="s">
+        <v>662</v>
+      </c>
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
       <c r="D59" s="30" t="s">
@@ -4467,17 +4641,28 @@
       <c r="N70" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="22">
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A12:A14"/>
     <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="D15:D17"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="D24:D26"/>
+    <mergeCell ref="A27:A29"/>
     <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A33:A35"/>
     <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A36:A39"/>
     <mergeCell ref="D36:D39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4498,7 +4683,7 @@
   <dimension ref="A2:N41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="F57:N57 E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4564,7 +4749,7 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>629</v>
+        <v>663</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -4598,7 +4783,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>630</v>
+        <v>664</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -4648,7 +4833,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>631</v>
+        <v>665</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -4666,7 +4851,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>632</v>
+        <v>666</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -4684,7 +4869,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>633</v>
+        <v>667</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -4702,7 +4887,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>634</v>
+        <v>668</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -4736,7 +4921,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>635</v>
+        <v>669</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -4754,7 +4939,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>636</v>
+        <v>670</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -4772,7 +4957,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>637</v>
+        <v>671</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -4790,7 +4975,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>638</v>
+        <v>672</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -4824,7 +5009,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>639</v>
+        <v>673</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -4842,7 +5027,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>640</v>
+        <v>674</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -4876,7 +5061,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>641</v>
+        <v>675</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -4894,7 +5079,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>642</v>
+        <v>676</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -4928,7 +5113,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>643</v>
+        <v>677</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -4946,7 +5131,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>644</v>
+        <v>678</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -4964,7 +5149,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>645</v>
+        <v>679</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -5236,7 +5421,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F57:N57 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5247,7 +5432,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>646</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -5271,7 +5456,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topRight" activeCell="D6" activeCellId="1" sqref="F57:N57 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -33861,7 +34046,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="F57:N57 C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34083,7 +34268,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E7" activeCellId="1" sqref="F57:N57 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34836,7 +35021,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="F57:N57 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34984,7 +35169,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F57:N57 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35150,7 +35335,7 @@
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="F57:N57 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35269,7 +35454,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="F57:N57 D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -36135,7 +36320,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F57:N57 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Business domain - fixed typos/errors in user stories
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="682">
   <si>
     <t>Term</t>
   </si>
@@ -2195,6 +2195,9 @@
   </si>
   <si>
     <t>BDGT_28</t>
+  </si>
+  <si>
+    <t>When an item is cancelled or replaced from subscription, appropriate item cancellation event should be fired from subscriber domain and they should debit booking amount.</t>
   </si>
   <si>
     <t>BDGT_29</t>
@@ -2776,7 +2779,7 @@
   <dimension ref="C1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="1" sqref="F57:N57 D47"/>
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2874,7 +2877,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F57:N57 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2962,10 +2965,10 @@
   </sheetPr>
   <dimension ref="A2:N70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F57" activeCellId="0" sqref="F57:N57"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4301,7 +4304,7 @@
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
       <c r="D53" s="30" t="s">
-        <v>479</v>
+        <v>656</v>
       </c>
       <c r="E53" s="30" t="s">
         <v>480</v>
@@ -4318,7 +4321,7 @@
     </row>
     <row r="54" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="51" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
@@ -4340,7 +4343,7 @@
     </row>
     <row r="55" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="51" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
@@ -4362,7 +4365,7 @@
     </row>
     <row r="56" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="51" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
@@ -4384,7 +4387,7 @@
     </row>
     <row r="57" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="51" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
@@ -4392,7 +4395,7 @@
         <v>486</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F57" s="51" t="s">
         <v>567</v>
@@ -4422,7 +4425,7 @@
     </row>
     <row r="58" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="51" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
@@ -4444,7 +4447,7 @@
     </row>
     <row r="59" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="51" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
@@ -4683,7 +4686,7 @@
   <dimension ref="A2:N41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="F57:N57 E26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4749,7 +4752,7 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
@@ -4783,7 +4786,7 @@
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
@@ -4833,7 +4836,7 @@
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -4851,7 +4854,7 @@
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
@@ -4869,7 +4872,7 @@
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
@@ -4887,7 +4890,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="51" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -4921,7 +4924,7 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -4939,7 +4942,7 @@
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -4957,7 +4960,7 @@
       <c r="B15" s="51"/>
       <c r="C15" s="51"/>
       <c r="D15" s="51" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -4975,7 +4978,7 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -5009,7 +5012,7 @@
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -5027,7 +5030,7 @@
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -5061,7 +5064,7 @@
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="51" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -5079,7 +5082,7 @@
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="51" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -5113,7 +5116,7 @@
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
       <c r="D24" s="51" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -5131,7 +5134,7 @@
       <c r="B25" s="51"/>
       <c r="C25" s="51"/>
       <c r="D25" s="51" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -5149,7 +5152,7 @@
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
       <c r="D26" s="51" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -5421,7 +5424,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="F57:N57 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5432,7 +5435,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -5456,7 +5459,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="0" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D6" activeCellId="1" sqref="F57:N57 D6"/>
+      <selection pane="topRight" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34046,7 +34049,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="F57:N57 C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34268,7 +34271,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E7" activeCellId="1" sqref="F57:N57 E7"/>
+      <selection pane="bottomLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35021,7 +35024,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="F57:N57 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35169,7 +35172,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F57:N57 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35335,7 +35338,7 @@
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="F57:N57 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35454,7 +35457,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="F57:N57 D25"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -36320,7 +36323,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F57:N57 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Moved Performance trackers on read side and some code cleanup
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -743,12 +743,6 @@
     <t>PR_06</t>
   </si>
   <si>
-    <t>Replicate actuals of last year as forecast of current year</t>
-  </si>
-  <si>
-    <t>As a System I will replicate actuals of last year in the forecast of current year in an yearly batch job so as to provide default values for the forecast for current year which administrator can modify wherever required.</t>
-  </si>
-  <si>
     <t>Yearly/half yearly batch,product account</t>
   </si>
   <si>
@@ -756,31 +750,6 @@
   </si>
   <si>
     <t>Calculate foreasted values of defined metrics for a product</t>
-  </si>
-  <si>
-    <t>As a System I will calculate the following metrics when subscriber enters forecast details for a product
-1. Monthly operating expenses per product( sum of commong expenses and subscription specific expenses)
-2. Monthly sales and marketing expenses per product??
-3. Net new subscribers per period(month)
-4. Total subscribers per period(month)
-5. Total churned subscribers per period(month)
-6. Percentage churned subscribers per period(month)
-7.Monthly recurring revenue due to new subscribers( MRR New)
-8. Monthly churned revenue due loosing subscribers associated with each price bucket.
-9. Total Monthly churned revenue
-10. Percentage net revenue churn
-11. Monthly average revenue per subscriber(ARPS New)
-12. Monthly average revenue per total subscribers(ARPS)
-13. Total monthly revenue
-14. Total cost of goods sold
-15. Selling price derived from margin percentage
-16. Operating profit/loss
-17. Percentage operating profit/loss
-18. Subscriber lifetime value(SLV)
-19. Subscriber lifetime period
-20. Cost of acquiring a subscriber(CAS)
-21. SLV to CAS ratio
-22. Months to recover CAS</t>
   </si>
   <si>
     <t>PR_09</t>
@@ -2611,6 +2580,29 @@
     <t>Configure product  with pricing paramters</t>
   </si>
   <si>
+    <t>As an administrator I manually create demand and churn forecast for a product so as to compare the actual performance of that product against these predictions. The structure(for every product) will have following attributes.
+1. New subscriptions per period(week/month)
+2. Churned subscriptions per period(week/month) affiliated to each price bucket
+3. Total subscriptions per period
+3. From date of forecast
+4. To Date of Forecast
+5. purchase price per unit
+6. sale price per unit.</t>
+  </si>
+  <si>
+    <t>Capture demand and churn pseuo actuals for next day</t>
+  </si>
+  <si>
+    <t>As an administrator I manually create demand and churn forecast for a product  for next day so as to use it for calculating offer price for that product for the first time. The structure(for every product) will have following attributes.
+1. New subscriptions per period(week/month)
+2. Churned subscriptions per period(week/month) affiliated to each price bucket
+3. Total subscriptions per period
+3. From date of forecast
+4. To Date of Forecast
+5. purchase price per unit
+6. sale price per unit.</t>
+  </si>
+  <si>
     <t>As an Adminstrator I will define which Parameters shuld be used for detemining the product price so as to decide which data should be captured in product forecast
 1. Product Pricing Policy
  1.1 Instanteneous pricing
@@ -2619,32 +2611,40 @@
 3. Whether to include cross price elasticity(optional) in pricing calculation: true/false
 4. Whether to include advertising expenses(optional) in pricing calculation : true/false
 5. period for which daily actuals should be aggregated to, in order to compare with target figures( weekly ,monthly,quarterly)
-6. next forecast date ( derived by the prcing logic)
+6. next forecast date ( derived by the pricing logic)
 7. demand curve period( period for which historical data should be used for forecasting( last one year,last two years etc).
 8. Pricing options(if the system generated price shoul dbe automatically accepted as offered price, if system generated price should be ignored and price should be manually overridden by merchant  OR if the system generated price should be prompted to merchant for him to make a decision on its acceptance or overriding)</t>
   </si>
   <si>
-    <t>As an administrator I manually create demand and churn forecast for a product so as to compare the actual performance of that product against these predictions. The structure(for every product) will have following attributes.
-1. New subscriptions per period(week/month)
-2. Churned subscriptions per period(week/month) affiliated to each price bucket
-3. Total subscriptions per period
-3. From date of forecast
-4. To Date of Forecast
-5. purchase price per unit
-6. sale price per unit.</t>
-  </si>
-  <si>
-    <t>Capture demand and churn pseuo actuals for next day</t>
-  </si>
-  <si>
-    <t>As an administrator I manually create demand and churn forecast for a product  for next day so as to use it for calculating offer price for that product for the first time. The structure(for every product) will have following attributes.
-1. New subscriptions per period(week/month)
-2. Churned subscriptions per period(week/month) affiliated to each price bucket
-3. Total subscriptions per period
-3. From date of forecast
-4. To Date of Forecast
-5. purchase price per unit
-6. sale price per unit.</t>
+    <t>Define forecast of next yer using actuals of current year</t>
+  </si>
+  <si>
+    <t>As a System I will forecast consumption and churn of next year using actuals of current year in an yearly batch job so as to provide default values for the targets and forecasts for next year which administrator can modify wherever required.</t>
+  </si>
+  <si>
+    <t>As a System I will calculate the following metrics when subscriber enters forecast details for a product
+1. Monthly operating expenses per product( sum of common expenses and subscription specific expenses)
+2. Monthly sales and marketing expenses per product??
+3. Net new subscribers per period(month)
+4. Total subscribers per period(month)
+5. Total churned subscribers per period(month)
+6. Percentage churned subscribers per period(month)
+7.Monthly recurring revenue due to new subscribers( MRR New)
+8. Monthly churned revenue due loosing subscribers associated with each price bucket.
+9. Total Monthly churned revenue
+10. Percentage net revenue churn
+11. Monthly average revenue per subscriber(ARPS New)
+12. Monthly average revenue per total subscribers(ARPS)
+13. Total monthly revenue
+14. Total cost of goods sold
+15. Selling price derived from margin percentage
+16. Operating profit/loss
+17. Percentage operating profit/loss
+18. Subscriber lifetime value(SLV)
+19. Subscriber lifetime period
+20. Cost of acquiring a subscriber(CAS)
+21. SLV to CAS ratio
+22. Months to recover CAS</t>
   </si>
 </sst>
 </file>
@@ -3480,7 +3480,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>20</v>
@@ -3509,15 +3509,15 @@
     </row>
     <row r="3" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="D3" s="23" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
@@ -3531,15 +3531,15 @@
     </row>
     <row r="4" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
       <c r="D4" s="23" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -3553,15 +3553,15 @@
     </row>
     <row r="5" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
       <c r="D5" s="23" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -3575,40 +3575,40 @@
     </row>
     <row r="6" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="58" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
       <c r="D6" s="59" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>481</v>
+      </c>
+      <c r="G6" s="38" t="s">
         <v>482</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>483</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>484</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>485</v>
       </c>
       <c r="H6" s="38"/>
       <c r="I6" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L6" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="M6" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="N6" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M6" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N6" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -3617,7 +3617,7 @@
       <c r="C7" s="38"/>
       <c r="D7" s="59"/>
       <c r="E7" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -3635,7 +3635,7 @@
       <c r="C8" s="38"/>
       <c r="D8" s="59"/>
       <c r="E8" s="23" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -3649,40 +3649,40 @@
     </row>
     <row r="9" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="58" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="59" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J9" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K9" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L9" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="M9" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="N9" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L9" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M9" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N9" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -3691,7 +3691,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="59"/>
       <c r="E10" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
@@ -3709,7 +3709,7 @@
       <c r="C11" s="38"/>
       <c r="D11" s="59"/>
       <c r="E11" s="23" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
@@ -3723,40 +3723,40 @@
     </row>
     <row r="12" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="58" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
       <c r="D12" s="59" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H12" s="38"/>
       <c r="I12" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L12" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="M12" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K12" s="41" t="s">
+      <c r="N12" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L12" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M12" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N12" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -3765,7 +3765,7 @@
       <c r="C13" s="38"/>
       <c r="D13" s="59"/>
       <c r="E13" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -3783,7 +3783,7 @@
       <c r="C14" s="38"/>
       <c r="D14" s="59"/>
       <c r="E14" s="23" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
@@ -3797,40 +3797,40 @@
     </row>
     <row r="15" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="58" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="59" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L15" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="M15" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="N15" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L15" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M15" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N15" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -3839,7 +3839,7 @@
       <c r="C16" s="38"/>
       <c r="D16" s="59"/>
       <c r="E16" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F16" s="38"/>
       <c r="G16" s="38"/>
@@ -3857,7 +3857,7 @@
       <c r="C17" s="38"/>
       <c r="D17" s="59"/>
       <c r="E17" s="23" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
@@ -3871,40 +3871,40 @@
     </row>
     <row r="18" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="58" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="59" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H18" s="38"/>
       <c r="I18" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J18" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L18" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J18" s="41" t="s">
+      <c r="M18" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K18" s="41" t="s">
+      <c r="N18" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L18" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M18" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N18" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -3913,7 +3913,7 @@
       <c r="C19" s="38"/>
       <c r="D19" s="59"/>
       <c r="E19" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
@@ -3931,7 +3931,7 @@
       <c r="C20" s="38"/>
       <c r="D20" s="59"/>
       <c r="E20" s="23" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
@@ -3945,40 +3945,40 @@
     </row>
     <row r="21" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="58" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="59" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H21" s="38"/>
       <c r="I21" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K21" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L21" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J21" s="41" t="s">
+      <c r="M21" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K21" s="41" t="s">
+      <c r="N21" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L21" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M21" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N21" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -3987,7 +3987,7 @@
       <c r="C22" s="38"/>
       <c r="D22" s="59"/>
       <c r="E22" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F22" s="38"/>
       <c r="G22" s="38"/>
@@ -4005,7 +4005,7 @@
       <c r="C23" s="38"/>
       <c r="D23" s="59"/>
       <c r="E23" s="23" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="38"/>
@@ -4019,40 +4019,40 @@
     </row>
     <row r="24" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="58" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="59" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H24" s="38"/>
       <c r="I24" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J24" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K24" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L24" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J24" s="41" t="s">
+      <c r="M24" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="N24" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L24" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M24" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N24" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -4061,7 +4061,7 @@
       <c r="C25" s="38"/>
       <c r="D25" s="59"/>
       <c r="E25" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
@@ -4079,7 +4079,7 @@
       <c r="C26" s="38"/>
       <c r="D26" s="59"/>
       <c r="E26" s="23" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
@@ -4093,40 +4093,40 @@
     </row>
     <row r="27" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="58" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="59" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H27" s="38"/>
       <c r="I27" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J27" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K27" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L27" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J27" s="41" t="s">
+      <c r="M27" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K27" s="41" t="s">
+      <c r="N27" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L27" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M27" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N27" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -4135,7 +4135,7 @@
       <c r="C28" s="38"/>
       <c r="D28" s="59"/>
       <c r="E28" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -4153,7 +4153,7 @@
       <c r="C29" s="38"/>
       <c r="D29" s="59"/>
       <c r="E29" s="23" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
@@ -4167,40 +4167,40 @@
     </row>
     <row r="30" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B30" s="38"/>
       <c r="C30" s="38"/>
       <c r="D30" s="59" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H30" s="38"/>
       <c r="I30" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J30" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K30" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L30" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J30" s="41" t="s">
+      <c r="M30" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K30" s="41" t="s">
+      <c r="N30" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L30" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M30" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N30" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -4209,7 +4209,7 @@
       <c r="C31" s="38"/>
       <c r="D31" s="59"/>
       <c r="E31" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F31" s="38"/>
       <c r="G31" s="38"/>
@@ -4227,7 +4227,7 @@
       <c r="C32" s="38"/>
       <c r="D32" s="59"/>
       <c r="E32" s="23" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="38"/>
@@ -4241,40 +4241,40 @@
     </row>
     <row r="33" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="58" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
       <c r="D33" s="59" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G33" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H33" s="38"/>
       <c r="I33" s="41" t="s">
+        <v>483</v>
+      </c>
+      <c r="J33" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="K33" s="41" t="s">
+        <v>485</v>
+      </c>
+      <c r="L33" s="41" t="s">
         <v>486</v>
       </c>
-      <c r="J33" s="41" t="s">
+      <c r="M33" s="41" t="s">
         <v>487</v>
       </c>
-      <c r="K33" s="41" t="s">
+      <c r="N33" s="41" t="s">
         <v>488</v>
-      </c>
-      <c r="L33" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M33" s="41" t="s">
-        <v>490</v>
-      </c>
-      <c r="N33" s="41" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
@@ -4283,7 +4283,7 @@
       <c r="C34" s="38"/>
       <c r="D34" s="59"/>
       <c r="E34" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F34" s="38"/>
       <c r="G34" s="38"/>
@@ -4301,7 +4301,7 @@
       <c r="C35" s="38"/>
       <c r="D35" s="59"/>
       <c r="E35" s="23" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F35" s="38"/>
       <c r="G35" s="38"/>
@@ -4315,15 +4315,15 @@
     </row>
     <row r="36" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="58" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
       <c r="D36" s="59" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
@@ -4341,7 +4341,7 @@
       <c r="C37" s="38"/>
       <c r="D37" s="59"/>
       <c r="E37" s="42" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
@@ -4359,7 +4359,7 @@
       <c r="C38" s="38"/>
       <c r="D38" s="59"/>
       <c r="E38" s="43" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44"/>
@@ -4377,83 +4377,83 @@
       <c r="C39" s="38"/>
       <c r="D39" s="59"/>
       <c r="E39" s="43" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H39" s="41"/>
       <c r="I39" s="41" t="s">
+        <v>533</v>
+      </c>
+      <c r="J39" s="41" t="s">
+        <v>534</v>
+      </c>
+      <c r="K39" s="41" t="s">
+        <v>535</v>
+      </c>
+      <c r="L39" s="41" t="s">
+        <v>486</v>
+      </c>
+      <c r="M39" s="41" t="s">
         <v>536</v>
       </c>
-      <c r="J39" s="41" t="s">
+      <c r="N39" s="41" t="s">
         <v>537</v>
-      </c>
-      <c r="K39" s="41" t="s">
-        <v>538</v>
-      </c>
-      <c r="L39" s="41" t="s">
-        <v>489</v>
-      </c>
-      <c r="M39" s="41" t="s">
-        <v>539</v>
-      </c>
-      <c r="N39" s="41" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A40" s="38" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
       <c r="D40" s="40" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E40" s="45" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H40" s="38"/>
       <c r="I40" s="38" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J40" s="41" t="s">
+        <v>540</v>
+      </c>
+      <c r="K40" s="41" t="s">
+        <v>541</v>
+      </c>
+      <c r="L40" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="M40" s="38" t="s">
+        <v>542</v>
+      </c>
+      <c r="N40" s="38" t="s">
         <v>543</v>
-      </c>
-      <c r="K40" s="41" t="s">
-        <v>544</v>
-      </c>
-      <c r="L40" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="M40" s="38" t="s">
-        <v>545</v>
-      </c>
-      <c r="N40" s="38" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="38" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B41" s="38"/>
       <c r="C41" s="38"/>
       <c r="D41" s="23" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
@@ -4467,15 +4467,15 @@
     </row>
     <row r="42" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="38" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B42" s="38"/>
       <c r="C42" s="38"/>
       <c r="D42" s="23" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F42" s="38"/>
       <c r="G42" s="38"/>
@@ -4489,15 +4489,15 @@
     </row>
     <row r="43" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="38" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B43" s="38"/>
       <c r="C43" s="38"/>
       <c r="D43" s="23" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F43" s="38"/>
       <c r="G43" s="38"/>
@@ -4511,15 +4511,15 @@
     </row>
     <row r="44" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="38" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B44" s="38"/>
       <c r="C44" s="38"/>
       <c r="D44" s="40" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="F44" s="38"/>
       <c r="G44" s="38"/>
@@ -4533,129 +4533,129 @@
     </row>
     <row r="45" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="38" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B45" s="38"/>
       <c r="C45" s="38"/>
       <c r="D45" s="40" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H45" s="38"/>
       <c r="I45" s="38" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J45" s="38" t="s">
+        <v>558</v>
+      </c>
+      <c r="K45" s="38" t="s">
+        <v>559</v>
+      </c>
+      <c r="L45" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="M45" s="38" t="s">
+        <v>560</v>
+      </c>
+      <c r="N45" s="38" t="s">
         <v>561</v>
-      </c>
-      <c r="K45" s="38" t="s">
-        <v>562</v>
-      </c>
-      <c r="L45" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="M45" s="38" t="s">
-        <v>563</v>
-      </c>
-      <c r="N45" s="38" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" s="38" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B46" s="38"/>
       <c r="C46" s="38"/>
       <c r="D46" s="40" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H46" s="38"/>
       <c r="I46" s="38" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J46" s="38" t="s">
+        <v>565</v>
+      </c>
+      <c r="K46" s="38" t="s">
+        <v>566</v>
+      </c>
+      <c r="L46" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="M46" s="38" t="s">
+        <v>567</v>
+      </c>
+      <c r="N46" s="38" t="s">
         <v>568</v>
-      </c>
-      <c r="K46" s="38" t="s">
-        <v>569</v>
-      </c>
-      <c r="L46" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="M46" s="38" t="s">
-        <v>570</v>
-      </c>
-      <c r="N46" s="38" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A47" s="38" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B47" s="38"/>
       <c r="C47" s="38"/>
       <c r="D47" s="40" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G47" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H47" s="38"/>
       <c r="I47" s="38" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J47" s="38" t="s">
+        <v>565</v>
+      </c>
+      <c r="K47" s="38" t="s">
+        <v>566</v>
+      </c>
+      <c r="L47" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="M47" s="38" t="s">
+        <v>567</v>
+      </c>
+      <c r="N47" s="38" t="s">
         <v>568</v>
-      </c>
-      <c r="K47" s="38" t="s">
-        <v>569</v>
-      </c>
-      <c r="L47" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="M47" s="38" t="s">
-        <v>570</v>
-      </c>
-      <c r="N47" s="38" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="38" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B48" s="38"/>
       <c r="C48" s="38"/>
       <c r="D48" s="23" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F48" s="38"/>
       <c r="G48" s="38"/>
@@ -4669,91 +4669,91 @@
     </row>
     <row r="49" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A49" s="38" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
       <c r="D49" s="40" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F49" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G49" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H49" s="38"/>
       <c r="I49" s="38" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J49" s="38" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="K49" s="38" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="L49" s="38" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="M49" s="38" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="N49" s="38" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A50" s="38" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
       <c r="D50" s="40" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E50" s="46" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G50" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H50" s="38"/>
       <c r="I50" s="38" t="s">
+        <v>583</v>
+      </c>
+      <c r="J50" s="38" t="s">
+        <v>584</v>
+      </c>
+      <c r="K50" s="38" t="s">
+        <v>585</v>
+      </c>
+      <c r="L50" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="M50" s="38" t="s">
         <v>586</v>
       </c>
-      <c r="J50" s="38" t="s">
+      <c r="N50" s="38" t="s">
         <v>587</v>
-      </c>
-      <c r="K50" s="38" t="s">
-        <v>588</v>
-      </c>
-      <c r="L50" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="M50" s="38" t="s">
-        <v>589</v>
-      </c>
-      <c r="N50" s="38" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="38" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B51" s="38"/>
       <c r="C51" s="38"/>
       <c r="D51" s="23" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F51" s="38"/>
       <c r="G51" s="38"/>
@@ -4767,15 +4767,15 @@
     </row>
     <row r="52" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A52" s="38" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B52" s="38"/>
       <c r="C52" s="38"/>
       <c r="D52" s="23" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F52" s="38"/>
       <c r="G52" s="38"/>
@@ -4789,15 +4789,15 @@
     </row>
     <row r="53" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="38" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B53" s="38"/>
       <c r="C53" s="38"/>
       <c r="D53" s="23" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F53" s="38"/>
       <c r="G53" s="38"/>
@@ -4811,15 +4811,15 @@
     </row>
     <row r="54" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A54" s="38" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B54" s="38"/>
       <c r="C54" s="38"/>
       <c r="D54" s="23" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F54" s="38"/>
       <c r="G54" s="38"/>
@@ -4833,15 +4833,15 @@
     </row>
     <row r="55" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A55" s="38" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B55" s="38"/>
       <c r="C55" s="38"/>
       <c r="D55" s="23" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F55" s="38"/>
       <c r="G55" s="38"/>
@@ -4855,15 +4855,15 @@
     </row>
     <row r="56" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" s="38" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B56" s="38"/>
       <c r="C56" s="38"/>
       <c r="D56" s="23" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F56" s="38"/>
       <c r="G56" s="38"/>
@@ -4877,53 +4877,53 @@
     </row>
     <row r="57" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A57" s="38" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B57" s="38"/>
       <c r="C57" s="38"/>
       <c r="D57" s="40" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F57" s="38" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G57" s="38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H57" s="38"/>
       <c r="I57" s="38" t="s">
+        <v>583</v>
+      </c>
+      <c r="J57" s="38" t="s">
+        <v>584</v>
+      </c>
+      <c r="K57" s="38" t="s">
+        <v>585</v>
+      </c>
+      <c r="L57" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="M57" s="38" t="s">
         <v>586</v>
       </c>
-      <c r="J57" s="38" t="s">
+      <c r="N57" s="38" t="s">
         <v>587</v>
-      </c>
-      <c r="K57" s="38" t="s">
-        <v>588</v>
-      </c>
-      <c r="L57" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="M57" s="38" t="s">
-        <v>589</v>
-      </c>
-      <c r="N57" s="38" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" s="38" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B58" s="38"/>
       <c r="C58" s="38"/>
       <c r="D58" s="23" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F58" s="38"/>
       <c r="G58" s="38"/>
@@ -4937,15 +4937,15 @@
     </row>
     <row r="59" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="38" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B59" s="38"/>
       <c r="C59" s="38"/>
       <c r="D59" s="23" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F59" s="38"/>
       <c r="G59" s="38"/>
@@ -5227,12 +5227,12 @@
     </row>
     <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
@@ -5266,7 +5266,7 @@
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
       <c r="D5" s="38" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E5" s="38"/>
       <c r="F5" s="38"/>
@@ -5316,7 +5316,7 @@
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
@@ -5334,7 +5334,7 @@
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
@@ -5352,7 +5352,7 @@
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
@@ -5370,7 +5370,7 @@
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
@@ -5404,7 +5404,7 @@
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
       <c r="D13" s="38" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="38"/>
@@ -5422,7 +5422,7 @@
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
@@ -5440,7 +5440,7 @@
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="E15" s="38"/>
       <c r="F15" s="38"/>
@@ -5458,7 +5458,7 @@
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="38"/>
@@ -5492,7 +5492,7 @@
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="38"/>
@@ -5510,7 +5510,7 @@
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
@@ -5544,7 +5544,7 @@
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E21" s="38"/>
       <c r="F21" s="38"/>
@@ -5562,7 +5562,7 @@
       <c r="B22" s="38"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="38"/>
@@ -5596,7 +5596,7 @@
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="38" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
@@ -5614,7 +5614,7 @@
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
       <c r="D25" s="38" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="38"/>
@@ -5632,7 +5632,7 @@
       <c r="B26" s="38"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="38"/>
@@ -5907,7 +5907,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>
@@ -5941,22 +5941,22 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
+        <v>630</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>631</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>632</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>633</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="E2" s="47" t="s">
         <v>634</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="F2" s="47" t="s">
         <v>635</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>636</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>637</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -5964,19 +5964,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
+        <v>636</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>637</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>638</v>
+      </c>
+      <c r="E3" s="48" t="s">
         <v>639</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="F3" s="48" t="s">
         <v>640</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>641</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>642</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -5984,19 +5984,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="38" t="s">
+        <v>641</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>643</v>
+      </c>
+      <c r="E4" s="38" t="s">
         <v>644</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="F4" s="38" t="s">
         <v>645</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>646</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>647</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6004,19 +6004,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="38" t="s">
+        <v>646</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>647</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>648</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>649</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="F5" s="38" t="s">
         <v>650</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>651</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>652</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6024,19 +6024,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="38" t="s">
+        <v>651</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>652</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>653</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>654</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="F6" s="38" t="s">
         <v>655</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>656</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>657</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6044,17 +6044,17 @@
         <v>4</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="38" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6062,17 +6062,17 @@
         <v>5</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -6083,10 +6083,10 @@
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -6097,7 +6097,7 @@
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="F10" s="38"/>
     </row>
@@ -6109,7 +6109,7 @@
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="F11" s="38"/>
     </row>
@@ -6148,7 +6148,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="39"/>
       <c r="B16" s="48" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
@@ -6158,7 +6158,7 @@
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="39"/>
       <c r="B17" s="60" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C17" s="60"/>
       <c r="D17" s="38"/>
@@ -6168,7 +6168,7 @@
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="39"/>
       <c r="B18" s="60" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C18" s="60"/>
       <c r="D18" s="38"/>
@@ -6178,7 +6178,7 @@
     <row r="19" spans="1:6" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="39"/>
       <c r="B19" s="60" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C19" s="60"/>
       <c r="D19" s="38"/>
@@ -6188,7 +6188,7 @@
     <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="39"/>
       <c r="B20" s="60" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C20" s="60"/>
       <c r="D20" s="38"/>
@@ -6279,50 +6279,50 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
+        <v>673</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>674</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="D1" s="49" t="s">
         <v>676</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="E1" s="49" t="s">
         <v>677</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="F1" s="49" t="s">
         <v>678</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="G1" s="49" t="s">
         <v>679</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="H1" s="50" t="s">
         <v>680</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>681</v>
-      </c>
-      <c r="G1" s="49" t="s">
-        <v>682</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51"/>
       <c r="B2" s="61" t="s">
+        <v>681</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>682</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>683</v>
+      </c>
+      <c r="E2" s="61" t="s">
         <v>684</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="F2" s="61" t="s">
         <v>685</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>686</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>687</v>
-      </c>
-      <c r="F2" s="61" t="s">
-        <v>688</v>
       </c>
       <c r="G2" s="61"/>
       <c r="H2" s="62" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -6331,10 +6331,10 @@
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="51" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E3" s="61"/>
       <c r="F3" s="61"/>
@@ -6345,16 +6345,16 @@
       <c r="A4" s="51"/>
       <c r="B4" s="61"/>
       <c r="C4" s="52" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="G4" s="64"/>
     </row>
@@ -6362,10 +6362,10 @@
       <c r="A5" s="51"/>
       <c r="B5" s="61"/>
       <c r="C5" s="52" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="63"/>
@@ -6375,13 +6375,13 @@
       <c r="A6" s="51"/>
       <c r="B6" s="61"/>
       <c r="C6" s="52" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="F6" s="63"/>
       <c r="G6" s="64"/>
@@ -6399,13 +6399,13 @@
       <c r="A8" s="51"/>
       <c r="B8" s="61"/>
       <c r="C8" s="52" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="F8" s="63"/>
       <c r="G8" s="53"/>
@@ -6414,30 +6414,30 @@
       <c r="A9" s="51"/>
       <c r="B9" s="61"/>
       <c r="C9" s="51" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="F9" s="63"/>
       <c r="G9" s="51" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A10" s="51"/>
       <c r="B10" s="61"/>
       <c r="C10" s="51" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="F10" s="63"/>
       <c r="G10" s="51"/>
@@ -6446,50 +6446,50 @@
       <c r="A11" s="51"/>
       <c r="B11" s="61"/>
       <c r="C11" s="51" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
       <c r="H11" s="32" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="91" x14ac:dyDescent="0.35">
       <c r="A12" s="51"/>
       <c r="B12" s="54"/>
       <c r="C12" s="51" t="s">
+        <v>708</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>709</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>710</v>
+      </c>
+      <c r="F12" s="51" t="s">
         <v>711</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>712</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>713</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>714</v>
       </c>
       <c r="G12" s="51"/>
       <c r="H12" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="51"/>
       <c r="B13" s="65" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="51"/>
@@ -6499,10 +6499,10 @@
       <c r="A14" s="51"/>
       <c r="B14" s="65"/>
       <c r="C14" s="51" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
@@ -6512,10 +6512,10 @@
       <c r="A15" s="51"/>
       <c r="B15" s="65"/>
       <c r="C15" s="51" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
@@ -6525,10 +6525,10 @@
       <c r="A16" s="51"/>
       <c r="B16" s="65"/>
       <c r="C16" s="51" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="51"/>
@@ -6538,10 +6538,10 @@
       <c r="A17" s="51"/>
       <c r="B17" s="65"/>
       <c r="C17" s="51" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="51"/>
@@ -6551,10 +6551,10 @@
       <c r="A18" s="51"/>
       <c r="B18" s="65"/>
       <c r="C18" s="51" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
@@ -6564,10 +6564,10 @@
       <c r="A19" s="51"/>
       <c r="B19" s="65"/>
       <c r="C19" s="51" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
@@ -6577,10 +6577,10 @@
       <c r="A20" s="51"/>
       <c r="B20" s="65"/>
       <c r="C20" s="51" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E20" s="51"/>
       <c r="F20" s="51"/>
@@ -6590,10 +6590,10 @@
       <c r="A21" s="51"/>
       <c r="B21" s="65"/>
       <c r="C21" s="51" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
@@ -6603,10 +6603,10 @@
       <c r="A22" s="51"/>
       <c r="B22" s="65"/>
       <c r="C22" s="51" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
@@ -6616,10 +6616,10 @@
       <c r="A23" s="51"/>
       <c r="B23" s="65"/>
       <c r="C23" s="51" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E23" s="51"/>
       <c r="F23" s="51"/>
@@ -6629,10 +6629,10 @@
       <c r="A24" s="51"/>
       <c r="B24" s="65"/>
       <c r="C24" s="51" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E24" s="51"/>
       <c r="F24" s="51"/>
@@ -6642,10 +6642,10 @@
       <c r="A25" s="51"/>
       <c r="B25" s="65"/>
       <c r="C25" s="51" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
@@ -6655,10 +6655,10 @@
       <c r="A26" s="51"/>
       <c r="B26" s="65"/>
       <c r="C26" s="51" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D26" s="46" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -6668,10 +6668,10 @@
       <c r="A27" s="51"/>
       <c r="B27" s="65"/>
       <c r="C27" s="51" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="E27" s="51"/>
       <c r="F27" s="51"/>
@@ -6681,10 +6681,10 @@
       <c r="A28" s="51"/>
       <c r="B28" s="65"/>
       <c r="C28" s="51" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
@@ -6694,10 +6694,10 @@
       <c r="A29" s="51"/>
       <c r="B29" s="65"/>
       <c r="C29" s="51" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E29" s="51"/>
       <c r="F29" s="51"/>
@@ -6707,10 +6707,10 @@
       <c r="A30" s="51"/>
       <c r="B30" s="65"/>
       <c r="C30" s="51" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E30" s="51"/>
       <c r="F30" s="51"/>
@@ -6720,10 +6720,10 @@
       <c r="A31" s="51"/>
       <c r="B31" s="65"/>
       <c r="C31" s="51" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E31" s="51"/>
       <c r="F31" s="51"/>
@@ -6733,10 +6733,10 @@
       <c r="A32" s="51"/>
       <c r="B32" s="65"/>
       <c r="C32" s="51" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E32" s="51"/>
       <c r="F32" s="51"/>
@@ -6746,10 +6746,10 @@
       <c r="A33" s="51"/>
       <c r="B33" s="65"/>
       <c r="C33" s="51" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E33" s="51"/>
       <c r="F33" s="51"/>
@@ -6759,10 +6759,10 @@
       <c r="A34" s="51"/>
       <c r="B34" s="65"/>
       <c r="C34" s="51" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D34" s="51" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E34" s="51"/>
       <c r="F34" s="51"/>
@@ -6772,10 +6772,10 @@
       <c r="A35" s="51"/>
       <c r="B35" s="65"/>
       <c r="C35" s="51" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D35" s="51" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E35" s="51"/>
       <c r="F35" s="51"/>
@@ -6785,10 +6785,10 @@
       <c r="A36" s="51"/>
       <c r="B36" s="65"/>
       <c r="C36" s="51" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D36" s="51" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E36" s="51"/>
       <c r="F36" s="51"/>
@@ -6798,10 +6798,10 @@
       <c r="A37" s="51"/>
       <c r="B37" s="65"/>
       <c r="C37" s="51" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E37" s="51"/>
       <c r="F37" s="51"/>
@@ -6811,10 +6811,10 @@
       <c r="A38" s="51"/>
       <c r="B38" s="65"/>
       <c r="C38" s="51" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="E38" s="51"/>
       <c r="F38" s="51"/>
@@ -6824,10 +6824,10 @@
       <c r="A39" s="51"/>
       <c r="B39" s="65"/>
       <c r="C39" s="51" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E39" s="51"/>
       <c r="F39" s="51"/>
@@ -6837,10 +6837,10 @@
       <c r="A40" s="51"/>
       <c r="B40" s="65"/>
       <c r="C40" s="51" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E40" s="51"/>
       <c r="F40" s="51"/>
@@ -6850,10 +6850,10 @@
       <c r="A41" s="51"/>
       <c r="B41" s="65"/>
       <c r="C41" s="51" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D41" s="51" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E41" s="51"/>
       <c r="F41" s="51"/>
@@ -6921,32 +6921,32 @@
         <v>45</v>
       </c>
       <c r="C48" s="51" t="s">
+        <v>724</v>
+      </c>
+      <c r="D48" s="51" t="s">
+        <v>725</v>
+      </c>
+      <c r="E48" s="51" t="s">
+        <v>726</v>
+      </c>
+      <c r="F48" s="51" t="s">
         <v>727</v>
-      </c>
-      <c r="D48" s="51" t="s">
-        <v>728</v>
-      </c>
-      <c r="E48" s="51" t="s">
-        <v>729</v>
-      </c>
-      <c r="F48" s="51" t="s">
-        <v>730</v>
       </c>
       <c r="G48" s="51"/>
     </row>
     <row r="49" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="51"/>
       <c r="B49" s="61" t="s">
+        <v>728</v>
+      </c>
+      <c r="C49" s="51" t="s">
+        <v>729</v>
+      </c>
+      <c r="D49" s="51" t="s">
+        <v>730</v>
+      </c>
+      <c r="E49" s="51" t="s">
         <v>731</v>
-      </c>
-      <c r="C49" s="51" t="s">
-        <v>732</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>733</v>
-      </c>
-      <c r="E49" s="51" t="s">
-        <v>734</v>
       </c>
       <c r="F49" s="51"/>
       <c r="G49" s="51"/>
@@ -6955,13 +6955,13 @@
       <c r="A50" s="51"/>
       <c r="B50" s="61"/>
       <c r="C50" s="51" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D50" s="51" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="E50" s="51" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
@@ -6970,13 +6970,13 @@
       <c r="A51" s="51"/>
       <c r="B51" s="61"/>
       <c r="C51" s="51" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D51" s="51" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E51" s="51" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -6985,13 +6985,13 @@
       <c r="A52" s="51"/>
       <c r="B52" s="61"/>
       <c r="C52" s="51" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D52" s="51" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="E52" s="51" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
@@ -7000,13 +7000,13 @@
       <c r="A53" s="51"/>
       <c r="B53" s="61"/>
       <c r="C53" s="51" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D53" s="51" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="E53" s="51" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="F53" s="51"/>
       <c r="G53" s="51"/>
@@ -7015,13 +7015,13 @@
       <c r="A54" s="51"/>
       <c r="B54" s="61"/>
       <c r="C54" s="51" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="D54" s="51" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="E54" s="51" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="51"/>
@@ -7033,10 +7033,10 @@
         <v>121</v>
       </c>
       <c r="D55" s="51" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="E55" s="51" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="51"/>
@@ -7044,16 +7044,16 @@
     <row r="56" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A56" s="51"/>
       <c r="B56" s="51" t="s">
+        <v>749</v>
+      </c>
+      <c r="C56" s="51" t="s">
+        <v>750</v>
+      </c>
+      <c r="D56" s="51" t="s">
+        <v>751</v>
+      </c>
+      <c r="E56" s="51" t="s">
         <v>752</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>753</v>
-      </c>
-      <c r="D56" s="51" t="s">
-        <v>754</v>
-      </c>
-      <c r="E56" s="51" t="s">
-        <v>755</v>
       </c>
       <c r="F56" s="51"/>
       <c r="G56" s="51"/>
@@ -7061,16 +7061,16 @@
     <row r="57" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A57" s="51"/>
       <c r="B57" s="51" t="s">
+        <v>753</v>
+      </c>
+      <c r="C57" s="51" t="s">
+        <v>754</v>
+      </c>
+      <c r="D57" s="51" t="s">
+        <v>755</v>
+      </c>
+      <c r="E57" s="51" t="s">
         <v>756</v>
-      </c>
-      <c r="C57" s="51" t="s">
-        <v>757</v>
-      </c>
-      <c r="D57" s="51" t="s">
-        <v>758</v>
-      </c>
-      <c r="E57" s="51" t="s">
-        <v>759</v>
       </c>
       <c r="F57" s="51"/>
       <c r="G57" s="51"/>
@@ -7078,16 +7078,16 @@
     <row r="58" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="51"/>
       <c r="B58" s="61" t="s">
+        <v>757</v>
+      </c>
+      <c r="C58" s="51" t="s">
+        <v>758</v>
+      </c>
+      <c r="D58" s="51" t="s">
+        <v>759</v>
+      </c>
+      <c r="E58" s="51" t="s">
         <v>760</v>
-      </c>
-      <c r="C58" s="51" t="s">
-        <v>761</v>
-      </c>
-      <c r="D58" s="51" t="s">
-        <v>762</v>
-      </c>
-      <c r="E58" s="51" t="s">
-        <v>763</v>
       </c>
       <c r="F58" s="51"/>
       <c r="G58" s="51"/>
@@ -7096,13 +7096,13 @@
       <c r="A59" s="51"/>
       <c r="B59" s="61"/>
       <c r="C59" s="51" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D59" s="51" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="E59" s="51" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="F59" s="51"/>
       <c r="G59" s="51"/>
@@ -7110,7 +7110,7 @@
     <row r="60" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A60" s="51"/>
       <c r="B60" s="51" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C60" s="51"/>
       <c r="D60" s="51"/>
@@ -7151,7 +7151,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -7159,7 +7159,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -7167,7 +7167,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -7175,7 +7175,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -7183,7 +7183,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7191,7 +7191,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -7199,7 +7199,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7207,7 +7207,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7215,7 +7215,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
@@ -7223,7 +7223,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7231,7 +7231,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -7239,7 +7239,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7247,7 +7247,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7255,7 +7255,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -7263,7 +7263,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -7271,7 +7271,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
   </sheetData>
@@ -8506,8 +8506,8 @@
   <dimension ref="A1:AMK45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8614,10 +8614,10 @@
         <v>31</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="25" t="s">
@@ -8653,7 +8653,7 @@
         <v>212</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>213</v>
@@ -8688,7 +8688,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>790</v>
@@ -8729,7 +8729,7 @@
         <v>223</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>219</v>
@@ -8752,10 +8752,10 @@
         <v>222</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -8804,13 +8804,13 @@
         <v>31</v>
       </c>
       <c r="D10" s="25" t="s">
+        <v>791</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>792</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>231</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>233</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -8823,17 +8823,17 @@
     </row>
     <row r="11" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>236</v>
+        <v>793</v>
       </c>
       <c r="F11" s="25" t="s">
         <v>213</v>
@@ -8849,20 +8849,20 @@
     </row>
     <row r="12" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>238</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>241</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -8875,20 +8875,20 @@
     </row>
     <row r="13" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -8901,20 +8901,20 @@
     </row>
     <row r="14" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -8927,20 +8927,20 @@
     </row>
     <row r="15" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -8953,20 +8953,20 @@
     </row>
     <row r="16" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="F16" s="25" t="s">
         <v>255</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>258</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -8981,13 +8981,13 @@
       <c r="A17" s="26"/>
       <c r="B17" s="1"/>
       <c r="C17" s="25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17"/>
@@ -9003,13 +9003,13 @@
       <c r="A18" s="26"/>
       <c r="B18" s="1"/>
       <c r="C18" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>262</v>
-      </c>
       <c r="E18" s="25" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18"/>
@@ -9023,20 +9023,20 @@
     </row>
     <row r="19" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="25" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
@@ -9049,20 +9049,20 @@
     </row>
     <row r="20" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="F20" s="25" t="s">
         <v>269</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>270</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>271</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>272</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
@@ -9075,20 +9075,20 @@
     </row>
     <row r="21" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B21"/>
       <c r="C21" s="25" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
@@ -9106,48 +9106,48 @@
         <v>31</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="26" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="J22" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="L22" s="26" t="s">
         <v>279</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>282</v>
       </c>
       <c r="M22" s="29"/>
       <c r="N22" s="26" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>285</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>288</v>
       </c>
       <c r="F23" s="26" t="s">
         <v>213</v>
@@ -9163,17 +9163,17 @@
     </row>
     <row r="24" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="26" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F24" s="26" t="s">
         <v>213</v>
@@ -9189,209 +9189,209 @@
     </row>
     <row r="25" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="F25" s="25" t="s">
         <v>293</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A26" s="26" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C26" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="F26" s="25" t="s">
         <v>293</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>300</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A28" s="26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="F29" s="25" t="s">
         <v>307</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>309</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="26" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="26" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="26" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="26" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="26" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="26" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -9423,7 +9423,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>18</v>
@@ -9452,85 +9452,85 @@
     </row>
     <row r="2" spans="1:12" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="C8" s="32" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="C9" s="32"/>
       <c r="D9" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E9" s="32"/>
     </row>
@@ -9562,7 +9562,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>18</v>
@@ -9591,72 +9591,72 @@
     </row>
     <row r="2" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="19"/>
       <c r="D5" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="19" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="19"/>
       <c r="D7" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E7" s="32"/>
     </row>
@@ -9664,10 +9664,10 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="19" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E8" s="32"/>
     </row>
@@ -9676,7 +9676,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="19"/>
       <c r="D9" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E9" s="32"/>
     </row>
@@ -9717,7 +9717,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -9742,10 +9742,10 @@
       </c>
       <c r="B4"/>
       <c r="C4" s="19" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -9756,46 +9756,46 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="19" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B6"/>
       <c r="C6" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>363</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>364</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>365</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>367</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>370</v>
       </c>
       <c r="E7"/>
     </row>
@@ -9808,43 +9808,43 @@
         <v>168</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>372</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>373</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>374</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>375</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11" spans="1:6" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
@@ -9859,11 +9859,11 @@
     </row>
     <row r="12" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>177</v>
@@ -9874,7 +9874,7 @@
     </row>
     <row r="13" spans="1:6" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
@@ -9940,10 +9940,10 @@
     </row>
     <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -9991,14 +9991,14 @@
     </row>
     <row r="4" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>32</v>
@@ -10006,55 +10006,55 @@
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4" s="34" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="L5" s="34" t="s">
         <v>392</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>386</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>394</v>
-      </c>
-      <c r="L5" s="34" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>54</v>
@@ -10066,14 +10066,14 @@
     </row>
     <row r="7" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>54</v>
@@ -10085,14 +10085,14 @@
     </row>
     <row r="8" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>32</v>
@@ -10104,14 +10104,14 @@
     </row>
     <row r="9" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E9" s="21"/>
       <c r="H9"/>
@@ -10121,14 +10121,14 @@
     </row>
     <row r="10" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E10" s="21"/>
       <c r="H10"/>
@@ -10138,14 +10138,14 @@
     </row>
     <row r="11" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E11" s="21"/>
       <c r="H11"/>
@@ -10155,13 +10155,13 @@
     </row>
     <row r="12" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E12" s="21"/>
       <c r="H12"/>
@@ -10171,13 +10171,13 @@
     </row>
     <row r="13" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E13" s="21"/>
       <c r="H13"/>
@@ -10187,13 +10187,13 @@
     </row>
     <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E14" s="21"/>
       <c r="H14"/>
@@ -10203,13 +10203,13 @@
     </row>
     <row r="15" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E15" s="21"/>
       <c r="H15"/>
@@ -10219,13 +10219,13 @@
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E16" s="21"/>
       <c r="H16"/>
@@ -10235,13 +10235,13 @@
     </row>
     <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E17" s="21"/>
       <c r="H17"/>
@@ -10251,13 +10251,13 @@
     </row>
     <row r="18" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>122</v>
@@ -10269,13 +10269,13 @@
     </row>
     <row r="19" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E19" s="21"/>
       <c r="H19"/>
@@ -10285,90 +10285,90 @@
     </row>
     <row r="20" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>32</v>
       </c>
       <c r="H20" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>439</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>440</v>
+      </c>
+      <c r="L20" s="19" t="s">
         <v>441</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>442</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>386</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>443</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E25" s="21"/>
     </row>
@@ -10403,60 +10403,60 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>460</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>461</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>462</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added attributed breakEvenPrice to PriceTaggedWIthProductVersion and implemented logic to calculate logic with variable expense are changed. The same needs to be done. when fixed expense are changed or when purchase price is changed. IN progress.
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="796">
   <si>
     <t>Term</t>
   </si>
@@ -2645,6 +2645,12 @@
 20. Cost of acquiring a subscriber(CAS)
 21. SLV to CAS ratio
 22. Months to recover CAS</t>
+  </si>
+  <si>
+    <t>Calculate breakevenr price whenever either of purchase price,fixed expense per unit or variable expense per unit undergoes change</t>
+  </si>
+  <si>
+    <t>As a system I will calculate breakevenr price whenever either of purchase price,fixed expense per unit and variable expense per unit undergoes change. The calculated breakeven price will be stored in associated PriceTaggedWithProduct version( which stores changed purchase price).</t>
   </si>
 </sst>
 </file>
@@ -2984,6 +2990,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2994,9 +3003,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5135,6 +5141,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="D21:D23"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="D33:D35"/>
     <mergeCell ref="A36:A39"/>
@@ -5145,18 +5163,6 @@
     <mergeCell ref="D27:D29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="D30:D32"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6305,7 +6311,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="62" t="s">
         <v>681</v>
       </c>
       <c r="C2" s="51" t="s">
@@ -6314,14 +6320,14 @@
       <c r="D2" s="51" t="s">
         <v>683</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="62" t="s">
         <v>684</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="62" t="s">
         <v>685</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62" t="s">
+      <c r="G2" s="62"/>
+      <c r="H2" s="63" t="s">
         <v>686</v>
       </c>
     </row>
@@ -6329,21 +6335,21 @@
       <c r="A3" s="51">
         <v>1</v>
       </c>
-      <c r="B3" s="61"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="51" t="s">
         <v>687</v>
       </c>
       <c r="D3" s="51" t="s">
         <v>688</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="51"/>
-      <c r="B4" s="61"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="52" t="s">
         <v>689</v>
       </c>
@@ -6353,14 +6359,14 @@
       <c r="E4" s="52" t="s">
         <v>690</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="64" t="s">
         <v>691</v>
       </c>
-      <c r="G4" s="64"/>
+      <c r="G4" s="65"/>
     </row>
     <row r="5" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="51"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="52" t="s">
         <v>781</v>
       </c>
@@ -6368,12 +6374,12 @@
         <v>782</v>
       </c>
       <c r="E5" s="52"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
     </row>
     <row r="6" spans="1:8" ht="91" x14ac:dyDescent="0.35">
       <c r="A6" s="51"/>
-      <c r="B6" s="61"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="52" t="s">
         <v>692</v>
       </c>
@@ -6383,21 +6389,21 @@
       <c r="E6" s="52" t="s">
         <v>694</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="51"/>
-      <c r="B7" s="61"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
-      <c r="F7" s="63"/>
+      <c r="F7" s="64"/>
       <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:8" ht="104" x14ac:dyDescent="0.35">
       <c r="A8" s="51"/>
-      <c r="B8" s="61"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="52" t="s">
         <v>695</v>
       </c>
@@ -6407,12 +6413,12 @@
       <c r="E8" s="52" t="s">
         <v>697</v>
       </c>
-      <c r="F8" s="63"/>
+      <c r="F8" s="64"/>
       <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:8" ht="91" x14ac:dyDescent="0.35">
       <c r="A9" s="51"/>
-      <c r="B9" s="61"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="51" t="s">
         <v>698</v>
       </c>
@@ -6422,14 +6428,14 @@
       <c r="E9" s="51" t="s">
         <v>700</v>
       </c>
-      <c r="F9" s="63"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="51" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A10" s="51"/>
-      <c r="B10" s="61"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="51" t="s">
         <v>702</v>
       </c>
@@ -6439,12 +6445,12 @@
       <c r="E10" s="51" t="s">
         <v>703</v>
       </c>
-      <c r="F10" s="63"/>
+      <c r="F10" s="64"/>
       <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:8" ht="169" x14ac:dyDescent="0.35">
       <c r="A11" s="51"/>
-      <c r="B11" s="61"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="51" t="s">
         <v>704</v>
       </c>
@@ -6482,7 +6488,7 @@
     </row>
     <row r="13" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="51"/>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="61" t="s">
         <v>713</v>
       </c>
       <c r="C13" s="51" t="s">
@@ -6497,7 +6503,7 @@
     </row>
     <row r="14" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
-      <c r="B14" s="65"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="51" t="s">
         <v>474</v>
       </c>
@@ -6510,7 +6516,7 @@
     </row>
     <row r="15" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A15" s="51"/>
-      <c r="B15" s="65"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="51" t="s">
         <v>476</v>
       </c>
@@ -6523,7 +6529,7 @@
     </row>
     <row r="16" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="51"/>
-      <c r="B16" s="65"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="51" t="s">
         <v>479</v>
       </c>
@@ -6536,7 +6542,7 @@
     </row>
     <row r="17" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A17" s="51"/>
-      <c r="B17" s="65"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="51" t="s">
         <v>492</v>
       </c>
@@ -6549,7 +6555,7 @@
     </row>
     <row r="18" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="51"/>
-      <c r="B18" s="65"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="51" t="s">
         <v>496</v>
       </c>
@@ -6562,7 +6568,7 @@
     </row>
     <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A19" s="51"/>
-      <c r="B19" s="65"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="51" t="s">
         <v>500</v>
       </c>
@@ -6575,7 +6581,7 @@
     </row>
     <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="51"/>
-      <c r="B20" s="65"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="51" t="s">
         <v>529</v>
       </c>
@@ -6588,7 +6594,7 @@
     </row>
     <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="51"/>
-      <c r="B21" s="65"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="51" t="s">
         <v>715</v>
       </c>
@@ -6601,7 +6607,7 @@
     </row>
     <row r="22" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A22" s="51"/>
-      <c r="B22" s="65"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="51" t="s">
         <v>545</v>
       </c>
@@ -6614,7 +6620,7 @@
     </row>
     <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="51"/>
-      <c r="B23" s="65"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="51" t="s">
         <v>548</v>
       </c>
@@ -6627,7 +6633,7 @@
     </row>
     <row r="24" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A24" s="51"/>
-      <c r="B24" s="65"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="51" t="s">
         <v>551</v>
       </c>
@@ -6640,7 +6646,7 @@
     </row>
     <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="51"/>
-      <c r="B25" s="65"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="51" t="s">
         <v>716</v>
       </c>
@@ -6653,7 +6659,7 @@
     </row>
     <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A26" s="51"/>
-      <c r="B26" s="65"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="51" t="s">
         <v>556</v>
       </c>
@@ -6666,7 +6672,7 @@
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="51"/>
-      <c r="B27" s="65"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="51" t="s">
         <v>717</v>
       </c>
@@ -6679,7 +6685,7 @@
     </row>
     <row r="28" spans="1:7" ht="65" x14ac:dyDescent="0.35">
       <c r="A28" s="51"/>
-      <c r="B28" s="65"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="51" t="s">
         <v>570</v>
       </c>
@@ -6692,7 +6698,7 @@
     </row>
     <row r="29" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" s="51"/>
-      <c r="B29" s="65"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="51" t="s">
         <v>573</v>
       </c>
@@ -6705,7 +6711,7 @@
     </row>
     <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="51"/>
-      <c r="B30" s="65"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="51" t="s">
         <v>576</v>
       </c>
@@ -6718,7 +6724,7 @@
     </row>
     <row r="31" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A31" s="51"/>
-      <c r="B31" s="65"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="51" t="s">
         <v>581</v>
       </c>
@@ -6731,7 +6737,7 @@
     </row>
     <row r="32" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A32" s="51"/>
-      <c r="B32" s="65"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="51" t="s">
         <v>589</v>
       </c>
@@ -6744,7 +6750,7 @@
     </row>
     <row r="33" spans="1:7" ht="65" x14ac:dyDescent="0.35">
       <c r="A33" s="51"/>
-      <c r="B33" s="65"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="51" t="s">
         <v>592</v>
       </c>
@@ -6757,7 +6763,7 @@
     </row>
     <row r="34" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A34" s="51"/>
-      <c r="B34" s="65"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="51" t="s">
         <v>720</v>
       </c>
@@ -6770,7 +6776,7 @@
     </row>
     <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="51"/>
-      <c r="B35" s="65"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="51" t="s">
         <v>597</v>
       </c>
@@ -6783,7 +6789,7 @@
     </row>
     <row r="36" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A36" s="51"/>
-      <c r="B36" s="65"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="51" t="s">
         <v>599</v>
       </c>
@@ -6796,7 +6802,7 @@
     </row>
     <row r="37" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A37" s="51"/>
-      <c r="B37" s="65"/>
+      <c r="B37" s="61"/>
       <c r="C37" s="51" t="s">
         <v>602</v>
       </c>
@@ -6809,7 +6815,7 @@
     </row>
     <row r="38" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A38" s="51"/>
-      <c r="B38" s="65"/>
+      <c r="B38" s="61"/>
       <c r="C38" s="51" t="s">
         <v>605</v>
       </c>
@@ -6822,7 +6828,7 @@
     </row>
     <row r="39" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A39" s="51"/>
-      <c r="B39" s="65"/>
+      <c r="B39" s="61"/>
       <c r="C39" s="51" t="s">
         <v>608</v>
       </c>
@@ -6835,7 +6841,7 @@
     </row>
     <row r="40" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A40" s="51"/>
-      <c r="B40" s="65"/>
+      <c r="B40" s="61"/>
       <c r="C40" s="51" t="s">
         <v>610</v>
       </c>
@@ -6848,7 +6854,7 @@
     </row>
     <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A41" s="51"/>
-      <c r="B41" s="65"/>
+      <c r="B41" s="61"/>
       <c r="C41" s="51" t="s">
         <v>722</v>
       </c>
@@ -6936,7 +6942,7 @@
     </row>
     <row r="49" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="51"/>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="62" t="s">
         <v>728</v>
       </c>
       <c r="C49" s="51" t="s">
@@ -6953,7 +6959,7 @@
     </row>
     <row r="50" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="51"/>
-      <c r="B50" s="61"/>
+      <c r="B50" s="62"/>
       <c r="C50" s="51" t="s">
         <v>732</v>
       </c>
@@ -6968,7 +6974,7 @@
     </row>
     <row r="51" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A51" s="51"/>
-      <c r="B51" s="61"/>
+      <c r="B51" s="62"/>
       <c r="C51" s="51" t="s">
         <v>735</v>
       </c>
@@ -6983,7 +6989,7 @@
     </row>
     <row r="52" spans="1:7" ht="91" x14ac:dyDescent="0.35">
       <c r="A52" s="51"/>
-      <c r="B52" s="61"/>
+      <c r="B52" s="62"/>
       <c r="C52" s="51" t="s">
         <v>738</v>
       </c>
@@ -6998,7 +7004,7 @@
     </row>
     <row r="53" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A53" s="51"/>
-      <c r="B53" s="61"/>
+      <c r="B53" s="62"/>
       <c r="C53" s="51" t="s">
         <v>741</v>
       </c>
@@ -7013,7 +7019,7 @@
     </row>
     <row r="54" spans="1:7" ht="65" x14ac:dyDescent="0.35">
       <c r="A54" s="51"/>
-      <c r="B54" s="61"/>
+      <c r="B54" s="62"/>
       <c r="C54" s="51" t="s">
         <v>744</v>
       </c>
@@ -7028,7 +7034,7 @@
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A55" s="51"/>
-      <c r="B55" s="61"/>
+      <c r="B55" s="62"/>
       <c r="C55" s="53" t="s">
         <v>121</v>
       </c>
@@ -7077,7 +7083,7 @@
     </row>
     <row r="58" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="51"/>
-      <c r="B58" s="61" t="s">
+      <c r="B58" s="62" t="s">
         <v>757</v>
       </c>
       <c r="C58" s="51" t="s">
@@ -7094,7 +7100,7 @@
     </row>
     <row r="59" spans="1:7" ht="234" x14ac:dyDescent="0.35">
       <c r="A59" s="51"/>
-      <c r="B59" s="61"/>
+      <c r="B59" s="62"/>
       <c r="C59" s="51" t="s">
         <v>761</v>
       </c>
@@ -7120,16 +7126,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="B13:B41"/>
     <mergeCell ref="B49:B55"/>
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="B2:B11"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="F4:F10"/>
-    <mergeCell ref="G4:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8181,7 +8187,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="65" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>163</v>
       </c>
@@ -8503,7 +8509,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK45"/>
+  <dimension ref="A1:AMK46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
@@ -8821,23 +8827,17 @@
       <c r="M10"/>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
-        <v>232</v>
-      </c>
+    <row r="11" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="26"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="25" t="s">
-        <v>31</v>
-      </c>
+      <c r="C11" s="25"/>
       <c r="D11" s="25" t="s">
-        <v>233</v>
+        <v>794</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>793</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>213</v>
-      </c>
+        <v>795</v>
+      </c>
+      <c r="F11" s="25"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
@@ -8847,22 +8847,22 @@
       <c r="M11"/>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="25" t="s">
-        <v>235</v>
+        <v>31</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>237</v>
+        <v>793</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -8873,22 +8873,22 @@
       <c r="M12"/>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="25" t="s">
         <v>235</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -8899,22 +8899,22 @@
       <c r="M13"/>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="25" t="s">
         <v>235</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -8927,20 +8927,20 @@
     </row>
     <row r="15" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="25" t="s">
         <v>235</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -8951,22 +8951,22 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="25" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -8978,18 +8978,22 @@
       <c r="N16"/>
     </row>
     <row r="17" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
+      <c r="A17" s="26" t="s">
+        <v>251</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="25" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="F17" s="25"/>
+        <v>254</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>255</v>
+      </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
@@ -9006,10 +9010,10 @@
         <v>256</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18"/>
@@ -9022,22 +9026,18 @@
       <c r="N18"/>
     </row>
     <row r="19" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="26" t="s">
-        <v>261</v>
-      </c>
+      <c r="A19" s="26"/>
       <c r="B19" s="1"/>
       <c r="C19" s="25" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>263</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>264</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="F19" s="25"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
@@ -9049,20 +9049,20 @@
     </row>
     <row r="20" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="25" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
@@ -9075,20 +9075,20 @@
     </row>
     <row r="21" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="B21"/>
+        <v>265</v>
+      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="25" t="s">
         <v>266</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
@@ -9099,81 +9099,81 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" ht="261" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="26" t="s">
+    <row r="22" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14" ht="261" x14ac:dyDescent="0.35">
+      <c r="A23" s="26"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D23" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E23" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="26" t="s">
+      <c r="F23" s="28"/>
+      <c r="G23" s="26" t="s">
         <v>275</v>
       </c>
-      <c r="H22" s="29"/>
-      <c r="I22" s="26" t="s">
+      <c r="H23" s="29"/>
+      <c r="I23" s="26" t="s">
         <v>276</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J23" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="K22" s="26" t="s">
+      <c r="K23" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="L22" s="26" t="s">
+      <c r="L23" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="26" t="s">
+      <c r="M23" s="29"/>
+      <c r="N23" s="26" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+    <row r="24" spans="1:14" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B24" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-    </row>
-    <row r="24" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="B24" s="26"/>
       <c r="C24" s="26" t="s">
         <v>283</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F24" s="26" t="s">
         <v>213</v>
@@ -9189,208 +9189,234 @@
     </row>
     <row r="25" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+    </row>
+    <row r="26" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="26" t="s">
         <v>289</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>291</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="26" t="s">
-        <v>294</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>290</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F26" s="25" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A27" s="26" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>290</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="26" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>290</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>290</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>290</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C31" s="25" t="s">
         <v>290</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F31" s="25" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>315</v>
+        <v>311</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="26" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="26" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E38" s="30" t="s">
         <v>325</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="26" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="26" t="s">
         <v>333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commented all serializers/deserializers associated with enums
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="990" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="990" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="859">
   <si>
     <t>Term</t>
   </si>
@@ -3066,12 +3066,37 @@
     <t>As a system,I receive ManualForecastAddedEvent from  a product when merchant adds manual forecast for that product and calculate expected provision for purchase cost for that product by multiplying forecasted total subscriptions for each product with  its current purchase cost and add this  amount to ProviosionalPurchaseCostAccount recommendation section and respective view.
 After all the products are registered with their manual forecast,the recommendation for total purchase cost is visible to the merchant which he can accept or override with higher/lower amount.</t>
   </si>
+  <si>
+    <t>Created Payment account on subscription confirmation</t>
+  </si>
+  <si>
+    <t>Register new product with payment account</t>
+  </si>
+  <si>
+    <t>As a system I should receive ProductRegisteredEvent from Product domain and register the product(already registered with Product domain) with payment domain, so as to refer to it's attrbutes such as pricing cateogry,offer price/discount,purchase price/MRP etc. while calculating and adjusting the total payment due ot it.</t>
+  </si>
+  <si>
+    <t>As a system I should receive subscription confirmation event from Subscriber domain, containing subscriber Id, subscription id, subscription confirmation date,pre-created deliveries containing productwise subscription count per delivery,offer prices /percent discounts for each at the time of subscription confirmation.
+The subscription confirmation event should create a new payment account for the said subscription,regsiter delivery details of each delivery with this account, calculate tentative cost per deivery (with reference to latest offer prices/discounts) as well as tentative total subscription  cost, and register them with DeliveryCostAccount and TotalSubscriptionCost account respectively.</t>
+  </si>
+  <si>
+    <t>Update the latest tagged price for each product when it undergoes change</t>
+  </si>
+  <si>
+    <t>As a system I should receive ProductStatusUpdatedEvent from Product/Integration domain,thereby receive changes in the tagged price of a product. The received tagged price will make earlier tagged price for the same product expired and register the new tagged price instead. The latest tagged price is referred while correcting the due amount of products with percent discount commited product as their percentage of discount is applied on latestMRP.</t>
+  </si>
+  <si>
+    <t>Update the changes in latest offer price in Payments domain</t>
+  </si>
+  <si>
+    <t>As a system I should receive OfferPriceChangedEvent( which indicates change in offer price or percent discount for a product). The newly reeived offered price/percent discount will make expiry of existing offer price/percent discount of that product and set the new value for it. In case of products falling in none committed price cateogry, the offer price is simply overriden by new value.The latest offer price/discount price is referred while correcting the due amount of products in differnt pricing categories.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3135,8 +3160,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3171,6 +3202,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3251,7 +3288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3439,6 +3476,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3454,9 +3500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3468,6 +3511,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4081,7 +4130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
@@ -4615,12 +4664,12 @@
       <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="72" t="s">
         <v>553</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="70" t="s">
+      <c r="D20" s="73" t="s">
         <v>554</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -4637,10 +4686,10 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="69"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="70"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="47" t="s">
         <v>556</v>
       </c>
@@ -4655,10 +4704,10 @@
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="69"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="70"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="48" t="s">
         <v>557</v>
       </c>
@@ -4673,10 +4722,10 @@
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="69"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="70"/>
+      <c r="D23" s="73"/>
       <c r="E23" s="48" t="s">
         <v>558</v>
       </c>
@@ -5712,48 +5761,48 @@
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="74" t="s">
         <v>678</v>
       </c>
-      <c r="C17" s="71"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="74" t="s">
         <v>679</v>
       </c>
-      <c r="C18" s="71"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="74" t="s">
         <v>680</v>
       </c>
-      <c r="C19" s="71"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="74" t="s">
         <v>681</v>
       </c>
-      <c r="C20" s="71"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -5860,7 +5909,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="75" t="s">
         <v>690</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -5869,14 +5918,14 @@
       <c r="D2" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="75" t="s">
         <v>693</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="75" t="s">
         <v>694</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="76" t="s">
         <v>695</v>
       </c>
     </row>
@@ -5884,21 +5933,21 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="73"/>
+      <c r="B3" s="75"/>
       <c r="C3" s="9" t="s">
         <v>696</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="4" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
-      <c r="B4" s="73"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="55" t="s">
         <v>698</v>
       </c>
@@ -5908,14 +5957,14 @@
       <c r="E4" s="55" t="s">
         <v>700</v>
       </c>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="77" t="s">
         <v>701</v>
       </c>
-      <c r="G4" s="76"/>
+      <c r="G4" s="78"/>
     </row>
     <row r="5" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="73"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="55" t="s">
         <v>702</v>
       </c>
@@ -5923,12 +5972,12 @@
         <v>703</v>
       </c>
       <c r="E5" s="55"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="76"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="78"/>
     </row>
     <row r="6" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="73"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="55" t="s">
         <v>704</v>
       </c>
@@ -5938,21 +5987,21 @@
       <c r="E6" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="76"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="73"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="75"/>
+      <c r="F7" s="77"/>
       <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:8" ht="52" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
-      <c r="B8" s="73"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="55" t="s">
         <v>707</v>
       </c>
@@ -5962,12 +6011,12 @@
       <c r="E8" s="55" t="s">
         <v>709</v>
       </c>
-      <c r="F8" s="75"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="56"/>
     </row>
     <row r="9" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="73"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="9" t="s">
         <v>710</v>
       </c>
@@ -5977,14 +6026,14 @@
       <c r="E9" s="9" t="s">
         <v>712</v>
       </c>
-      <c r="F9" s="75"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="9" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="73"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="9" t="s">
         <v>714</v>
       </c>
@@ -5994,12 +6043,12 @@
       <c r="E10" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="F10" s="75"/>
+      <c r="F10" s="77"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="156" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="73"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="9" t="s">
         <v>716</v>
       </c>
@@ -6037,7 +6086,7 @@
     </row>
     <row r="13" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="79" t="s">
         <v>725</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -6052,7 +6101,7 @@
     </row>
     <row r="14" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="72"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="9" t="s">
         <v>531</v>
       </c>
@@ -6065,7 +6114,7 @@
     </row>
     <row r="15" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="72"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="9" t="s">
         <v>533</v>
       </c>
@@ -6078,7 +6127,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
-      <c r="B16" s="72"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="9" t="s">
         <v>536</v>
       </c>
@@ -6091,7 +6140,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="72"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="9" t="s">
         <v>546</v>
       </c>
@@ -6104,7 +6153,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="72"/>
+      <c r="B18" s="79"/>
       <c r="C18" s="9" t="s">
         <v>548</v>
       </c>
@@ -6117,7 +6166,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="72"/>
+      <c r="B19" s="79"/>
       <c r="C19" s="9" t="s">
         <v>550</v>
       </c>
@@ -6130,7 +6179,7 @@
     </row>
     <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="72"/>
+      <c r="B20" s="79"/>
       <c r="C20" s="9" t="s">
         <v>555</v>
       </c>
@@ -6143,7 +6192,7 @@
     </row>
     <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="72"/>
+      <c r="B21" s="79"/>
       <c r="C21" s="9" t="s">
         <v>727</v>
       </c>
@@ -6156,7 +6205,7 @@
     </row>
     <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="72"/>
+      <c r="B22" s="79"/>
       <c r="C22" s="9" t="s">
         <v>570</v>
       </c>
@@ -6169,7 +6218,7 @@
     </row>
     <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="72"/>
+      <c r="B23" s="79"/>
       <c r="C23" s="9" t="s">
         <v>573</v>
       </c>
@@ -6182,7 +6231,7 @@
     </row>
     <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="72"/>
+      <c r="B24" s="79"/>
       <c r="C24" s="9" t="s">
         <v>576</v>
       </c>
@@ -6195,7 +6244,7 @@
     </row>
     <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
-      <c r="B25" s="72"/>
+      <c r="B25" s="79"/>
       <c r="C25" s="9" t="s">
         <v>728</v>
       </c>
@@ -6208,7 +6257,7 @@
     </row>
     <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
-      <c r="B26" s="72"/>
+      <c r="B26" s="79"/>
       <c r="C26" s="9" t="s">
         <v>581</v>
       </c>
@@ -6221,7 +6270,7 @@
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
-      <c r="B27" s="72"/>
+      <c r="B27" s="79"/>
       <c r="C27" s="9" t="s">
         <v>729</v>
       </c>
@@ -6234,7 +6283,7 @@
     </row>
     <row r="28" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
-      <c r="B28" s="72"/>
+      <c r="B28" s="79"/>
       <c r="C28" s="9" t="s">
         <v>595</v>
       </c>
@@ -6247,7 +6296,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
-      <c r="B29" s="72"/>
+      <c r="B29" s="79"/>
       <c r="C29" s="9" t="s">
         <v>598</v>
       </c>
@@ -6260,7 +6309,7 @@
     </row>
     <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="72"/>
+      <c r="B30" s="79"/>
       <c r="C30" s="9" t="s">
         <v>601</v>
       </c>
@@ -6273,7 +6322,7 @@
     </row>
     <row r="31" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="72"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="9" t="s">
         <v>606</v>
       </c>
@@ -6286,7 +6335,7 @@
     </row>
     <row r="32" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="72"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="9" t="s">
         <v>614</v>
       </c>
@@ -6299,7 +6348,7 @@
     </row>
     <row r="33" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="72"/>
+      <c r="B33" s="79"/>
       <c r="C33" s="9" t="s">
         <v>617</v>
       </c>
@@ -6312,7 +6361,7 @@
     </row>
     <row r="34" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
-      <c r="B34" s="72"/>
+      <c r="B34" s="79"/>
       <c r="C34" s="9" t="s">
         <v>732</v>
       </c>
@@ -6325,7 +6374,7 @@
     </row>
     <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
-      <c r="B35" s="72"/>
+      <c r="B35" s="79"/>
       <c r="C35" s="9" t="s">
         <v>622</v>
       </c>
@@ -6338,7 +6387,7 @@
     </row>
     <row r="36" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
-      <c r="B36" s="72"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="9" t="s">
         <v>624</v>
       </c>
@@ -6351,7 +6400,7 @@
     </row>
     <row r="37" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
-      <c r="B37" s="72"/>
+      <c r="B37" s="79"/>
       <c r="C37" s="9" t="s">
         <v>627</v>
       </c>
@@ -6364,7 +6413,7 @@
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
-      <c r="B38" s="72"/>
+      <c r="B38" s="79"/>
       <c r="C38" s="9" t="s">
         <v>630</v>
       </c>
@@ -6377,7 +6426,7 @@
     </row>
     <row r="39" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
-      <c r="B39" s="72"/>
+      <c r="B39" s="79"/>
       <c r="C39" s="9" t="s">
         <v>633</v>
       </c>
@@ -6390,7 +6439,7 @@
     </row>
     <row r="40" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
-      <c r="B40" s="72"/>
+      <c r="B40" s="79"/>
       <c r="C40" s="9" t="s">
         <v>635</v>
       </c>
@@ -6403,7 +6452,7 @@
     </row>
     <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
-      <c r="B41" s="72"/>
+      <c r="B41" s="79"/>
       <c r="C41" s="9" t="s">
         <v>734</v>
       </c>
@@ -6491,7 +6540,7 @@
     </row>
     <row r="49" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="75" t="s">
         <v>740</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -6508,7 +6557,7 @@
     </row>
     <row r="50" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
-      <c r="B50" s="73"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="9" t="s">
         <v>744</v>
       </c>
@@ -6523,7 +6572,7 @@
     </row>
     <row r="51" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
-      <c r="B51" s="73"/>
+      <c r="B51" s="75"/>
       <c r="C51" s="9" t="s">
         <v>747</v>
       </c>
@@ -6538,7 +6587,7 @@
     </row>
     <row r="52" spans="1:7" ht="78" x14ac:dyDescent="0.35">
       <c r="A52" s="9"/>
-      <c r="B52" s="73"/>
+      <c r="B52" s="75"/>
       <c r="C52" s="9" t="s">
         <v>750</v>
       </c>
@@ -6553,7 +6602,7 @@
     </row>
     <row r="53" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
-      <c r="B53" s="73"/>
+      <c r="B53" s="75"/>
       <c r="C53" s="9" t="s">
         <v>753</v>
       </c>
@@ -6568,7 +6617,7 @@
     </row>
     <row r="54" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
-      <c r="B54" s="73"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="9" t="s">
         <v>756</v>
       </c>
@@ -6583,7 +6632,7 @@
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
-      <c r="B55" s="73"/>
+      <c r="B55" s="75"/>
       <c r="C55" s="56" t="s">
         <v>123</v>
       </c>
@@ -6632,7 +6681,7 @@
     </row>
     <row r="58" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
-      <c r="B58" s="73" t="s">
+      <c r="B58" s="75" t="s">
         <v>769</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -6649,7 +6698,7 @@
     </row>
     <row r="59" spans="1:7" ht="208" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
-      <c r="B59" s="73"/>
+      <c r="B59" s="75"/>
       <c r="C59" s="9" t="s">
         <v>773</v>
       </c>
@@ -6675,16 +6724,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B13:B41"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="F4:F10"/>
     <mergeCell ref="G4:G6"/>
-    <mergeCell ref="B13:B41"/>
-    <mergeCell ref="B49:B55"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8249,7 +8298,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="70" t="s">
         <v>186</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -8258,28 +8307,28 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="67"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="21" t="s">
         <v>188</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="67"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="21" t="s">
         <v>189</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C6" s="67"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="4" t="s">
         <v>190</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="67"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="4" t="s">
         <v>191</v>
       </c>
@@ -8333,7 +8382,7 @@
       <c r="E14"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="71" t="s">
         <v>198</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -8344,37 +8393,37 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C16" s="68"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="4" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17" s="68"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="4" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C18" s="68"/>
+      <c r="C18" s="71"/>
       <c r="D18" s="4" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C19" s="68"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C20" s="68"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C21" s="68"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="1" t="s">
         <v>206</v>
       </c>
@@ -9863,11 +9912,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK25"/>
+  <dimension ref="A1:AMK29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9951,152 +10000,144 @@
       <c r="K3"/>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>418</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20" t="s">
-        <v>419</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>420</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>32</v>
-      </c>
+    <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="80" t="s">
+        <v>852</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>853</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
       <c r="H4"/>
       <c r="I4"/>
-      <c r="J4" s="35" t="s">
-        <v>421</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>422</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
-        <v>424</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20" t="s">
-        <v>425</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>426</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>427</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J5" s="35" t="s">
-        <v>421</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>429</v>
-      </c>
-      <c r="L5" s="35" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
-        <v>431</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>52</v>
-      </c>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="80" t="s">
+        <v>851</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>854</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="69"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="80" t="s">
+        <v>855</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>856</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
-        <v>434</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20" t="s">
-        <v>435</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>436</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>52</v>
-      </c>
+    <row r="7" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="80" t="s">
+        <v>857</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>858</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>32</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="J8" s="35" t="s">
+        <v>421</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>442</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+        <v>426</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>421</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="20" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>445</v>
-      </c>
-      <c r="E10" s="22"/>
+        <v>433</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -10105,16 +10146,18 @@
     </row>
     <row r="11" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>448</v>
-      </c>
-      <c r="E11" s="22"/>
+        <v>436</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -10123,30 +10166,34 @@
     </row>
     <row r="12" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>450</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>451</v>
-      </c>
-      <c r="E12" s="22"/>
+        <v>437</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>452</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>453</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>454</v>
+        <v>440</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>442</v>
       </c>
       <c r="E13" s="22"/>
       <c r="H13"/>
@@ -10155,15 +10202,16 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>455</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>456</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>457</v>
+        <v>443</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>445</v>
       </c>
       <c r="E14" s="22"/>
       <c r="H14"/>
@@ -10174,13 +10222,14 @@
     </row>
     <row r="15" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>458</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>459</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>460</v>
+        <v>446</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>448</v>
       </c>
       <c r="E15" s="22"/>
       <c r="H15"/>
@@ -10189,15 +10238,15 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>462</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>463</v>
+        <v>450</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>451</v>
       </c>
       <c r="E16" s="22"/>
       <c r="H16"/>
@@ -10208,13 +10257,13 @@
     </row>
     <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="E17" s="22"/>
       <c r="H17"/>
@@ -10223,19 +10272,17 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>469</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>124</v>
-      </c>
+        <v>457</v>
+      </c>
+      <c r="E18" s="22"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -10244,13 +10291,13 @@
     </row>
     <row r="19" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="E19" s="22"/>
       <c r="H19"/>
@@ -10259,104 +10306,174 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>462</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>463</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>464</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>468</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>471</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>472</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C24" s="35" t="s">
         <v>474</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D24" s="35" t="s">
         <v>475</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E24" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="H24" s="35" t="s">
         <v>476</v>
       </c>
-      <c r="I20" s="35" t="s">
+      <c r="I24" s="35" t="s">
         <v>477</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J24" s="35" t="s">
         <v>421</v>
       </c>
-      <c r="K20" s="20" t="s">
+      <c r="K24" s="20" t="s">
         <v>478</v>
       </c>
-      <c r="L20" s="20" t="s">
+      <c r="L24" s="20" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+    <row r="25" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C25" s="35" t="s">
         <v>481</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D25" s="35" t="s">
         <v>482</v>
       </c>
-      <c r="E21" s="22"/>
-    </row>
-    <row r="22" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
+      <c r="E25" s="22"/>
+    </row>
+    <row r="26" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C26" s="35" t="s">
         <v>484</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D26" s="35" t="s">
         <v>485</v>
       </c>
-      <c r="E22" s="22"/>
-    </row>
-    <row r="23" spans="1:12" ht="116" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+      <c r="A27" s="20" t="s">
         <v>486</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C27" s="35" t="s">
         <v>487</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D27" s="35" t="s">
         <v>488</v>
       </c>
-      <c r="E23" s="22"/>
-    </row>
-    <row r="24" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A28" s="20" t="s">
         <v>489</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C28" s="35" t="s">
         <v>490</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D28" s="35" t="s">
         <v>491</v>
       </c>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C29" s="35" t="s">
         <v>493</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D29" s="35" t="s">
         <v>494</v>
       </c>
-      <c r="E25" s="22"/>
+      <c r="E29" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E29">
       <formula1>"Not Started,Completed,In Progress"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
workflow of the total subscription lifecycle
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="990" firstSheet="3" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="990" firstSheet="4" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="PendingQuestions" sheetId="16" r:id="rId14"/>
     <sheet name="workflows" sheetId="15" r:id="rId15"/>
     <sheet name="Sheet1" sheetId="17" r:id="rId16"/>
+    <sheet name="Pending" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="1018">
   <si>
     <t>Term</t>
   </si>
@@ -3450,9 +3451,6 @@
     <t>Manual creation of Business Account</t>
   </si>
   <si>
-    <t>Admin creates a business account for a desired financial year in order to initiate subscription business</t>
-  </si>
-  <si>
     <t>Creation of Business Account for a financial Year.</t>
   </si>
   <si>
@@ -3489,7 +3487,152 @@
     </r>
   </si>
   <si>
-    <t>Admin creates business account</t>
+    <t>Subscriber accessing products of different categories on shopping portal</t>
+  </si>
+  <si>
+    <t>read APIs in subscriber domain</t>
+  </si>
+  <si>
+    <t>Ability to search for a product by brand name,category name, product name</t>
+  </si>
+  <si>
+    <t>Elastic search implementation(where?)</t>
+  </si>
+  <si>
+    <t>Subscriber should be able to see his subscription content,delivery calender for each</t>
+  </si>
+  <si>
+    <t>Susbcriber should be able to see the payment history, total payment, due payment, next payment date</t>
+  </si>
+  <si>
+    <t>read Api in payment domain</t>
+  </si>
+  <si>
+    <t>Subscriber should be able to see his /her reward points accumulated (vested and not yeat vested) and have an option to use them as payment toward current/future</t>
+  </si>
+  <si>
+    <t>Benefits domain</t>
+  </si>
+  <si>
+    <t>Susbcriber syndicate formation</t>
+  </si>
+  <si>
+    <t>Subscriber domain</t>
+  </si>
+  <si>
+    <t>Benefit schemes only applicable for syndicates</t>
+  </si>
+  <si>
+    <t>Each product should be able to tell how much it can contributes in rewards provisioning.. So as to arrive at benefits provisioning</t>
+  </si>
+  <si>
+    <t>Product-&gt;Business domain</t>
+  </si>
+  <si>
+    <t>Ability to devide the available provision for benefits among available/future benefit schemes</t>
+  </si>
+  <si>
+    <t>Business domain</t>
+  </si>
+  <si>
+    <t>Ability for the system to find out closest benefit schemes to which a subscriber will be eligible to gain with minor additions to his subscription content</t>
+  </si>
+  <si>
+    <t>Benefits -&gt;Subscriber</t>
+  </si>
+  <si>
+    <t>Admin creates a business account for a desired financial year in order to initiate subscription business ( through BusinessAccountConfigurationController)</t>
+  </si>
+  <si>
+    <t>If there is any existing business account then it should be closed.
+business account view should get populated with business account details such as id,merchant id,start date,end date, provision date)</t>
+  </si>
+  <si>
+    <t>Admin configures business account</t>
+  </si>
+  <si>
+    <t>Following configuration should be set through UI
+1. budget adjustment options: If the merchant wants to manually configure the budget,or want recommendations by system,or set in auto pilot mode.
+2. Setting of Fiscal year applicable to the country(April to march or Jan to december)
+3. Tax percentage fo annual revenue: How much total tax percentage is going from the annual revenue</t>
+  </si>
+  <si>
+    <t>The same information should be stored in BusinessAccount Configuration View for read purpose</t>
+  </si>
+  <si>
+    <t>Primary outcome</t>
+  </si>
+  <si>
+    <t>Secondary outcome</t>
+  </si>
+  <si>
+    <t>Manual Setting of budgets(optional)</t>
+  </si>
+  <si>
+    <t>Admin sets budget for purchase cost through UI</t>
+  </si>
+  <si>
+    <t>Business Account aggregate should be created followed by following child account members
+1. subscription receivable account
+2. provisional purchase cost account
+3. provisional losses account
+4. provisional benefits account
+5. provisional taxes account
+6. provisional others account
+7. provisional common expenses account
+8. provisional subscription specific expenses account.
+9. revenue account
+10. interest gain account
+11. profit account
+12. refund account</t>
+  </si>
+  <si>
+    <t>RefundAccountView is not connected to events coming from refund account- to be added</t>
+  </si>
+  <si>
+    <t>Admin sets provision for benefits through UI</t>
+  </si>
+  <si>
+    <t>Following budget information reg. purchase cost provision is set in Purchase cost account.
+1. Start Date of the provision
+2. End Date of the provision
+3. provision of purchase goods
+The provision is distributed across the year.
+The provision calendar inside purchase cost account will distribute the amount evenly across the period segments in the financial year.
+(need to remove even distribution in future and instead introduce DistributionPolicy based on demand growth rate)</t>
+  </si>
+  <si>
+    <t>Following budget information reg.  is set in account.
+1. Start Date of the provision
+2. End Date of the provision
+3. provision amount
+The provision is distributed across the year.
+The provision calendar inside purchase cost account will distribute the amount evenly across the period segments in the financial year.
+(need to remove even distribution in future and instead introduce DistributionPolicy based on demand growth rate)</t>
+  </si>
+  <si>
+    <t>The same info should be stored in PurchaseCostAccountViewRepository as well as PurchaseCostAccountTransactionViewRepository.</t>
+  </si>
+  <si>
+    <t>The same info should be stored in BenefitAccountViewRepository as well as PurchaseCostAccountTransactionViewRepository.</t>
+  </si>
+  <si>
+    <t>Admin sets provision for losses thru UI ( Currently not being used anywhere)</t>
+  </si>
+  <si>
+    <t>Following budget information reg.  is set in account.
+1. Start Date of the provision
+2. End Date of the provision
+3. provision amount</t>
+  </si>
+  <si>
+    <t>The same info should be stored in LossesAccountViewRepository as well as LossesAccountTransactionViewRepository.</t>
+  </si>
+  <si>
+    <t>Admin sets provision for Taxes thru UI</t>
+  </si>
+  <si>
+    <t>The same info should be stored in TaxesAccountViewRepository as well as TaxesAccountTransactionViewRepository.</t>
   </si>
 </sst>
 </file>
@@ -3784,7 +3927,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4107,6 +4250,42 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4207,6 +4386,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5355,12 +5537,12 @@
       <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="114" t="s">
+      <c r="A20" s="126" t="s">
         <v>553</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="115" t="s">
+      <c r="D20" s="127" t="s">
         <v>554</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -5377,10 +5559,10 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="114"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="115"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="47" t="s">
         <v>556</v>
       </c>
@@ -5395,10 +5577,10 @@
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="114"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="115"/>
+      <c r="D22" s="127"/>
       <c r="E22" s="48" t="s">
         <v>557</v>
       </c>
@@ -5413,10 +5595,10 @@
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="114"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="115"/>
+      <c r="D23" s="127"/>
       <c r="E23" s="48" t="s">
         <v>558</v>
       </c>
@@ -6423,48 +6605,48 @@
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="128" t="s">
         <v>678</v>
       </c>
-      <c r="C17" s="116"/>
+      <c r="C17" s="128"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="128" t="s">
         <v>679</v>
       </c>
-      <c r="C18" s="116"/>
+      <c r="C18" s="128"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="128" t="s">
         <v>680</v>
       </c>
-      <c r="C19" s="116"/>
+      <c r="C19" s="128"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
-      <c r="B20" s="116" t="s">
+      <c r="B20" s="128" t="s">
         <v>681</v>
       </c>
-      <c r="C20" s="116"/>
+      <c r="C20" s="128"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
+      <c r="B21" s="128"/>
+      <c r="C21" s="128"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -6840,7 +7022,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="130" t="s">
         <v>690</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -6849,14 +7031,14 @@
       <c r="D2" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="E2" s="118" t="s">
+      <c r="E2" s="130" t="s">
         <v>693</v>
       </c>
-      <c r="F2" s="118" t="s">
+      <c r="F2" s="130" t="s">
         <v>694</v>
       </c>
-      <c r="G2" s="118"/>
-      <c r="H2" s="119" t="s">
+      <c r="G2" s="130"/>
+      <c r="H2" s="131" t="s">
         <v>695</v>
       </c>
     </row>
@@ -6864,21 +7046,21 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="118"/>
+      <c r="B3" s="130"/>
       <c r="C3" s="9" t="s">
         <v>696</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="119"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="131"/>
     </row>
     <row r="4" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
-      <c r="B4" s="118"/>
+      <c r="B4" s="130"/>
       <c r="C4" s="55" t="s">
         <v>698</v>
       </c>
@@ -6888,14 +7070,14 @@
       <c r="E4" s="55" t="s">
         <v>700</v>
       </c>
-      <c r="F4" s="120" t="s">
+      <c r="F4" s="132" t="s">
         <v>701</v>
       </c>
-      <c r="G4" s="121"/>
+      <c r="G4" s="133"/>
     </row>
     <row r="5" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="118"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="55" t="s">
         <v>702</v>
       </c>
@@ -6903,12 +7085,12 @@
         <v>703</v>
       </c>
       <c r="E5" s="55"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="121"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="133"/>
     </row>
     <row r="6" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="118"/>
+      <c r="B6" s="130"/>
       <c r="C6" s="55" t="s">
         <v>704</v>
       </c>
@@ -6918,21 +7100,21 @@
       <c r="E6" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="F6" s="120"/>
-      <c r="G6" s="121"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="133"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="118"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="120"/>
+      <c r="F7" s="132"/>
       <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:8" ht="52" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
-      <c r="B8" s="118"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="55" t="s">
         <v>707</v>
       </c>
@@ -6942,12 +7124,12 @@
       <c r="E8" s="55" t="s">
         <v>709</v>
       </c>
-      <c r="F8" s="120"/>
+      <c r="F8" s="132"/>
       <c r="G8" s="56"/>
     </row>
     <row r="9" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="118"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="9" t="s">
         <v>710</v>
       </c>
@@ -6957,14 +7139,14 @@
       <c r="E9" s="9" t="s">
         <v>712</v>
       </c>
-      <c r="F9" s="120"/>
+      <c r="F9" s="132"/>
       <c r="G9" s="9" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="118"/>
+      <c r="B10" s="130"/>
       <c r="C10" s="9" t="s">
         <v>714</v>
       </c>
@@ -6974,12 +7156,12 @@
       <c r="E10" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="F10" s="120"/>
+      <c r="F10" s="132"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="156" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="118"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="9" t="s">
         <v>716</v>
       </c>
@@ -7017,7 +7199,7 @@
     </row>
     <row r="13" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="129" t="s">
         <v>725</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -7032,7 +7214,7 @@
     </row>
     <row r="14" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="117"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="9" t="s">
         <v>531</v>
       </c>
@@ -7045,7 +7227,7 @@
     </row>
     <row r="15" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="117"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="9" t="s">
         <v>533</v>
       </c>
@@ -7058,7 +7240,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
-      <c r="B16" s="117"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="9" t="s">
         <v>536</v>
       </c>
@@ -7071,7 +7253,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="117"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="9" t="s">
         <v>546</v>
       </c>
@@ -7084,7 +7266,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="117"/>
+      <c r="B18" s="129"/>
       <c r="C18" s="9" t="s">
         <v>548</v>
       </c>
@@ -7097,7 +7279,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="117"/>
+      <c r="B19" s="129"/>
       <c r="C19" s="9" t="s">
         <v>550</v>
       </c>
@@ -7110,7 +7292,7 @@
     </row>
     <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="117"/>
+      <c r="B20" s="129"/>
       <c r="C20" s="9" t="s">
         <v>555</v>
       </c>
@@ -7123,7 +7305,7 @@
     </row>
     <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="117"/>
+      <c r="B21" s="129"/>
       <c r="C21" s="9" t="s">
         <v>727</v>
       </c>
@@ -7136,7 +7318,7 @@
     </row>
     <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="117"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="9" t="s">
         <v>570</v>
       </c>
@@ -7149,7 +7331,7 @@
     </row>
     <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="117"/>
+      <c r="B23" s="129"/>
       <c r="C23" s="9" t="s">
         <v>573</v>
       </c>
@@ -7162,7 +7344,7 @@
     </row>
     <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="117"/>
+      <c r="B24" s="129"/>
       <c r="C24" s="9" t="s">
         <v>576</v>
       </c>
@@ -7175,7 +7357,7 @@
     </row>
     <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
-      <c r="B25" s="117"/>
+      <c r="B25" s="129"/>
       <c r="C25" s="9" t="s">
         <v>728</v>
       </c>
@@ -7188,7 +7370,7 @@
     </row>
     <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
-      <c r="B26" s="117"/>
+      <c r="B26" s="129"/>
       <c r="C26" s="9" t="s">
         <v>581</v>
       </c>
@@ -7201,7 +7383,7 @@
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
-      <c r="B27" s="117"/>
+      <c r="B27" s="129"/>
       <c r="C27" s="9" t="s">
         <v>729</v>
       </c>
@@ -7214,7 +7396,7 @@
     </row>
     <row r="28" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
-      <c r="B28" s="117"/>
+      <c r="B28" s="129"/>
       <c r="C28" s="9" t="s">
         <v>595</v>
       </c>
@@ -7227,7 +7409,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
-      <c r="B29" s="117"/>
+      <c r="B29" s="129"/>
       <c r="C29" s="9" t="s">
         <v>598</v>
       </c>
@@ -7240,7 +7422,7 @@
     </row>
     <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="117"/>
+      <c r="B30" s="129"/>
       <c r="C30" s="9" t="s">
         <v>601</v>
       </c>
@@ -7253,7 +7435,7 @@
     </row>
     <row r="31" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="117"/>
+      <c r="B31" s="129"/>
       <c r="C31" s="9" t="s">
         <v>606</v>
       </c>
@@ -7266,7 +7448,7 @@
     </row>
     <row r="32" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="117"/>
+      <c r="B32" s="129"/>
       <c r="C32" s="9" t="s">
         <v>614</v>
       </c>
@@ -7279,7 +7461,7 @@
     </row>
     <row r="33" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="117"/>
+      <c r="B33" s="129"/>
       <c r="C33" s="9" t="s">
         <v>617</v>
       </c>
@@ -7292,7 +7474,7 @@
     </row>
     <row r="34" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
-      <c r="B34" s="117"/>
+      <c r="B34" s="129"/>
       <c r="C34" s="9" t="s">
         <v>732</v>
       </c>
@@ -7305,7 +7487,7 @@
     </row>
     <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
-      <c r="B35" s="117"/>
+      <c r="B35" s="129"/>
       <c r="C35" s="9" t="s">
         <v>622</v>
       </c>
@@ -7318,7 +7500,7 @@
     </row>
     <row r="36" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
-      <c r="B36" s="117"/>
+      <c r="B36" s="129"/>
       <c r="C36" s="9" t="s">
         <v>624</v>
       </c>
@@ -7331,7 +7513,7 @@
     </row>
     <row r="37" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
-      <c r="B37" s="117"/>
+      <c r="B37" s="129"/>
       <c r="C37" s="9" t="s">
         <v>627</v>
       </c>
@@ -7344,7 +7526,7 @@
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
-      <c r="B38" s="117"/>
+      <c r="B38" s="129"/>
       <c r="C38" s="9" t="s">
         <v>630</v>
       </c>
@@ -7357,7 +7539,7 @@
     </row>
     <row r="39" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
-      <c r="B39" s="117"/>
+      <c r="B39" s="129"/>
       <c r="C39" s="9" t="s">
         <v>633</v>
       </c>
@@ -7370,7 +7552,7 @@
     </row>
     <row r="40" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
-      <c r="B40" s="117"/>
+      <c r="B40" s="129"/>
       <c r="C40" s="9" t="s">
         <v>635</v>
       </c>
@@ -7383,7 +7565,7 @@
     </row>
     <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
-      <c r="B41" s="117"/>
+      <c r="B41" s="129"/>
       <c r="C41" s="9" t="s">
         <v>734</v>
       </c>
@@ -7471,7 +7653,7 @@
     </row>
     <row r="49" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
-      <c r="B49" s="118" t="s">
+      <c r="B49" s="130" t="s">
         <v>740</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -7488,7 +7670,7 @@
     </row>
     <row r="50" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
-      <c r="B50" s="118"/>
+      <c r="B50" s="130"/>
       <c r="C50" s="9" t="s">
         <v>744</v>
       </c>
@@ -7503,7 +7685,7 @@
     </row>
     <row r="51" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
-      <c r="B51" s="118"/>
+      <c r="B51" s="130"/>
       <c r="C51" s="9" t="s">
         <v>747</v>
       </c>
@@ -7518,7 +7700,7 @@
     </row>
     <row r="52" spans="1:7" ht="78" x14ac:dyDescent="0.35">
       <c r="A52" s="9"/>
-      <c r="B52" s="118"/>
+      <c r="B52" s="130"/>
       <c r="C52" s="9" t="s">
         <v>750</v>
       </c>
@@ -7533,7 +7715,7 @@
     </row>
     <row r="53" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
-      <c r="B53" s="118"/>
+      <c r="B53" s="130"/>
       <c r="C53" s="9" t="s">
         <v>753</v>
       </c>
@@ -7548,7 +7730,7 @@
     </row>
     <row r="54" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
-      <c r="B54" s="118"/>
+      <c r="B54" s="130"/>
       <c r="C54" s="9" t="s">
         <v>756</v>
       </c>
@@ -7563,7 +7745,7 @@
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
-      <c r="B55" s="118"/>
+      <c r="B55" s="130"/>
       <c r="C55" s="56" t="s">
         <v>123</v>
       </c>
@@ -7612,7 +7794,7 @@
     </row>
     <row r="58" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
-      <c r="B58" s="118" t="s">
+      <c r="B58" s="130" t="s">
         <v>769</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -7629,7 +7811,7 @@
     </row>
     <row r="59" spans="1:7" ht="208" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
-      <c r="B59" s="118"/>
+      <c r="B59" s="130"/>
       <c r="C59" s="9" t="s">
         <v>773</v>
       </c>
@@ -7673,25 +7855,27 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" style="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" style="75" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="75" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="75"/>
     <col min="4" max="4" width="51.7265625" style="75" customWidth="1"/>
     <col min="5" max="5" width="30.90625" style="75" customWidth="1"/>
-    <col min="6" max="6" width="37" style="75" customWidth="1"/>
-    <col min="7" max="7" width="42" style="75" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="75"/>
+    <col min="6" max="6" width="60.08984375" style="75" customWidth="1"/>
+    <col min="7" max="7" width="33.1796875" style="75" customWidth="1"/>
+    <col min="8" max="8" width="37" style="75" customWidth="1"/>
+    <col min="9" max="9" width="42" style="75" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="74" t="s">
         <v>519</v>
       </c>
@@ -7706,1219 +7890,1607 @@
         <v>893</v>
       </c>
       <c r="F1" s="74" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H1" s="74" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52" x14ac:dyDescent="0.35">
-      <c r="A2" s="74" t="s">
+    <row r="2" spans="1:9" ht="182" x14ac:dyDescent="0.35">
+      <c r="A2" s="121" t="s">
         <v>542</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="114" t="s">
         <v>970</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="71" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="85" t="s">
+        <v>997</v>
+      </c>
+      <c r="E2" s="114" t="s">
         <v>971</v>
       </c>
-      <c r="E2" s="106" t="s">
+      <c r="F2" s="114" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G2" s="114" t="s">
+        <v>998</v>
+      </c>
+      <c r="H2" s="74" t="s">
         <v>972</v>
       </c>
-      <c r="F2" s="74" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A3" s="74"/>
       <c r="B3" s="106"/>
       <c r="C3" s="74"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="74"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="74" t="s">
-        <v>861</v>
-      </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="71" t="s">
-        <v>980</v>
+      <c r="D3" s="85" t="s">
+        <v>999</v>
+      </c>
+      <c r="F3" s="114" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="114" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H3" s="74"/>
+    </row>
+    <row r="4" spans="1:9" ht="130" x14ac:dyDescent="0.35">
+      <c r="B4" s="121" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C4" s="121"/>
+      <c r="D4" s="85" t="s">
+        <v>1005</v>
       </c>
       <c r="E4" s="106"/>
-      <c r="F4" s="74"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F4" s="114" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G4" s="114" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H4" s="74"/>
+    </row>
+    <row r="5" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A5" s="74"/>
       <c r="B5" s="106"/>
       <c r="C5" s="74"/>
-      <c r="D5" s="71"/>
+      <c r="D5" s="85" t="s">
+        <v>1008</v>
+      </c>
       <c r="E5" s="106"/>
-      <c r="F5" s="74"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5" s="114" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G5" s="114" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H5" s="74"/>
+    </row>
+    <row r="6" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A6" s="74"/>
       <c r="B6" s="106"/>
       <c r="C6" s="74"/>
-      <c r="D6" s="71"/>
+      <c r="D6" s="121" t="s">
+        <v>1013</v>
+      </c>
       <c r="E6" s="106"/>
-      <c r="F6" s="74"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6" s="114" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G6" s="114" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H6" s="74"/>
+    </row>
+    <row r="7" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A7" s="74"/>
       <c r="B7" s="106"/>
       <c r="C7" s="74"/>
-      <c r="D7" s="71"/>
+      <c r="D7" s="121" t="s">
+        <v>1016</v>
+      </c>
       <c r="E7" s="106"/>
-      <c r="F7" s="74"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" s="114" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G7" s="114" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H7" s="74"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="74"/>
       <c r="B8" s="106"/>
       <c r="C8" s="74"/>
-      <c r="D8" s="71"/>
       <c r="E8" s="106"/>
-      <c r="F8" s="74"/>
-    </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="74"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="74"/>
-      <c r="B9" s="127" t="s">
+      <c r="B9" s="106"/>
+      <c r="C9" s="74"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="74"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="74"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="74"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="74"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="74"/>
+      <c r="B11" s="106"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="74"/>
+    </row>
+    <row r="12" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A12" s="74"/>
+      <c r="B12" s="139" t="s">
         <v>877</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77" t="s">
+      <c r="C12" s="76"/>
+      <c r="D12" s="77" t="s">
         <v>959</v>
       </c>
-      <c r="E9" s="127" t="s">
+      <c r="E12" s="139" t="s">
         <v>895</v>
       </c>
-      <c r="F9" s="74" t="s">
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="74" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="78" x14ac:dyDescent="0.35">
-      <c r="A10" s="131" t="s">
+    <row r="13" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+      <c r="A13" s="143" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="123"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77" t="s">
+      <c r="B13" s="135"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77" t="s">
         <v>889</v>
       </c>
-      <c r="E10" s="123"/>
-      <c r="F10" s="78" t="s">
+      <c r="E13" s="135"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="78" t="s">
         <v>962</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="I13" s="75" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="131"/>
-      <c r="B11" s="123"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="79" t="s">
-        <v>862</v>
-      </c>
-      <c r="E11" s="123"/>
-      <c r="F11" s="78" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A12" s="131"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="79" t="s">
-        <v>891</v>
-      </c>
-      <c r="E12" s="123"/>
-      <c r="F12" s="78" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A13" s="131"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="79" t="s">
-        <v>963</v>
-      </c>
-      <c r="E13" s="124"/>
-      <c r="F13" s="78" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A14" s="131"/>
-      <c r="B14" s="124"/>
+    <row r="14" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A14" s="143"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="76"/>
       <c r="D14" s="79" t="s">
-        <v>890</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>899</v>
-      </c>
-      <c r="F14" s="78" t="s">
+        <v>862</v>
+      </c>
+      <c r="E14" s="135"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="78" t="s">
         <v>964</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="109" t="s">
-        <v>974</v>
-      </c>
-      <c r="B15" s="107" t="s">
-        <v>976</v>
-      </c>
-      <c r="C15" s="108"/>
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A15" s="143"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="79" t="s">
-        <v>975</v>
-      </c>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="78"/>
-      <c r="B16" s="76"/>
+        <v>891</v>
+      </c>
+      <c r="E15" s="135"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="78" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A16" s="143"/>
+      <c r="B16" s="135"/>
       <c r="C16" s="76"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="78"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="131" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="130" t="s">
-        <v>878</v>
-      </c>
+      <c r="D16" s="79" t="s">
+        <v>963</v>
+      </c>
+      <c r="E16" s="136"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="78" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A17" s="143"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="76"/>
       <c r="D17" s="79" t="s">
-        <v>707</v>
-      </c>
-      <c r="E17" s="127" t="s">
-        <v>894</v>
-      </c>
-      <c r="F17" s="122" t="s">
-        <v>962</v>
-      </c>
-      <c r="G17" s="125" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="131"/>
-      <c r="B18" s="130"/>
-      <c r="C18" s="76"/>
+        <v>890</v>
+      </c>
+      <c r="E17" s="76" t="s">
+        <v>899</v>
+      </c>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="78" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="109" t="s">
+        <v>973</v>
+      </c>
+      <c r="B18" s="107" t="s">
+        <v>975</v>
+      </c>
+      <c r="C18" s="108"/>
       <c r="D18" s="79" t="s">
-        <v>892</v>
-      </c>
-      <c r="E18" s="128"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="126"/>
-    </row>
-    <row r="19" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A19" s="131"/>
-      <c r="B19" s="130"/>
+        <v>974</v>
+      </c>
+      <c r="E18" s="108"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
+      <c r="H18" s="109" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="78"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="76"/>
-      <c r="D19" s="79" t="s">
-        <v>863</v>
-      </c>
-      <c r="E19" s="128"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="126"/>
-    </row>
-    <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A20" s="131"/>
-      <c r="B20" s="130"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+      <c r="H19" s="78"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="143" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="142" t="s">
+        <v>878</v>
+      </c>
       <c r="C20" s="76"/>
       <c r="D20" s="79" t="s">
+        <v>707</v>
+      </c>
+      <c r="E20" s="139" t="s">
+        <v>894</v>
+      </c>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="134" t="s">
+        <v>962</v>
+      </c>
+      <c r="I20" s="137" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A21" s="143"/>
+      <c r="B21" s="142"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="79" t="s">
+        <v>892</v>
+      </c>
+      <c r="E21" s="140"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="135"/>
+      <c r="I21" s="138"/>
+    </row>
+    <row r="22" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A22" s="143"/>
+      <c r="B22" s="142"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="79" t="s">
+        <v>863</v>
+      </c>
+      <c r="E22" s="140"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="138"/>
+    </row>
+    <row r="23" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A23" s="143"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="79" t="s">
         <v>864</v>
       </c>
-      <c r="E20" s="128"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="126"/>
-    </row>
-    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A21" s="131"/>
-      <c r="B21" s="130"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="77" t="s">
-        <v>868</v>
-      </c>
-      <c r="E21" s="129"/>
-      <c r="F21" s="78" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A22" s="131"/>
-      <c r="B22" s="130"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="77" t="s">
-        <v>896</v>
-      </c>
-      <c r="E22" s="130" t="s">
-        <v>900</v>
-      </c>
-      <c r="F22" s="78" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="78" x14ac:dyDescent="0.35">
-      <c r="A23" s="131"/>
-      <c r="B23" s="130"/>
-      <c r="C23" s="111" t="s">
-        <v>978</v>
-      </c>
-      <c r="D23" s="79" t="s">
-        <v>977</v>
-      </c>
-      <c r="E23" s="130"/>
-      <c r="F23" s="110"/>
-    </row>
-    <row r="24" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A24" s="131"/>
-      <c r="B24" s="130"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="123"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="138"/>
+    </row>
+    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A24" s="143"/>
+      <c r="B24" s="142"/>
       <c r="C24" s="76"/>
       <c r="D24" s="77" t="s">
-        <v>897</v>
-      </c>
-      <c r="E24" s="130"/>
-      <c r="F24" s="78" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A25" s="131"/>
-      <c r="B25" s="130"/>
+        <v>868</v>
+      </c>
+      <c r="E24" s="141"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="78" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A25" s="143"/>
+      <c r="B25" s="142"/>
       <c r="C25" s="76"/>
       <c r="D25" s="77" t="s">
-        <v>898</v>
-      </c>
-      <c r="E25" s="130"/>
-      <c r="F25" s="78" t="s">
+        <v>896</v>
+      </c>
+      <c r="E25" s="142" t="s">
+        <v>900</v>
+      </c>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="78" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="78"/>
-      <c r="B26" s="76"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="78"/>
-    </row>
-    <row r="27" spans="1:7" ht="39" x14ac:dyDescent="0.35">
-      <c r="A27" s="131" t="s">
-        <v>537</v>
-      </c>
-      <c r="B27" s="130" t="s">
-        <v>879</v>
-      </c>
+    <row r="26" spans="1:9" ht="78" x14ac:dyDescent="0.35">
+      <c r="A26" s="143"/>
+      <c r="B26" s="142"/>
+      <c r="C26" s="111" t="s">
+        <v>977</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>976</v>
+      </c>
+      <c r="E26" s="142"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="110"/>
+    </row>
+    <row r="27" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A27" s="143"/>
+      <c r="B27" s="142"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="79" t="s">
-        <v>885</v>
-      </c>
-      <c r="E27" s="127" t="s">
-        <v>902</v>
-      </c>
-      <c r="F27" s="78" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="91" x14ac:dyDescent="0.35">
-      <c r="A28" s="131"/>
-      <c r="B28" s="130"/>
+      <c r="D27" s="77" t="s">
+        <v>897</v>
+      </c>
+      <c r="E27" s="142"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+      <c r="H27" s="78" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="143"/>
+      <c r="B28" s="142"/>
       <c r="C28" s="76"/>
       <c r="D28" s="77" t="s">
+        <v>898</v>
+      </c>
+      <c r="E28" s="142"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="122"/>
+      <c r="H28" s="78" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="78"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="122"/>
+      <c r="H29" s="78"/>
+    </row>
+    <row r="30" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A30" s="143" t="s">
+        <v>537</v>
+      </c>
+      <c r="B30" s="142" t="s">
+        <v>879</v>
+      </c>
+      <c r="C30" s="76"/>
+      <c r="D30" s="79" t="s">
+        <v>885</v>
+      </c>
+      <c r="E30" s="139" t="s">
+        <v>902</v>
+      </c>
+      <c r="F30" s="115"/>
+      <c r="G30" s="115"/>
+      <c r="H30" s="78" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="91" x14ac:dyDescent="0.35">
+      <c r="A31" s="143"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77" t="s">
         <v>865</v>
       </c>
-      <c r="E28" s="129"/>
-      <c r="F28" s="78" t="s">
+      <c r="E31" s="141"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="78" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="117" x14ac:dyDescent="0.35">
-      <c r="A29" s="104" t="s">
+    <row r="32" spans="1:9" ht="117" x14ac:dyDescent="0.35">
+      <c r="A32" s="104" t="s">
         <v>968</v>
       </c>
-      <c r="B29" s="105" t="s">
+      <c r="B32" s="105" t="s">
         <v>969</v>
       </c>
-      <c r="C29" s="105"/>
-      <c r="D29" s="86" t="s">
+      <c r="C32" s="105"/>
+      <c r="D32" s="86" t="s">
         <v>967</v>
       </c>
-      <c r="E29" s="103" t="s">
-        <v>979</v>
-      </c>
-      <c r="F29" s="104" t="s">
+      <c r="E32" s="103" t="s">
+        <v>978</v>
+      </c>
+      <c r="F32" s="116"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="104" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="78"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="78"/>
-    </row>
-    <row r="31" spans="1:7" ht="117" x14ac:dyDescent="0.35">
-      <c r="A31" s="80" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="78"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="78"/>
+    </row>
+    <row r="34" spans="1:8" ht="117" x14ac:dyDescent="0.35">
+      <c r="A34" s="80" t="s">
         <v>871</v>
       </c>
-      <c r="B31" s="81" t="s">
+      <c r="B34" s="81" t="s">
         <v>869</v>
       </c>
-      <c r="C31" s="81"/>
-      <c r="D31" s="82" t="s">
+      <c r="C34" s="81"/>
+      <c r="D34" s="82" t="s">
         <v>886</v>
       </c>
-      <c r="E31" s="83" t="s">
+      <c r="E34" s="83" t="s">
         <v>870</v>
       </c>
-      <c r="F31" s="78"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="78"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="78"/>
-    </row>
-    <row r="33" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A33" s="131" t="s">
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
+      <c r="H34" s="78"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="78"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="78"/>
+    </row>
+    <row r="36" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A36" s="143" t="s">
         <v>861</v>
       </c>
-      <c r="B33" s="130" t="s">
+      <c r="B36" s="142" t="s">
         <v>880</v>
       </c>
-      <c r="C33" s="76"/>
-      <c r="D33" s="77" t="s">
+      <c r="C36" s="76"/>
+      <c r="D36" s="77" t="s">
         <v>872</v>
       </c>
-      <c r="E33" s="127" t="s">
+      <c r="E36" s="139" t="s">
         <v>903</v>
       </c>
-      <c r="F33" s="78"/>
-    </row>
-    <row r="34" spans="1:6" ht="52" x14ac:dyDescent="0.35">
-      <c r="A34" s="131"/>
-      <c r="B34" s="130"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="77" t="s">
-        <v>873</v>
-      </c>
-      <c r="E34" s="129"/>
-      <c r="F34" s="78"/>
-    </row>
-    <row r="35" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A35" s="131"/>
-      <c r="B35" s="130"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="77" t="s">
-        <v>536</v>
-      </c>
-      <c r="E35" s="84" t="s">
-        <v>904</v>
-      </c>
-      <c r="F35" s="85" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="104" x14ac:dyDescent="0.35">
-      <c r="A36" s="131"/>
-      <c r="B36" s="130"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="86" t="s">
-        <v>888</v>
-      </c>
-      <c r="E36" s="76" t="s">
-        <v>905</v>
-      </c>
-      <c r="F36" s="87" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A37" s="131"/>
-      <c r="B37" s="130"/>
+      <c r="F36" s="115"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="78"/>
+    </row>
+    <row r="37" spans="1:8" ht="52" x14ac:dyDescent="0.35">
+      <c r="A37" s="143"/>
+      <c r="B37" s="142"/>
       <c r="C37" s="76"/>
       <c r="D37" s="77" t="s">
-        <v>548</v>
-      </c>
-      <c r="E37" s="84" t="s">
-        <v>906</v>
-      </c>
-      <c r="F37" s="78" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A38" s="131"/>
-      <c r="B38" s="130"/>
+        <v>873</v>
+      </c>
+      <c r="E37" s="141"/>
+      <c r="F37" s="116"/>
+      <c r="G37" s="116"/>
+      <c r="H37" s="78"/>
+    </row>
+    <row r="38" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A38" s="143"/>
+      <c r="B38" s="142"/>
       <c r="C38" s="76"/>
       <c r="D38" s="77" t="s">
-        <v>874</v>
-      </c>
-      <c r="E38" s="76" t="s">
-        <v>907</v>
-      </c>
-      <c r="F38" s="78"/>
-    </row>
-    <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A39" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="B39" s="76"/>
+        <v>536</v>
+      </c>
+      <c r="E38" s="84" t="s">
+        <v>904</v>
+      </c>
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="85" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="104" x14ac:dyDescent="0.35">
+      <c r="A39" s="143"/>
+      <c r="B39" s="142"/>
       <c r="C39" s="76"/>
-      <c r="D39" s="77" t="s">
-        <v>911</v>
-      </c>
-      <c r="E39" s="76"/>
-      <c r="F39" s="78"/>
-    </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A40" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="B40" s="76"/>
+      <c r="D39" s="86" t="s">
+        <v>888</v>
+      </c>
+      <c r="E39" s="76" t="s">
+        <v>905</v>
+      </c>
+      <c r="F39" s="122"/>
+      <c r="G39" s="122"/>
+      <c r="H39" s="87" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A40" s="143"/>
+      <c r="B40" s="142"/>
       <c r="C40" s="76"/>
       <c r="D40" s="77" t="s">
-        <v>901</v>
-      </c>
-      <c r="E40" s="77" t="s">
-        <v>908</v>
-      </c>
-      <c r="F40" s="78"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="137" t="s">
-        <v>884</v>
-      </c>
-      <c r="B41" s="138"/>
-      <c r="C41" s="138"/>
-      <c r="D41" s="138"/>
-      <c r="E41" s="138"/>
-      <c r="F41" s="139"/>
-    </row>
-    <row r="42" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+        <v>548</v>
+      </c>
+      <c r="E40" s="84" t="s">
+        <v>906</v>
+      </c>
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="78" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A41" s="143"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="77" t="s">
+        <v>874</v>
+      </c>
+      <c r="E41" s="76" t="s">
+        <v>907</v>
+      </c>
+      <c r="F41" s="122"/>
+      <c r="G41" s="122"/>
+      <c r="H41" s="78"/>
+    </row>
+    <row r="42" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A42" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="B42" s="140" t="s">
-        <v>919</v>
-      </c>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88" t="s">
-        <v>910</v>
-      </c>
-      <c r="E42" s="88" t="s">
-        <v>915</v>
-      </c>
-      <c r="F42" s="89"/>
-    </row>
-    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="77" t="s">
+        <v>911</v>
+      </c>
+      <c r="E42" s="76"/>
+      <c r="F42" s="122"/>
+      <c r="G42" s="122"/>
+      <c r="H42" s="78"/>
+    </row>
+    <row r="43" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A43" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="B43" s="140"/>
-      <c r="C43" s="88"/>
-      <c r="D43" s="88" t="s">
-        <v>912</v>
-      </c>
-      <c r="E43" s="88" t="s">
-        <v>916</v>
-      </c>
-      <c r="F43" s="89"/>
-    </row>
-    <row r="44" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A44" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="140"/>
-      <c r="C44" s="88"/>
-      <c r="D44" s="88" t="s">
-        <v>913</v>
-      </c>
-      <c r="E44" s="88" t="s">
-        <v>917</v>
-      </c>
-      <c r="F44" s="89"/>
-    </row>
-    <row r="45" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="77" t="s">
+        <v>901</v>
+      </c>
+      <c r="E43" s="77" t="s">
+        <v>908</v>
+      </c>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="78"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="149" t="s">
+        <v>884</v>
+      </c>
+      <c r="B44" s="150"/>
+      <c r="C44" s="150"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="150"/>
+      <c r="F44" s="150"/>
+      <c r="G44" s="150"/>
+      <c r="H44" s="151"/>
+    </row>
+    <row r="45" spans="1:8" ht="39" x14ac:dyDescent="0.35">
       <c r="A45" s="78" t="s">
-        <v>861</v>
-      </c>
-      <c r="B45" s="140"/>
+        <v>216</v>
+      </c>
+      <c r="B45" s="152" t="s">
+        <v>919</v>
+      </c>
       <c r="C45" s="88"/>
       <c r="D45" s="88" t="s">
+        <v>910</v>
+      </c>
+      <c r="E45" s="88" t="s">
+        <v>915</v>
+      </c>
+      <c r="F45" s="117"/>
+      <c r="G45" s="117"/>
+      <c r="H45" s="89"/>
+    </row>
+    <row r="46" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A46" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="152"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="88" t="s">
+        <v>912</v>
+      </c>
+      <c r="E46" s="88" t="s">
+        <v>916</v>
+      </c>
+      <c r="F46" s="117"/>
+      <c r="G46" s="117"/>
+      <c r="H46" s="89"/>
+    </row>
+    <row r="47" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A47" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="152"/>
+      <c r="C47" s="88"/>
+      <c r="D47" s="88" t="s">
+        <v>913</v>
+      </c>
+      <c r="E47" s="88" t="s">
+        <v>917</v>
+      </c>
+      <c r="F47" s="117"/>
+      <c r="G47" s="117"/>
+      <c r="H47" s="89"/>
+    </row>
+    <row r="48" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A48" s="78" t="s">
+        <v>861</v>
+      </c>
+      <c r="B48" s="152"/>
+      <c r="C48" s="88"/>
+      <c r="D48" s="88" t="s">
         <v>914</v>
       </c>
-      <c r="E45" s="88" t="s">
+      <c r="E48" s="88" t="s">
         <v>918</v>
       </c>
-      <c r="F45" s="89"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="141" t="s">
+      <c r="F48" s="117"/>
+      <c r="G48" s="117"/>
+      <c r="H48" s="89"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="153" t="s">
         <v>920</v>
       </c>
-      <c r="B46" s="141"/>
-      <c r="C46" s="141"/>
-      <c r="D46" s="141"/>
-      <c r="E46" s="141"/>
-      <c r="F46" s="141"/>
-    </row>
-    <row r="47" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="90"/>
-      <c r="B47" s="90"/>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="91"/>
-    </row>
-    <row r="48" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A48" s="89" t="s">
-        <v>956</v>
-      </c>
-      <c r="B48" s="132" t="s">
-        <v>957</v>
-      </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="72" t="s">
-        <v>955</v>
-      </c>
-      <c r="E48" s="135" t="s">
-        <v>958</v>
-      </c>
-      <c r="F48" s="91"/>
-    </row>
-    <row r="49" spans="1:6" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A49" s="89" t="s">
-        <v>421</v>
-      </c>
-      <c r="B49" s="134"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="72" t="s">
-        <v>954</v>
-      </c>
-      <c r="E49" s="136"/>
-      <c r="F49" s="91"/>
-    </row>
-    <row r="50" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="94"/>
-      <c r="B50" s="102"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="153"/>
+      <c r="E49" s="153"/>
+      <c r="F49" s="153"/>
+      <c r="G49" s="153"/>
+      <c r="H49" s="153"/>
+    </row>
+    <row r="50" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="90"/>
+      <c r="B50" s="90"/>
       <c r="C50" s="90"/>
       <c r="D50" s="90"/>
-      <c r="E50" s="102"/>
+      <c r="E50" s="90"/>
       <c r="F50" s="91"/>
-    </row>
-    <row r="51" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="132" t="s">
+      <c r="G50" s="91"/>
+      <c r="H50" s="91"/>
+    </row>
+    <row r="51" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A51" s="89" t="s">
+        <v>956</v>
+      </c>
+      <c r="B51" s="144" t="s">
+        <v>957</v>
+      </c>
+      <c r="C51" s="90"/>
+      <c r="D51" s="72" t="s">
+        <v>955</v>
+      </c>
+      <c r="E51" s="147" t="s">
+        <v>958</v>
+      </c>
+      <c r="F51" s="158"/>
+      <c r="G51" s="158"/>
+      <c r="H51" s="91"/>
+    </row>
+    <row r="52" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A52" s="89" t="s">
+        <v>421</v>
+      </c>
+      <c r="B52" s="146"/>
+      <c r="C52" s="90"/>
+      <c r="D52" s="72" t="s">
+        <v>954</v>
+      </c>
+      <c r="E52" s="148"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="91"/>
+    </row>
+    <row r="53" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="94"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="90"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="102"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+    </row>
+    <row r="54" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="143" t="s">
+      <c r="B54" s="155" t="s">
         <v>929</v>
       </c>
-      <c r="C51" s="93"/>
-      <c r="D51" s="73" t="s">
+      <c r="C54" s="93"/>
+      <c r="D54" s="73" t="s">
         <v>921</v>
       </c>
-      <c r="E51" s="143" t="s">
+      <c r="E54" s="155" t="s">
         <v>930</v>
       </c>
-      <c r="F51" s="94"/>
-    </row>
-    <row r="52" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A52" s="133"/>
-      <c r="B52" s="144"/>
-      <c r="C52" s="93"/>
-      <c r="D52" s="95" t="s">
+      <c r="F54" s="118"/>
+      <c r="G54" s="118"/>
+      <c r="H54" s="94"/>
+    </row>
+    <row r="55" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A55" s="145"/>
+      <c r="B55" s="156"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="95" t="s">
         <v>922</v>
       </c>
-      <c r="E52" s="144"/>
-      <c r="F52" s="94" t="s">
+      <c r="E55" s="156"/>
+      <c r="F55" s="119"/>
+      <c r="G55" s="119"/>
+      <c r="H55" s="94" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A53" s="133"/>
-      <c r="B53" s="144"/>
-      <c r="C53" s="93"/>
-      <c r="D53" s="95" t="s">
-        <v>744</v>
-      </c>
-      <c r="E53" s="144"/>
-      <c r="F53" s="94" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A54" s="133"/>
-      <c r="B54" s="144"/>
-      <c r="C54" s="93"/>
-      <c r="D54" s="95" t="s">
-        <v>923</v>
-      </c>
-      <c r="E54" s="144"/>
-      <c r="F54" s="94"/>
-    </row>
-    <row r="55" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="133"/>
-      <c r="B55" s="144"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="96" t="s">
-        <v>750</v>
-      </c>
-      <c r="E55" s="144"/>
-      <c r="F55" s="94"/>
-    </row>
-    <row r="56" spans="1:6" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A56" s="133"/>
-      <c r="B56" s="144"/>
+    <row r="56" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A56" s="145"/>
+      <c r="B56" s="156"/>
       <c r="C56" s="93"/>
       <c r="D56" s="95" t="s">
-        <v>924</v>
-      </c>
-      <c r="E56" s="144"/>
-      <c r="F56" s="94"/>
-    </row>
-    <row r="57" spans="1:6" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A57" s="133"/>
-      <c r="B57" s="144"/>
+        <v>744</v>
+      </c>
+      <c r="E56" s="156"/>
+      <c r="F56" s="119"/>
+      <c r="G56" s="119"/>
+      <c r="H56" s="94" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A57" s="145"/>
+      <c r="B57" s="156"/>
       <c r="C57" s="93"/>
       <c r="D57" s="95" t="s">
-        <v>925</v>
-      </c>
-      <c r="E57" s="144"/>
-      <c r="F57" s="94"/>
-    </row>
-    <row r="58" spans="1:6" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A58" s="133"/>
-      <c r="B58" s="144"/>
+        <v>923</v>
+      </c>
+      <c r="E57" s="156"/>
+      <c r="F57" s="119"/>
+      <c r="G57" s="119"/>
+      <c r="H57" s="94"/>
+    </row>
+    <row r="58" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="145"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="93"/>
-      <c r="D58" s="95" t="s">
-        <v>926</v>
-      </c>
-      <c r="E58" s="144"/>
-      <c r="F58" s="94"/>
-    </row>
-    <row r="59" spans="1:6" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A59" s="133"/>
-      <c r="B59" s="144"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="95" t="s">
-        <v>927</v>
-      </c>
-      <c r="E59" s="144"/>
-      <c r="F59" s="94"/>
-    </row>
-    <row r="60" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="133"/>
-      <c r="B60" s="144"/>
+      <c r="D58" s="96" t="s">
+        <v>750</v>
+      </c>
+      <c r="E58" s="156"/>
+      <c r="F58" s="119"/>
+      <c r="G58" s="119"/>
+      <c r="H58" s="94"/>
+    </row>
+    <row r="59" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A59" s="145"/>
+      <c r="B59" s="156"/>
+      <c r="C59" s="93" t="s">
+        <v>977</v>
+      </c>
+      <c r="D59" s="96"/>
+      <c r="E59" s="156"/>
+      <c r="F59" s="119"/>
+      <c r="G59" s="119"/>
+      <c r="H59" s="94"/>
+    </row>
+    <row r="60" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A60" s="145"/>
+      <c r="B60" s="156"/>
       <c r="C60" s="93"/>
       <c r="D60" s="95" t="s">
-        <v>753</v>
-      </c>
-      <c r="E60" s="144"/>
-      <c r="F60" s="94"/>
-    </row>
-    <row r="61" spans="1:6" s="92" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="142"/>
-      <c r="B61" s="145"/>
+        <v>924</v>
+      </c>
+      <c r="E60" s="156"/>
+      <c r="F60" s="119"/>
+      <c r="G60" s="119"/>
+      <c r="H60" s="94"/>
+    </row>
+    <row r="61" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A61" s="145"/>
+      <c r="B61" s="156"/>
       <c r="C61" s="93"/>
       <c r="D61" s="95" t="s">
+        <v>925</v>
+      </c>
+      <c r="E61" s="156"/>
+      <c r="F61" s="119"/>
+      <c r="G61" s="119"/>
+      <c r="H61" s="94"/>
+    </row>
+    <row r="62" spans="1:8" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A62" s="145"/>
+      <c r="B62" s="156"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="95" t="s">
+        <v>926</v>
+      </c>
+      <c r="E62" s="156"/>
+      <c r="F62" s="119"/>
+      <c r="G62" s="119"/>
+      <c r="H62" s="94"/>
+    </row>
+    <row r="63" spans="1:8" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A63" s="145"/>
+      <c r="B63" s="156"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="95" t="s">
+        <v>927</v>
+      </c>
+      <c r="E63" s="156"/>
+      <c r="F63" s="119"/>
+      <c r="G63" s="119"/>
+      <c r="H63" s="94"/>
+    </row>
+    <row r="64" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="145"/>
+      <c r="B64" s="156"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="95" t="s">
+        <v>753</v>
+      </c>
+      <c r="E64" s="156"/>
+      <c r="F64" s="119"/>
+      <c r="G64" s="119"/>
+      <c r="H64" s="94"/>
+    </row>
+    <row r="65" spans="1:8" s="92" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="154"/>
+      <c r="B65" s="157"/>
+      <c r="C65" s="93"/>
+      <c r="D65" s="95" t="s">
         <v>928</v>
       </c>
-      <c r="E61" s="145"/>
-      <c r="F61" s="94"/>
-    </row>
-    <row r="62" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="72"/>
-      <c r="B62" s="90"/>
-      <c r="C62" s="90"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="90"/>
-      <c r="F62" s="94"/>
-    </row>
-    <row r="63" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A63" s="72" t="s">
+      <c r="E65" s="157"/>
+      <c r="F65" s="120"/>
+      <c r="G65" s="120"/>
+      <c r="H65" s="94"/>
+    </row>
+    <row r="66" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="72"/>
+      <c r="B66" s="90"/>
+      <c r="C66" s="90"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="90"/>
+      <c r="F66" s="90"/>
+      <c r="G66" s="90"/>
+      <c r="H66" s="94"/>
+    </row>
+    <row r="67" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A67" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="132" t="s">
+      <c r="B67" s="144" t="s">
         <v>950</v>
       </c>
-      <c r="C63" s="90"/>
-      <c r="D63" s="72" t="s">
+      <c r="C67" s="90"/>
+      <c r="D67" s="72" t="s">
         <v>933</v>
       </c>
-      <c r="E63" s="90"/>
-      <c r="F63" s="94"/>
-    </row>
-    <row r="64" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A64" s="72" t="s">
-        <v>934</v>
-      </c>
-      <c r="B64" s="133"/>
-      <c r="C64" s="90"/>
-      <c r="D64" s="85" t="s">
-        <v>938</v>
-      </c>
-      <c r="E64" s="90" t="s">
-        <v>935</v>
-      </c>
-      <c r="F64" s="94"/>
-    </row>
-    <row r="65" spans="1:6" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A65" s="72" t="s">
-        <v>934</v>
-      </c>
-      <c r="B65" s="133"/>
-      <c r="C65" s="90"/>
-      <c r="D65" s="85" t="s">
-        <v>581</v>
-      </c>
-      <c r="E65" s="90"/>
-      <c r="F65" s="94"/>
-    </row>
-    <row r="66" spans="1:6" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A66" s="72" t="s">
-        <v>937</v>
-      </c>
-      <c r="B66" s="133"/>
-      <c r="C66" s="90"/>
-      <c r="D66" s="85" t="s">
-        <v>936</v>
-      </c>
-      <c r="E66" s="90"/>
-      <c r="F66" s="94"/>
-    </row>
-    <row r="67" spans="1:6" s="92" customFormat="1" ht="117" x14ac:dyDescent="0.35">
-      <c r="A67" s="72" t="s">
-        <v>934</v>
-      </c>
-      <c r="B67" s="133"/>
-      <c r="C67" s="90"/>
-      <c r="D67" s="85" t="s">
-        <v>939</v>
-      </c>
-      <c r="E67" s="90" t="s">
-        <v>935</v>
-      </c>
-      <c r="F67" s="94"/>
-    </row>
-    <row r="68" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="E67" s="90"/>
+      <c r="F67" s="90"/>
+      <c r="G67" s="90"/>
+      <c r="H67" s="94"/>
+    </row>
+    <row r="68" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A68" s="72" t="s">
         <v>934</v>
       </c>
-      <c r="B68" s="133"/>
+      <c r="B68" s="145"/>
       <c r="C68" s="90"/>
       <c r="D68" s="85" t="s">
-        <v>598</v>
+        <v>938</v>
       </c>
       <c r="E68" s="90" t="s">
         <v>935</v>
       </c>
-      <c r="F68" s="94"/>
-    </row>
-    <row r="69" spans="1:6" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="F68" s="90"/>
+      <c r="G68" s="90"/>
+      <c r="H68" s="94"/>
+    </row>
+    <row r="69" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
       <c r="A69" s="72" t="s">
         <v>934</v>
       </c>
-      <c r="B69" s="133"/>
+      <c r="B69" s="145"/>
       <c r="C69" s="90"/>
       <c r="D69" s="85" t="s">
+        <v>581</v>
+      </c>
+      <c r="E69" s="90"/>
+      <c r="F69" s="90"/>
+      <c r="G69" s="90"/>
+      <c r="H69" s="94"/>
+    </row>
+    <row r="70" spans="1:8" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A70" s="72" t="s">
+        <v>937</v>
+      </c>
+      <c r="B70" s="145"/>
+      <c r="C70" s="90"/>
+      <c r="D70" s="85" t="s">
+        <v>936</v>
+      </c>
+      <c r="E70" s="90"/>
+      <c r="F70" s="90"/>
+      <c r="G70" s="90"/>
+      <c r="H70" s="94"/>
+    </row>
+    <row r="71" spans="1:8" s="92" customFormat="1" ht="117" x14ac:dyDescent="0.35">
+      <c r="A71" s="72" t="s">
+        <v>934</v>
+      </c>
+      <c r="B71" s="145"/>
+      <c r="C71" s="90"/>
+      <c r="D71" s="85" t="s">
+        <v>939</v>
+      </c>
+      <c r="E71" s="90" t="s">
+        <v>935</v>
+      </c>
+      <c r="F71" s="90"/>
+      <c r="G71" s="90"/>
+      <c r="H71" s="94"/>
+    </row>
+    <row r="72" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A72" s="72" t="s">
+        <v>934</v>
+      </c>
+      <c r="B72" s="145"/>
+      <c r="C72" s="90"/>
+      <c r="D72" s="85" t="s">
+        <v>598</v>
+      </c>
+      <c r="E72" s="90" t="s">
+        <v>935</v>
+      </c>
+      <c r="F72" s="90"/>
+      <c r="G72" s="90"/>
+      <c r="H72" s="94"/>
+    </row>
+    <row r="73" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A73" s="72" t="s">
+        <v>934</v>
+      </c>
+      <c r="B73" s="145"/>
+      <c r="C73" s="90"/>
+      <c r="D73" s="85" t="s">
         <v>940</v>
       </c>
-      <c r="E69" s="90"/>
-      <c r="F69" s="94"/>
-    </row>
-    <row r="70" spans="1:6" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A70" s="72" t="s">
+      <c r="E73" s="90"/>
+      <c r="F73" s="90"/>
+      <c r="G73" s="90"/>
+      <c r="H73" s="94"/>
+    </row>
+    <row r="74" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A74" s="72" t="s">
         <v>941</v>
       </c>
-      <c r="B70" s="123"/>
-      <c r="C70" s="90"/>
-      <c r="D70" s="99" t="s">
-        <v>942</v>
-      </c>
-      <c r="E70" s="90"/>
-      <c r="F70" s="94"/>
-    </row>
-    <row r="71" spans="1:6" s="92" customFormat="1" ht="117" x14ac:dyDescent="0.35">
-      <c r="A71" s="72" t="s">
-        <v>941</v>
-      </c>
-      <c r="B71" s="124"/>
-      <c r="C71" s="90"/>
-      <c r="D71" s="99" t="s">
-        <v>943</v>
-      </c>
-      <c r="E71" s="90"/>
-      <c r="F71" s="94"/>
-    </row>
-    <row r="72" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="72"/>
-      <c r="B72" s="98"/>
-      <c r="C72" s="90"/>
-      <c r="D72" s="99"/>
-      <c r="E72" s="90"/>
-      <c r="F72" s="94"/>
-    </row>
-    <row r="73" spans="1:6" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A73" s="72" t="s">
-        <v>941</v>
-      </c>
-      <c r="B73" s="122" t="s">
-        <v>953</v>
-      </c>
-      <c r="C73" s="90"/>
-      <c r="D73" s="99" t="s">
-        <v>944</v>
-      </c>
-      <c r="E73" s="90"/>
-      <c r="F73" s="94"/>
-    </row>
-    <row r="74" spans="1:6" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A74" s="72" t="s">
-        <v>951</v>
-      </c>
-      <c r="B74" s="123"/>
+      <c r="B74" s="135"/>
       <c r="C74" s="90"/>
       <c r="D74" s="99" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="E74" s="90"/>
-      <c r="F74" s="94"/>
-    </row>
-    <row r="75" spans="1:6" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="F74" s="90"/>
+      <c r="G74" s="90"/>
+      <c r="H74" s="94"/>
+    </row>
+    <row r="75" spans="1:8" s="92" customFormat="1" ht="117" x14ac:dyDescent="0.35">
       <c r="A75" s="72" t="s">
-        <v>951</v>
-      </c>
-      <c r="B75" s="123"/>
+        <v>941</v>
+      </c>
+      <c r="B75" s="136"/>
       <c r="C75" s="90"/>
       <c r="D75" s="99" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="E75" s="90"/>
-      <c r="F75" s="94"/>
-    </row>
-    <row r="76" spans="1:6" s="92" customFormat="1" ht="78" x14ac:dyDescent="0.35">
-      <c r="A76" s="72" t="s">
+      <c r="F75" s="90"/>
+      <c r="G75" s="90"/>
+      <c r="H75" s="94"/>
+    </row>
+    <row r="76" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="72"/>
+      <c r="B76" s="98"/>
+      <c r="C76" s="90"/>
+      <c r="D76" s="99"/>
+      <c r="E76" s="90"/>
+      <c r="F76" s="90"/>
+      <c r="G76" s="90"/>
+      <c r="H76" s="94"/>
+    </row>
+    <row r="77" spans="1:8" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A77" s="72" t="s">
         <v>941</v>
       </c>
-      <c r="B76" s="123"/>
-      <c r="C76" s="90"/>
-      <c r="D76" s="99" t="s">
-        <v>947</v>
-      </c>
-      <c r="E76" s="90"/>
-      <c r="F76" s="94"/>
-    </row>
-    <row r="77" spans="1:6" s="92" customFormat="1" ht="130" x14ac:dyDescent="0.35">
-      <c r="A77" s="72" t="s">
-        <v>951</v>
-      </c>
-      <c r="B77" s="123"/>
+      <c r="B77" s="134" t="s">
+        <v>953</v>
+      </c>
       <c r="C77" s="90"/>
       <c r="D77" s="99" t="s">
+        <v>944</v>
+      </c>
+      <c r="E77" s="90"/>
+      <c r="F77" s="90"/>
+      <c r="G77" s="90"/>
+      <c r="H77" s="94"/>
+    </row>
+    <row r="78" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A78" s="72" t="s">
+        <v>951</v>
+      </c>
+      <c r="B78" s="135"/>
+      <c r="C78" s="90"/>
+      <c r="D78" s="99" t="s">
+        <v>945</v>
+      </c>
+      <c r="E78" s="90"/>
+      <c r="F78" s="90"/>
+      <c r="G78" s="90"/>
+      <c r="H78" s="94"/>
+    </row>
+    <row r="79" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+      <c r="A79" s="72" t="s">
+        <v>951</v>
+      </c>
+      <c r="B79" s="135"/>
+      <c r="C79" s="90"/>
+      <c r="D79" s="99" t="s">
+        <v>946</v>
+      </c>
+      <c r="E79" s="90"/>
+      <c r="F79" s="90"/>
+      <c r="G79" s="90"/>
+      <c r="H79" s="94"/>
+    </row>
+    <row r="80" spans="1:8" s="92" customFormat="1" ht="78" x14ac:dyDescent="0.35">
+      <c r="A80" s="72" t="s">
+        <v>941</v>
+      </c>
+      <c r="B80" s="135"/>
+      <c r="C80" s="90"/>
+      <c r="D80" s="99" t="s">
+        <v>947</v>
+      </c>
+      <c r="E80" s="90"/>
+      <c r="F80" s="90"/>
+      <c r="G80" s="90"/>
+      <c r="H80" s="94"/>
+    </row>
+    <row r="81" spans="1:8" s="92" customFormat="1" ht="130" x14ac:dyDescent="0.35">
+      <c r="A81" s="72" t="s">
+        <v>951</v>
+      </c>
+      <c r="B81" s="135"/>
+      <c r="C81" s="90"/>
+      <c r="D81" s="99" t="s">
         <v>949</v>
       </c>
-      <c r="E77" s="90"/>
-      <c r="F77" s="94"/>
-    </row>
-    <row r="78" spans="1:6" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A78" s="72" t="s">
+      <c r="E81" s="90"/>
+      <c r="F81" s="90"/>
+      <c r="G81" s="90"/>
+      <c r="H81" s="94"/>
+    </row>
+    <row r="82" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A82" s="72" t="s">
         <v>952</v>
       </c>
-      <c r="B78" s="124"/>
-      <c r="C78" s="90"/>
-      <c r="D78" s="85" t="s">
+      <c r="B82" s="136"/>
+      <c r="C82" s="90"/>
+      <c r="D82" s="85" t="s">
         <v>948</v>
       </c>
-      <c r="E78" s="90"/>
-      <c r="F78" s="94"/>
-    </row>
-    <row r="79" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="72"/>
-      <c r="B79" s="98"/>
-      <c r="C79" s="90"/>
-      <c r="D79" s="99"/>
-      <c r="E79" s="90"/>
-      <c r="F79" s="94"/>
-    </row>
-    <row r="80" spans="1:6" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="90"/>
-      <c r="B80" s="90"/>
-      <c r="C80" s="90"/>
-      <c r="D80" s="90"/>
-      <c r="E80" s="90"/>
-      <c r="F80" s="94"/>
-    </row>
-    <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A81" s="98" t="s">
+      <c r="E82" s="90"/>
+      <c r="F82" s="90"/>
+      <c r="G82" s="90"/>
+      <c r="H82" s="94"/>
+    </row>
+    <row r="83" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="72"/>
+      <c r="B83" s="98"/>
+      <c r="C83" s="90"/>
+      <c r="D83" s="99"/>
+      <c r="E83" s="90"/>
+      <c r="F83" s="90"/>
+      <c r="G83" s="90"/>
+      <c r="H83" s="94"/>
+    </row>
+    <row r="84" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="90"/>
+      <c r="B84" s="90"/>
+      <c r="C84" s="90"/>
+      <c r="D84" s="90"/>
+      <c r="E84" s="90"/>
+      <c r="F84" s="90"/>
+      <c r="G84" s="90"/>
+      <c r="H84" s="94"/>
+    </row>
+    <row r="85" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A85" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="B81" s="98" t="s">
+      <c r="B85" s="98" t="s">
         <v>317</v>
       </c>
-      <c r="C81" s="98"/>
-      <c r="D81" s="99" t="s">
+      <c r="C85" s="98"/>
+      <c r="D85" s="99" t="s">
         <v>720</v>
       </c>
-      <c r="E81" s="100"/>
-      <c r="F81" s="78"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" s="101"/>
-      <c r="B82" s="101"/>
-      <c r="C82" s="101"/>
-      <c r="D82" s="101"/>
-      <c r="E82" s="101"/>
-      <c r="F82" s="78"/>
-    </row>
-    <row r="83" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A83" s="78" t="s">
+      <c r="E85" s="100"/>
+      <c r="F85" s="100"/>
+      <c r="G85" s="100"/>
+      <c r="H85" s="78"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="101"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="101"/>
+      <c r="D86" s="101"/>
+      <c r="E86" s="101"/>
+      <c r="F86" s="101"/>
+      <c r="G86" s="101"/>
+      <c r="H86" s="78"/>
+    </row>
+    <row r="87" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A87" s="78" t="s">
         <v>881</v>
-      </c>
-      <c r="B83" s="78"/>
-      <c r="C83" s="78"/>
-      <c r="D83" s="85" t="s">
-        <v>883</v>
-      </c>
-      <c r="E83" s="78"/>
-      <c r="F83" s="78"/>
-    </row>
-    <row r="84" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="78"/>
-      <c r="B84" s="78"/>
-      <c r="C84" s="78"/>
-      <c r="D84" s="78"/>
-      <c r="E84" s="78"/>
-      <c r="F84" s="78"/>
-    </row>
-    <row r="85" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A85" s="78" t="s">
-        <v>881</v>
-      </c>
-      <c r="B85" s="78"/>
-      <c r="C85" s="78"/>
-      <c r="D85" s="85" t="s">
-        <v>727</v>
-      </c>
-      <c r="E85" s="78"/>
-      <c r="F85" s="78"/>
-    </row>
-    <row r="86" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A86" s="78" t="s">
-        <v>881</v>
-      </c>
-      <c r="B86" s="78"/>
-      <c r="C86" s="78"/>
-      <c r="D86" s="85" t="s">
-        <v>570</v>
-      </c>
-      <c r="E86" s="78"/>
-      <c r="F86" s="78"/>
-    </row>
-    <row r="87" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A87" s="78" t="s">
-        <v>882</v>
       </c>
       <c r="B87" s="78"/>
       <c r="C87" s="78"/>
       <c r="D87" s="85" t="s">
-        <v>573</v>
+        <v>883</v>
       </c>
       <c r="E87" s="78"/>
-      <c r="F87" s="78"/>
-    </row>
-    <row r="88" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A88" s="78" t="s">
-        <v>882</v>
-      </c>
+      <c r="F87" s="121"/>
+      <c r="G87" s="121"/>
+      <c r="H87" s="78"/>
+    </row>
+    <row r="88" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="78"/>
       <c r="B88" s="78"/>
       <c r="C88" s="78"/>
-      <c r="D88" s="85" t="s">
-        <v>576</v>
-      </c>
+      <c r="D88" s="78"/>
       <c r="E88" s="78"/>
-      <c r="F88" s="78"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" s="78"/>
+      <c r="F88" s="121"/>
+      <c r="G88" s="121"/>
+      <c r="H88" s="78"/>
+    </row>
+    <row r="89" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A89" s="78" t="s">
+        <v>881</v>
+      </c>
       <c r="B89" s="78"/>
       <c r="C89" s="78"/>
+      <c r="D89" s="85" t="s">
+        <v>727</v>
+      </c>
       <c r="E89" s="78"/>
-      <c r="F89" s="78"/>
-    </row>
-    <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.35">
-      <c r="A90" s="78"/>
+      <c r="F89" s="121"/>
+      <c r="G89" s="121"/>
+      <c r="H89" s="78"/>
+    </row>
+    <row r="90" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A90" s="78" t="s">
+        <v>881</v>
+      </c>
       <c r="B90" s="78"/>
       <c r="C90" s="78"/>
       <c r="D90" s="85" t="s">
-        <v>614</v>
+        <v>570</v>
       </c>
       <c r="E90" s="78"/>
-      <c r="F90" s="78"/>
-    </row>
-    <row r="91" spans="1:6" ht="65" x14ac:dyDescent="0.35">
-      <c r="A91" s="78"/>
+      <c r="F90" s="121"/>
+      <c r="G90" s="121"/>
+      <c r="H90" s="78"/>
+    </row>
+    <row r="91" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A91" s="78" t="s">
+        <v>882</v>
+      </c>
       <c r="B91" s="78"/>
       <c r="C91" s="78"/>
       <c r="D91" s="85" t="s">
-        <v>617</v>
+        <v>573</v>
       </c>
       <c r="E91" s="78"/>
-      <c r="F91" s="78"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="78"/>
+      <c r="F91" s="121"/>
+      <c r="G91" s="121"/>
+      <c r="H91" s="78"/>
+    </row>
+    <row r="92" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A92" s="78" t="s">
+        <v>882</v>
+      </c>
       <c r="B92" s="78"/>
       <c r="C92" s="78"/>
-      <c r="D92" s="85"/>
+      <c r="D92" s="85" t="s">
+        <v>576</v>
+      </c>
       <c r="E92" s="78"/>
-      <c r="F92" s="78"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F92" s="121"/>
+      <c r="G92" s="121"/>
+      <c r="H92" s="78"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="78"/>
       <c r="B93" s="78"/>
       <c r="C93" s="78"/>
-      <c r="D93" s="85"/>
       <c r="E93" s="78"/>
-      <c r="F93" s="78"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F93" s="121"/>
+      <c r="G93" s="121"/>
+      <c r="H93" s="78"/>
+    </row>
+    <row r="94" spans="1:8" ht="39" x14ac:dyDescent="0.35">
       <c r="A94" s="78"/>
       <c r="B94" s="78"/>
       <c r="C94" s="78"/>
+      <c r="D94" s="85" t="s">
+        <v>614</v>
+      </c>
       <c r="E94" s="78"/>
-      <c r="F94" s="78"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F94" s="121"/>
+      <c r="G94" s="121"/>
+      <c r="H94" s="78"/>
+    </row>
+    <row r="95" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A95" s="78"/>
       <c r="B95" s="78"/>
       <c r="C95" s="78"/>
-      <c r="D95" s="85"/>
+      <c r="D95" s="85" t="s">
+        <v>617</v>
+      </c>
       <c r="E95" s="78"/>
-      <c r="F95" s="78"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F95" s="121"/>
+      <c r="G95" s="121"/>
+      <c r="H95" s="78"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="78"/>
       <c r="B96" s="78"/>
       <c r="C96" s="78"/>
       <c r="D96" s="85"/>
       <c r="E96" s="78"/>
-      <c r="F96" s="78"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F96" s="121"/>
+      <c r="G96" s="121"/>
+      <c r="H96" s="78"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="78"/>
       <c r="B97" s="78"/>
       <c r="C97" s="78"/>
       <c r="D97" s="85"/>
       <c r="E97" s="78"/>
-      <c r="F97" s="78"/>
-    </row>
-    <row r="98" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+      <c r="F97" s="121"/>
+      <c r="G97" s="121"/>
+      <c r="H97" s="78"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="78"/>
       <c r="B98" s="78"/>
       <c r="C98" s="78"/>
-      <c r="D98" s="85" t="s">
-        <v>734</v>
-      </c>
       <c r="E98" s="78"/>
-      <c r="F98" s="78"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F98" s="121"/>
+      <c r="G98" s="121"/>
+      <c r="H98" s="78"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="78"/>
       <c r="B99" s="78"/>
       <c r="C99" s="78"/>
+      <c r="D99" s="85"/>
       <c r="E99" s="78"/>
-      <c r="F99" s="78"/>
-    </row>
-    <row r="100" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="F99" s="121"/>
+      <c r="G99" s="121"/>
+      <c r="H99" s="78"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="78"/>
       <c r="B100" s="78"/>
       <c r="C100" s="78"/>
-      <c r="D100" s="85" t="s">
-        <v>762</v>
-      </c>
+      <c r="D100" s="85"/>
       <c r="E100" s="78"/>
-      <c r="F100" s="78"/>
-    </row>
-    <row r="101" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="F100" s="121"/>
+      <c r="G100" s="121"/>
+      <c r="H100" s="78"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="78"/>
       <c r="B101" s="78"/>
       <c r="C101" s="78"/>
-      <c r="D101" s="85" t="s">
-        <v>766</v>
-      </c>
+      <c r="D101" s="85"/>
       <c r="E101" s="78"/>
-      <c r="F101" s="78"/>
-    </row>
-    <row r="102" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+      <c r="F101" s="121"/>
+      <c r="G101" s="121"/>
+      <c r="H101" s="78"/>
+    </row>
+    <row r="102" spans="1:8" ht="52" x14ac:dyDescent="0.35">
       <c r="A102" s="78"/>
       <c r="B102" s="78"/>
       <c r="C102" s="78"/>
       <c r="D102" s="85" t="s">
-        <v>866</v>
+        <v>734</v>
       </c>
       <c r="E102" s="78"/>
-      <c r="F102" s="78"/>
-    </row>
-    <row r="103" spans="1:6" ht="78" x14ac:dyDescent="0.35">
+      <c r="F102" s="121"/>
+      <c r="G102" s="121"/>
+      <c r="H102" s="78"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="78"/>
       <c r="B103" s="78"/>
       <c r="C103" s="78"/>
-      <c r="D103" s="85" t="s">
-        <v>867</v>
-      </c>
       <c r="E103" s="78"/>
-      <c r="F103" s="78"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F103" s="121"/>
+      <c r="G103" s="121"/>
+      <c r="H103" s="78"/>
+    </row>
+    <row r="104" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A104" s="78"/>
       <c r="B104" s="78"/>
       <c r="C104" s="78"/>
-      <c r="D104" s="85"/>
+      <c r="D104" s="85" t="s">
+        <v>762</v>
+      </c>
       <c r="E104" s="78"/>
-      <c r="F104" s="78"/>
+      <c r="F104" s="121"/>
+      <c r="G104" s="121"/>
+      <c r="H104" s="78"/>
+    </row>
+    <row r="105" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A105" s="78"/>
+      <c r="B105" s="78"/>
+      <c r="C105" s="78"/>
+      <c r="D105" s="85" t="s">
+        <v>766</v>
+      </c>
+      <c r="E105" s="78"/>
+      <c r="F105" s="121"/>
+      <c r="G105" s="121"/>
+      <c r="H105" s="78"/>
+    </row>
+    <row r="106" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A106" s="78"/>
+      <c r="B106" s="78"/>
+      <c r="C106" s="78"/>
+      <c r="D106" s="85" t="s">
+        <v>866</v>
+      </c>
+      <c r="E106" s="78"/>
+      <c r="F106" s="121"/>
+      <c r="G106" s="121"/>
+      <c r="H106" s="78"/>
+    </row>
+    <row r="107" spans="1:8" ht="78" x14ac:dyDescent="0.35">
+      <c r="A107" s="78"/>
+      <c r="B107" s="78"/>
+      <c r="C107" s="78"/>
+      <c r="D107" s="85" t="s">
+        <v>867</v>
+      </c>
+      <c r="E107" s="78"/>
+      <c r="F107" s="121"/>
+      <c r="G107" s="121"/>
+      <c r="H107" s="78"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108" s="78"/>
+      <c r="B108" s="78"/>
+      <c r="C108" s="78"/>
+      <c r="D108" s="85"/>
+      <c r="E108" s="78"/>
+      <c r="F108" s="121"/>
+      <c r="G108" s="121"/>
+      <c r="H108" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A51:A61"/>
-    <mergeCell ref="B51:B61"/>
-    <mergeCell ref="E51:E61"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B67:B75"/>
+    <mergeCell ref="B77:B82"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A54:A65"/>
+    <mergeCell ref="B54:B65"/>
+    <mergeCell ref="E54:E65"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="87.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C3" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C4" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C5" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="C6" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C7" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="C8" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="C9" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="C10" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C11" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C12" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C13" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10240,7 +10812,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="112" t="s">
+      <c r="C3" s="124" t="s">
         <v>186</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -10249,28 +10821,28 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="112"/>
+      <c r="C4" s="124"/>
       <c r="D4" s="21" t="s">
         <v>188</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="112"/>
+      <c r="C5" s="124"/>
       <c r="D5" s="21" t="s">
         <v>189</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C6" s="112"/>
+      <c r="C6" s="124"/>
       <c r="D6" s="4" t="s">
         <v>190</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="112"/>
+      <c r="C7" s="124"/>
       <c r="D7" s="4" t="s">
         <v>191</v>
       </c>
@@ -10324,7 +10896,7 @@
       <c r="E14"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="125" t="s">
         <v>198</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -10335,37 +10907,37 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C16" s="113"/>
+      <c r="C16" s="125"/>
       <c r="D16" s="4" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17" s="113"/>
+      <c r="C17" s="125"/>
       <c r="D17" s="4" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C18" s="113"/>
+      <c r="C18" s="125"/>
       <c r="D18" s="4" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C19" s="113"/>
+      <c r="C19" s="125"/>
       <c r="D19" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C20" s="113"/>
+      <c r="C20" s="125"/>
       <c r="D20" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C21" s="113"/>
+      <c r="C21" s="125"/>
       <c r="D21" s="1" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
modification of stream definition in dataflow-pipeline.bat
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -31,16 +31,12 @@
     <sheet name="Pending" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="1040">
   <si>
     <t>Term</t>
   </si>
@@ -3445,9 +3441,6 @@
     <t>Product-&gt;BusinessAccount</t>
   </si>
   <si>
-    <t>Setting of manual forecast will trigger ManualForecastCreation event which is received by Business domain. Business domain then updates the purchase budget with the total demand count per period*purchase price,for each received forecast.</t>
-  </si>
-  <si>
     <t>Update of purchase budget with manual forecast</t>
   </si>
   <si>
@@ -4479,9 +4472,12 @@
     <t>Administrator sets manual forecast for each registered product/or through mass upload of product forecasts.(ForecastController)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Instance of ProductAnalyseraggregate is created.
-It usesManualForecastHelper to add the manual forecast for a product in </t>
+    <t xml:space="preserve">Instance of ProductAnalyseraggregate is created.
+</t>
+  </si>
+  <si>
+    <r>
+      <t>It uses</t>
     </r>
     <r>
       <rPr>
@@ -4491,7 +4487,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>ProductForecastView</t>
+      <t>ManualForecastHelper</t>
     </r>
     <r>
       <rPr>
@@ -4500,7 +4496,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">. Also the </t>
+      <t xml:space="preserve"> to add the manual forecast for a product in </t>
     </r>
     <r>
       <rPr>
@@ -4510,7 +4506,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>ProductActivationStatusView</t>
+      <t>ProductForecastView.</t>
     </r>
     <r>
       <rPr>
@@ -4519,8 +4515,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> is updated with the status "FORECASTED".
-Pseudo actuals(daily forecast values) are then derived out of forecast view using interpolation and then sotred in </t>
+      <t xml:space="preserve"> Also the </t>
     </r>
     <r>
       <rPr>
@@ -4530,7 +4525,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>ProductPseudoActualsView</t>
+      <t>ProductActivationStatusView</t>
     </r>
     <r>
       <rPr>
@@ -4539,8 +4534,8 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">.
-Finally the change of demand forecast from 0 to new value has been calculated dayon day/month on month by </t>
+      <t xml:space="preserve"> is updated with the status "FORECASTED".
+Pseudo actuals(daily forecast values) are then derived out of forecast view using interpolation and then sotred in </t>
     </r>
     <r>
       <rPr>
@@ -4550,15 +4545,17 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ProductTrendChangeDetector </t>
+      <t>ProductPseudoActualsView.</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">and it fires either of </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Finally the change of demand forecast from 0 to new value has been calculated dayon day/month on month by </t>
     </r>
     <r>
       <rPr>
@@ -4568,15 +4565,16 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">IncreaseInProductTotalCountEvent </t>
+      <t>ProductTrendChangeDetector</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">or </t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and it fires either of </t>
     </r>
     <r>
       <rPr>
@@ -4586,7 +4584,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>DecreaseInProductTotalCountEvent</t>
+      <t>IncreaseInProductTotalCountEvent</t>
     </r>
     <r>
       <rPr>
@@ -4595,8 +4593,454 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>DecreaseInProductTotalCountEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">
 depending upon comparison of earlier demand forecast trend and new demand forecast trend. This informaiton is not stored in product domain but passed to Business Account.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">AddToPurchaseCostAccountCommand </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">causes storing of additional budget amount to provision recommendation account ,if the budget adjustment option configured by admin is "RECOMMEND BUDGET ADJUSTEMENT". Else it is added to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PurchaseCostAccount.
+PurchaseCostCreditedEvent </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>stores the additional purchase cost provsion to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> PurchaseCostAccount.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">In case of recommendation </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AdditionalBudgetRecommendationAddedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is added to recommendations list.</t>
+    </r>
+  </si>
+  <si>
+    <t>transaction view is yet to be updated.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PurchaseCostCreditedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> also adds the additional budget to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PurchaseCostAccountView.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AdditionalBudgetRecommendationAddedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> adds the recommendation to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BudgetChangeRecommendationView</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Setting of manual forecast will trigger </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>IncreaseInProductTotalCountEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">DecreaseInProductTotalCountEvent.
+The IncreaseInProductTotalCountEvent </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>causes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">comparison of current forecast for the same period with new one brought by event. In case there is a difference then ProductForecastView in Business domain is updated with revised total subscription count.
+Since there is a change in forecasted demand the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">AddToPurchaseCostAccountCommand </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>is fired to adjust the PurchaseBudget.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>DecreaseInProductTotalCountEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> causes comparison of current forecast for the same period with new one brought by event. In case there is a difference then ProductForecastView in Business domain is updated with revised total subscription count.
+Since there is a change in forecasted demand the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ReduceFromPurchaseCostAccountCommand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is fired to adjust the PurchaseBudget.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ReduceFromPurchaseCostAccountCommand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> causes storing of reduced budget amount to provision recommendation account ,if the budget adjustment option configured by admin is "RECOMMEND BUDGET ADJUSTEMENT". Else it is reduced from PurchaseCostAccount.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PurchaseCostDebitedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> stores the reduced purchase cost provsion to PurchaseCostAccount.
+In case of recommendation </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BudgetReductionRecommendationAddedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is added to recommendations list.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PurchaseCostDebitedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> also sets reduced budget to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PurchaseCostAccountView.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> BudgetReductionRecommendationAddedEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> adds the recommendation to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BudgetChangeRecommendationView</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -4725,7 +5169,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4770,30 +5214,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -4866,73 +5292,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5132,188 +5496,8 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5348,79 +5532,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6569,12 +6717,12 @@
       <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="135" t="s">
+      <c r="A20" s="75" t="s">
         <v>553</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="136" t="s">
+      <c r="D20" s="76" t="s">
         <v>554</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -6591,10 +6739,10 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="135"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="136"/>
+      <c r="D21" s="76"/>
       <c r="E21" s="47" t="s">
         <v>556</v>
       </c>
@@ -6609,10 +6757,10 @@
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="135"/>
+      <c r="A22" s="75"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="136"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="48" t="s">
         <v>557</v>
       </c>
@@ -6627,10 +6775,10 @@
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="135"/>
+      <c r="A23" s="75"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="136"/>
+      <c r="D23" s="76"/>
       <c r="E23" s="48" t="s">
         <v>558</v>
       </c>
@@ -7637,48 +7785,48 @@
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
-      <c r="B17" s="137" t="s">
+      <c r="B17" s="77" t="s">
         <v>678</v>
       </c>
-      <c r="C17" s="137"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="77" t="s">
         <v>679</v>
       </c>
-      <c r="C18" s="137"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
-      <c r="B19" s="137" t="s">
+      <c r="B19" s="77" t="s">
         <v>680</v>
       </c>
-      <c r="C19" s="137"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
-      <c r="B20" s="137" t="s">
+      <c r="B20" s="77" t="s">
         <v>681</v>
       </c>
-      <c r="C20" s="137"/>
+      <c r="C20" s="77"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
-      <c r="B21" s="137"/>
-      <c r="C21" s="137"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -8054,7 +8202,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="79" t="s">
         <v>690</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -8063,14 +8211,14 @@
       <c r="D2" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="E2" s="139" t="s">
+      <c r="E2" s="79" t="s">
         <v>693</v>
       </c>
-      <c r="F2" s="139" t="s">
+      <c r="F2" s="79" t="s">
         <v>694</v>
       </c>
-      <c r="G2" s="139"/>
-      <c r="H2" s="140" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="80" t="s">
         <v>695</v>
       </c>
     </row>
@@ -8078,21 +8226,21 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="139"/>
+      <c r="B3" s="79"/>
       <c r="C3" s="9" t="s">
         <v>696</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="140"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
     </row>
     <row r="4" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
-      <c r="B4" s="139"/>
+      <c r="B4" s="79"/>
       <c r="C4" s="55" t="s">
         <v>698</v>
       </c>
@@ -8102,14 +8250,14 @@
       <c r="E4" s="55" t="s">
         <v>700</v>
       </c>
-      <c r="F4" s="141" t="s">
+      <c r="F4" s="81" t="s">
         <v>701</v>
       </c>
-      <c r="G4" s="142"/>
+      <c r="G4" s="82"/>
     </row>
     <row r="5" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="139"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="55" t="s">
         <v>702</v>
       </c>
@@ -8117,12 +8265,12 @@
         <v>703</v>
       </c>
       <c r="E5" s="55"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="142"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="82"/>
     </row>
     <row r="6" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="139"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="55" t="s">
         <v>704</v>
       </c>
@@ -8132,21 +8280,21 @@
       <c r="E6" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="F6" s="141"/>
-      <c r="G6" s="142"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="82"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="139"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="141"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:8" ht="52" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
-      <c r="B8" s="139"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="55" t="s">
         <v>707</v>
       </c>
@@ -8156,12 +8304,12 @@
       <c r="E8" s="55" t="s">
         <v>709</v>
       </c>
-      <c r="F8" s="141"/>
+      <c r="F8" s="81"/>
       <c r="G8" s="56"/>
     </row>
     <row r="9" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="139"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="9" t="s">
         <v>710</v>
       </c>
@@ -8171,14 +8319,14 @@
       <c r="E9" s="9" t="s">
         <v>712</v>
       </c>
-      <c r="F9" s="141"/>
+      <c r="F9" s="81"/>
       <c r="G9" s="9" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="139"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="9" t="s">
         <v>714</v>
       </c>
@@ -8188,12 +8336,12 @@
       <c r="E10" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="F10" s="141"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="156" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="139"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="9" t="s">
         <v>716</v>
       </c>
@@ -8231,7 +8379,7 @@
     </row>
     <row r="13" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="138" t="s">
+      <c r="B13" s="78" t="s">
         <v>725</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -8246,7 +8394,7 @@
     </row>
     <row r="14" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="138"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="9" t="s">
         <v>531</v>
       </c>
@@ -8259,7 +8407,7 @@
     </row>
     <row r="15" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="138"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="9" t="s">
         <v>533</v>
       </c>
@@ -8272,7 +8420,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
-      <c r="B16" s="138"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="9" t="s">
         <v>536</v>
       </c>
@@ -8285,7 +8433,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="138"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="9" t="s">
         <v>546</v>
       </c>
@@ -8298,7 +8446,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="138"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="9" t="s">
         <v>548</v>
       </c>
@@ -8311,7 +8459,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="138"/>
+      <c r="B19" s="78"/>
       <c r="C19" s="9" t="s">
         <v>550</v>
       </c>
@@ -8324,7 +8472,7 @@
     </row>
     <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="138"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="9" t="s">
         <v>555</v>
       </c>
@@ -8337,7 +8485,7 @@
     </row>
     <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="138"/>
+      <c r="B21" s="78"/>
       <c r="C21" s="9" t="s">
         <v>727</v>
       </c>
@@ -8350,7 +8498,7 @@
     </row>
     <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="138"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="9" t="s">
         <v>570</v>
       </c>
@@ -8363,7 +8511,7 @@
     </row>
     <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="138"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="9" t="s">
         <v>573</v>
       </c>
@@ -8376,7 +8524,7 @@
     </row>
     <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="138"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="9" t="s">
         <v>576</v>
       </c>
@@ -8389,7 +8537,7 @@
     </row>
     <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
-      <c r="B25" s="138"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="9" t="s">
         <v>728</v>
       </c>
@@ -8402,7 +8550,7 @@
     </row>
     <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
-      <c r="B26" s="138"/>
+      <c r="B26" s="78"/>
       <c r="C26" s="9" t="s">
         <v>581</v>
       </c>
@@ -8415,7 +8563,7 @@
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
-      <c r="B27" s="138"/>
+      <c r="B27" s="78"/>
       <c r="C27" s="9" t="s">
         <v>729</v>
       </c>
@@ -8428,7 +8576,7 @@
     </row>
     <row r="28" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
-      <c r="B28" s="138"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="9" t="s">
         <v>595</v>
       </c>
@@ -8441,7 +8589,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
-      <c r="B29" s="138"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="9" t="s">
         <v>598</v>
       </c>
@@ -8454,7 +8602,7 @@
     </row>
     <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="138"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="9" t="s">
         <v>601</v>
       </c>
@@ -8467,7 +8615,7 @@
     </row>
     <row r="31" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="138"/>
+      <c r="B31" s="78"/>
       <c r="C31" s="9" t="s">
         <v>606</v>
       </c>
@@ -8480,7 +8628,7 @@
     </row>
     <row r="32" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="138"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="9" t="s">
         <v>614</v>
       </c>
@@ -8493,7 +8641,7 @@
     </row>
     <row r="33" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="138"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="9" t="s">
         <v>617</v>
       </c>
@@ -8506,7 +8654,7 @@
     </row>
     <row r="34" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
-      <c r="B34" s="138"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="9" t="s">
         <v>732</v>
       </c>
@@ -8519,7 +8667,7 @@
     </row>
     <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
-      <c r="B35" s="138"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="9" t="s">
         <v>622</v>
       </c>
@@ -8532,7 +8680,7 @@
     </row>
     <row r="36" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
-      <c r="B36" s="138"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="9" t="s">
         <v>624</v>
       </c>
@@ -8545,7 +8693,7 @@
     </row>
     <row r="37" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
-      <c r="B37" s="138"/>
+      <c r="B37" s="78"/>
       <c r="C37" s="9" t="s">
         <v>627</v>
       </c>
@@ -8558,7 +8706,7 @@
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
-      <c r="B38" s="138"/>
+      <c r="B38" s="78"/>
       <c r="C38" s="9" t="s">
         <v>630</v>
       </c>
@@ -8571,7 +8719,7 @@
     </row>
     <row r="39" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
-      <c r="B39" s="138"/>
+      <c r="B39" s="78"/>
       <c r="C39" s="9" t="s">
         <v>633</v>
       </c>
@@ -8584,7 +8732,7 @@
     </row>
     <row r="40" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
-      <c r="B40" s="138"/>
+      <c r="B40" s="78"/>
       <c r="C40" s="9" t="s">
         <v>635</v>
       </c>
@@ -8597,7 +8745,7 @@
     </row>
     <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
-      <c r="B41" s="138"/>
+      <c r="B41" s="78"/>
       <c r="C41" s="9" t="s">
         <v>734</v>
       </c>
@@ -8685,7 +8833,7 @@
     </row>
     <row r="49" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
-      <c r="B49" s="139" t="s">
+      <c r="B49" s="79" t="s">
         <v>740</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -8702,7 +8850,7 @@
     </row>
     <row r="50" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
-      <c r="B50" s="139"/>
+      <c r="B50" s="79"/>
       <c r="C50" s="9" t="s">
         <v>744</v>
       </c>
@@ -8717,7 +8865,7 @@
     </row>
     <row r="51" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
-      <c r="B51" s="139"/>
+      <c r="B51" s="79"/>
       <c r="C51" s="9" t="s">
         <v>747</v>
       </c>
@@ -8732,7 +8880,7 @@
     </row>
     <row r="52" spans="1:7" ht="78" x14ac:dyDescent="0.35">
       <c r="A52" s="9"/>
-      <c r="B52" s="139"/>
+      <c r="B52" s="79"/>
       <c r="C52" s="9" t="s">
         <v>750</v>
       </c>
@@ -8747,7 +8895,7 @@
     </row>
     <row r="53" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
-      <c r="B53" s="139"/>
+      <c r="B53" s="79"/>
       <c r="C53" s="9" t="s">
         <v>753</v>
       </c>
@@ -8762,7 +8910,7 @@
     </row>
     <row r="54" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
-      <c r="B54" s="139"/>
+      <c r="B54" s="79"/>
       <c r="C54" s="9" t="s">
         <v>756</v>
       </c>
@@ -8777,7 +8925,7 @@
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
-      <c r="B55" s="139"/>
+      <c r="B55" s="79"/>
       <c r="C55" s="56" t="s">
         <v>123</v>
       </c>
@@ -8826,7 +8974,7 @@
     </row>
     <row r="58" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
-      <c r="B58" s="139" t="s">
+      <c r="B58" s="79" t="s">
         <v>769</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -8843,7 +8991,7 @@
     </row>
     <row r="59" spans="1:7" ht="208" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
-      <c r="B59" s="139"/>
+      <c r="B59" s="79"/>
       <c r="C59" s="9" t="s">
         <v>773</v>
       </c>
@@ -8887,1574 +9035,1264 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" style="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="75" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" style="75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.36328125" style="75" customWidth="1"/>
-    <col min="5" max="5" width="30.90625" style="75" customWidth="1"/>
-    <col min="6" max="6" width="60.08984375" style="75" customWidth="1"/>
-    <col min="7" max="7" width="49.453125" style="75" customWidth="1"/>
-    <col min="8" max="8" width="37" style="75" customWidth="1"/>
-    <col min="9" max="9" width="42" style="75" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="75"/>
+    <col min="1" max="1" width="18" style="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="72" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="72" customWidth="1"/>
+    <col min="4" max="4" width="65.36328125" style="72" customWidth="1"/>
+    <col min="5" max="5" width="30.90625" style="72" customWidth="1"/>
+    <col min="6" max="6" width="60.08984375" style="72" customWidth="1"/>
+    <col min="7" max="7" width="68.6328125" style="72" customWidth="1"/>
+    <col min="8" max="8" width="37" style="72" customWidth="1"/>
+    <col min="9" max="9" width="42" style="72" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="71" t="s">
         <v>519</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="71" t="s">
         <v>859</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="71" t="s">
+      <c r="C1" s="71"/>
+      <c r="D1" s="84" t="s">
         <v>684</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="71" t="s">
         <v>890</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="71" t="s">
+        <v>992</v>
+      </c>
+      <c r="G1" s="71" t="s">
         <v>993</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="H1" s="71" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="182" x14ac:dyDescent="0.35">
+      <c r="A2" s="72" t="s">
+        <v>542</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>965</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>966</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G2" s="72" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="91" x14ac:dyDescent="0.35">
+      <c r="A3" s="71"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="85" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>991</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H3" s="71"/>
+    </row>
+    <row r="4" spans="1:9" ht="130" x14ac:dyDescent="0.35">
+      <c r="B4" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="H1" s="74" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="182" x14ac:dyDescent="0.35">
-      <c r="A2" s="121" t="s">
-        <v>542</v>
-      </c>
-      <c r="B2" s="114" t="s">
-        <v>965</v>
-      </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="85" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E2" s="114" t="s">
-        <v>966</v>
-      </c>
-      <c r="F2" s="114" t="s">
-        <v>1004</v>
-      </c>
-      <c r="G2" s="114" t="s">
-        <v>1005</v>
-      </c>
-      <c r="H2" s="74" t="s">
+      <c r="D4" s="85" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E4" s="71"/>
+      <c r="F4" s="72" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H4" s="71"/>
+    </row>
+    <row r="5" spans="1:9" ht="117" x14ac:dyDescent="0.35">
+      <c r="A5" s="71"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="85" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H5" s="71"/>
+    </row>
+    <row r="6" spans="1:9" ht="52" x14ac:dyDescent="0.35">
+      <c r="A6" s="71"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G6" s="72" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H6" s="71"/>
+    </row>
+    <row r="7" spans="1:9" ht="117" x14ac:dyDescent="0.35">
+      <c r="A7" s="71"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G7" s="72" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H7" s="71"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="71"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+    </row>
+    <row r="9" spans="1:9" ht="65" x14ac:dyDescent="0.35">
+      <c r="A9" s="71"/>
+      <c r="B9" s="72" t="s">
+        <v>876</v>
+      </c>
+      <c r="D9" s="85" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E9" s="83" t="s">
+        <v>892</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H9" s="71" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="93"/>
+      <c r="D10" s="85" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E10" s="94"/>
+      <c r="F10" s="93" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G10" s="93" t="s">
+        <v>1022</v>
+      </c>
+      <c r="H10" s="72" t="s">
+        <v>957</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="83"/>
+      <c r="B11" s="93" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E11" s="94"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="85" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="83"/>
+      <c r="B12" s="93" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E12" s="94"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="85" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A13" s="83"/>
+      <c r="B13" s="93"/>
+      <c r="D13" s="86" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E13" s="94"/>
+      <c r="F13" s="92" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G13" s="83" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A14" s="83"/>
+      <c r="B14" s="93"/>
+      <c r="D14" s="86" t="s">
+        <v>888</v>
+      </c>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="72" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A15" s="83"/>
+      <c r="B15" s="93"/>
+      <c r="D15" s="87" t="s">
+        <v>958</v>
+      </c>
+      <c r="E15" s="94"/>
+      <c r="F15" s="93"/>
+      <c r="H15" s="72" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="143" x14ac:dyDescent="0.35">
+      <c r="A16" s="83"/>
+      <c r="B16" s="93"/>
+      <c r="D16" s="86" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>896</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G16" s="72" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H16" s="72" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="195" x14ac:dyDescent="0.35">
+      <c r="A17" s="72" t="s">
+        <v>968</v>
+      </c>
+      <c r="B17" s="93" t="s">
+        <v>969</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>968</v>
+      </c>
+      <c r="D17" s="86"/>
+      <c r="G17" s="72" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H17" s="72" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="91" x14ac:dyDescent="0.35">
-      <c r="A3" s="74"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="85" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>1001</v>
-      </c>
-      <c r="F3" s="114" t="s">
-        <v>992</v>
-      </c>
-      <c r="G3" s="114" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H3" s="74"/>
-    </row>
-    <row r="4" spans="1:9" ht="130" x14ac:dyDescent="0.35">
-      <c r="B4" s="121" t="s">
-        <v>995</v>
-      </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="85" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="114" t="s">
-        <v>1011</v>
-      </c>
-      <c r="G4" s="114" t="s">
-        <v>1012</v>
-      </c>
-      <c r="H4" s="74"/>
-    </row>
-    <row r="5" spans="1:9" ht="117" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="85" t="s">
-        <v>1010</v>
-      </c>
-      <c r="E5" s="106"/>
-      <c r="F5" s="114" t="s">
-        <v>1007</v>
-      </c>
-      <c r="G5" s="114" t="s">
-        <v>1008</v>
-      </c>
-      <c r="H5" s="74"/>
-    </row>
-    <row r="6" spans="1:9" ht="52" x14ac:dyDescent="0.35">
-      <c r="A6" s="74"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="121" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E6" s="106"/>
-      <c r="F6" s="114" t="s">
-        <v>1014</v>
-      </c>
-      <c r="G6" s="114" t="s">
-        <v>1015</v>
-      </c>
-      <c r="H6" s="74"/>
-    </row>
-    <row r="7" spans="1:9" ht="117" x14ac:dyDescent="0.35">
-      <c r="A7" s="74"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="121" t="s">
-        <v>1016</v>
-      </c>
-      <c r="E7" s="106"/>
-      <c r="F7" s="114" t="s">
-        <v>1017</v>
-      </c>
-      <c r="G7" s="114" t="s">
-        <v>1018</v>
-      </c>
-      <c r="H7" s="74"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="74"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="74"/>
-    </row>
-    <row r="9" spans="1:9" ht="65" x14ac:dyDescent="0.35">
-      <c r="A9" s="74"/>
-      <c r="B9" s="126" t="s">
-        <v>876</v>
-      </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77" t="s">
-        <v>1019</v>
-      </c>
-      <c r="E9" s="148" t="s">
-        <v>892</v>
-      </c>
-      <c r="F9" s="115" t="s">
-        <v>1020</v>
-      </c>
-      <c r="G9" s="115"/>
-      <c r="H9" s="74" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="152" t="s">
+    <row r="18" spans="1:9" ht="104" x14ac:dyDescent="0.35">
+      <c r="D18" s="86"/>
+      <c r="F18" s="72" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G18" s="72" t="s">
+        <v>1036</v>
+      </c>
+      <c r="H18" s="72" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="104" x14ac:dyDescent="0.35">
+      <c r="D19" s="86"/>
+      <c r="F19" s="72" t="s">
+        <v>1038</v>
+      </c>
+      <c r="G19" s="72" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="83" t="s">
+        <v>877</v>
+      </c>
+      <c r="D20" s="86" t="s">
+        <v>707</v>
+      </c>
+      <c r="E20" s="83" t="s">
+        <v>891</v>
+      </c>
+      <c r="H20" s="83" t="s">
+        <v>957</v>
+      </c>
+      <c r="I20" s="83" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="D21" s="86" t="s">
+        <v>889</v>
+      </c>
+      <c r="E21" s="83"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
+    </row>
+    <row r="22" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
+      <c r="D22" s="86" t="s">
+        <v>862</v>
+      </c>
+      <c r="E22" s="83"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="94"/>
+    </row>
+    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A23" s="83"/>
+      <c r="B23" s="83"/>
+      <c r="D23" s="86" t="s">
+        <v>863</v>
+      </c>
+      <c r="E23" s="83"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="94"/>
+    </row>
+    <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
+      <c r="D24" s="85" t="s">
+        <v>867</v>
+      </c>
+      <c r="E24" s="83"/>
+      <c r="H24" s="72" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="39" x14ac:dyDescent="0.35">
+      <c r="A25" s="83"/>
+      <c r="B25" s="83"/>
+      <c r="D25" s="85" t="s">
+        <v>893</v>
+      </c>
+      <c r="E25" s="83" t="s">
+        <v>897</v>
+      </c>
+      <c r="H25" s="72" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="52" x14ac:dyDescent="0.35">
+      <c r="A26" s="83"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="72" t="s">
+        <v>971</v>
+      </c>
+      <c r="D26" s="86" t="s">
+        <v>970</v>
+      </c>
+      <c r="E26" s="83"/>
+    </row>
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A27" s="83"/>
+      <c r="B27" s="83"/>
+      <c r="D27" s="85" t="s">
+        <v>894</v>
+      </c>
+      <c r="E27" s="83"/>
+      <c r="H27" s="72" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A28" s="83"/>
+      <c r="B28" s="83"/>
+      <c r="D28" s="85" t="s">
+        <v>895</v>
+      </c>
+      <c r="E28" s="83"/>
+      <c r="H28" s="72" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D29" s="86"/>
+    </row>
+    <row r="30" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A30" s="83" t="s">
+        <v>537</v>
+      </c>
+      <c r="B30" s="83" t="s">
+        <v>878</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>884</v>
+      </c>
+      <c r="E30" s="83" t="s">
+        <v>899</v>
+      </c>
+      <c r="H30" s="72" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="65" x14ac:dyDescent="0.35">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83"/>
+      <c r="D31" s="85" t="s">
+        <v>864</v>
+      </c>
+      <c r="E31" s="83"/>
+      <c r="H31" s="72" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="117" x14ac:dyDescent="0.35">
+      <c r="A32" s="72" t="s">
+        <v>963</v>
+      </c>
+      <c r="B32" s="72" t="s">
+        <v>964</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>962</v>
+      </c>
+      <c r="E32" s="72" t="s">
+        <v>972</v>
+      </c>
+      <c r="H32" s="72" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D33" s="85"/>
+    </row>
+    <row r="34" spans="1:8" ht="91" x14ac:dyDescent="0.35">
+      <c r="A34" s="88" t="s">
+        <v>870</v>
+      </c>
+      <c r="B34" s="88" t="s">
+        <v>868</v>
+      </c>
+      <c r="C34" s="88"/>
+      <c r="D34" s="89" t="s">
+        <v>885</v>
+      </c>
+      <c r="E34" s="72" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D35" s="85"/>
+    </row>
+    <row r="36" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A36" s="83" t="s">
+        <v>861</v>
+      </c>
+      <c r="B36" s="83" t="s">
+        <v>879</v>
+      </c>
+      <c r="D36" s="85" t="s">
+        <v>871</v>
+      </c>
+      <c r="E36" s="83" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A37" s="83"/>
+      <c r="B37" s="83"/>
+      <c r="D37" s="85" t="s">
+        <v>872</v>
+      </c>
+      <c r="E37" s="83"/>
+    </row>
+    <row r="38" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="D38" s="85" t="s">
+        <v>536</v>
+      </c>
+      <c r="E38" s="72" t="s">
+        <v>901</v>
+      </c>
+      <c r="H38" s="85" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="78" x14ac:dyDescent="0.35">
+      <c r="A39" s="83"/>
+      <c r="B39" s="83"/>
+      <c r="D39" s="87" t="s">
+        <v>887</v>
+      </c>
+      <c r="E39" s="72" t="s">
+        <v>902</v>
+      </c>
+      <c r="H39" s="90" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A40" s="83"/>
+      <c r="B40" s="83"/>
+      <c r="D40" s="85" t="s">
+        <v>548</v>
+      </c>
+      <c r="E40" s="72" t="s">
+        <v>903</v>
+      </c>
+      <c r="H40" s="72" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A41" s="83"/>
+      <c r="B41" s="83"/>
+      <c r="D41" s="85" t="s">
+        <v>873</v>
+      </c>
+      <c r="E41" s="72" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A42" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="124"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E10" s="144"/>
-      <c r="F10" s="112" t="s">
-        <v>1022</v>
-      </c>
-      <c r="G10" s="112" t="s">
-        <v>1023</v>
-      </c>
-      <c r="H10" s="78" t="s">
-        <v>957</v>
-      </c>
-      <c r="I10" s="75" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="152"/>
-      <c r="B11" s="124" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C11" s="127"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="77" t="s">
-        <v>1024</v>
-      </c>
-      <c r="H11" s="128"/>
-    </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="152"/>
-      <c r="B12" s="124" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C12" s="127"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="77" t="s">
-        <v>1025</v>
-      </c>
-      <c r="H12" s="128"/>
-    </row>
-    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A13" s="152"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="79" t="s">
-        <v>1028</v>
-      </c>
-      <c r="E13" s="144"/>
-      <c r="F13" s="155" t="s">
-        <v>1029</v>
-      </c>
-      <c r="G13" s="143" t="s">
-        <v>1030</v>
-      </c>
-      <c r="H13" s="78" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A14" s="152"/>
-      <c r="B14" s="124"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="79" t="s">
-        <v>888</v>
-      </c>
-      <c r="E14" s="144"/>
-      <c r="F14" s="144"/>
-      <c r="G14" s="144"/>
-      <c r="H14" s="78" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.35">
-      <c r="A15" s="152"/>
-      <c r="B15" s="124"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="86" t="s">
-        <v>958</v>
-      </c>
-      <c r="E15" s="145"/>
-      <c r="F15" s="113"/>
-      <c r="H15" s="78" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="169" x14ac:dyDescent="0.35">
-      <c r="A16" s="152"/>
-      <c r="B16" s="125"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="79" t="s">
-        <v>1032</v>
-      </c>
-      <c r="E16" s="76" t="s">
-        <v>896</v>
-      </c>
-      <c r="F16" s="122" t="s">
-        <v>1033</v>
-      </c>
-      <c r="G16" s="122"/>
-      <c r="H16" s="78" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="109" t="s">
-        <v>968</v>
-      </c>
-      <c r="B17" s="107" t="s">
-        <v>970</v>
-      </c>
-      <c r="C17" s="108"/>
-      <c r="D17" s="79" t="s">
-        <v>969</v>
-      </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="122"/>
-      <c r="H17" s="109" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="78"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="122"/>
-      <c r="H18" s="78"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="152" t="s">
+      <c r="D42" s="85" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A43" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" s="85" t="s">
+        <v>898</v>
+      </c>
+      <c r="E43" s="85" t="s">
+        <v>905</v>
+      </c>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="91" t="s">
+        <v>883</v>
+      </c>
+      <c r="B44" s="91"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="91"/>
+      <c r="E44" s="91"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+    </row>
+    <row r="45" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A45" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="83" t="s">
+        <v>916</v>
+      </c>
+      <c r="D45" s="72" t="s">
+        <v>907</v>
+      </c>
+      <c r="E45" s="72" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A46" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="83"/>
+      <c r="D46" s="72" t="s">
+        <v>909</v>
+      </c>
+      <c r="E46" s="72" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A47" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="151" t="s">
-        <v>877</v>
-      </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="79" t="s">
-        <v>707</v>
-      </c>
-      <c r="E19" s="148" t="s">
-        <v>891</v>
-      </c>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
-      <c r="H19" s="143" t="s">
-        <v>957</v>
-      </c>
-      <c r="I19" s="146" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="152"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="79" t="s">
-        <v>889</v>
-      </c>
-      <c r="E20" s="149"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="147"/>
-    </row>
-    <row r="21" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A21" s="152"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="79" t="s">
-        <v>862</v>
-      </c>
-      <c r="E21" s="149"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="147"/>
-    </row>
-    <row r="22" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="152"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="79" t="s">
-        <v>863</v>
-      </c>
-      <c r="E22" s="149"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="145"/>
-      <c r="I22" s="147"/>
-    </row>
-    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A23" s="152"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="77" t="s">
-        <v>867</v>
-      </c>
-      <c r="E23" s="150"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="78" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="39" x14ac:dyDescent="0.35">
-      <c r="A24" s="152"/>
-      <c r="B24" s="151"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="77" t="s">
-        <v>893</v>
-      </c>
-      <c r="E24" s="151" t="s">
-        <v>897</v>
-      </c>
-      <c r="F24" s="122"/>
-      <c r="G24" s="122"/>
-      <c r="H24" s="78" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="52" x14ac:dyDescent="0.35">
-      <c r="A25" s="152"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="111" t="s">
-        <v>972</v>
-      </c>
-      <c r="D25" s="79" t="s">
-        <v>971</v>
-      </c>
-      <c r="E25" s="151"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="122"/>
-      <c r="H25" s="110"/>
-    </row>
-    <row r="26" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A26" s="152"/>
-      <c r="B26" s="151"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77" t="s">
-        <v>894</v>
-      </c>
-      <c r="E26" s="151"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="78" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A27" s="152"/>
-      <c r="B27" s="151"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="77" t="s">
-        <v>895</v>
-      </c>
-      <c r="E27" s="151"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="78" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="78"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="78"/>
-    </row>
-    <row r="29" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A29" s="152" t="s">
-        <v>537</v>
-      </c>
-      <c r="B29" s="151" t="s">
-        <v>878</v>
-      </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="79" t="s">
-        <v>884</v>
-      </c>
-      <c r="E29" s="148" t="s">
-        <v>899</v>
-      </c>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="78" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="65" x14ac:dyDescent="0.35">
-      <c r="A30" s="152"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="77" t="s">
-        <v>864</v>
-      </c>
-      <c r="E30" s="150"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="78" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="117" x14ac:dyDescent="0.35">
-      <c r="A31" s="104" t="s">
-        <v>963</v>
-      </c>
-      <c r="B31" s="105" t="s">
-        <v>964</v>
-      </c>
-      <c r="C31" s="105"/>
-      <c r="D31" s="86" t="s">
-        <v>962</v>
-      </c>
-      <c r="E31" s="103" t="s">
-        <v>973</v>
-      </c>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="104" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="78"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="122"/>
-      <c r="G32" s="122"/>
-      <c r="H32" s="78"/>
-    </row>
-    <row r="33" spans="1:8" ht="91" x14ac:dyDescent="0.35">
-      <c r="A33" s="80" t="s">
-        <v>870</v>
-      </c>
-      <c r="B33" s="81" t="s">
-        <v>868</v>
-      </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82" t="s">
-        <v>885</v>
-      </c>
-      <c r="E33" s="83" t="s">
-        <v>869</v>
-      </c>
-      <c r="F33" s="115"/>
-      <c r="G33" s="115"/>
-      <c r="H33" s="78"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="78"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="122"/>
-      <c r="G34" s="122"/>
-      <c r="H34" s="78"/>
-    </row>
-    <row r="35" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A35" s="152" t="s">
+      <c r="B47" s="83"/>
+      <c r="D47" s="72" t="s">
+        <v>910</v>
+      </c>
+      <c r="E47" s="72" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A48" s="72" t="s">
         <v>861</v>
       </c>
-      <c r="B35" s="151" t="s">
-        <v>879</v>
-      </c>
-      <c r="C35" s="76"/>
-      <c r="D35" s="77" t="s">
-        <v>871</v>
-      </c>
-      <c r="E35" s="148" t="s">
-        <v>900</v>
-      </c>
-      <c r="F35" s="115"/>
-      <c r="G35" s="115"/>
-      <c r="H35" s="78"/>
-    </row>
-    <row r="36" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A36" s="152"/>
-      <c r="B36" s="151"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="77" t="s">
-        <v>872</v>
-      </c>
-      <c r="E36" s="150"/>
-      <c r="F36" s="116"/>
-      <c r="G36" s="116"/>
-      <c r="H36" s="78"/>
-    </row>
-    <row r="37" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A37" s="152"/>
-      <c r="B37" s="151"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="77" t="s">
-        <v>536</v>
-      </c>
-      <c r="E37" s="84" t="s">
-        <v>901</v>
-      </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="85" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="78" x14ac:dyDescent="0.35">
-      <c r="A38" s="152"/>
-      <c r="B38" s="151"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="86" t="s">
-        <v>887</v>
-      </c>
-      <c r="E38" s="76" t="s">
-        <v>902</v>
-      </c>
-      <c r="F38" s="122"/>
-      <c r="G38" s="122"/>
-      <c r="H38" s="87" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A39" s="152"/>
-      <c r="B39" s="151"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="77" t="s">
-        <v>548</v>
-      </c>
-      <c r="E39" s="84" t="s">
-        <v>903</v>
-      </c>
-      <c r="F39" s="84"/>
-      <c r="G39" s="84"/>
-      <c r="H39" s="78" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A40" s="152"/>
-      <c r="B40" s="151"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="77" t="s">
-        <v>873</v>
-      </c>
-      <c r="E40" s="76" t="s">
-        <v>904</v>
-      </c>
-      <c r="F40" s="122"/>
-      <c r="G40" s="122"/>
-      <c r="H40" s="78"/>
-    </row>
-    <row r="41" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A41" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="77" t="s">
-        <v>908</v>
-      </c>
-      <c r="E41" s="76"/>
-      <c r="F41" s="122"/>
-      <c r="G41" s="122"/>
-      <c r="H41" s="78"/>
-    </row>
-    <row r="42" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A42" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="77" t="s">
-        <v>898</v>
-      </c>
-      <c r="E42" s="77" t="s">
-        <v>905</v>
-      </c>
-      <c r="F42" s="77"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="78"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="158" t="s">
-        <v>883</v>
-      </c>
-      <c r="B43" s="159"/>
-      <c r="C43" s="159"/>
-      <c r="D43" s="159"/>
-      <c r="E43" s="159"/>
-      <c r="F43" s="159"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="160"/>
-    </row>
-    <row r="44" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A44" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="B44" s="161" t="s">
-        <v>916</v>
-      </c>
-      <c r="C44" s="88"/>
-      <c r="D44" s="88" t="s">
-        <v>907</v>
-      </c>
-      <c r="E44" s="88" t="s">
-        <v>912</v>
-      </c>
-      <c r="F44" s="117"/>
-      <c r="G44" s="117"/>
-      <c r="H44" s="89"/>
-    </row>
-    <row r="45" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A45" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="B45" s="161"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="88" t="s">
-        <v>909</v>
-      </c>
-      <c r="E45" s="88" t="s">
-        <v>913</v>
-      </c>
-      <c r="F45" s="117"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="89"/>
-    </row>
-    <row r="46" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A46" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="161"/>
-      <c r="C46" s="88"/>
-      <c r="D46" s="88" t="s">
-        <v>910</v>
-      </c>
-      <c r="E46" s="88" t="s">
-        <v>914</v>
-      </c>
-      <c r="F46" s="117"/>
-      <c r="G46" s="117"/>
-      <c r="H46" s="89"/>
-    </row>
-    <row r="47" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A47" s="78" t="s">
-        <v>861</v>
-      </c>
-      <c r="B47" s="161"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="88" t="s">
+      <c r="B48" s="83"/>
+      <c r="D48" s="72" t="s">
         <v>911</v>
       </c>
-      <c r="E47" s="88" t="s">
+      <c r="E48" s="72" t="s">
         <v>915</v>
       </c>
-      <c r="F47" s="117"/>
-      <c r="G47" s="117"/>
-      <c r="H47" s="89"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="162" t="s">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="91" t="s">
         <v>917</v>
       </c>
-      <c r="B48" s="162"/>
-      <c r="C48" s="162"/>
-      <c r="D48" s="162"/>
-      <c r="E48" s="162"/>
-      <c r="F48" s="162"/>
-      <c r="G48" s="162"/>
-      <c r="H48" s="162"/>
-    </row>
-    <row r="49" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="90"/>
-      <c r="B49" s="90"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="91"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
       <c r="F49" s="91"/>
       <c r="G49" s="91"/>
       <c r="H49" s="91"/>
     </row>
-    <row r="50" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A50" s="89" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="71"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="71"/>
+    </row>
+    <row r="51" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A51" s="72" t="s">
         <v>952</v>
       </c>
-      <c r="B50" s="153" t="s">
+      <c r="B51" s="83" t="s">
         <v>953</v>
       </c>
-      <c r="C50" s="90"/>
-      <c r="D50" s="72" t="s">
+      <c r="C51" s="71"/>
+      <c r="D51" s="72" t="s">
         <v>951</v>
       </c>
-      <c r="E50" s="156" t="s">
+      <c r="E51" s="83" t="s">
         <v>954</v>
       </c>
-      <c r="F50" s="129"/>
-      <c r="G50" s="129"/>
-      <c r="H50" s="91"/>
-    </row>
-    <row r="51" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A51" s="89" t="s">
+      <c r="H51" s="71"/>
+    </row>
+    <row r="52" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A52" s="72" t="s">
         <v>421</v>
       </c>
-      <c r="B51" s="155"/>
-      <c r="C51" s="90"/>
-      <c r="D51" s="72" t="s">
+      <c r="B52" s="92"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72" t="s">
         <v>950</v>
       </c>
-      <c r="E51" s="157"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="91"/>
-    </row>
-    <row r="52" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="94"/>
-      <c r="B52" s="102"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="102"/>
-      <c r="F52" s="91"/>
-      <c r="G52" s="91"/>
-      <c r="H52" s="91"/>
-    </row>
-    <row r="53" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="153" t="s">
+      <c r="E52" s="92"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="95"/>
+      <c r="H52" s="71"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="71"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="164" t="s">
+      <c r="B54" s="83" t="s">
         <v>926</v>
       </c>
-      <c r="C53" s="93"/>
-      <c r="D53" s="73" t="s">
+      <c r="C54" s="71"/>
+      <c r="D54" s="72" t="s">
         <v>918</v>
       </c>
-      <c r="E53" s="164" t="s">
+      <c r="E54" s="83" t="s">
         <v>927</v>
       </c>
-      <c r="F53" s="118"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="94"/>
-    </row>
-    <row r="54" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A54" s="154"/>
-      <c r="B54" s="165"/>
-      <c r="C54" s="93"/>
-      <c r="D54" s="95" t="s">
+      <c r="H54" s="71"/>
+    </row>
+    <row r="55" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A55" s="83"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="85" t="s">
         <v>919</v>
       </c>
-      <c r="E54" s="165"/>
-      <c r="F54" s="119"/>
-      <c r="G54" s="119"/>
-      <c r="H54" s="94" t="s">
+      <c r="E55" s="83"/>
+      <c r="H55" s="71" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="154"/>
-      <c r="B55" s="165"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="95" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="83"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="85" t="s">
         <v>744</v>
       </c>
-      <c r="E55" s="165"/>
-      <c r="F55" s="119"/>
-      <c r="G55" s="119"/>
-      <c r="H55" s="94" t="s">
+      <c r="E56" s="83"/>
+      <c r="H56" s="71" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A56" s="154"/>
-      <c r="B56" s="165"/>
-      <c r="C56" s="93"/>
-      <c r="D56" s="95" t="s">
+    <row r="57" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A57" s="83"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="85" t="s">
         <v>920</v>
       </c>
-      <c r="E56" s="165"/>
-      <c r="F56" s="119"/>
-      <c r="G56" s="119"/>
-      <c r="H56" s="94"/>
-    </row>
-    <row r="57" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="154"/>
-      <c r="B57" s="165"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="96" t="s">
+      <c r="E57" s="83"/>
+      <c r="H57" s="71"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="83"/>
+      <c r="B58" s="83"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="72" t="s">
         <v>750</v>
       </c>
-      <c r="E57" s="165"/>
-      <c r="F57" s="119"/>
-      <c r="G57" s="119"/>
-      <c r="H57" s="94"/>
-    </row>
-    <row r="58" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A58" s="154"/>
-      <c r="B58" s="165"/>
-      <c r="C58" s="130" t="s">
-        <v>972</v>
-      </c>
-      <c r="D58" s="132"/>
-      <c r="E58" s="167"/>
-      <c r="F58" s="119"/>
-      <c r="G58" s="119"/>
-      <c r="H58" s="94"/>
-    </row>
-    <row r="59" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A59" s="154"/>
-      <c r="B59" s="165"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="131" t="s">
+      <c r="E58" s="83"/>
+      <c r="H58" s="71"/>
+    </row>
+    <row r="59" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A59" s="83"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="71" t="s">
+        <v>971</v>
+      </c>
+      <c r="E59" s="83"/>
+      <c r="H59" s="71"/>
+    </row>
+    <row r="60" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A60" s="83"/>
+      <c r="B60" s="83"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="85" t="s">
         <v>921</v>
       </c>
-      <c r="E59" s="165"/>
-      <c r="F59" s="119"/>
-      <c r="G59" s="119"/>
-      <c r="H59" s="94"/>
-    </row>
-    <row r="60" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A60" s="154"/>
-      <c r="B60" s="165"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="95" t="s">
+      <c r="E60" s="83"/>
+      <c r="H60" s="71"/>
+    </row>
+    <row r="61" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A61" s="83"/>
+      <c r="B61" s="83"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="85" t="s">
         <v>922</v>
       </c>
-      <c r="E60" s="165"/>
-      <c r="F60" s="119"/>
-      <c r="G60" s="119"/>
-      <c r="H60" s="94"/>
-    </row>
-    <row r="61" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A61" s="154"/>
-      <c r="B61" s="165"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="95" t="s">
+      <c r="E61" s="83"/>
+      <c r="H61" s="71"/>
+    </row>
+    <row r="62" spans="1:8" ht="52" x14ac:dyDescent="0.35">
+      <c r="A62" s="83"/>
+      <c r="B62" s="83"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="85" t="s">
         <v>923</v>
       </c>
-      <c r="E61" s="165"/>
-      <c r="F61" s="119"/>
-      <c r="G61" s="119"/>
-      <c r="H61" s="94"/>
-    </row>
-    <row r="62" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A62" s="154"/>
-      <c r="B62" s="165"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="95" t="s">
+      <c r="E62" s="83"/>
+      <c r="H62" s="71"/>
+    </row>
+    <row r="63" spans="1:8" ht="52" x14ac:dyDescent="0.35">
+      <c r="A63" s="83"/>
+      <c r="B63" s="83"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="85" t="s">
         <v>924</v>
       </c>
-      <c r="E62" s="165"/>
-      <c r="F62" s="119"/>
-      <c r="G62" s="119"/>
-      <c r="H62" s="94"/>
-    </row>
-    <row r="63" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="154"/>
-      <c r="B63" s="165"/>
-      <c r="C63" s="93"/>
-      <c r="D63" s="95" t="s">
+      <c r="E63" s="83"/>
+      <c r="H63" s="71"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="83"/>
+      <c r="B64" s="83"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="85" t="s">
         <v>753</v>
       </c>
-      <c r="E63" s="165"/>
-      <c r="F63" s="119"/>
-      <c r="G63" s="119"/>
-      <c r="H63" s="94"/>
-    </row>
-    <row r="64" spans="1:8" s="92" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="163"/>
-      <c r="B64" s="166"/>
-      <c r="C64" s="93"/>
-      <c r="D64" s="95" t="s">
+      <c r="E64" s="83"/>
+      <c r="H64" s="71"/>
+    </row>
+    <row r="65" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="83"/>
+      <c r="B65" s="83"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="85" t="s">
         <v>925</v>
       </c>
-      <c r="E64" s="166"/>
-      <c r="F64" s="120"/>
-      <c r="G64" s="120"/>
-      <c r="H64" s="94"/>
-    </row>
-    <row r="65" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="72"/>
-      <c r="B65" s="90"/>
-      <c r="C65" s="90"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="90"/>
-      <c r="F65" s="90"/>
-      <c r="G65" s="90"/>
-      <c r="H65" s="94"/>
-    </row>
-    <row r="66" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A66" s="72" t="s">
+      <c r="E65" s="83"/>
+      <c r="H65" s="71"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="71"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="71"/>
+      <c r="G66" s="71"/>
+      <c r="H66" s="71"/>
+    </row>
+    <row r="67" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A67" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="153" t="s">
+      <c r="B67" s="83" t="s">
         <v>946</v>
       </c>
-      <c r="C66" s="90"/>
-      <c r="D66" s="72" t="s">
-        <v>997</v>
-      </c>
-      <c r="E66" s="90"/>
-      <c r="F66" s="90"/>
-      <c r="G66" s="90"/>
-      <c r="H66" s="94"/>
-    </row>
-    <row r="67" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A67" s="72" t="s">
-        <v>930</v>
-      </c>
-      <c r="B67" s="154"/>
-      <c r="C67" s="90"/>
-      <c r="D67" s="85" t="s">
-        <v>934</v>
-      </c>
-      <c r="E67" s="90" t="s">
-        <v>931</v>
-      </c>
-      <c r="F67" s="90"/>
-      <c r="G67" s="90"/>
-      <c r="H67" s="94"/>
-    </row>
-    <row r="68" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="C67" s="71"/>
+      <c r="D67" s="72" t="s">
+        <v>996</v>
+      </c>
+      <c r="E67" s="71"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
+    </row>
+    <row r="68" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A68" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B68" s="154"/>
-      <c r="C68" s="90"/>
+      <c r="B68" s="83"/>
+      <c r="C68" s="71"/>
       <c r="D68" s="85" t="s">
+        <v>934</v>
+      </c>
+      <c r="E68" s="71" t="s">
+        <v>931</v>
+      </c>
+      <c r="F68" s="71"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="71"/>
+    </row>
+    <row r="69" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A69" s="72" t="s">
+        <v>930</v>
+      </c>
+      <c r="B69" s="83"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="85" t="s">
         <v>581</v>
       </c>
-      <c r="E68" s="90"/>
-      <c r="F68" s="90"/>
-      <c r="G68" s="90"/>
-      <c r="H68" s="94"/>
-    </row>
-    <row r="69" spans="1:8" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A69" s="72" t="s">
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
+      <c r="G69" s="71"/>
+      <c r="H69" s="71"/>
+    </row>
+    <row r="70" spans="1:8" ht="65" x14ac:dyDescent="0.35">
+      <c r="A70" s="72" t="s">
+        <v>997</v>
+      </c>
+      <c r="B70" s="83"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="85" t="s">
         <v>998</v>
       </c>
-      <c r="B69" s="154"/>
-      <c r="C69" s="90"/>
-      <c r="D69" s="85" t="s">
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
+    </row>
+    <row r="71" spans="1:8" ht="312" x14ac:dyDescent="0.35">
+      <c r="A71" s="72" t="s">
+        <v>997</v>
+      </c>
+      <c r="B71" s="83"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="85" t="s">
         <v>999</v>
       </c>
-      <c r="E69" s="90"/>
-      <c r="F69" s="90"/>
-      <c r="G69" s="90"/>
-      <c r="H69" s="94"/>
-    </row>
-    <row r="70" spans="1:8" s="92" customFormat="1" ht="312" x14ac:dyDescent="0.35">
-      <c r="A70" s="72" t="s">
-        <v>998</v>
-      </c>
-      <c r="B70" s="154"/>
-      <c r="C70" s="90"/>
-      <c r="D70" s="85" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E70" s="90"/>
-      <c r="F70" s="90"/>
-      <c r="G70" s="90"/>
-      <c r="H70" s="94"/>
-    </row>
-    <row r="71" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A71" s="72" t="s">
+      <c r="E71" s="71"/>
+      <c r="F71" s="71"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="71"/>
+    </row>
+    <row r="72" spans="1:8" ht="52" x14ac:dyDescent="0.35">
+      <c r="A72" s="72" t="s">
         <v>933</v>
       </c>
-      <c r="B71" s="154"/>
-      <c r="C71" s="90"/>
-      <c r="D71" s="85" t="s">
+      <c r="B72" s="83"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="85" t="s">
         <v>932</v>
       </c>
-      <c r="E71" s="90"/>
-      <c r="F71" s="90"/>
-      <c r="G71" s="90"/>
-      <c r="H71" s="94"/>
-    </row>
-    <row r="72" spans="1:8" s="92" customFormat="1" ht="91" x14ac:dyDescent="0.35">
-      <c r="A72" s="72" t="s">
-        <v>930</v>
-      </c>
-      <c r="B72" s="154"/>
-      <c r="C72" s="90"/>
-      <c r="D72" s="85" t="s">
-        <v>935</v>
-      </c>
-      <c r="E72" s="90" t="s">
-        <v>931</v>
-      </c>
-      <c r="F72" s="90"/>
-      <c r="G72" s="90"/>
-      <c r="H72" s="94"/>
-    </row>
-    <row r="73" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E72" s="71"/>
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+    </row>
+    <row r="73" spans="1:8" ht="91" x14ac:dyDescent="0.35">
       <c r="A73" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B73" s="154"/>
-      <c r="C73" s="90"/>
+      <c r="B73" s="83"/>
+      <c r="C73" s="71"/>
       <c r="D73" s="85" t="s">
-        <v>598</v>
-      </c>
-      <c r="E73" s="90" t="s">
+        <v>935</v>
+      </c>
+      <c r="E73" s="71" t="s">
         <v>931</v>
       </c>
-      <c r="F73" s="90"/>
-      <c r="G73" s="90"/>
-      <c r="H73" s="94"/>
-    </row>
-    <row r="74" spans="1:8" s="92" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="F73" s="71"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B74" s="154"/>
-      <c r="C74" s="90"/>
+      <c r="B74" s="83"/>
+      <c r="C74" s="71"/>
       <c r="D74" s="85" t="s">
+        <v>598</v>
+      </c>
+      <c r="E74" s="71" t="s">
+        <v>931</v>
+      </c>
+      <c r="F74" s="71"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="71"/>
+    </row>
+    <row r="75" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A75" s="72" t="s">
+        <v>930</v>
+      </c>
+      <c r="B75" s="83"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="85" t="s">
         <v>936</v>
       </c>
-      <c r="E74" s="90"/>
-      <c r="F74" s="90"/>
-      <c r="G74" s="90"/>
-      <c r="H74" s="94"/>
-    </row>
-    <row r="75" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A75" s="72" t="s">
-        <v>937</v>
-      </c>
-      <c r="B75" s="144"/>
-      <c r="C75" s="90"/>
-      <c r="D75" s="99" t="s">
-        <v>938</v>
-      </c>
-      <c r="E75" s="90"/>
-      <c r="F75" s="90"/>
-      <c r="G75" s="90"/>
-      <c r="H75" s="94"/>
-    </row>
-    <row r="76" spans="1:8" s="92" customFormat="1" ht="91" x14ac:dyDescent="0.35">
+      <c r="E75" s="71"/>
+      <c r="F75" s="71"/>
+      <c r="G75" s="71"/>
+      <c r="H75" s="71"/>
+    </row>
+    <row r="76" spans="1:8" ht="39" x14ac:dyDescent="0.35">
       <c r="A76" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B76" s="145"/>
-      <c r="C76" s="90"/>
-      <c r="D76" s="99" t="s">
+      <c r="B76" s="94"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="85" t="s">
+        <v>938</v>
+      </c>
+      <c r="E76" s="71"/>
+      <c r="F76" s="71"/>
+      <c r="G76" s="71"/>
+      <c r="H76" s="71"/>
+    </row>
+    <row r="77" spans="1:8" ht="91" x14ac:dyDescent="0.35">
+      <c r="A77" s="72" t="s">
+        <v>937</v>
+      </c>
+      <c r="B77" s="94"/>
+      <c r="C77" s="71"/>
+      <c r="D77" s="85" t="s">
         <v>939</v>
       </c>
-      <c r="E76" s="90"/>
-      <c r="F76" s="90"/>
-      <c r="G76" s="90"/>
-      <c r="H76" s="94"/>
-    </row>
-    <row r="77" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="72"/>
-      <c r="B77" s="98"/>
-      <c r="C77" s="90"/>
-      <c r="D77" s="99"/>
-      <c r="E77" s="90"/>
-      <c r="F77" s="90"/>
-      <c r="G77" s="90"/>
-      <c r="H77" s="94"/>
-    </row>
-    <row r="78" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A78" s="72" t="s">
+      <c r="E77" s="71"/>
+      <c r="F77" s="71"/>
+      <c r="G77" s="71"/>
+      <c r="H77" s="71"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C78" s="71"/>
+      <c r="D78" s="85"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="71"/>
+      <c r="H78" s="71"/>
+    </row>
+    <row r="79" spans="1:8" ht="52" x14ac:dyDescent="0.35">
+      <c r="A79" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B78" s="143" t="s">
+      <c r="B79" s="83" t="s">
         <v>949</v>
       </c>
-      <c r="C78" s="90"/>
-      <c r="D78" s="99" t="s">
+      <c r="C79" s="71"/>
+      <c r="D79" s="85" t="s">
         <v>940</v>
       </c>
-      <c r="E78" s="90"/>
-      <c r="F78" s="90"/>
-      <c r="G78" s="90"/>
-      <c r="H78" s="94"/>
-    </row>
-    <row r="79" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A79" s="72" t="s">
-        <v>947</v>
-      </c>
-      <c r="B79" s="144"/>
-      <c r="C79" s="90"/>
-      <c r="D79" s="99" t="s">
-        <v>941</v>
-      </c>
-      <c r="E79" s="90"/>
-      <c r="F79" s="90"/>
-      <c r="G79" s="90"/>
-      <c r="H79" s="94"/>
-    </row>
-    <row r="80" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="E79" s="71"/>
+      <c r="F79" s="71"/>
+      <c r="G79" s="71"/>
+      <c r="H79" s="71"/>
+    </row>
+    <row r="80" spans="1:8" ht="39" x14ac:dyDescent="0.35">
       <c r="A80" s="72" t="s">
         <v>947</v>
       </c>
-      <c r="B80" s="144"/>
-      <c r="C80" s="90"/>
-      <c r="D80" s="99" t="s">
+      <c r="B80" s="94"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="85" t="s">
+        <v>941</v>
+      </c>
+      <c r="E80" s="71"/>
+      <c r="F80" s="71"/>
+      <c r="G80" s="71"/>
+      <c r="H80" s="71"/>
+    </row>
+    <row r="81" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A81" s="72" t="s">
+        <v>947</v>
+      </c>
+      <c r="B81" s="94"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="85" t="s">
         <v>942</v>
       </c>
-      <c r="E80" s="90"/>
-      <c r="F80" s="90"/>
-      <c r="G80" s="90"/>
-      <c r="H80" s="94"/>
-    </row>
-    <row r="81" spans="1:8" s="92" customFormat="1" ht="52" x14ac:dyDescent="0.35">
-      <c r="A81" s="72" t="s">
+      <c r="E81" s="71"/>
+      <c r="F81" s="71"/>
+      <c r="G81" s="71"/>
+      <c r="H81" s="71"/>
+    </row>
+    <row r="82" spans="1:8" ht="52" x14ac:dyDescent="0.35">
+      <c r="A82" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B81" s="144"/>
-      <c r="C81" s="90"/>
-      <c r="D81" s="99" t="s">
+      <c r="B82" s="94"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="85" t="s">
         <v>943</v>
       </c>
-      <c r="E81" s="90"/>
-      <c r="F81" s="90"/>
-      <c r="G81" s="90"/>
-      <c r="H81" s="94"/>
-    </row>
-    <row r="82" spans="1:8" s="92" customFormat="1" ht="104" x14ac:dyDescent="0.35">
-      <c r="A82" s="72" t="s">
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="71"/>
+    </row>
+    <row r="83" spans="1:8" ht="104" x14ac:dyDescent="0.35">
+      <c r="A83" s="72" t="s">
         <v>947</v>
       </c>
-      <c r="B82" s="144"/>
-      <c r="C82" s="90"/>
-      <c r="D82" s="99" t="s">
+      <c r="B83" s="94"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="85" t="s">
         <v>945</v>
       </c>
-      <c r="E82" s="90"/>
-      <c r="F82" s="90"/>
-      <c r="G82" s="90"/>
-      <c r="H82" s="94"/>
-    </row>
-    <row r="83" spans="1:8" s="92" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A83" s="72" t="s">
+      <c r="E83" s="71"/>
+      <c r="F83" s="71"/>
+      <c r="G83" s="71"/>
+      <c r="H83" s="71"/>
+    </row>
+    <row r="84" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A84" s="72" t="s">
         <v>948</v>
       </c>
-      <c r="B83" s="145"/>
-      <c r="C83" s="90"/>
-      <c r="D83" s="85" t="s">
+      <c r="B84" s="94"/>
+      <c r="C84" s="71"/>
+      <c r="D84" s="85" t="s">
         <v>944</v>
       </c>
-      <c r="E83" s="90"/>
-      <c r="F83" s="90"/>
-      <c r="G83" s="90"/>
-      <c r="H83" s="94"/>
-    </row>
-    <row r="84" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="72"/>
-      <c r="B84" s="98"/>
-      <c r="C84" s="90"/>
-      <c r="D84" s="99"/>
-      <c r="E84" s="90"/>
-      <c r="F84" s="90"/>
-      <c r="G84" s="90"/>
-      <c r="H84" s="94"/>
-    </row>
-    <row r="85" spans="1:8" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="90"/>
-      <c r="B85" s="90"/>
-      <c r="C85" s="90"/>
-      <c r="D85" s="90"/>
-      <c r="E85" s="90"/>
-      <c r="F85" s="90"/>
-      <c r="G85" s="90"/>
-      <c r="H85" s="94"/>
-    </row>
-    <row r="86" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A86" s="98" t="s">
+      <c r="E84" s="71"/>
+      <c r="F84" s="71"/>
+      <c r="G84" s="71"/>
+      <c r="H84" s="71"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C85" s="71"/>
+      <c r="D85" s="85"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="71"/>
+      <c r="G85" s="71"/>
+      <c r="H85" s="71"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="71"/>
+      <c r="B86" s="71"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="71"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="71"/>
+      <c r="G86" s="71"/>
+      <c r="H86" s="71"/>
+    </row>
+    <row r="87" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A87" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="B86" s="98" t="s">
+      <c r="B87" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="C86" s="98"/>
-      <c r="D86" s="99" t="s">
+      <c r="D87" s="85" t="s">
         <v>720</v>
       </c>
-      <c r="E86" s="100"/>
-      <c r="F86" s="100"/>
-      <c r="G86" s="100"/>
-      <c r="H86" s="78"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A87" s="101"/>
-      <c r="B87" s="101"/>
-      <c r="C87" s="101"/>
-      <c r="D87" s="101"/>
-      <c r="E87" s="101"/>
-      <c r="F87" s="101"/>
-      <c r="G87" s="101"/>
-      <c r="H87" s="78"/>
-    </row>
-    <row r="88" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A88" s="78" t="s">
+    </row>
+    <row r="89" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A89" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="B88" s="78"/>
-      <c r="C88" s="78"/>
-      <c r="D88" s="85" t="s">
+      <c r="D89" s="85" t="s">
         <v>882</v>
       </c>
-      <c r="E88" s="78"/>
-      <c r="F88" s="121"/>
-      <c r="G88" s="121"/>
-      <c r="H88" s="78"/>
-    </row>
-    <row r="89" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="78"/>
-      <c r="B89" s="78"/>
-      <c r="C89" s="78"/>
-      <c r="D89" s="78"/>
-      <c r="E89" s="78"/>
-      <c r="F89" s="121"/>
-      <c r="G89" s="121"/>
-      <c r="H89" s="78"/>
-    </row>
-    <row r="90" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A90" s="78" t="s">
+    </row>
+    <row r="90" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A91" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="B90" s="78"/>
-      <c r="C90" s="78"/>
-      <c r="D90" s="85" t="s">
+      <c r="D91" s="85" t="s">
         <v>727</v>
       </c>
-      <c r="E90" s="78"/>
-      <c r="F90" s="121"/>
-      <c r="G90" s="121"/>
-      <c r="H90" s="78"/>
-    </row>
-    <row r="91" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A91" s="78" t="s">
+    </row>
+    <row r="92" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A92" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="B91" s="78"/>
-      <c r="C91" s="78"/>
-      <c r="D91" s="85" t="s">
+      <c r="D92" s="85" t="s">
         <v>570</v>
       </c>
-      <c r="E91" s="78"/>
-      <c r="F91" s="121"/>
-      <c r="G91" s="121"/>
-      <c r="H91" s="78"/>
-    </row>
-    <row r="92" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A92" s="78" t="s">
+    </row>
+    <row r="93" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A93" s="72" t="s">
         <v>881</v>
       </c>
-      <c r="B92" s="78"/>
-      <c r="C92" s="78"/>
-      <c r="D92" s="85" t="s">
+      <c r="D93" s="85" t="s">
         <v>573</v>
       </c>
-      <c r="E92" s="78"/>
-      <c r="F92" s="121"/>
-      <c r="G92" s="121"/>
-      <c r="H92" s="78"/>
-    </row>
-    <row r="93" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A93" s="78" t="s">
+    </row>
+    <row r="94" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A94" s="72" t="s">
         <v>881</v>
       </c>
-      <c r="B93" s="78"/>
-      <c r="C93" s="78"/>
-      <c r="D93" s="85" t="s">
+      <c r="D94" s="85" t="s">
         <v>576</v>
       </c>
-      <c r="E93" s="78"/>
-      <c r="F93" s="121"/>
-      <c r="G93" s="121"/>
-      <c r="H93" s="78"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A94" s="78"/>
-      <c r="B94" s="78"/>
-      <c r="C94" s="78"/>
-      <c r="E94" s="78"/>
-      <c r="F94" s="121"/>
-      <c r="G94" s="121"/>
-      <c r="H94" s="78"/>
-    </row>
-    <row r="95" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A95" s="78"/>
-      <c r="B95" s="78"/>
-      <c r="C95" s="78"/>
-      <c r="D95" s="85" t="s">
+    </row>
+    <row r="96" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="D96" s="85" t="s">
         <v>614</v>
       </c>
-      <c r="E95" s="78"/>
-      <c r="F95" s="121"/>
-      <c r="G95" s="121"/>
-      <c r="H95" s="78"/>
-    </row>
-    <row r="96" spans="1:8" ht="52" x14ac:dyDescent="0.35">
-      <c r="A96" s="78"/>
-      <c r="B96" s="78"/>
-      <c r="C96" s="78"/>
-      <c r="D96" s="85" t="s">
+    </row>
+    <row r="97" spans="4:4" ht="52" x14ac:dyDescent="0.35">
+      <c r="D97" s="85" t="s">
         <v>617</v>
       </c>
-      <c r="E96" s="78"/>
-      <c r="F96" s="121"/>
-      <c r="G96" s="121"/>
-      <c r="H96" s="78"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="78"/>
-      <c r="B97" s="78"/>
-      <c r="C97" s="78"/>
-      <c r="D97" s="85"/>
-      <c r="E97" s="78"/>
-      <c r="F97" s="121"/>
-      <c r="G97" s="121"/>
-      <c r="H97" s="78"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A98" s="78"/>
-      <c r="B98" s="78"/>
-      <c r="C98" s="78"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D98" s="85"/>
-      <c r="E98" s="78"/>
-      <c r="F98" s="121"/>
-      <c r="G98" s="121"/>
-      <c r="H98" s="78"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A99" s="78"/>
-      <c r="B99" s="78"/>
-      <c r="C99" s="78"/>
-      <c r="E99" s="78"/>
-      <c r="F99" s="121"/>
-      <c r="G99" s="121"/>
-      <c r="H99" s="78"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A100" s="78"/>
-      <c r="B100" s="78"/>
-      <c r="C100" s="78"/>
-      <c r="D100" s="85"/>
-      <c r="E100" s="78"/>
-      <c r="F100" s="121"/>
-      <c r="G100" s="121"/>
-      <c r="H100" s="78"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A101" s="78"/>
-      <c r="B101" s="78"/>
-      <c r="C101" s="78"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D99" s="85"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D101" s="85"/>
-      <c r="E101" s="78"/>
-      <c r="F101" s="121"/>
-      <c r="G101" s="121"/>
-      <c r="H101" s="78"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A102" s="78"/>
-      <c r="B102" s="78"/>
-      <c r="C102" s="78"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D102" s="85"/>
-      <c r="E102" s="78"/>
-      <c r="F102" s="121"/>
-      <c r="G102" s="121"/>
-      <c r="H102" s="78"/>
-    </row>
-    <row r="103" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A103" s="78"/>
-      <c r="B103" s="78"/>
-      <c r="C103" s="78"/>
-      <c r="D103" s="85" t="s">
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D103" s="85"/>
+    </row>
+    <row r="104" spans="4:4" ht="39" x14ac:dyDescent="0.35">
+      <c r="D104" s="85" t="s">
         <v>734</v>
       </c>
-      <c r="E103" s="78"/>
-      <c r="F103" s="121"/>
-      <c r="G103" s="121"/>
-      <c r="H103" s="78"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A104" s="78"/>
-      <c r="B104" s="78"/>
-      <c r="C104" s="78"/>
-      <c r="E104" s="78"/>
-      <c r="F104" s="121"/>
-      <c r="G104" s="121"/>
-      <c r="H104" s="78"/>
-    </row>
-    <row r="105" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A105" s="78"/>
-      <c r="B105" s="78"/>
-      <c r="C105" s="78"/>
-      <c r="D105" s="85" t="s">
+    </row>
+    <row r="106" spans="4:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="D106" s="85" t="s">
         <v>762</v>
       </c>
-      <c r="E105" s="78"/>
-      <c r="F105" s="121"/>
-      <c r="G105" s="121"/>
-      <c r="H105" s="78"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A106" s="78"/>
-      <c r="B106" s="78"/>
-      <c r="C106" s="78"/>
-      <c r="D106" s="85" t="s">
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D107" s="85" t="s">
         <v>766</v>
       </c>
-      <c r="E106" s="78"/>
-      <c r="F106" s="121"/>
-      <c r="G106" s="121"/>
-      <c r="H106" s="78"/>
-    </row>
-    <row r="107" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A107" s="78"/>
-      <c r="B107" s="78"/>
-      <c r="C107" s="78"/>
-      <c r="D107" s="85" t="s">
+    </row>
+    <row r="108" spans="4:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="D108" s="85" t="s">
         <v>865</v>
       </c>
-      <c r="E107" s="78"/>
-      <c r="F107" s="121"/>
-      <c r="G107" s="121"/>
-      <c r="H107" s="78"/>
-    </row>
-    <row r="108" spans="1:8" ht="78" x14ac:dyDescent="0.35">
-      <c r="A108" s="78"/>
-      <c r="B108" s="78"/>
-      <c r="C108" s="78"/>
-      <c r="D108" s="85" t="s">
+    </row>
+    <row r="109" spans="4:4" ht="78" x14ac:dyDescent="0.35">
+      <c r="D109" s="85" t="s">
         <v>866</v>
       </c>
-      <c r="E108" s="78"/>
-      <c r="F108" s="121"/>
-      <c r="G108" s="121"/>
-      <c r="H108" s="78"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A109" s="78"/>
-      <c r="B109" s="78"/>
-      <c r="C109" s="78"/>
-      <c r="D109" s="85"/>
-      <c r="E109" s="78"/>
-      <c r="F109" s="121"/>
-      <c r="G109" s="121"/>
-      <c r="H109" s="78"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D110" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="26">
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B66:B76"/>
-    <mergeCell ref="B78:B83"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A53:A64"/>
-    <mergeCell ref="B53:B64"/>
-    <mergeCell ref="E53:E64"/>
+    <mergeCell ref="B67:B77"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A54:A65"/>
+    <mergeCell ref="B54:B65"/>
+    <mergeCell ref="E54:E65"/>
     <mergeCell ref="E9:E15"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="A36:A41"/>
     <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="E19:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10477,87 +10315,87 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C3" t="s">
         <v>974</v>
-      </c>
-      <c r="C3" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C4" t="s">
         <v>976</v>
-      </c>
-      <c r="C4" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C5" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C6" t="s">
         <v>979</v>
-      </c>
-      <c r="C6" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C7" t="s">
         <v>981</v>
-      </c>
-      <c r="C7" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C8" t="s">
         <v>983</v>
-      </c>
-      <c r="C8" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C9" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C10" t="s">
         <v>986</v>
-      </c>
-      <c r="C10" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C11" t="s">
         <v>988</v>
-      </c>
-      <c r="C11" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="C12" t="s">
         <v>990</v>
-      </c>
-      <c r="C12" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C13" t="s">
         <v>537</v>
@@ -11886,7 +11724,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="73" t="s">
         <v>186</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -11895,28 +11733,28 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="133"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="21" t="s">
         <v>188</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="133"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="21" t="s">
         <v>189</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C6" s="133"/>
+      <c r="C6" s="73"/>
       <c r="D6" s="4" t="s">
         <v>190</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="133"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="4" t="s">
         <v>191</v>
       </c>
@@ -11970,7 +11808,7 @@
       <c r="E14"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="134" t="s">
+      <c r="C15" s="74" t="s">
         <v>198</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -11981,37 +11819,37 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C16" s="134"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="4" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17" s="134"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="4" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C18" s="134"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="4" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C19" s="134"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C20" s="134"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C21" s="134"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="1" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
FLOW AND DETAILS DOC
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.004.xlsx
@@ -31,7 +31,6 @@
     <sheet name="Pending" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -5296,7 +5295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5502,39 +5501,6 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5556,8 +5522,41 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5565,11 +5564,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6717,12 +6719,12 @@
       <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="84" t="s">
         <v>553</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="76" t="s">
+      <c r="D20" s="85" t="s">
         <v>554</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -6739,10 +6741,10 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="75"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="76"/>
+      <c r="D21" s="85"/>
       <c r="E21" s="47" t="s">
         <v>556</v>
       </c>
@@ -6757,10 +6759,10 @@
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="75"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="76"/>
+      <c r="D22" s="85"/>
       <c r="E22" s="48" t="s">
         <v>557</v>
       </c>
@@ -6775,10 +6777,10 @@
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="1:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="75"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
-      <c r="D23" s="76"/>
+      <c r="D23" s="85"/>
       <c r="E23" s="48" t="s">
         <v>558</v>
       </c>
@@ -7785,48 +7787,48 @@
     </row>
     <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="86" t="s">
         <v>678</v>
       </c>
-      <c r="C17" s="77"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="86" t="s">
         <v>679</v>
       </c>
-      <c r="C18" s="77"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="86" t="s">
         <v>680</v>
       </c>
-      <c r="C19" s="77"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="86" t="s">
         <v>681</v>
       </c>
-      <c r="C20" s="77"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -8202,7 +8204,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="87" t="s">
         <v>690</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -8211,14 +8213,14 @@
       <c r="D2" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="87" t="s">
         <v>693</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="87" t="s">
         <v>694</v>
       </c>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80" t="s">
+      <c r="G2" s="87"/>
+      <c r="H2" s="88" t="s">
         <v>695</v>
       </c>
     </row>
@@ -8226,21 +8228,21 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="9" t="s">
         <v>696</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="80"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88"/>
     </row>
     <row r="4" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
-      <c r="B4" s="79"/>
+      <c r="B4" s="87"/>
       <c r="C4" s="55" t="s">
         <v>698</v>
       </c>
@@ -8250,14 +8252,14 @@
       <c r="E4" s="55" t="s">
         <v>700</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="89" t="s">
         <v>701</v>
       </c>
-      <c r="G4" s="82"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="1:8" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="79"/>
+      <c r="B5" s="87"/>
       <c r="C5" s="55" t="s">
         <v>702</v>
       </c>
@@ -8265,12 +8267,12 @@
         <v>703</v>
       </c>
       <c r="E5" s="55"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="82"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="90"/>
     </row>
     <row r="6" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="79"/>
+      <c r="B6" s="87"/>
       <c r="C6" s="55" t="s">
         <v>704</v>
       </c>
@@ -8280,21 +8282,21 @@
       <c r="E6" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="F6" s="81"/>
-      <c r="G6" s="82"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="90"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="79"/>
+      <c r="B7" s="87"/>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="81"/>
+      <c r="F7" s="89"/>
       <c r="G7" s="56"/>
     </row>
     <row r="8" spans="1:8" ht="52" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
-      <c r="B8" s="79"/>
+      <c r="B8" s="87"/>
       <c r="C8" s="55" t="s">
         <v>707</v>
       </c>
@@ -8304,12 +8306,12 @@
       <c r="E8" s="55" t="s">
         <v>709</v>
       </c>
-      <c r="F8" s="81"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="56"/>
     </row>
     <row r="9" spans="1:8" ht="78" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="79"/>
+      <c r="B9" s="87"/>
       <c r="C9" s="9" t="s">
         <v>710</v>
       </c>
@@ -8319,14 +8321,14 @@
       <c r="E9" s="9" t="s">
         <v>712</v>
       </c>
-      <c r="F9" s="81"/>
+      <c r="F9" s="89"/>
       <c r="G9" s="9" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="79"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="9" t="s">
         <v>714</v>
       </c>
@@ -8336,12 +8338,12 @@
       <c r="E10" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="89"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="156" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="79"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="9" t="s">
         <v>716</v>
       </c>
@@ -8379,7 +8381,7 @@
     </row>
     <row r="13" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="91" t="s">
         <v>725</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -8394,7 +8396,7 @@
     </row>
     <row r="14" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="78"/>
+      <c r="B14" s="91"/>
       <c r="C14" s="9" t="s">
         <v>531</v>
       </c>
@@ -8407,7 +8409,7 @@
     </row>
     <row r="15" spans="1:8" ht="65" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="78"/>
+      <c r="B15" s="91"/>
       <c r="C15" s="9" t="s">
         <v>533</v>
       </c>
@@ -8420,7 +8422,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
-      <c r="B16" s="78"/>
+      <c r="B16" s="91"/>
       <c r="C16" s="9" t="s">
         <v>536</v>
       </c>
@@ -8433,7 +8435,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="78"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="9" t="s">
         <v>546</v>
       </c>
@@ -8446,7 +8448,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="78"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="9" t="s">
         <v>548</v>
       </c>
@@ -8459,7 +8461,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="78"/>
+      <c r="B19" s="91"/>
       <c r="C19" s="9" t="s">
         <v>550</v>
       </c>
@@ -8472,7 +8474,7 @@
     </row>
     <row r="20" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="78"/>
+      <c r="B20" s="91"/>
       <c r="C20" s="9" t="s">
         <v>555</v>
       </c>
@@ -8485,7 +8487,7 @@
     </row>
     <row r="21" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="78"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="9" t="s">
         <v>727</v>
       </c>
@@ -8498,7 +8500,7 @@
     </row>
     <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="78"/>
+      <c r="B22" s="91"/>
       <c r="C22" s="9" t="s">
         <v>570</v>
       </c>
@@ -8511,7 +8513,7 @@
     </row>
     <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="78"/>
+      <c r="B23" s="91"/>
       <c r="C23" s="9" t="s">
         <v>573</v>
       </c>
@@ -8524,7 +8526,7 @@
     </row>
     <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="78"/>
+      <c r="B24" s="91"/>
       <c r="C24" s="9" t="s">
         <v>576</v>
       </c>
@@ -8537,7 +8539,7 @@
     </row>
     <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
-      <c r="B25" s="78"/>
+      <c r="B25" s="91"/>
       <c r="C25" s="9" t="s">
         <v>728</v>
       </c>
@@ -8550,7 +8552,7 @@
     </row>
     <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
-      <c r="B26" s="78"/>
+      <c r="B26" s="91"/>
       <c r="C26" s="9" t="s">
         <v>581</v>
       </c>
@@ -8563,7 +8565,7 @@
     </row>
     <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
-      <c r="B27" s="78"/>
+      <c r="B27" s="91"/>
       <c r="C27" s="9" t="s">
         <v>729</v>
       </c>
@@ -8576,7 +8578,7 @@
     </row>
     <row r="28" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
-      <c r="B28" s="78"/>
+      <c r="B28" s="91"/>
       <c r="C28" s="9" t="s">
         <v>595</v>
       </c>
@@ -8589,7 +8591,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
-      <c r="B29" s="78"/>
+      <c r="B29" s="91"/>
       <c r="C29" s="9" t="s">
         <v>598</v>
       </c>
@@ -8602,7 +8604,7 @@
     </row>
     <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="78"/>
+      <c r="B30" s="91"/>
       <c r="C30" s="9" t="s">
         <v>601</v>
       </c>
@@ -8615,7 +8617,7 @@
     </row>
     <row r="31" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="78"/>
+      <c r="B31" s="91"/>
       <c r="C31" s="9" t="s">
         <v>606</v>
       </c>
@@ -8628,7 +8630,7 @@
     </row>
     <row r="32" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="78"/>
+      <c r="B32" s="91"/>
       <c r="C32" s="9" t="s">
         <v>614</v>
       </c>
@@ -8641,7 +8643,7 @@
     </row>
     <row r="33" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="78"/>
+      <c r="B33" s="91"/>
       <c r="C33" s="9" t="s">
         <v>617</v>
       </c>
@@ -8654,7 +8656,7 @@
     </row>
     <row r="34" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
-      <c r="B34" s="78"/>
+      <c r="B34" s="91"/>
       <c r="C34" s="9" t="s">
         <v>732</v>
       </c>
@@ -8667,7 +8669,7 @@
     </row>
     <row r="35" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
-      <c r="B35" s="78"/>
+      <c r="B35" s="91"/>
       <c r="C35" s="9" t="s">
         <v>622</v>
       </c>
@@ -8680,7 +8682,7 @@
     </row>
     <row r="36" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
-      <c r="B36" s="78"/>
+      <c r="B36" s="91"/>
       <c r="C36" s="9" t="s">
         <v>624</v>
       </c>
@@ -8693,7 +8695,7 @@
     </row>
     <row r="37" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
-      <c r="B37" s="78"/>
+      <c r="B37" s="91"/>
       <c r="C37" s="9" t="s">
         <v>627</v>
       </c>
@@ -8706,7 +8708,7 @@
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
-      <c r="B38" s="78"/>
+      <c r="B38" s="91"/>
       <c r="C38" s="9" t="s">
         <v>630</v>
       </c>
@@ -8719,7 +8721,7 @@
     </row>
     <row r="39" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
-      <c r="B39" s="78"/>
+      <c r="B39" s="91"/>
       <c r="C39" s="9" t="s">
         <v>633</v>
       </c>
@@ -8732,7 +8734,7 @@
     </row>
     <row r="40" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
-      <c r="B40" s="78"/>
+      <c r="B40" s="91"/>
       <c r="C40" s="9" t="s">
         <v>635</v>
       </c>
@@ -8745,7 +8747,7 @@
     </row>
     <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
-      <c r="B41" s="78"/>
+      <c r="B41" s="91"/>
       <c r="C41" s="9" t="s">
         <v>734</v>
       </c>
@@ -8833,7 +8835,7 @@
     </row>
     <row r="49" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
-      <c r="B49" s="79" t="s">
+      <c r="B49" s="87" t="s">
         <v>740</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -8850,7 +8852,7 @@
     </row>
     <row r="50" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
-      <c r="B50" s="79"/>
+      <c r="B50" s="87"/>
       <c r="C50" s="9" t="s">
         <v>744</v>
       </c>
@@ -8865,7 +8867,7 @@
     </row>
     <row r="51" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A51" s="9"/>
-      <c r="B51" s="79"/>
+      <c r="B51" s="87"/>
       <c r="C51" s="9" t="s">
         <v>747</v>
       </c>
@@ -8880,7 +8882,7 @@
     </row>
     <row r="52" spans="1:7" ht="78" x14ac:dyDescent="0.35">
       <c r="A52" s="9"/>
-      <c r="B52" s="79"/>
+      <c r="B52" s="87"/>
       <c r="C52" s="9" t="s">
         <v>750</v>
       </c>
@@ -8895,7 +8897,7 @@
     </row>
     <row r="53" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
-      <c r="B53" s="79"/>
+      <c r="B53" s="87"/>
       <c r="C53" s="9" t="s">
         <v>753</v>
       </c>
@@ -8910,7 +8912,7 @@
     </row>
     <row r="54" spans="1:7" ht="52" x14ac:dyDescent="0.35">
       <c r="A54" s="9"/>
-      <c r="B54" s="79"/>
+      <c r="B54" s="87"/>
       <c r="C54" s="9" t="s">
         <v>756</v>
       </c>
@@ -8925,7 +8927,7 @@
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
-      <c r="B55" s="79"/>
+      <c r="B55" s="87"/>
       <c r="C55" s="56" t="s">
         <v>123</v>
       </c>
@@ -8974,7 +8976,7 @@
     </row>
     <row r="58" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
-      <c r="B58" s="79" t="s">
+      <c r="B58" s="87" t="s">
         <v>769</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -8991,7 +8993,7 @@
     </row>
     <row r="59" spans="1:7" ht="208" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
-      <c r="B59" s="79"/>
+      <c r="B59" s="87"/>
       <c r="C59" s="9" t="s">
         <v>773</v>
       </c>
@@ -9017,16 +9019,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B13:B41"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="F4:F10"/>
     <mergeCell ref="G4:G6"/>
-    <mergeCell ref="B13:B41"/>
-    <mergeCell ref="B49:B55"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9037,8 +9039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -9063,7 +9065,7 @@
         <v>859</v>
       </c>
       <c r="C1" s="71"/>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="73" t="s">
         <v>684</v>
       </c>
       <c r="E1" s="71" t="s">
@@ -9086,7 +9088,7 @@
       <c r="B2" s="72" t="s">
         <v>965</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="74" t="s">
         <v>1002</v>
       </c>
       <c r="E2" s="72" t="s">
@@ -9106,7 +9108,7 @@
       <c r="A3" s="71"/>
       <c r="B3" s="71"/>
       <c r="C3" s="71"/>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="74" t="s">
         <v>1005</v>
       </c>
       <c r="E3" s="72" t="s">
@@ -9124,7 +9126,7 @@
       <c r="B4" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="74" t="s">
         <v>1008</v>
       </c>
       <c r="E4" s="71"/>
@@ -9140,7 +9142,7 @@
       <c r="A5" s="71"/>
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="74" t="s">
         <v>1009</v>
       </c>
       <c r="E5" s="71"/>
@@ -9188,7 +9190,7 @@
       <c r="A8" s="71"/>
       <c r="B8" s="71"/>
       <c r="C8" s="71"/>
-      <c r="D8" s="84"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="71"/>
       <c r="F8" s="71"/>
       <c r="G8" s="71"/>
@@ -9199,10 +9201,10 @@
       <c r="B9" s="72" t="s">
         <v>876</v>
       </c>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="74" t="s">
         <v>1018</v>
       </c>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="94" t="s">
         <v>892</v>
       </c>
       <c r="F9" s="72" t="s">
@@ -9213,18 +9215,18 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="D10" s="85" t="s">
+      <c r="B10" s="80"/>
+      <c r="D10" s="74" t="s">
         <v>1020</v>
       </c>
-      <c r="E10" s="94"/>
-      <c r="F10" s="93" t="s">
+      <c r="E10" s="93"/>
+      <c r="F10" s="80" t="s">
         <v>1021</v>
       </c>
-      <c r="G10" s="93" t="s">
+      <c r="G10" s="80" t="s">
         <v>1022</v>
       </c>
       <c r="H10" s="72" t="s">
@@ -9235,38 +9237,38 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="83"/>
-      <c r="B11" s="93" t="s">
+      <c r="A11" s="94"/>
+      <c r="B11" s="80" t="s">
         <v>1025</v>
       </c>
-      <c r="E11" s="94"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="85" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="74" t="s">
         <v>1023</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="83"/>
-      <c r="B12" s="93" t="s">
+      <c r="A12" s="94"/>
+      <c r="B12" s="80" t="s">
         <v>1026</v>
       </c>
-      <c r="E12" s="94"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="85" t="s">
+      <c r="E12" s="93"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="74" t="s">
         <v>1024</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A13" s="83"/>
-      <c r="B13" s="93"/>
-      <c r="D13" s="86" t="s">
+      <c r="A13" s="94"/>
+      <c r="B13" s="80"/>
+      <c r="D13" s="75" t="s">
         <v>1027</v>
       </c>
-      <c r="E13" s="94"/>
+      <c r="E13" s="93"/>
       <c r="F13" s="92" t="s">
         <v>1028</v>
       </c>
-      <c r="G13" s="83" t="s">
+      <c r="G13" s="94" t="s">
         <v>1029</v>
       </c>
       <c r="H13" s="72" t="s">
@@ -9274,34 +9276,34 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A14" s="83"/>
-      <c r="B14" s="93"/>
-      <c r="D14" s="86" t="s">
+      <c r="A14" s="94"/>
+      <c r="B14" s="80"/>
+      <c r="D14" s="75" t="s">
         <v>888</v>
       </c>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
       <c r="H14" s="72" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="39" x14ac:dyDescent="0.35">
-      <c r="A15" s="83"/>
-      <c r="B15" s="93"/>
-      <c r="D15" s="87" t="s">
+      <c r="A15" s="94"/>
+      <c r="B15" s="80"/>
+      <c r="D15" s="96" t="s">
         <v>958</v>
       </c>
-      <c r="E15" s="94"/>
-      <c r="F15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="80"/>
       <c r="H15" s="72" t="s">
         <v>1030</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="143" x14ac:dyDescent="0.35">
-      <c r="A16" s="83"/>
-      <c r="B16" s="93"/>
-      <c r="D16" s="86" t="s">
+      <c r="A16" s="94"/>
+      <c r="B16" s="80"/>
+      <c r="D16" s="75" t="s">
         <v>1031</v>
       </c>
       <c r="E16" s="72" t="s">
@@ -9321,13 +9323,13 @@
       <c r="A17" s="72" t="s">
         <v>968</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="80" t="s">
         <v>969</v>
       </c>
       <c r="C17" s="72" t="s">
         <v>968</v>
       </c>
-      <c r="D17" s="86"/>
+      <c r="D17" s="75"/>
       <c r="G17" s="72" t="s">
         <v>1037</v>
       </c>
@@ -9336,7 +9338,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="104" x14ac:dyDescent="0.35">
-      <c r="D18" s="86"/>
+      <c r="D18" s="75"/>
       <c r="F18" s="72" t="s">
         <v>1034</v>
       </c>
@@ -9348,7 +9350,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="104" x14ac:dyDescent="0.35">
-      <c r="D19" s="86"/>
+      <c r="D19" s="75"/>
       <c r="F19" s="72" t="s">
         <v>1038</v>
       </c>
@@ -9357,73 +9359,73 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="83" t="s">
+      <c r="A20" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="94" t="s">
         <v>877</v>
       </c>
-      <c r="D20" s="86" t="s">
+      <c r="D20" s="75" t="s">
         <v>707</v>
       </c>
-      <c r="E20" s="83" t="s">
+      <c r="E20" s="94" t="s">
         <v>891</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="94" t="s">
         <v>957</v>
       </c>
-      <c r="I20" s="83" t="s">
+      <c r="I20" s="94" t="s">
         <v>960</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83"/>
-      <c r="D21" s="86" t="s">
+      <c r="A21" s="94"/>
+      <c r="B21" s="94"/>
+      <c r="D21" s="75" t="s">
         <v>889</v>
       </c>
-      <c r="E21" s="83"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
     </row>
     <row r="22" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="83"/>
-      <c r="B22" s="83"/>
-      <c r="D22" s="86" t="s">
+      <c r="A22" s="94"/>
+      <c r="B22" s="94"/>
+      <c r="D22" s="75" t="s">
         <v>862</v>
       </c>
-      <c r="E22" s="83"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
     </row>
     <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
-      <c r="D23" s="86" t="s">
+      <c r="A23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="D23" s="75" t="s">
         <v>863</v>
       </c>
-      <c r="E23" s="83"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="93"/>
     </row>
     <row r="24" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="D24" s="85" t="s">
+      <c r="A24" s="94"/>
+      <c r="B24" s="94"/>
+      <c r="D24" s="74" t="s">
         <v>867</v>
       </c>
-      <c r="E24" s="83"/>
+      <c r="E24" s="94"/>
       <c r="H24" s="72" t="s">
         <v>957</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="39" x14ac:dyDescent="0.35">
-      <c r="A25" s="83"/>
-      <c r="B25" s="83"/>
-      <c r="D25" s="85" t="s">
+      <c r="A25" s="94"/>
+      <c r="B25" s="94"/>
+      <c r="D25" s="74" t="s">
         <v>893</v>
       </c>
-      <c r="E25" s="83" t="s">
+      <c r="E25" s="94" t="s">
         <v>897</v>
       </c>
       <c r="H25" s="72" t="s">
@@ -9431,52 +9433,52 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="52" x14ac:dyDescent="0.35">
-      <c r="A26" s="83"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="94"/>
+      <c r="B26" s="94"/>
       <c r="C26" s="72" t="s">
         <v>971</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="75" t="s">
         <v>970</v>
       </c>
-      <c r="E26" s="83"/>
+      <c r="E26" s="94"/>
     </row>
     <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A27" s="83"/>
-      <c r="B27" s="83"/>
-      <c r="D27" s="85" t="s">
+      <c r="A27" s="94"/>
+      <c r="B27" s="94"/>
+      <c r="D27" s="74" t="s">
         <v>894</v>
       </c>
-      <c r="E27" s="83"/>
+      <c r="E27" s="94"/>
       <c r="H27" s="72" t="s">
         <v>961</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A28" s="83"/>
-      <c r="B28" s="83"/>
-      <c r="D28" s="85" t="s">
+      <c r="A28" s="94"/>
+      <c r="B28" s="94"/>
+      <c r="D28" s="74" t="s">
         <v>895</v>
       </c>
-      <c r="E28" s="83"/>
+      <c r="E28" s="94"/>
       <c r="H28" s="72" t="s">
         <v>961</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D29" s="86"/>
+      <c r="D29" s="75"/>
     </row>
     <row r="30" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A30" s="83" t="s">
+      <c r="A30" s="94" t="s">
         <v>537</v>
       </c>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="94" t="s">
         <v>878</v>
       </c>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="75" t="s">
         <v>884</v>
       </c>
-      <c r="E30" s="83" t="s">
+      <c r="E30" s="94" t="s">
         <v>899</v>
       </c>
       <c r="H30" s="72" t="s">
@@ -9484,12 +9486,12 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="65" x14ac:dyDescent="0.35">
-      <c r="A31" s="83"/>
-      <c r="B31" s="83"/>
-      <c r="D31" s="85" t="s">
+      <c r="A31" s="94"/>
+      <c r="B31" s="94"/>
+      <c r="D31" s="74" t="s">
         <v>864</v>
       </c>
-      <c r="E31" s="83"/>
+      <c r="E31" s="94"/>
       <c r="H31" s="72" t="s">
         <v>860</v>
       </c>
@@ -9501,7 +9503,7 @@
       <c r="B32" s="72" t="s">
         <v>964</v>
       </c>
-      <c r="D32" s="87" t="s">
+      <c r="D32" s="76" t="s">
         <v>962</v>
       </c>
       <c r="E32" s="72" t="s">
@@ -9512,17 +9514,17 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D33" s="85"/>
+      <c r="D33" s="74"/>
     </row>
     <row r="34" spans="1:8" ht="91" x14ac:dyDescent="0.35">
-      <c r="A34" s="88" t="s">
+      <c r="A34" s="77" t="s">
         <v>870</v>
       </c>
-      <c r="B34" s="88" t="s">
+      <c r="B34" s="77" t="s">
         <v>868</v>
       </c>
-      <c r="C34" s="88"/>
-      <c r="D34" s="89" t="s">
+      <c r="C34" s="77"/>
+      <c r="D34" s="78" t="s">
         <v>885</v>
       </c>
       <c r="E34" s="72" t="s">
@@ -9530,60 +9532,60 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D35" s="85"/>
+      <c r="D35" s="74"/>
     </row>
     <row r="36" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A36" s="83" t="s">
+      <c r="A36" s="94" t="s">
         <v>861</v>
       </c>
-      <c r="B36" s="83" t="s">
+      <c r="B36" s="94" t="s">
         <v>879</v>
       </c>
-      <c r="D36" s="85" t="s">
+      <c r="D36" s="74" t="s">
         <v>871</v>
       </c>
-      <c r="E36" s="83" t="s">
+      <c r="E36" s="94" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A37" s="83"/>
-      <c r="B37" s="83"/>
-      <c r="D37" s="85" t="s">
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="D37" s="74" t="s">
         <v>872</v>
       </c>
-      <c r="E37" s="83"/>
+      <c r="E37" s="94"/>
     </row>
     <row r="38" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A38" s="83"/>
-      <c r="B38" s="83"/>
-      <c r="D38" s="85" t="s">
+      <c r="A38" s="94"/>
+      <c r="B38" s="94"/>
+      <c r="D38" s="74" t="s">
         <v>536</v>
       </c>
       <c r="E38" s="72" t="s">
         <v>901</v>
       </c>
-      <c r="H38" s="85" t="s">
+      <c r="H38" s="74" t="s">
         <v>886</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="78" x14ac:dyDescent="0.35">
-      <c r="A39" s="83"/>
-      <c r="B39" s="83"/>
-      <c r="D39" s="87" t="s">
+      <c r="A39" s="94"/>
+      <c r="B39" s="94"/>
+      <c r="D39" s="76" t="s">
         <v>887</v>
       </c>
       <c r="E39" s="72" t="s">
         <v>902</v>
       </c>
-      <c r="H39" s="90" t="s">
+      <c r="H39" s="79" t="s">
         <v>874</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A40" s="83"/>
-      <c r="B40" s="83"/>
-      <c r="D40" s="85" t="s">
+      <c r="A40" s="94"/>
+      <c r="B40" s="94"/>
+      <c r="D40" s="74" t="s">
         <v>548</v>
       </c>
       <c r="E40" s="72" t="s">
@@ -9594,9 +9596,9 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A41" s="83"/>
-      <c r="B41" s="83"/>
-      <c r="D41" s="85" t="s">
+      <c r="A41" s="94"/>
+      <c r="B41" s="94"/>
+      <c r="D41" s="74" t="s">
         <v>873</v>
       </c>
       <c r="E41" s="72" t="s">
@@ -9607,7 +9609,7 @@
       <c r="A42" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="D42" s="85" t="s">
+      <c r="D42" s="74" t="s">
         <v>908</v>
       </c>
     </row>
@@ -9615,32 +9617,32 @@
       <c r="A43" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="D43" s="85" t="s">
+      <c r="D43" s="74" t="s">
         <v>898</v>
       </c>
-      <c r="E43" s="85" t="s">
+      <c r="E43" s="74" t="s">
         <v>905</v>
       </c>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="91" t="s">
+      <c r="A44" s="95" t="s">
         <v>883</v>
       </c>
-      <c r="B44" s="91"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="91"/>
-      <c r="H44" s="91"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="95"/>
+      <c r="F44" s="95"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="95"/>
     </row>
     <row r="45" spans="1:8" ht="39" x14ac:dyDescent="0.35">
       <c r="A45" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="94" t="s">
         <v>916</v>
       </c>
       <c r="D45" s="72" t="s">
@@ -9654,7 +9656,7 @@
       <c r="A46" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="B46" s="83"/>
+      <c r="B46" s="94"/>
       <c r="D46" s="72" t="s">
         <v>909</v>
       </c>
@@ -9666,7 +9668,7 @@
       <c r="A47" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="83"/>
+      <c r="B47" s="94"/>
       <c r="D47" s="72" t="s">
         <v>910</v>
       </c>
@@ -9678,7 +9680,7 @@
       <c r="A48" s="72" t="s">
         <v>861</v>
       </c>
-      <c r="B48" s="83"/>
+      <c r="B48" s="94"/>
       <c r="D48" s="72" t="s">
         <v>911</v>
       </c>
@@ -9687,16 +9689,16 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="91" t="s">
+      <c r="A49" s="95" t="s">
         <v>917</v>
       </c>
-      <c r="B49" s="91"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="91"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="91"/>
-      <c r="G49" s="91"/>
-      <c r="H49" s="91"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="95"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="95"/>
+      <c r="H49" s="95"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="71"/>
@@ -9712,14 +9714,14 @@
       <c r="A51" s="72" t="s">
         <v>952</v>
       </c>
-      <c r="B51" s="83" t="s">
+      <c r="B51" s="94" t="s">
         <v>953</v>
       </c>
       <c r="C51" s="71"/>
       <c r="D51" s="72" t="s">
         <v>951</v>
       </c>
-      <c r="E51" s="83" t="s">
+      <c r="E51" s="94" t="s">
         <v>954</v>
       </c>
       <c r="H51" s="71"/>
@@ -9734,8 +9736,8 @@
         <v>950</v>
       </c>
       <c r="E52" s="92"/>
-      <c r="F52" s="95"/>
-      <c r="G52" s="95"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="81"/>
       <c r="H52" s="71"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -9749,138 +9751,138 @@
       <c r="H53" s="71"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="83" t="s">
+      <c r="A54" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="83" t="s">
+      <c r="B54" s="94" t="s">
         <v>926</v>
       </c>
       <c r="C54" s="71"/>
       <c r="D54" s="72" t="s">
         <v>918</v>
       </c>
-      <c r="E54" s="83" t="s">
+      <c r="E54" s="94" t="s">
         <v>927</v>
       </c>
       <c r="H54" s="71"/>
     </row>
     <row r="55" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A55" s="83"/>
-      <c r="B55" s="83"/>
+      <c r="A55" s="94"/>
+      <c r="B55" s="94"/>
       <c r="C55" s="71"/>
-      <c r="D55" s="85" t="s">
+      <c r="D55" s="74" t="s">
         <v>919</v>
       </c>
-      <c r="E55" s="83"/>
+      <c r="E55" s="94"/>
       <c r="H55" s="71" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="83"/>
-      <c r="B56" s="83"/>
+      <c r="A56" s="94"/>
+      <c r="B56" s="94"/>
       <c r="C56" s="71"/>
-      <c r="D56" s="85" t="s">
+      <c r="D56" s="74" t="s">
         <v>744</v>
       </c>
-      <c r="E56" s="83"/>
+      <c r="E56" s="94"/>
       <c r="H56" s="71" t="s">
         <v>929</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A57" s="83"/>
-      <c r="B57" s="83"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="94"/>
       <c r="C57" s="71"/>
-      <c r="D57" s="85" t="s">
+      <c r="D57" s="74" t="s">
         <v>920</v>
       </c>
-      <c r="E57" s="83"/>
+      <c r="E57" s="94"/>
       <c r="H57" s="71"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="83"/>
-      <c r="B58" s="83"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="94"/>
       <c r="C58" s="71"/>
       <c r="D58" s="72" t="s">
         <v>750</v>
       </c>
-      <c r="E58" s="83"/>
+      <c r="E58" s="94"/>
       <c r="H58" s="71"/>
     </row>
     <row r="59" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A59" s="83"/>
-      <c r="B59" s="83"/>
+      <c r="A59" s="94"/>
+      <c r="B59" s="94"/>
       <c r="C59" s="71" t="s">
         <v>971</v>
       </c>
-      <c r="E59" s="83"/>
+      <c r="E59" s="94"/>
       <c r="H59" s="71"/>
     </row>
     <row r="60" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A60" s="83"/>
-      <c r="B60" s="83"/>
+      <c r="A60" s="94"/>
+      <c r="B60" s="94"/>
       <c r="C60" s="71"/>
-      <c r="D60" s="85" t="s">
+      <c r="D60" s="74" t="s">
         <v>921</v>
       </c>
-      <c r="E60" s="83"/>
+      <c r="E60" s="94"/>
       <c r="H60" s="71"/>
     </row>
     <row r="61" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A61" s="83"/>
-      <c r="B61" s="83"/>
+      <c r="A61" s="94"/>
+      <c r="B61" s="94"/>
       <c r="C61" s="71"/>
-      <c r="D61" s="85" t="s">
+      <c r="D61" s="74" t="s">
         <v>922</v>
       </c>
-      <c r="E61" s="83"/>
+      <c r="E61" s="94"/>
       <c r="H61" s="71"/>
     </row>
     <row r="62" spans="1:8" ht="52" x14ac:dyDescent="0.35">
-      <c r="A62" s="83"/>
-      <c r="B62" s="83"/>
+      <c r="A62" s="94"/>
+      <c r="B62" s="94"/>
       <c r="C62" s="71"/>
-      <c r="D62" s="85" t="s">
+      <c r="D62" s="74" t="s">
         <v>923</v>
       </c>
-      <c r="E62" s="83"/>
+      <c r="E62" s="94"/>
       <c r="H62" s="71"/>
     </row>
     <row r="63" spans="1:8" ht="52" x14ac:dyDescent="0.35">
-      <c r="A63" s="83"/>
-      <c r="B63" s="83"/>
+      <c r="A63" s="94"/>
+      <c r="B63" s="94"/>
       <c r="C63" s="71"/>
-      <c r="D63" s="85" t="s">
+      <c r="D63" s="74" t="s">
         <v>924</v>
       </c>
-      <c r="E63" s="83"/>
+      <c r="E63" s="94"/>
       <c r="H63" s="71"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="83"/>
-      <c r="B64" s="83"/>
+      <c r="A64" s="94"/>
+      <c r="B64" s="94"/>
       <c r="C64" s="71"/>
-      <c r="D64" s="85" t="s">
+      <c r="D64" s="74" t="s">
         <v>753</v>
       </c>
-      <c r="E64" s="83"/>
+      <c r="E64" s="94"/>
       <c r="H64" s="71"/>
     </row>
     <row r="65" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="83"/>
-      <c r="B65" s="83"/>
+      <c r="A65" s="94"/>
+      <c r="B65" s="94"/>
       <c r="C65" s="71"/>
-      <c r="D65" s="85" t="s">
+      <c r="D65" s="74" t="s">
         <v>925</v>
       </c>
-      <c r="E65" s="83"/>
+      <c r="E65" s="94"/>
       <c r="H65" s="71"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B66" s="71"/>
       <c r="C66" s="71"/>
-      <c r="D66" s="87"/>
+      <c r="D66" s="76"/>
       <c r="E66" s="71"/>
       <c r="F66" s="71"/>
       <c r="G66" s="71"/>
@@ -9890,7 +9892,7 @@
       <c r="A67" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="83" t="s">
+      <c r="B67" s="94" t="s">
         <v>946</v>
       </c>
       <c r="C67" s="71"/>
@@ -9906,9 +9908,9 @@
       <c r="A68" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B68" s="83"/>
+      <c r="B68" s="94"/>
       <c r="C68" s="71"/>
-      <c r="D68" s="85" t="s">
+      <c r="D68" s="74" t="s">
         <v>934</v>
       </c>
       <c r="E68" s="71" t="s">
@@ -9922,9 +9924,9 @@
       <c r="A69" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B69" s="83"/>
+      <c r="B69" s="94"/>
       <c r="C69" s="71"/>
-      <c r="D69" s="85" t="s">
+      <c r="D69" s="74" t="s">
         <v>581</v>
       </c>
       <c r="E69" s="71"/>
@@ -9936,9 +9938,9 @@
       <c r="A70" s="72" t="s">
         <v>997</v>
       </c>
-      <c r="B70" s="83"/>
+      <c r="B70" s="94"/>
       <c r="C70" s="71"/>
-      <c r="D70" s="85" t="s">
+      <c r="D70" s="74" t="s">
         <v>998</v>
       </c>
       <c r="E70" s="71"/>
@@ -9950,9 +9952,9 @@
       <c r="A71" s="72" t="s">
         <v>997</v>
       </c>
-      <c r="B71" s="83"/>
+      <c r="B71" s="94"/>
       <c r="C71" s="71"/>
-      <c r="D71" s="85" t="s">
+      <c r="D71" s="74" t="s">
         <v>999</v>
       </c>
       <c r="E71" s="71"/>
@@ -9964,9 +9966,9 @@
       <c r="A72" s="72" t="s">
         <v>933</v>
       </c>
-      <c r="B72" s="83"/>
+      <c r="B72" s="94"/>
       <c r="C72" s="71"/>
-      <c r="D72" s="85" t="s">
+      <c r="D72" s="74" t="s">
         <v>932</v>
       </c>
       <c r="E72" s="71"/>
@@ -9978,9 +9980,9 @@
       <c r="A73" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B73" s="83"/>
+      <c r="B73" s="94"/>
       <c r="C73" s="71"/>
-      <c r="D73" s="85" t="s">
+      <c r="D73" s="74" t="s">
         <v>935</v>
       </c>
       <c r="E73" s="71" t="s">
@@ -9994,9 +9996,9 @@
       <c r="A74" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B74" s="83"/>
+      <c r="B74" s="94"/>
       <c r="C74" s="71"/>
-      <c r="D74" s="85" t="s">
+      <c r="D74" s="74" t="s">
         <v>598</v>
       </c>
       <c r="E74" s="71" t="s">
@@ -10010,9 +10012,9 @@
       <c r="A75" s="72" t="s">
         <v>930</v>
       </c>
-      <c r="B75" s="83"/>
+      <c r="B75" s="94"/>
       <c r="C75" s="71"/>
-      <c r="D75" s="85" t="s">
+      <c r="D75" s="74" t="s">
         <v>936</v>
       </c>
       <c r="E75" s="71"/>
@@ -10024,9 +10026,9 @@
       <c r="A76" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B76" s="94"/>
+      <c r="B76" s="93"/>
       <c r="C76" s="71"/>
-      <c r="D76" s="85" t="s">
+      <c r="D76" s="74" t="s">
         <v>938</v>
       </c>
       <c r="E76" s="71"/>
@@ -10038,9 +10040,9 @@
       <c r="A77" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B77" s="94"/>
+      <c r="B77" s="93"/>
       <c r="C77" s="71"/>
-      <c r="D77" s="85" t="s">
+      <c r="D77" s="74" t="s">
         <v>939</v>
       </c>
       <c r="E77" s="71"/>
@@ -10050,7 +10052,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C78" s="71"/>
-      <c r="D78" s="85"/>
+      <c r="D78" s="74"/>
       <c r="E78" s="71"/>
       <c r="F78" s="71"/>
       <c r="G78" s="71"/>
@@ -10060,11 +10062,11 @@
       <c r="A79" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B79" s="83" t="s">
+      <c r="B79" s="94" t="s">
         <v>949</v>
       </c>
       <c r="C79" s="71"/>
-      <c r="D79" s="85" t="s">
+      <c r="D79" s="74" t="s">
         <v>940</v>
       </c>
       <c r="E79" s="71"/>
@@ -10076,9 +10078,9 @@
       <c r="A80" s="72" t="s">
         <v>947</v>
       </c>
-      <c r="B80" s="94"/>
+      <c r="B80" s="93"/>
       <c r="C80" s="71"/>
-      <c r="D80" s="85" t="s">
+      <c r="D80" s="74" t="s">
         <v>941</v>
       </c>
       <c r="E80" s="71"/>
@@ -10090,9 +10092,9 @@
       <c r="A81" s="72" t="s">
         <v>947</v>
       </c>
-      <c r="B81" s="94"/>
+      <c r="B81" s="93"/>
       <c r="C81" s="71"/>
-      <c r="D81" s="85" t="s">
+      <c r="D81" s="74" t="s">
         <v>942</v>
       </c>
       <c r="E81" s="71"/>
@@ -10104,9 +10106,9 @@
       <c r="A82" s="72" t="s">
         <v>937</v>
       </c>
-      <c r="B82" s="94"/>
+      <c r="B82" s="93"/>
       <c r="C82" s="71"/>
-      <c r="D82" s="85" t="s">
+      <c r="D82" s="74" t="s">
         <v>943</v>
       </c>
       <c r="E82" s="71"/>
@@ -10118,9 +10120,9 @@
       <c r="A83" s="72" t="s">
         <v>947</v>
       </c>
-      <c r="B83" s="94"/>
+      <c r="B83" s="93"/>
       <c r="C83" s="71"/>
-      <c r="D83" s="85" t="s">
+      <c r="D83" s="74" t="s">
         <v>945</v>
       </c>
       <c r="E83" s="71"/>
@@ -10132,9 +10134,9 @@
       <c r="A84" s="72" t="s">
         <v>948</v>
       </c>
-      <c r="B84" s="94"/>
+      <c r="B84" s="93"/>
       <c r="C84" s="71"/>
-      <c r="D84" s="85" t="s">
+      <c r="D84" s="74" t="s">
         <v>944</v>
       </c>
       <c r="E84" s="71"/>
@@ -10144,7 +10146,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C85" s="71"/>
-      <c r="D85" s="85"/>
+      <c r="D85" s="74"/>
       <c r="E85" s="71"/>
       <c r="F85" s="71"/>
       <c r="G85" s="71"/>
@@ -10167,7 +10169,7 @@
       <c r="B87" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="D87" s="85" t="s">
+      <c r="D87" s="74" t="s">
         <v>720</v>
       </c>
     </row>
@@ -10175,7 +10177,7 @@
       <c r="A89" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="D89" s="85" t="s">
+      <c r="D89" s="74" t="s">
         <v>882</v>
       </c>
     </row>
@@ -10184,7 +10186,7 @@
       <c r="A91" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="D91" s="85" t="s">
+      <c r="D91" s="74" t="s">
         <v>727</v>
       </c>
     </row>
@@ -10192,7 +10194,7 @@
       <c r="A92" s="72" t="s">
         <v>880</v>
       </c>
-      <c r="D92" s="85" t="s">
+      <c r="D92" s="74" t="s">
         <v>570</v>
       </c>
     </row>
@@ -10200,7 +10202,7 @@
       <c r="A93" s="72" t="s">
         <v>881</v>
       </c>
-      <c r="D93" s="85" t="s">
+      <c r="D93" s="74" t="s">
         <v>573</v>
       </c>
     </row>
@@ -10208,65 +10210,75 @@
       <c r="A94" s="72" t="s">
         <v>881</v>
       </c>
-      <c r="D94" s="85" t="s">
+      <c r="D94" s="74" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="D96" s="85" t="s">
+      <c r="D96" s="74" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="97" spans="4:4" ht="52" x14ac:dyDescent="0.35">
-      <c r="D97" s="85" t="s">
+      <c r="D97" s="74" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D98" s="85"/>
+      <c r="D98" s="74"/>
     </row>
     <row r="99" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D99" s="85"/>
+      <c r="D99" s="74"/>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D101" s="85"/>
+      <c r="D101" s="74"/>
     </row>
     <row r="102" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D102" s="85"/>
+      <c r="D102" s="74"/>
     </row>
     <row r="103" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D103" s="85"/>
+      <c r="D103" s="74"/>
     </row>
     <row r="104" spans="4:4" ht="39" x14ac:dyDescent="0.35">
-      <c r="D104" s="85" t="s">
+      <c r="D104" s="74" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="106" spans="4:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="D106" s="85" t="s">
+      <c r="D106" s="74" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="107" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D107" s="85" t="s">
+      <c r="D107" s="74" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="108" spans="4:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="D108" s="85" t="s">
+      <c r="D108" s="74" t="s">
         <v>865</v>
       </c>
     </row>
     <row r="109" spans="4:4" ht="78" x14ac:dyDescent="0.35">
-      <c r="D109" s="85" t="s">
+      <c r="D109" s="74" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D110" s="85"/>
+      <c r="D110" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B36:B41"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="B67:B77"/>
@@ -10283,16 +10295,6 @@
     <mergeCell ref="E9:E15"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B20:B28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11724,7 +11726,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="82" t="s">
         <v>186</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -11733,28 +11735,28 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="73"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="21" t="s">
         <v>188</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="73"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="21" t="s">
         <v>189</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C6" s="73"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="4" t="s">
         <v>190</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C7" s="73"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="4" t="s">
         <v>191</v>
       </c>
@@ -11808,7 +11810,7 @@
       <c r="E14"/>
     </row>
     <row r="15" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="83" t="s">
         <v>198</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -11819,37 +11821,37 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="C16" s="74"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="4" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17" s="74"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="4" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C18" s="74"/>
+      <c r="C18" s="83"/>
       <c r="D18" s="4" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C19" s="74"/>
+      <c r="C19" s="83"/>
       <c r="D19" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C20" s="74"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="C21" s="74"/>
+      <c r="C21" s="83"/>
       <c r="D21" s="1" t="s">
         <v>206</v>
       </c>

</xml_diff>